<commit_message>
Ditto (only chapter title)
</commit_message>
<xml_diff>
--- a/win11_en.xlsx
+++ b/win11_en.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpsuzuki\Documents\2022_03\fresta2022\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE086A3D-DB4C-4F28-811A-13D4F72CE1B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D87FFB22-2781-490A-A225-0269834D6CA9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="15468" windowHeight="6384" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="15468" windowHeight="6384" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -50,9 +50,6 @@
     <t>description</t>
   </si>
   <si>
-    <t>Know your PC's spec</t>
-  </si>
-  <si>
     <t>win10-1-01.svg</t>
   </si>
   <si>
@@ -442,10 +439,6 @@
   </si>
   <si>
     <t>win10-4-10e.svg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Initial setting of your PC</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1313,6 +1306,14 @@
   </si>
   <si>
     <t>win11en-winhello.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Initial setting of your PC (you can execute this chapter before getting your student ID.)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Know your PC's spec (you can do this chapter before getting student ID.)</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1735,7 +1736,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1743,7 +1744,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -1751,7 +1752,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -1765,7 +1766,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -1783,10 +1784,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF0FC8B8-3740-45D4-A5FA-75052BCDA48C}">
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B40" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D47" sqref="D47"/>
+    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.2"/>
@@ -1803,7 +1804,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1811,7 +1812,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>106</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1819,7 +1820,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1827,7 +1828,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="6" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1847,7 +1848,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s" ph="1">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C7" t="s" ph="1">
         <v>4</v>
@@ -1861,13 +1862,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s" ph="1">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
@@ -1875,13 +1876,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s" ph="1">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C9" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
@@ -1889,21 +1890,21 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s" ph="1">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>185</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s" ph="1">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C11" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>186</v>
+        <v>184</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="48.6" customHeight="1" ph="1" x14ac:dyDescent="0.2">
@@ -1911,24 +1912,24 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s" ph="1">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C12" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s" ph="1">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C13" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>188</v>
+        <v>186</v>
       </c>
     </row>
     <row r="14" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1936,13 +1937,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s" ph="1">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C14" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>189</v>
+        <v>187</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
@@ -1950,13 +1951,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s" ph="1">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C15" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>190</v>
+        <v>188</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
@@ -1964,13 +1965,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s" ph="1">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C16" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="17" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1979,7 +1980,7 @@
         <v>5</v>
       </c>
       <c r="D17" t="s" ph="1">
-        <v>192</v>
+        <v>190</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="120" customHeight="1" ph="1" x14ac:dyDescent="0.2">
@@ -1987,13 +1988,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s" ph="1">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C18" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>193</v>
+        <v>191</v>
       </c>
     </row>
     <row r="19" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -2001,24 +2002,24 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s" ph="1">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C19" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D19" t="s" ph="1">
-        <v>194</v>
+        <v>192</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s" ph="1">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C20" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="61.2" ph="1" x14ac:dyDescent="0.2">
@@ -2026,13 +2027,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s" ph="1">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C21" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>196</v>
+        <v>194</v>
       </c>
     </row>
     <row r="22" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -2040,13 +2041,13 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s" ph="1">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C22" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>197</v>
+        <v>195</v>
       </c>
     </row>
     <row r="23" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -2054,281 +2055,278 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s" ph="1">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C23" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>198</v>
+        <v>196</v>
       </c>
     </row>
     <row r="24" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s" ph="1">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C24" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s" ph="1">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C25" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="26" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s" ph="1">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C26" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D26" t="s" ph="1">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="27" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s" ph="1">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C27" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D27" t="s" ph="1">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s" ph="1">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C28" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D28" t="s" ph="1">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s" ph="1">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C29" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D29" t="s" ph="1">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="61.2" ph="1" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s" ph="1">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C30" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D30" t="s" ph="1">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="31" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s" ph="1">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C31" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D31" t="s" ph="1">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="81.599999999999994" ph="1" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s" ph="1">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C32" t="s" ph="1">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D32" t="s" ph="1">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="33" spans="2:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C33" t="s" ph="1">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D33" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="34" spans="2:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="C34" t="s" ph="1">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D34" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C35" t="s" ph="1">
+        <v>235</v>
+      </c>
+      <c r="D35" t="s">
         <v>236</v>
-      </c>
-      <c r="C35" t="s" ph="1">
-        <v>237</v>
-      </c>
-      <c r="D35" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s" ph="1">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C36" t="s" ph="1">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D36" t="s" ph="1">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s" ph="1">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C37" t="s" ph="1">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D37" t="s" ph="1">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s" ph="1">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="C38" t="s" ph="1">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D38" t="s" ph="1">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="39" spans="2:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s" ph="1">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="C39" t="s" ph="1">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D39" t="s" ph="1">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="40" spans="2:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s" ph="1">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="C40" t="s" ph="1">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D40" t="s" ph="1">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="41" spans="2:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s" ph="1">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="C41" t="s" ph="1">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D41" t="s" ph="1">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="42" spans="2:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s" ph="1">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="C42" t="s" ph="1">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D42" t="s" ph="1">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="43" spans="2:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s" ph="1">
+        <v>255</v>
+      </c>
+      <c r="C43" t="s" ph="1">
+        <v>256</v>
+      </c>
+      <c r="D43" t="s" ph="1">
         <v>257</v>
-      </c>
-      <c r="C43" t="s" ph="1">
-        <v>258</v>
-      </c>
-      <c r="D43" t="s" ph="1">
-        <v>259</v>
       </c>
     </row>
     <row r="44" spans="2:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="C44" t="s" ph="1">
+        <v>256</v>
+      </c>
+      <c r="D44" t="s" ph="1">
         <v>258</v>
-      </c>
-      <c r="D44" t="s" ph="1">
-        <v>260</v>
       </c>
     </row>
     <row r="45" spans="2:4" ht="61.2" ph="1" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s" ph="1">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C45" t="s" ph="1">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D45" t="s" ph="1">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="46" spans="2:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s" ph="1">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C46" t="s" ph="1">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D46" t="s" ph="1">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="47" spans="2:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s" ph="1">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C47" t="s" ph="1">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D47" t="s" ph="1">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="48" spans="2:4" customFormat="1" ht="13.2" x14ac:dyDescent="0.2">
-      <c r="B48" s="1"/>
+        <v>264</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -2341,8 +2339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -2358,7 +2356,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2366,7 +2364,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>7</v>
+        <v>266</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2374,7 +2372,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2382,7 +2380,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -2390,7 +2388,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -2404,13 +2402,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="184.8" x14ac:dyDescent="0.2">
@@ -2418,13 +2416,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -2432,13 +2430,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
         <v>10</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="145.19999999999999" x14ac:dyDescent="0.2">
@@ -2446,13 +2444,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -2483,7 +2481,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2491,7 +2489,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2499,7 +2497,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2507,12 +2505,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -2520,13 +2518,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="145.19999999999999" x14ac:dyDescent="0.2">
@@ -2534,13 +2532,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -2548,13 +2546,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
         <v>21</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -2562,13 +2560,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -2576,13 +2574,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" t="s">
         <v>24</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -2590,13 +2588,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
         <v>26</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -2604,21 +2602,21 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>31</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -2632,13 +2630,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" t="s">
         <v>5</v>
       </c>
       <c r="D15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -2668,7 +2666,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2676,7 +2674,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2684,7 +2682,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2692,7 +2690,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -2700,7 +2698,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -2711,7 +2709,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -2719,13 +2717,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" t="s">
         <v>36</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -2733,13 +2731,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
         <v>38</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -2747,13 +2745,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
         <v>40</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -2761,13 +2759,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -2775,18 +2773,18 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" t="s">
         <v>42</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -2794,13 +2792,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -2808,13 +2806,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
         <v>45</v>
-      </c>
-      <c r="C15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -2822,13 +2820,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -2836,13 +2834,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
         <v>48</v>
-      </c>
-      <c r="C17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -2850,13 +2848,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -2864,13 +2862,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -2901,7 +2899,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2909,7 +2907,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2917,7 +2915,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2925,7 +2923,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
@@ -2933,7 +2931,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -2944,7 +2942,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="158.4" x14ac:dyDescent="0.2">
@@ -2952,18 +2950,18 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -2971,37 +2969,37 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D11" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D12" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D13" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -3009,13 +3007,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -3023,18 +3021,18 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" t="s">
         <v>16</v>
-      </c>
-      <c r="C15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D15" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -3042,21 +3040,21 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C17" t="s">
         <v>4</v>
       </c>
       <c r="D17" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D18" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -3064,13 +3062,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -3078,13 +3076,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C20" t="s">
         <v>4</v>
       </c>
       <c r="D20" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -3092,13 +3090,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -3106,13 +3104,13 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
       <c r="D22" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -3120,13 +3118,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -3157,7 +3155,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3165,7 +3163,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3173,7 +3171,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -3181,7 +3179,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="211.2" x14ac:dyDescent="0.2">
@@ -3189,7 +3187,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -3200,7 +3198,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -3222,13 +3220,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" t="s">
         <v>53</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -3236,18 +3234,18 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" t="s">
         <v>55</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -3269,13 +3267,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" t="s">
         <v>58</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -3283,13 +3281,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -3297,13 +3295,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -3311,13 +3309,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -3325,13 +3323,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" t="s">
         <v>60</v>
-      </c>
-      <c r="C17" t="s">
-        <v>4</v>
-      </c>
-      <c r="D17" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
@@ -3339,13 +3337,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -3353,13 +3351,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -3367,18 +3365,18 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" t="s">
         <v>64</v>
-      </c>
-      <c r="C20" t="s">
-        <v>4</v>
-      </c>
-      <c r="D20" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -3400,13 +3398,13 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
         <v>67</v>
-      </c>
-      <c r="C23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -3414,13 +3412,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
       </c>
       <c r="D24" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -3428,18 +3426,18 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+      <c r="D25" t="s">
         <v>70</v>
-      </c>
-      <c r="C25" t="s">
-        <v>4</v>
-      </c>
-      <c r="D25" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -3461,13 +3459,13 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -3475,13 +3473,13 @@
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" t="s">
+        <v>4</v>
+      </c>
+      <c r="D29" t="s">
         <v>73</v>
-      </c>
-      <c r="C29" t="s">
-        <v>4</v>
-      </c>
-      <c r="D29" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -3489,13 +3487,13 @@
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C30" t="s">
+        <v>4</v>
+      </c>
+      <c r="D30" t="s">
         <v>75</v>
-      </c>
-      <c r="C30" t="s">
-        <v>4</v>
-      </c>
-      <c r="D30" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -3503,13 +3501,13 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C31" t="s">
         <v>4</v>
       </c>
       <c r="D31" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -3517,13 +3515,13 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C32" t="s">
+        <v>4</v>
+      </c>
+      <c r="D32" t="s">
         <v>78</v>
-      </c>
-      <c r="C32" t="s">
-        <v>4</v>
-      </c>
-      <c r="D32" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="184.8" x14ac:dyDescent="0.2">
@@ -3531,13 +3529,13 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C33" t="s">
         <v>4</v>
       </c>
       <c r="D33" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -3545,13 +3543,13 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C34" t="s">
         <v>4</v>
       </c>
       <c r="D34" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -3559,13 +3557,13 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -3573,13 +3571,13 @@
         <v>4</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C36" t="s">
         <v>4</v>
       </c>
       <c r="D36" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -3587,26 +3585,26 @@
         <v>4</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C37" t="s">
         <v>4</v>
       </c>
       <c r="D37" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D38" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -3614,7 +3612,7 @@
         <v>4</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C40" t="s">
         <v>4</v>
@@ -3628,13 +3626,13 @@
         <v>4</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C41" t="s">
         <v>5</v>
       </c>
       <c r="D41" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
@@ -3642,21 +3640,21 @@
         <v>4</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C42" t="s">
         <v>5</v>
       </c>
       <c r="D42" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D43" t="s" ph="1">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -3664,13 +3662,13 @@
         <v>4</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C44" t="s">
         <v>5</v>
       </c>
       <c r="D44" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -3701,7 +3699,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3709,7 +3707,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3717,7 +3715,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -3725,7 +3723,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -3736,7 +3734,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="198" x14ac:dyDescent="0.2">
@@ -3744,7 +3742,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -3755,7 +3753,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
@@ -3763,7 +3761,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
Update the preface in win11_en.win11_en.xlsx
</commit_message>
<xml_diff>
--- a/win11_en.xlsx
+++ b/win11_en.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpsuzuki\Documents\2022_03\fresta2022\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D87FFB22-2781-490A-A225-0269834D6CA9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA9639A-0837-4820-917A-74F2C42C45B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="15468" windowHeight="6384" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="15468" windowHeight="6384" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -853,151 +853,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>PCの電源を初めて入れて、デスクトップ画面が表示されるまでの設定手順について説明します。
-一番重要なのは、Windows11の初期設定にはネット環境とMicrosoftアカウントが必要なことです。広島大学の学生は広島大学が管理するMicrosoftアカウントを持ちますが、そのMicrosoftアカウントで初期設定すると卒業後にそのPCが使えなくなってしまいます。
-そのため、広島大学と無関係なMicrosoftアカウントを一時的に作成して初期設定を開始し、さらにネット環境が無くても使えるアカウントに変更します。容量は小さくても良いのでUSBフラッシュメモリを用意しておきましょう。
-すでにデスクトップが表示されている方は、この章をスキップして次の「パソコンのスペック確認」へ進んでください。 Windows11はバージョン番号が同じでもバリエーションがあったり、出荷時期によって違いがあります。以下の手順の中で拒否しや設定しないで進めるとなっている項目がそもそも表示されないこともありますが、あわてないでください。</t>
-    <rPh sb="3" eb="5">
-      <t>デンゲン</t>
-    </rPh>
-    <rPh sb="19" eb="21">
-      <t>ガメン</t>
-    </rPh>
-    <rPh sb="22" eb="24">
-      <t>ヒョウジ</t>
-    </rPh>
-    <rPh sb="30" eb="32">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="32" eb="34">
-      <t>テジュン</t>
-    </rPh>
-    <rPh sb="38" eb="40">
-      <t>セツメイ</t>
-    </rPh>
-    <rPh sb="45" eb="47">
-      <t>イチバン</t>
-    </rPh>
-    <rPh sb="47" eb="49">
-      <t>ジュウヨウ</t>
-    </rPh>
-    <rPh sb="63" eb="65">
-      <t>ショキ</t>
-    </rPh>
-    <rPh sb="65" eb="67">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="72" eb="74">
-      <t>カンキョウ</t>
-    </rPh>
-    <rPh sb="90" eb="92">
-      <t>ヒツヨウ</t>
-    </rPh>
-    <rPh sb="98" eb="100">
-      <t>ヒロシマ</t>
-    </rPh>
-    <rPh sb="100" eb="102">
-      <t>ダイガク</t>
-    </rPh>
-    <rPh sb="103" eb="105">
-      <t>ガクセイ</t>
-    </rPh>
-    <rPh sb="106" eb="108">
-      <t>ヒロシマ</t>
-    </rPh>
-    <rPh sb="108" eb="110">
-      <t>ダイガク</t>
-    </rPh>
-    <rPh sb="111" eb="113">
-      <t>カンリ</t>
-    </rPh>
-    <rPh sb="130" eb="131">
-      <t>モ</t>
-    </rPh>
-    <rPh sb="153" eb="155">
-      <t>ショキ</t>
-    </rPh>
-    <rPh sb="155" eb="157">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="160" eb="163">
-      <t>ソツギョウゴ</t>
-    </rPh>
-    <rPh sb="169" eb="170">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="187" eb="189">
-      <t>ヒロシマ</t>
-    </rPh>
-    <rPh sb="189" eb="191">
-      <t>ダイガク</t>
-    </rPh>
-    <rPh sb="193" eb="196">
-      <t>ムカンケイ</t>
-    </rPh>
-    <rPh sb="211" eb="214">
-      <t>イチジテキ</t>
-    </rPh>
-    <rPh sb="215" eb="217">
-      <t>サクセイ</t>
-    </rPh>
-    <rPh sb="220" eb="222">
-      <t>ショキ</t>
-    </rPh>
-    <rPh sb="222" eb="224">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="225" eb="227">
-      <t>カイシ</t>
-    </rPh>
-    <rPh sb="235" eb="237">
-      <t>カンキョウ</t>
-    </rPh>
-    <rPh sb="238" eb="239">
-      <t>ナ</t>
-    </rPh>
-    <rPh sb="242" eb="243">
-      <t>ツカ</t>
-    </rPh>
-    <rPh sb="251" eb="253">
-      <t>ヘンコウ</t>
-    </rPh>
-    <rPh sb="257" eb="259">
-      <t>ヨウリョウ</t>
-    </rPh>
-    <rPh sb="260" eb="261">
-      <t>チイ</t>
-    </rPh>
-    <rPh sb="265" eb="266">
-      <t>ヨ</t>
-    </rPh>
-    <rPh sb="281" eb="283">
-      <t>ヨウイ</t>
-    </rPh>
-    <rPh sb="362" eb="364">
-      <t>バンゴウ</t>
-    </rPh>
-    <rPh sb="365" eb="366">
-      <t>オナ</t>
-    </rPh>
-    <rPh sb="390" eb="391">
-      <t>チガ</t>
-    </rPh>
-    <rPh sb="410" eb="412">
-      <t>セッテイ</t>
-    </rPh>
-    <rPh sb="416" eb="417">
-      <t>スス</t>
-    </rPh>
-    <rPh sb="425" eb="427">
-      <t>コウモク</t>
-    </rPh>
-    <rPh sb="432" eb="434">
-      <t>ヒョウジ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>chartn</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1314,6 +1169,13 @@
   </si>
   <si>
     <t>Know your PC's spec (you can do this chapter before getting student ID.)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>In this chapter, the initialization procedure of your computer after the first power-on.
+The most important feature of Windows11 is the requirement of the Internet connectivity, and the requirement of a "Microsoft account". The students of Hirosima University would have a Microsoft account registered for Hiroshima University. But you should not use it for the initialization of your computer. Because when you graduate Hiroshima University, the account would be removed soon, and you would be disabled to use the Microsoft account provided by Hiroshima University, and you would loose the access of your computer. To avoid such trouble, you should obtain a Microsoft account for the initialization which is independent from Hiroshima University.
+In this chapter, you would create a new Microsoft account, and create another local account which is independent from Microsoft. The procedures in the chapter 1 and later should be operated by the local account.
+If you already have the desktop environment, you can skip this chapter and proceed to the chapter 1.</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1744,7 +1606,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -1752,7 +1614,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -1786,8 +1648,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF0FC8B8-3740-45D4-A5FA-75052BCDA48C}">
   <dimension ref="A1:D47"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="B4" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.2"/>
@@ -1812,7 +1674,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1828,7 +1690,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1843,12 +1705,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="183.6" ph="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="204" ph="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s" ph="1">
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s" ph="1">
-        <v>180</v>
+        <v>266</v>
       </c>
       <c r="C7" t="s" ph="1">
         <v>4</v>
@@ -1862,13 +1724,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s" ph="1">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D8" t="s" ph="1">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
@@ -1876,13 +1738,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s" ph="1">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C9" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
@@ -1890,21 +1752,21 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s" ph="1">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="11" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s" ph="1">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C11" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="48.6" customHeight="1" ph="1" x14ac:dyDescent="0.2">
@@ -1912,24 +1774,24 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s" ph="1">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C12" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s" ph="1">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C13" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="14" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1937,13 +1799,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s" ph="1">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C14" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
@@ -1951,13 +1813,13 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s" ph="1">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C15" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
@@ -1965,13 +1827,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s" ph="1">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C16" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="17" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1980,7 +1842,7 @@
         <v>5</v>
       </c>
       <c r="D17" t="s" ph="1">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="120" customHeight="1" ph="1" x14ac:dyDescent="0.2">
@@ -1988,13 +1850,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s" ph="1">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C18" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="19" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -2002,24 +1864,24 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s" ph="1">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C19" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D19" t="s" ph="1">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s" ph="1">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C20" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="61.2" ph="1" x14ac:dyDescent="0.2">
@@ -2027,13 +1889,13 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s" ph="1">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C21" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="22" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -2041,13 +1903,13 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s" ph="1">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C22" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="23" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -2055,277 +1917,277 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s" ph="1">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C23" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="24" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s" ph="1">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C24" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D24" t="s" ph="1">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s" ph="1">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C25" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="26" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s" ph="1">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C26" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D26" t="s" ph="1">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="27" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s" ph="1">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C27" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D27" t="s" ph="1">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s" ph="1">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C28" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D28" t="s" ph="1">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s" ph="1">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C29" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D29" t="s" ph="1">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="61.2" ph="1" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s" ph="1">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C30" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D30" t="s" ph="1">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="31" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s" ph="1">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C31" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D31" t="s" ph="1">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="81.599999999999994" ph="1" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s" ph="1">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C32" t="s" ph="1">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D32" t="s" ph="1">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="33" spans="2:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C33" t="s" ph="1">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D33" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="34" spans="2:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C34" t="s" ph="1">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D34" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="C35" t="s" ph="1">
         <v>234</v>
       </c>
-      <c r="C35" t="s" ph="1">
+      <c r="D35" t="s">
         <v>235</v>
-      </c>
-      <c r="D35" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s" ph="1">
+        <v>236</v>
+      </c>
+      <c r="C36" t="s" ph="1">
+        <v>234</v>
+      </c>
+      <c r="D36" t="s" ph="1">
         <v>237</v>
-      </c>
-      <c r="C36" t="s" ph="1">
-        <v>235</v>
-      </c>
-      <c r="D36" t="s" ph="1">
-        <v>238</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s" ph="1">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C37" t="s" ph="1">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D37" t="s" ph="1">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s" ph="1">
+        <v>240</v>
+      </c>
+      <c r="C38" t="s" ph="1">
+        <v>234</v>
+      </c>
+      <c r="D38" t="s" ph="1">
         <v>241</v>
-      </c>
-      <c r="C38" t="s" ph="1">
-        <v>235</v>
-      </c>
-      <c r="D38" t="s" ph="1">
-        <v>242</v>
       </c>
     </row>
     <row r="39" spans="2:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s" ph="1">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C39" t="s" ph="1">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D39" t="s" ph="1">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="40" spans="2:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s" ph="1">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C40" t="s" ph="1">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D40" t="s" ph="1">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="41" spans="2:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s" ph="1">
+        <v>246</v>
+      </c>
+      <c r="C41" t="s" ph="1">
+        <v>234</v>
+      </c>
+      <c r="D41" t="s" ph="1">
         <v>247</v>
-      </c>
-      <c r="C41" t="s" ph="1">
-        <v>235</v>
-      </c>
-      <c r="D41" t="s" ph="1">
-        <v>248</v>
       </c>
     </row>
     <row r="42" spans="2:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s" ph="1">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C42" t="s" ph="1">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D42" t="s" ph="1">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="43" spans="2:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s" ph="1">
+        <v>254</v>
+      </c>
+      <c r="C43" t="s" ph="1">
         <v>255</v>
       </c>
-      <c r="C43" t="s" ph="1">
+      <c r="D43" t="s" ph="1">
         <v>256</v>
-      </c>
-      <c r="D43" t="s" ph="1">
-        <v>257</v>
       </c>
     </row>
     <row r="44" spans="2:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C44" t="s" ph="1">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D44" t="s" ph="1">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="45" spans="2:4" ht="61.2" ph="1" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s" ph="1">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C45" t="s" ph="1">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D45" t="s" ph="1">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="46" spans="2:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s" ph="1">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C46" t="s" ph="1">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D46" t="s" ph="1">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="47" spans="2:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s" ph="1">
+        <v>262</v>
+      </c>
+      <c r="C47" t="s" ph="1">
+        <v>255</v>
+      </c>
+      <c r="D47" t="s" ph="1">
         <v>263</v>
-      </c>
-      <c r="C47" t="s" ph="1">
-        <v>256</v>
-      </c>
-      <c r="D47" t="s" ph="1">
-        <v>264</v>
       </c>
     </row>
   </sheetData>
@@ -2339,7 +2201,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -2364,7 +2226,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
English procedure to check a local administrator account.
</commit_message>
<xml_diff>
--- a/win11_en.xlsx
+++ b/win11_en.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mpsuzuki\Documents\2022_03\fresta2022\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8043D34-233E-4B07-803D-29BD52DF5F06}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17F9DA84-79E4-4F30-B371-E3986B04A692}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="15468" windowHeight="6384" tabRatio="729" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="15468" windowHeight="6384" tabRatio="729" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
     <sheet name="ch0" sheetId="9" r:id="rId2"/>
-    <sheet name="ch1" sheetId="3" r:id="rId3"/>
-    <sheet name="ch2" sheetId="6" r:id="rId4"/>
-    <sheet name="ch3" sheetId="4" r:id="rId5"/>
+    <sheet name="ch1" sheetId="4" r:id="rId3"/>
+    <sheet name="ch2" sheetId="3" r:id="rId4"/>
+    <sheet name="ch3" sheetId="6" r:id="rId5"/>
     <sheet name="ch4" sheetId="11" r:id="rId6"/>
     <sheet name="ch5" sheetId="7" r:id="rId7"/>
     <sheet name="ch6" sheetId="12" r:id="rId8"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="235">
   <si>
     <t>header1</t>
   </si>
@@ -493,10 +493,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>FRESTA-TEXT-2021 Win11en chap.1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>FRESTA-TEXT-2021 Win11en chap.7</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -509,9 +505,6 @@
   </si>
   <si>
     <t>win11en-gear.png</t>
-  </si>
-  <si>
-    <t>win11en-setting-system.png</t>
   </si>
   <si>
     <t>win11en-account-others-add.png</t>
@@ -708,14 +701,6 @@
   </si>
   <si>
     <t>Please search "google chrome download", and install it.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Login to Moodle and set multifactor authentication.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Login to Moodle and set multifactor authentication (student ID is needed)</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -937,6 +922,34 @@
   </si>
   <si>
     <t>fresta_en</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FRESTA-TEXT-2021 Win11 chap.5</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11en-account-type-check2.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11en-account-type-check.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FRESTA-TEXT-2022 Win11 chap.1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Creating a local account for the lectures</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>In this chapter, you would create a local account for the lectures. If you are using a local account already, and it is an administrator, you can skip this chapter. Please confirm the type of your current account in following procedure.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Your current account information is displayed at the top of the right side. If your current account is a local account and an administrator, you can jump to the next chapter.</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1442,7 +1455,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -1494,7 +1507,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58E70A2B-96AA-4C94-9421-5C006AEAF8E2}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -1509,7 +1522,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -1525,7 +1538,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1567,8 +1580,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF0FC8B8-3740-45D4-A5FA-75052BCDA48C}">
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46:D46"/>
+    <sheetView topLeftCell="A28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30:D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.2"/>
@@ -1637,7 +1650,7 @@
         <v>5</v>
       </c>
       <c r="D7" t="s" ph="1">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="61.2" ph="1" x14ac:dyDescent="0.2">
@@ -1679,7 +1692,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s" ph="1">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C11" t="s" ph="1">
         <v>5</v>
@@ -1732,7 +1745,7 @@
     </row>
     <row r="15" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s" ph="1">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C15" t="s" ph="1">
         <v>5</v>
@@ -1921,172 +1934,52 @@
         <v>64</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="C31" t="s" ph="1">
-        <v>42</v>
-      </c>
-      <c r="D31" t="s" ph="1">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
-      <c r="B32" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C32" t="s" ph="1">
-        <v>42</v>
-      </c>
-      <c r="D32" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="33" spans="2:4" ht="39.6" ph="1" x14ac:dyDescent="0.2">
-      <c r="B33" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="C33" t="s" ph="1">
-        <v>91</v>
-      </c>
-      <c r="D33" t="s" ph="1">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="34" spans="2:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="1" t="s" ph="1">
-        <v>92</v>
-      </c>
-      <c r="C34" t="s" ph="1">
-        <v>91</v>
-      </c>
-      <c r="D34" t="s" ph="1">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="35" spans="2:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
-      <c r="B35" s="1" t="s" ph="1">
-        <v>93</v>
-      </c>
-      <c r="C35" t="s" ph="1">
-        <v>91</v>
-      </c>
-      <c r="D35" t="s" ph="1">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="36" spans="2:4" ht="61.2" ph="1" x14ac:dyDescent="0.2">
-      <c r="B36" s="1" t="s" ph="1">
-        <v>94</v>
-      </c>
-      <c r="C36" t="s" ph="1">
-        <v>91</v>
-      </c>
-      <c r="D36" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="37" spans="2:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
-      <c r="B37" s="1" t="s" ph="1">
-        <v>96</v>
-      </c>
-      <c r="C37" t="s" ph="1">
-        <v>91</v>
-      </c>
-      <c r="D37" t="s" ph="1">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="38" spans="2:4" ph="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="1" t="s" ph="1">
-        <v>97</v>
-      </c>
-      <c r="C38" t="s" ph="1">
-        <v>91</v>
-      </c>
-      <c r="D38" t="s" ph="1">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="39" spans="2:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
-      <c r="B39" s="1" t="s" ph="1">
-        <v>98</v>
-      </c>
-      <c r="C39" t="s" ph="1">
-        <v>91</v>
-      </c>
-      <c r="D39" t="s" ph="1">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="40" spans="2:4" ph="1" x14ac:dyDescent="0.2">
-      <c r="B40" s="1" t="s" ph="1">
-        <v>100</v>
-      </c>
-      <c r="C40" t="s" ph="1">
-        <v>91</v>
-      </c>
-      <c r="D40" t="s" ph="1">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="41" spans="2:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
-      <c r="B41" s="1" t="s" ph="1">
-        <v>104</v>
-      </c>
-      <c r="C41" t="s" ph="1">
-        <v>105</v>
-      </c>
-      <c r="D41" t="s" ph="1">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="42" spans="2:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
-      <c r="B42" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="C42" t="s" ph="1">
-        <v>105</v>
-      </c>
-      <c r="D42" t="s" ph="1">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="43" spans="2:4" ht="81.599999999999994" ph="1" x14ac:dyDescent="0.2">
-      <c r="B43" s="1" t="s" ph="1">
-        <v>108</v>
-      </c>
-      <c r="C43" t="s" ph="1">
-        <v>105</v>
-      </c>
-      <c r="D43" t="s" ph="1">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="44" spans="2:4" ht="26.4" ph="1" x14ac:dyDescent="0.2">
-      <c r="B44" s="1" t="s">
-        <v>142</v>
-      </c>
-      <c r="C44" t="s" ph="1">
-        <v>105</v>
-      </c>
-      <c r="D44" t="s" ph="1">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="45" spans="2:4" ht="61.2" ph="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="1" t="s" ph="1">
-        <v>143</v>
-      </c>
-      <c r="C45" t="s" ph="1">
-        <v>105</v>
-      </c>
-      <c r="D45" t="s" ph="1">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="46" spans="2:4" ph="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" customFormat="1" ht="13.2" x14ac:dyDescent="0.2">
+      <c r="B31" s="1"/>
+    </row>
+    <row r="32" spans="1:4" customFormat="1" ht="13.2" x14ac:dyDescent="0.2">
+      <c r="B32" s="1"/>
+    </row>
+    <row r="33" spans="2:2" customFormat="1" ht="13.2" x14ac:dyDescent="0.2">
+      <c r="B33" s="1"/>
+    </row>
+    <row r="34" spans="2:2" customFormat="1" ht="13.2" x14ac:dyDescent="0.2">
+      <c r="B34" s="1"/>
+    </row>
+    <row r="35" spans="2:2" customFormat="1" ht="13.2" x14ac:dyDescent="0.2">
+      <c r="B35" s="1"/>
+    </row>
+    <row r="36" spans="2:2" customFormat="1" ht="13.2" x14ac:dyDescent="0.2">
+      <c r="B36" s="1"/>
+    </row>
+    <row r="37" spans="2:2" customFormat="1" ht="13.2" x14ac:dyDescent="0.2">
+      <c r="B37" s="1"/>
+    </row>
+    <row r="38" spans="2:2" customFormat="1" ht="13.2" x14ac:dyDescent="0.2">
+      <c r="B38" s="1"/>
+    </row>
+    <row r="39" spans="2:2" customFormat="1" ht="13.2" x14ac:dyDescent="0.2">
+      <c r="B39" s="1"/>
+    </row>
+    <row r="40" spans="2:2" customFormat="1" ht="13.2" x14ac:dyDescent="0.2">
+      <c r="B40" s="1"/>
+    </row>
+    <row r="41" spans="2:2" customFormat="1" ht="13.2" x14ac:dyDescent="0.2">
+      <c r="B41" s="1"/>
+    </row>
+    <row r="42" spans="2:2" customFormat="1" ht="13.2" x14ac:dyDescent="0.2">
+      <c r="B42" s="1"/>
+    </row>
+    <row r="43" spans="2:2" customFormat="1" ht="13.2" x14ac:dyDescent="0.2">
+      <c r="B43" s="1"/>
+    </row>
+    <row r="44" spans="2:2" customFormat="1" ht="13.2" x14ac:dyDescent="0.2">
+      <c r="B44" s="1"/>
+    </row>
+    <row r="45" spans="2:2" customFormat="1" ht="13.2" x14ac:dyDescent="0.2">
+      <c r="B45" s="1"/>
+    </row>
+    <row r="46" spans="2:2" ph="1" x14ac:dyDescent="0.2">
       <c r="B46" s="1" ph="1"/>
     </row>
   </sheetData>
@@ -2097,11 +1990,290 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:D40"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="66.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="34" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="A1" t="s" ph="1">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="A2" t="s" ph="1">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="A3" t="s" ph="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="A4" t="s" ph="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="A5" ph="1"/>
+    </row>
+    <row r="6" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="A6" ph="1"/>
+      <c r="B6" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="102" x14ac:dyDescent="0.2">
+      <c r="A7" ph="1"/>
+      <c r="B7" s="1" t="s" ph="1">
+        <v>102</v>
+      </c>
+      <c r="C7" t="s" ph="1">
+        <v>42</v>
+      </c>
+      <c r="D7" t="s" ph="1">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C8" t="s" ph="1">
+        <v>42</v>
+      </c>
+      <c r="D8" t="s" ph="1">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C9" t="s" ph="1">
+        <v>42</v>
+      </c>
+      <c r="D9" t="s" ph="1">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
+      <c r="B10" s="1"/>
+    </row>
+    <row r="11" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C11" t="s" ph="1">
+        <v>42</v>
+      </c>
+      <c r="D11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" t="s" ph="1">
+        <v>91</v>
+      </c>
+      <c r="D12" t="s" ph="1">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" customFormat="1" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s" ph="1">
+        <v>92</v>
+      </c>
+      <c r="C13" t="s" ph="1">
+        <v>91</v>
+      </c>
+      <c r="D13" t="s" ph="1">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" customFormat="1" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s" ph="1">
+        <v>93</v>
+      </c>
+      <c r="C14" t="s" ph="1">
+        <v>91</v>
+      </c>
+      <c r="D14" t="s" ph="1">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" customFormat="1" ht="61.2" ph="1" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s" ph="1">
+        <v>94</v>
+      </c>
+      <c r="C15" t="s" ph="1">
+        <v>91</v>
+      </c>
+      <c r="D15" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" customFormat="1" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s" ph="1">
+        <v>96</v>
+      </c>
+      <c r="C16" t="s" ph="1">
+        <v>91</v>
+      </c>
+      <c r="D16" t="s" ph="1">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s" ph="1">
+        <v>97</v>
+      </c>
+      <c r="C17" t="s" ph="1">
+        <v>91</v>
+      </c>
+      <c r="D17" t="s" ph="1">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" customFormat="1" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s" ph="1">
+        <v>98</v>
+      </c>
+      <c r="C18" t="s" ph="1">
+        <v>91</v>
+      </c>
+      <c r="D18" t="s" ph="1">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s" ph="1">
+        <v>100</v>
+      </c>
+      <c r="C19" t="s" ph="1">
+        <v>91</v>
+      </c>
+      <c r="D19" t="s" ph="1">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" customFormat="1" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s" ph="1">
+        <v>104</v>
+      </c>
+      <c r="C20" t="s" ph="1">
+        <v>105</v>
+      </c>
+      <c r="D20" t="s" ph="1">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="C21" t="s" ph="1">
+        <v>105</v>
+      </c>
+      <c r="D21" t="s" ph="1">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="22" spans="2:4" customFormat="1" ht="81.599999999999994" ph="1" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s" ph="1">
+        <v>108</v>
+      </c>
+      <c r="C22" t="s" ph="1">
+        <v>105</v>
+      </c>
+      <c r="D22" t="s" ph="1">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="23" spans="2:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C23" t="s" ph="1">
+        <v>105</v>
+      </c>
+      <c r="D23" t="s" ph="1">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" customFormat="1" ht="61.2" ph="1" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s" ph="1">
+        <v>141</v>
+      </c>
+      <c r="C24" t="s" ph="1">
+        <v>105</v>
+      </c>
+      <c r="D24" t="s" ph="1">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>4</v>
+      </c>
+      <c r="C36" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>4</v>
+      </c>
+      <c r="C38" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>4</v>
+      </c>
+      <c r="C40" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:D15"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -2141,7 +2313,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
@@ -2163,21 +2335,21 @@
         <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
       </c>
       <c r="D7" s="4" t="s" ph="1">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D8" s="4" t="s" ph="1">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="237.6" x14ac:dyDescent="0.2">
@@ -2191,7 +2363,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="4" t="s" ph="1">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
@@ -2220,12 +2392,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -2265,7 +2437,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
@@ -2292,13 +2464,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -2306,13 +2478,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -2328,21 +2500,21 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -2350,13 +2522,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -2364,13 +2536,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -2378,10 +2550,10 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -2396,172 +2568,6 @@
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="66.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B9" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="D9" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>171</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B11" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D11" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D12" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B13" s="1" t="s">
-        <v>174</v>
-      </c>
-      <c r="D13" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2577,13 +2583,13 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="100.6640625" customWidth="1"/>
+    <col min="2" max="2" width="66.5546875" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" customWidth="1"/>
     <col min="4" max="4" width="20.6640625" style="4" customWidth="1"/>
   </cols>
@@ -2593,24 +2599,27 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>175</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="D1"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>176</v>
-      </c>
+        <v>8</v>
+      </c>
+      <c r="D2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>231</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="D3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
@@ -2619,82 +2628,90 @@
       <c r="B4" s="1" t="s">
         <v>112</v>
       </c>
+      <c r="D4"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" s="1"/>
-    </row>
-    <row r="6" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="D5"/>
+    </row>
+    <row r="6" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="1"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7"/>
+    </row>
+    <row r="8" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>167</v>
+      </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>5</v>
+      </c>
+      <c r="D8" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>178</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+        <v>168</v>
+      </c>
+      <c r="D9" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="171.6" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
+      <c r="D10" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B12" s="1"/>
+        <v>170</v>
+      </c>
+      <c r="D11" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="D12" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="1"/>
-      <c r="C13" t="s">
-        <v>4</v>
+      <c r="B13" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D13" t="s">
+        <v>165</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -2705,15 +2722,10 @@
       <c r="C14" t="s">
         <v>4</v>
       </c>
+      <c r="D14"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>4</v>
-      </c>
       <c r="B15" s="1"/>
-      <c r="C15" t="s">
-        <v>4</v>
-      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -2724,10 +2736,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -2743,7 +2755,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2751,7 +2763,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2759,7 +2771,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2767,119 +2779,113 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>208</v>
+        <v>173</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
       </c>
-      <c r="D6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="D7" t="s">
-        <v>183</v>
-      </c>
+      <c r="D6" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D7" s="4"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="1" t="s">
-        <v>201</v>
-      </c>
-      <c r="D8" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>202</v>
-      </c>
-      <c r="D9" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>174</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>203</v>
-      </c>
-      <c r="D10" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>175</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="171.6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="D11" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>205</v>
-      </c>
-      <c r="D12" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B13" s="1" t="s">
-        <v>206</v>
+      <c r="C13" t="s">
+        <v>4</v>
       </c>
       <c r="D13" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
+        <v>196</v>
       </c>
       <c r="D14" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>4</v>
       </c>
-      <c r="C15" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D15" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>209</v>
+        <v>198</v>
+      </c>
+      <c r="D16" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -2887,13 +2893,10 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="C17" t="s">
-        <v>4</v>
+        <v>199</v>
       </c>
       <c r="D17" t="s">
-        <v>4</v>
+        <v>182</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -2901,68 +2904,64 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="D18" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>211</v>
-      </c>
-      <c r="C19" t="s">
-        <v>4</v>
+      <c r="B19" s="1" t="s">
+        <v>201</v>
       </c>
       <c r="D19" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B20" s="3" t="s">
-        <v>212</v>
+        <v>184</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>202</v>
       </c>
       <c r="D20" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>18</v>
+        <v>186</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>4</v>
       </c>
-      <c r="B22" s="1" t="s">
-        <v>214</v>
-      </c>
       <c r="C22" t="s">
         <v>4</v>
       </c>
-      <c r="D22" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="C24" t="s">
         <v>4</v>
@@ -2976,32 +2975,32 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="D25" t="s">
-        <v>20</v>
+        <v>178</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>4</v>
       </c>
-      <c r="B26" s="1" t="s">
-        <v>217</v>
+      <c r="B26" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
       </c>
       <c r="D26" t="s">
-        <v>21</v>
+        <v>187</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>4</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>219</v>
+      <c r="B27" s="3" t="s">
+        <v>208</v>
       </c>
       <c r="D27" t="s">
-        <v>181</v>
+        <v>130</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -3009,43 +3008,118 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>220</v>
+        <v>209</v>
+      </c>
+      <c r="C28" t="s">
+        <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>221</v>
+        <v>210</v>
+      </c>
+      <c r="C29" t="s">
+        <v>4</v>
       </c>
       <c r="D29" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>4</v>
+        <v>19</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="D32" ph="1"/>
+      <c r="B31" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="C31" t="s">
+        <v>4</v>
+      </c>
+      <c r="D31" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D32" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="D48" ph="1"/>
+      <c r="B33" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D33" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D34" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>4</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="D35" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>4</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D36" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="D39" ph="1"/>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="4:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="D55" ph="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -3075,7 +3149,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3083,7 +3157,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3091,7 +3165,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -3099,7 +3173,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -3110,7 +3184,7 @@
     </row>
     <row r="7" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -3118,21 +3192,21 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="D9" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -3140,13 +3214,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -3154,13 +3228,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -3168,13 +3242,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -3228,7 +3302,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -3269,13 +3343,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C9" t="s">
         <v>4</v>
       </c>
       <c r="D9" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -3283,13 +3357,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -3297,13 +3371,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
win11en: change chapter num
</commit_message>
<xml_diff>
--- a/win11_en.xlsx
+++ b/win11_en.xlsx
@@ -1,35 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20395"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20407"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{723A1DD0-19A7-474F-9864-209DC48183B4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{43EB432D-C892-455D-B241-1F97B0DAFD7D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6708" yWindow="-15096" windowWidth="21600" windowHeight="11592" tabRatio="729" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6708" yWindow="-15096" windowWidth="8652" windowHeight="11592" tabRatio="729" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
     <sheet name="ch0" sheetId="9" r:id="rId2"/>
-    <sheet name="ch1" sheetId="4" r:id="rId3"/>
-    <sheet name="ch2" sheetId="3" r:id="rId4"/>
-    <sheet name="ch3" sheetId="6" r:id="rId5"/>
-    <sheet name="ch4" sheetId="11" r:id="rId6"/>
-    <sheet name="ch5" sheetId="7" r:id="rId7"/>
-    <sheet name="ch6" sheetId="12" r:id="rId8"/>
-    <sheet name="ch7" sheetId="5" r:id="rId9"/>
-    <sheet name="ch8" sheetId="8" r:id="rId10"/>
+    <sheet name="ch1" sheetId="3" r:id="rId3"/>
+    <sheet name="ch2" sheetId="6" r:id="rId4"/>
+    <sheet name="ch3" sheetId="11" r:id="rId5"/>
+    <sheet name="ch4" sheetId="7" r:id="rId6"/>
+    <sheet name="ch5" sheetId="12" r:id="rId7"/>
+    <sheet name="ch6" sheetId="5" r:id="rId8"/>
+    <sheet name="ch7" sheetId="8" r:id="rId9"/>
+    <sheet name="ch8" sheetId="13" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="469" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="255">
   <si>
     <t>header1</t>
   </si>
@@ -79,17 +79,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">Here, you will set up Windows Update which keeps your Wndows10 and Office updated. 
-Furthermore, you will learn how to use Microsoft Defender&amp;apos;s full scan.
-&lt;ul&gt;&lt;li&gt;&lt;a href="#windows_update"&gt;Set up Windows Update &lt;/a&gt;
-&lt;/li&gt;
-&lt;li&gt;&lt;a href="#defender"&gt;Microsoft Defender -manual update and a full scan-&lt;/a&gt;
-&lt;/li&gt;
- &lt;/ul&gt;
- </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve">You are going to prepare your PC for your study life at Hiroshima University during this lecture. Here is the list of what you are going to do at this workshop.
 &lt;ol&gt; &lt;/ol&gt;
 * Some screenshots in this text are displayed in Japanese. Sorry for inconvenience. </t>
@@ -105,16 +94,6 @@
   </si>
   <si>
     <t>fresta_en</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">First of all, you will learn how to know your PC&amp;apos;s &amp;quot;spec&amp;quot;. Sometimes the word &amp;quot;spec&amp;quot; indicates some features which tell you the capability of your PC. Here, find these specs in the list below;
-&lt;ol&gt;&lt;li&gt; OS version &lt;/li&gt;
-&lt;li&gt; Main memory capacity &lt;/li&gt;
-&lt;li&gt; HDD/SSD capacity &lt;/li&gt;
-&lt;li&gt; Battery run time &lt;/li&gt;
-&lt;/ol&gt;
- </t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -205,9 +184,6 @@
     <t>win11en-desktop.png</t>
   </si>
   <si>
-    <t>win11en-setting-account.png</t>
-  </si>
-  <si>
     <t>For first, choose the regional culture which your computer is configured for.</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -264,10 +240,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>You would be asked to configure the identification by your face. You can skipt it for now.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Please set the "PIN" code to login your computer.</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -288,72 +260,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Please click "Add account" button on "Other users". If you add a family member, you would be asked to configure parental setting, it is not independent from the current "Microsoft account".</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>chartn</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>You would be asked for the method for the new account to sign in. Please choose "I don't have this person's sign-in information".</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>You would be asked for an email account for the new account. Please choose "Add a new account without a Microsoft account".</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>You would be asked to set the new account name, new password (2 times), and 3 secret questions. It is recommended to set the new account name by alphabets, digits, hyphen "-", plus "+" and underscore "_".</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11en-local-account-listed.png</t>
-  </si>
-  <si>
-    <t>You would find the new account is listed in "Other users". Please expand the list for this new local account.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Please click "Change account type" in the expanded list.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>You would receive a dialogue to choose the account type. Please choose the "Administrator" type for future maintenance, and push "OK".</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11en-change-account-type-adm.png</t>
-  </si>
-  <si>
-    <t>You would find that the new account is now typed as an Administrator for this computer.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>In the right side of the window to "Accounts" pane. Then, please click "Family &amp; other users" in the right side list.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Once the preparation is finished, you receive vanilla desktop environment with single "launcher" like window. This window is corresponding to the "start menu" in older Windows system. You can open this window by clicking the "window" button on the task bar at the lowest part of the window. Please click the "gear" icon to start the "Settings" application.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Please open the "start menu" window again, and choose the "Sign out" menu from the lower left "human icon" button.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>chartn</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>You would see the default login panel of Windows11. Please click somewhere on the background.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11en-login-panel-multi-account.png</t>
-  </si>
-  <si>
-    <t>You would find the list of the available account of this computer. Please choose the account which you have just created. Please remember that new local account was configured without PIN code. Thus, if you've asked "PIN" instead of "password", it would be the Microsoft account.</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -372,10 +279,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>FRESTA-TEXT-2021 Win11en chap.2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>FRESTA-TEXT-2021 Win11en chap.7</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -386,37 +289,6 @@
     <t>win11en-gear.png</t>
   </si>
   <si>
-    <t>win11en-account-others-add.png</t>
-  </si>
-  <si>
-    <t>win11en-new-account-signin-info.png</t>
-  </si>
-  <si>
-    <t>win11en-new-account-create.png</t>
-  </si>
-  <si>
-    <t>win11en-local-account-setting.png</t>
-  </si>
-  <si>
-    <t>win11en-local-account-type-menu.png</t>
-  </si>
-  <si>
-    <t>win11en-local-account-type.png</t>
-  </si>
-  <si>
-    <t>win11en-sign-out-button.png</t>
-  </si>
-  <si>
-    <t>win11en-login-panel.png</t>
-  </si>
-  <si>
-    <t>win11en-login-local-account.png</t>
-  </si>
-  <si>
-    <t>FRESTA-TEXT-2021 Win11en chap.8</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>moodle-login.png</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -441,14 +313,6 @@
   </si>
   <si>
     <t>You would be asked about the default backup throught the network (designed for the computer owned by the organization). Please choose "Set up for personal use".</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Please change the account which you have just created, the password would be asked because you have not set your PIN code for this local account.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>You would be asked the privacy settings again. You can disable them again. Depending with the version of your Windows11, you would be asked about "Windows Hello" for your face recognition. You can skip it again.</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -490,10 +354,6 @@
     <t>win11en-scan-progress.png</t>
   </si>
   <si>
-    <t>Please click start button and open "Setting" application. Then click "Windows Update" in the left list, and click "Check for update" button.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Please click "Virus &amp; threat protection". Should not touch with "Set up OneDrive" button.</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -548,14 +408,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Please search "google chrome download", and install it.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>FRESTA-TEXT-2021 Win11 chap.6</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>win11en-momiji-before-login0.png</t>
   </si>
   <si>
@@ -641,34 +493,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11en-account-type-check2.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11en-account-type-check.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Creating a local account for the lectures</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>In this chapter, you would create a local account for the lectures. If you are using a local account already, and it is an administrator, you can skip this chapter. Please confirm the type of your current account in following procedure.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Your current account information is displayed at the top of the right side. If your current account is a local account and an administrator, you can jump to the next chapter.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Once the preparation is finished, you receive vanilla desktop environment with single "launcher" like window. This window is corresponding to the "start menu" in older Windows system. You can open this window by clicking the "window" button on the task bar at the lowest part of the desktop. </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Please click the "gear" icon to start the "Settings" application. On the left side list of the "Settings" application window, you can find "Accounts" menu. Please select it.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>If your PC does not have preinstalled Office365, you can download it from your Office365 web page.</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -708,17 +532,6 @@
   </si>
   <si>
     <t>mymomiji-1stlogin-en.png</t>
-  </si>
-  <si>
-    <t>win11en-check-storage-size.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">Next, Check HDD/SDD capacity of your PC. Read and write speed of HDD, Hard Disk Drive, or SSD, Solid State Drive are not as fast as those of RAM. But their capacity is larger than that of RAM. And they can keep data after shutting down your PC.
-Click the File Explorer icon in the taskbar. Then click &amp;quot;This PC&amp;quot; in the left side of the window, 
-HDD/SSD capacity will be displayed with the label &amp;quot;Local Disk (C:)&amp;quot;.
-  </t>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>In the first login to MyMOMIJI, you would be asked about the permission to use your statistic info gathered in Momiji, Hirodai moodle, etc by Hiroshima University (you don't have to permit). For detail, please refer the FAQ linked in the page.</t>
@@ -776,15 +589,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">Please install Google Chrome on your PC.
-&lt;ul&gt;
-&lt;li&gt;&lt;a href="#chrome"&gt;Install Google Chrome&lt;/a&gt;
-&lt;/li&gt;
- &lt;/ul&gt;
- </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Set up Windows Update so that your Windows11 will keep updated. And set up anti-virus software, Microsoft Defender, to be updated automatically.</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -939,31 +743,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>FRESTA-TEXT-2023 Win11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;h3&gt;Windows11&lt;/h3&gt;
-Mar. 2023&lt;br&gt;
- Information Media Center, Hiroshima University&lt;br&gt;
- Hiroshima Univesity Coop shop 
- </t>
-  </si>
-  <si>
-    <t>FRESTA-TEXT-2023 Win11 chap.0</t>
-  </si>
-  <si>
-    <t>FRESTA-TEXT-2023 Win11 chap.1</t>
-  </si>
-  <si>
-    <t>FRESTA-TEXT-2023 Win11en chap.3</t>
-  </si>
-  <si>
-    <t>FRESTA-TEXT-2023 Win11en chap.4</t>
-  </si>
-  <si>
-    <t>FRESTA-TEXT-2023 Win11 chap.5</t>
-  </si>
-  <si>
     <t>You can connect to Wi-Fi called &amp;quot;HINET Wi-Fi&amp;quot; in shared facilities in Hiroshima University campus. Here you will set up your PC to connect to the internal network and the internet via Wi-Fi. As far as you connect to the same access point, you do not need to do this again.</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -979,10 +758,6 @@
 &lt;/span&gt;
 &amp;quot;Installed RAM&amp;quot; entry tells you the capacity of the main memory in your PC. The larger the size of RAM your PC have, the more data your PC can store or the greater multi-tasking ability your PC gets.
   </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>After the installation of the available update, click "Advanced options", and enable "Receive updates for other Microsoft products". Please check additional updates by "Chek for update" button.&lt;span class="check"&gt;check-4&lt;/span&gt;</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1044,12 +819,251 @@
     <t>The size of "OneDrive" for Hiroshima University students is 3TB. Please backup your important files here. It is also useful to share it with your teacher, classmates, etc in the university.</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>FRESTA-TEXT-2024 Win11</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;h3&gt;Windows11&lt;/h3&gt;
+Mar. 2024&lt;br&gt;
+ Information Media Center, Hiroshima University&lt;br&gt;
+ Hiroshima Univesity Coop shop 
+ </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FRESTA-TEXT-2024 Win11 chap.0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>You would be asked to solve a quiz to prove you are human</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>chartn</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11en-msaccoutn-quiz.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>You might be asked to configrue the identification by your fingerprint. You can skip it.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>You might be asked to configure the identification by your face. You can skip it for now.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11en-msaccount-fingerprint.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FRESTA-TEXT-2024 Win11en chap.1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Check the storage size of your PC. Click "System" menu on the left side menus, and select "Storage" in the "System" submenu on the right side.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">win11en-setting-storage-menu.png </t>
+  </si>
+  <si>
+    <t>The storage size of your system partition, and used / free sizes are displayed.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">win11en-setting-storage-detail.png </t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;strong&gt;This chapter should be operated under offline environment (without network connection)&lt;/strong&gt;, to avoid unexpected linkage of your personal files to your MS account. Because the non-charged MS account has a limitation of 5GB data size, your computer will soon fill it up. You must prevent the unexpected linkage.
+First of all, you will learn how to know your PC&amp;apos;s &amp;quot;spec&amp;quot;. Sometimes the word &amp;quot;spec&amp;quot; indicates some features which tell you the capability of your PC. Here, find these specs in the list below;
+&lt;ol&gt;&lt;li&gt; OS version &lt;/li&gt;
+&lt;li&gt; Main memory capacity &lt;/li&gt;
+&lt;li&gt; HDD/SSD capacity &lt;/li&gt;
+&lt;li&gt; Battery run time &lt;/li&gt;
+&lt;/ol&gt;
+ </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Before proceed to the next chapter, you should stop the OneDrive application. Please refer &lt;a href="ch8.html"&gt;Chapter 8&lt;/a&gt; for detailed instruction.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Please click start button and open "Setting" application. Select "System" menu in the left list, and proceed to "Activation".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11en-winlic-active-stat1.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;strong&gt;The operation in this chapter requires the network connection.&lt;/strong&gt;
+Here, you will set up Windows Update which keeps your Wndows10 and Office updated. 
+Furthermore, you will learn how to use Microsoft Defender&amp;apos;s full scan.
+&lt;ul&gt;&lt;li&gt;&lt;a href="#windows_update"&gt;Set up Windows Update &lt;/a&gt;
+&lt;/li&gt;
+&lt;li&gt;&lt;a href="#defender"&gt;Microsoft Defender -manual update and a full scan-&lt;/a&gt;
+&lt;/li&gt;
+ &lt;/ul&gt;
+ </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FRESTA-TEXT-2024 Win11en chap.2</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>If your Windows is "activated", you can use Windows Update properly.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11en-winlic-active-done.png</t>
+  </si>
+  <si>
+    <t>In the case that "Can't connect" is displayed, reconnect your PC to the network, reboot and wait a while. If it does not resolved, try to follow the instruction (e.g. activation by phone).</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11en-winlic-active-notyet.png</t>
+  </si>
+  <si>
+    <t>Please click start button and open "Setting" application. Then click "Advanced options", and enable "Receive updates for other Microsoft products". Please check additional updates by "Chek for update" button (①). After checking it, back to the main menu of Windows Update (②)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Click "Check for updates" button. The installations would be queued automatically &lt;span class="check"&gt;check-4&lt;/span&gt; The update of the Microsoft Defender virus database is done during this &lt;span class="check"&gt;check-5&lt;/span&gt;.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Open "Setting" application, and proceed to "Privacy &amp; Security". Then search "Device Encryption" menu in the right side.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>If you PC was originally sold with Window10 Home and somebody upgraded it to Windows 11 (in the other word, no preinstalled Windows11), there would be a case that there is no "Device Encryption". In such case, Windows cannot enable BitLocker, you can proceed to the next chapter safely.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">win11en-setting-bitlocker-able.png </t>
+  </si>
+  <si>
+    <t xml:space="preserve">win11en-setting-bitlocker-unable.png </t>
+  </si>
+  <si>
+    <t>win11en-setting-bitlocker-enabled.png</t>
+  </si>
+  <si>
+    <t>Sometimes the toggle switch is ON, but there is a warning as "Sign in with your Microsoft account to finish encryption this device". It is often happened in the offline environment. If you're online but it happens, and you cannot resolve it after the connection to the internet, please change the toggle switch to OFF. Under the situation this warning displayed, following operation cannnot be executed properly</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">win11en-setting-bitlocker-incomplete.png </t>
+  </si>
+  <si>
+    <t>win11en-open-ctrlpanel.png</t>
+  </si>
+  <si>
+    <t>① Click "Start Button" on the task bar ② Type "control panel" to the search form ③ Open "Control Panel".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">win11en-ctrl-syssec-bitlocker-mgr.png </t>
+  </si>
+  <si>
+    <t>Windows11 Pro has "BitLocker Device Encryption", Windows11 Home may have "Device Encryption". Click the one your PC has.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Since Windows10, there is a builtin tool to encrypt the system storage, named "BitLocker". In some Windows Updates, the encryption system is silently activated, and you may lose the access to the data in your PC. You should keep the recovery key out of your PC. In this section, we present how to check the status of the encryption and how to brose it.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>If there is "Device Encryption", click it &amp; expand the menu. If "Device Encryption" toggle switch is ON, BitLocker is already enabled. You should preserve the recovery key as soon as possible. If it is OFF, no encryption key is set yet, but you must understand this toggle switch can be enabled unexpectedly, by Windows Update.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Proceed to "Print the recovery key".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Choose "Microsoft Print to PDF".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Save print output on the desktop with recognizable filename.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Yet your PC has no configured PDF browsing software, keep the result PDF as it is.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11en-printer-desktop.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11en-printer-select.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11en-bitlocker-backup-print.png</t>
+  </si>
+  <si>
+    <t>FRESTA-TEXT-2024 Win11en chap.3</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Please install Google Chrome on your PC.
+&lt;ul&gt;
+&lt;li&gt;&lt;a href="#config_edge"&gt;Configure Microsoft Edge&lt;/a&gt;&lt;/li&gt;
+&lt;li&gt;&lt;a href="#chrome"&gt;Install Google Chrome&lt;/a&gt;&lt;/li&gt;
+&lt;li&gt;&lt;a href="#bitlocker_pdf"&gt;Browse BitLocker Recovery Key PDF&lt;/a&gt;&lt;/li&gt;
+&lt;/ul&gt;
+ </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Follow the instruction on the site.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Search "google chrome download". You should be careful about the advertisements by Microsoft and non-Google redistributors, because redistributions often include malwares.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Now, when you double click the PDF file of the BitLocker recovery key, the default application for PDF can be selected. The default is MS Edge, but you can use Google Chrome too..</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">win11en-bitlockerpdf-dblclick.png </t>
+  </si>
+  <si>
+    <t xml:space="preserve">win11en-bitlockerpdf-content.pdf </t>
+  </si>
+  <si>
+    <t>Take photo for the displayed recovery key in your smartphone, to prevent the case that you would be requested it.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FRESTA-TEXT-2023 Win11 chap.4</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FRESTA-TEXT-2021 Win11 chap.5</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>FRESTA-TEXT-2021 Win11en chap.6</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1064,13 +1078,28 @@
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="ＭＳ Ｐゴシック"/>
+      <family val="3"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1085,7 +1114,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1097,6 +1126,16 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -1440,7 +1479,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -1464,7 +1503,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1472,7 +1511,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>230</v>
+        <v>198</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -1480,7 +1519,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>231</v>
+        <v>199</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -1494,7 +1533,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -1511,114 +1550,24 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:D11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87D4E1FF-6B8C-4FDC-839A-EEEE7C41D6DF}">
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B5" s="1" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>172</v>
-      </c>
-      <c r="D6" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="D7" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D8" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B9" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="D9" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B10" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="D10" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B11" s="1" t="s">
-        <v>178</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <sheetData/>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF0FC8B8-3740-45D4-A5FA-75052BCDA48C}">
-  <dimension ref="A1:D46"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView topLeftCell="A17" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="20.399999999999999" x14ac:dyDescent="0.2"/>
@@ -1635,7 +1584,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1643,7 +1592,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1651,7 +1600,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1659,7 +1608,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>232</v>
+        <v>200</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="285.60000000000002" ph="1" x14ac:dyDescent="0.2">
@@ -1667,7 +1616,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s" ph="1">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="C6" t="s" ph="1">
         <v>4</v>
@@ -1681,13 +1630,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s" ph="1">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D7" t="s" ph="1">
-        <v>88</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="61.2" ph="1" x14ac:dyDescent="0.2">
@@ -1695,7 +1644,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s" ph="1">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C8" t="s" ph="1">
         <v>5</v>
@@ -1707,21 +1656,21 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s" ph="1">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="D9" t="s" ph="1">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s" ph="1">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C10" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D10" t="s" ph="1">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="48.6" customHeight="1" ph="1" x14ac:dyDescent="0.2">
@@ -1729,13 +1678,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s" ph="1">
-        <v>249</v>
+        <v>194</v>
       </c>
       <c r="C11" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D11" t="s" ph="1">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
@@ -1743,13 +1692,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s" ph="1">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D12" t="s" ph="1">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
@@ -1757,13 +1706,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s" ph="1">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D13" t="s" ph="1">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="61.2" ph="1" x14ac:dyDescent="0.2">
@@ -1771,24 +1720,24 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s" ph="1">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C14" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D14" t="s" ph="1">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s" ph="1">
-        <v>107</v>
+        <v>75</v>
       </c>
       <c r="C15" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D15" t="s" ph="1">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="120" customHeight="1" ph="1" x14ac:dyDescent="0.2">
@@ -1796,13 +1745,13 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s" ph="1">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="C16" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D16" t="s" ph="1">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1810,24 +1759,24 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s" ph="1">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="C17" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D17" t="s" ph="1">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s" ph="1">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="C18" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D18" t="s" ph="1">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="81.599999999999994" ph="1" x14ac:dyDescent="0.2">
@@ -1835,13 +1784,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s" ph="1">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C19" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D19" t="s" ph="1">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
@@ -1849,13 +1798,13 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s" ph="1">
-        <v>250</v>
+        <v>195</v>
       </c>
       <c r="C20" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D20" t="s" ph="1">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1863,116 +1812,138 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s" ph="1">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="C21" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D21" t="s" ph="1">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s" ph="1">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="C22" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D22" t="s" ph="1">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="61.2" ph="1" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s" ph="1">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C23" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D23" t="s" ph="1">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:4" ph="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="1" t="s" ph="1">
-        <v>59</v>
-      </c>
-      <c r="C24" t="s" ph="1">
-        <v>5</v>
-      </c>
-      <c r="D24" t="s" ph="1">
-        <v>37</v>
+      <c r="B24" s="5" t="s" ph="1">
+        <v>201</v>
+      </c>
+      <c r="C24" s="6" t="s" ph="1">
+        <v>202</v>
+      </c>
+      <c r="D24" s="6" t="s" ph="1">
+        <v>203</v>
       </c>
     </row>
     <row r="25" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s" ph="1">
-        <v>60</v>
+        <v>205</v>
       </c>
       <c r="C25" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D25" t="s" ph="1">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="61.2" ph="1" x14ac:dyDescent="0.2">
-      <c r="B26" s="1" t="s" ph="1">
-        <v>61</v>
-      </c>
-      <c r="C26" t="s" ph="1">
-        <v>5</v>
-      </c>
-      <c r="D26" t="s" ph="1">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="7" t="s" ph="1">
+        <v>204</v>
+      </c>
+      <c r="C26" s="8" t="s" ph="1">
+        <v>202</v>
+      </c>
+      <c r="D26" s="8" t="s" ph="1">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s" ph="1">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="C27" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D27" t="s" ph="1">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="81.599999999999994" ph="1" x14ac:dyDescent="0.2">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="61.2" ph="1" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s" ph="1">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C28" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D28" t="s" ph="1">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" ph="1" x14ac:dyDescent="0.2">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s" ph="1">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="C29" t="s" ph="1">
         <v>5</v>
       </c>
       <c r="D29" t="s" ph="1">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" ht="102" ph="1" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="81.599999999999994" ph="1" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s" ph="1">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="C30" t="s" ph="1">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="D30" t="s" ph="1">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="2:2" ph="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="1" ph="1"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ph="1" x14ac:dyDescent="0.2">
+      <c r="B31" s="1" t="s" ph="1">
+        <v>60</v>
+      </c>
+      <c r="C31" t="s" ph="1">
+        <v>5</v>
+      </c>
+      <c r="D31" t="s" ph="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="102" ph="1" x14ac:dyDescent="0.2">
+      <c r="B32" s="1" t="s" ph="1">
+        <v>61</v>
+      </c>
+      <c r="C32" t="s" ph="1">
+        <v>19</v>
+      </c>
+      <c r="D32" t="s" ph="1">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2" ph="1" x14ac:dyDescent="0.2">
+      <c r="B48" s="1" ph="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -1982,290 +1953,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:D40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="66.5546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="34" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="A1" t="s" ph="1">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="A2" t="s" ph="1">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="A3" t="s" ph="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="A4" t="s" ph="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="A5" ph="1"/>
-    </row>
-    <row r="6" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
-      <c r="A6" ph="1"/>
-      <c r="B6" s="1" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="81.599999999999994" x14ac:dyDescent="0.2">
-      <c r="A7" ph="1"/>
-      <c r="B7" s="1" t="s" ph="1">
-        <v>168</v>
-      </c>
-      <c r="C7" t="s" ph="1">
-        <v>21</v>
-      </c>
-      <c r="D7" t="s" ph="1">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="C8" t="s" ph="1">
-        <v>21</v>
-      </c>
-      <c r="D8" t="s" ph="1">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="C9" t="s" ph="1">
-        <v>21</v>
-      </c>
-      <c r="D9" t="s" ph="1">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
-      <c r="B10" s="1"/>
-    </row>
-    <row r="11" spans="1:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
-      <c r="B11" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C11" t="s" ph="1">
-        <v>21</v>
-      </c>
-      <c r="D11" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" customFormat="1" ht="39.6" ph="1" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="C12" t="s" ph="1">
-        <v>66</v>
-      </c>
-      <c r="D12" t="s" ph="1">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" customFormat="1" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
-      <c r="B13" s="1" t="s" ph="1">
-        <v>67</v>
-      </c>
-      <c r="C13" t="s" ph="1">
-        <v>66</v>
-      </c>
-      <c r="D13" t="s" ph="1">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" customFormat="1" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
-      <c r="B14" s="1" t="s" ph="1">
-        <v>68</v>
-      </c>
-      <c r="C14" t="s" ph="1">
-        <v>66</v>
-      </c>
-      <c r="D14" t="s" ph="1">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" customFormat="1" ht="61.2" ph="1" x14ac:dyDescent="0.2">
-      <c r="B15" s="1" t="s" ph="1">
-        <v>69</v>
-      </c>
-      <c r="C15" t="s" ph="1">
-        <v>66</v>
-      </c>
-      <c r="D15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" customFormat="1" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
-      <c r="B16" s="1" t="s" ph="1">
-        <v>71</v>
-      </c>
-      <c r="C16" t="s" ph="1">
-        <v>66</v>
-      </c>
-      <c r="D16" t="s" ph="1">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" customFormat="1" ht="20.399999999999999" ph="1" x14ac:dyDescent="0.2">
-      <c r="B17" s="1" t="s" ph="1">
-        <v>72</v>
-      </c>
-      <c r="C17" t="s" ph="1">
-        <v>66</v>
-      </c>
-      <c r="D17" t="s" ph="1">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" customFormat="1" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
-      <c r="B18" s="1" t="s" ph="1">
-        <v>73</v>
-      </c>
-      <c r="C18" t="s" ph="1">
-        <v>66</v>
-      </c>
-      <c r="D18" t="s" ph="1">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="19" spans="2:4" customFormat="1" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
-      <c r="B19" s="1" t="s" ph="1">
-        <v>75</v>
-      </c>
-      <c r="C19" t="s" ph="1">
-        <v>66</v>
-      </c>
-      <c r="D19" t="s" ph="1">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" customFormat="1" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
-      <c r="B20" s="1" t="s" ph="1">
-        <v>78</v>
-      </c>
-      <c r="C20" t="s" ph="1">
-        <v>79</v>
-      </c>
-      <c r="D20" t="s" ph="1">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
-      <c r="B21" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C21" t="s" ph="1">
-        <v>79</v>
-      </c>
-      <c r="D21" t="s" ph="1">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="22" spans="2:4" customFormat="1" ht="81.599999999999994" ph="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="1" t="s" ph="1">
-        <v>82</v>
-      </c>
-      <c r="C22" t="s" ph="1">
-        <v>79</v>
-      </c>
-      <c r="D22" t="s" ph="1">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="23" spans="2:4" customFormat="1" ht="26.4" ph="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="1" t="s">
-        <v>108</v>
-      </c>
-      <c r="C23" t="s" ph="1">
-        <v>79</v>
-      </c>
-      <c r="D23" t="s" ph="1">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" customFormat="1" ht="61.2" ph="1" x14ac:dyDescent="0.2">
-      <c r="B24" s="1" t="s" ph="1">
-        <v>109</v>
-      </c>
-      <c r="C24" t="s" ph="1">
-        <v>79</v>
-      </c>
-      <c r="D24" t="s" ph="1">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>4</v>
-      </c>
-      <c r="C36" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>4</v>
-      </c>
-      <c r="C38" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>4</v>
-      </c>
-      <c r="C40" t="s">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D11"/>
-  <sheetViews>
-    <sheetView topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -2289,7 +1981,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2297,7 +1989,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2305,15 +1997,153 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>86</v>
+        <v>207</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="184.8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="97.2" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="4" t="s" ph="1">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D8" s="4" t="s" ph="1">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="237.6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" s="4" t="s" ph="1">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C10" t="s">
+        <v>202</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C11" t="s">
+        <v>202</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B12" s="3" t="s">
+        <v>213</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:D30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="89.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" style="4" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>217</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>19</v>
+      <c r="B6" s="1" t="s">
+        <v>216</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -2322,59 +2152,223 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="97.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="4" t="s" ph="1">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D8" s="4" t="s" ph="1">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="237.6" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="3" t="s">
+      <c r="D15" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B28" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B29" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="C9" t="s">
-        <v>5</v>
-      </c>
-      <c r="D9" s="4" t="s" ph="1">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>4</v>
+      <c r="D29" s="4" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B30" s="1" t="s">
+        <v>240</v>
       </c>
     </row>
   </sheetData>
@@ -2385,197 +2379,11 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:D18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D3AC582-7A6D-4EA0-8C12-75B8749BA9E2}">
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" style="4" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="105.6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B7" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="C9" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B12" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>4</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D3AC582-7A6D-4EA0-8C12-75B8749BA9E2}">
-  <dimension ref="A1:D15"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -2591,7 +2399,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>177</v>
+        <v>133</v>
       </c>
       <c r="D1"/>
     </row>
@@ -2609,7 +2417,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3"/>
     </row>
@@ -2618,7 +2426,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>235</v>
+        <v>244</v>
       </c>
       <c r="D4"/>
     </row>
@@ -2626,12 +2434,12 @@
       <c r="B5" s="1"/>
       <c r="D5"/>
     </row>
-    <row r="6" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>194</v>
+        <v>245</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -2651,21 +2459,21 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>132</v>
+        <v>97</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>126</v>
+        <v>91</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>133</v>
+        <v>98</v>
       </c>
       <c r="D9" t="s">
-        <v>127</v>
+        <v>92</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -2673,51 +2481,65 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>134</v>
+        <v>99</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>128</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>135</v>
+        <v>100</v>
       </c>
       <c r="D11" t="s">
-        <v>129</v>
+        <v>94</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>136</v>
+        <v>101</v>
       </c>
       <c r="D12" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D13" t="s">
-        <v>131</v>
+        <v>247</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>246</v>
+      </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
-      <c r="D14"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B15" s="1"/>
+      <c r="D14" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>250</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -2726,12 +2548,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView topLeftCell="A30" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B46" sqref="B46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -2747,7 +2569,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>244</v>
+        <v>189</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2755,7 +2577,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>150</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2763,7 +2585,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>162</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2771,7 +2593,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>236</v>
+        <v>252</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -2779,7 +2601,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>184</v>
+        <v>138</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -2793,7 +2615,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>245</v>
+        <v>190</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -2809,12 +2631,12 @@
     </row>
     <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>197</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>198</v>
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -2836,13 +2658,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>223</v>
+        <v>176</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>199</v>
+        <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -2850,15 +2672,15 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>224</v>
+        <v>177</v>
       </c>
       <c r="D13" t="s">
-        <v>139</v>
+        <v>102</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>200</v>
+        <v>153</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -2866,29 +2688,29 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>247</v>
+        <v>192</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>246</v>
+        <v>191</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>201</v>
+        <v>154</v>
       </c>
       <c r="D16" t="s">
-        <v>202</v>
+        <v>155</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>203</v>
+        <v>156</v>
       </c>
       <c r="D17" t="s">
-        <v>100</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -2896,13 +2718,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>204</v>
+        <v>157</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>101</v>
+        <v>69</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -2910,18 +2732,18 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>205</v>
+        <v>158</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>206</v>
+        <v>159</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>207</v>
+        <v>160</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -2929,21 +2751,21 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>208</v>
+        <v>161</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>209</v>
+        <v>162</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>210</v>
+        <v>163</v>
       </c>
       <c r="D22" t="s">
-        <v>211</v>
+        <v>164</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -2951,21 +2773,21 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>212</v>
+        <v>165</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
       </c>
       <c r="D23" t="s">
-        <v>213</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>214</v>
+        <v>167</v>
       </c>
       <c r="D24" t="s">
-        <v>215</v>
+        <v>168</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -2973,13 +2795,13 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>228</v>
+        <v>181</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>216</v>
+        <v>169</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -2990,7 +2812,7 @@
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>222</v>
+        <v>175</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
@@ -3004,13 +2826,13 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>218</v>
+        <v>171</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>217</v>
+        <v>170</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -3018,10 +2840,10 @@
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>219</v>
+        <v>172</v>
       </c>
       <c r="D29" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -3029,18 +2851,18 @@
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>220</v>
+        <v>173</v>
       </c>
       <c r="D30" t="s">
-        <v>140</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>152</v>
+        <v>115</v>
       </c>
       <c r="D31" t="s">
-        <v>141</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -3048,10 +2870,10 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>153</v>
+        <v>116</v>
       </c>
       <c r="D32" t="s">
-        <v>142</v>
+        <v>105</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -3059,18 +2881,18 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>193</v>
+        <v>147</v>
       </c>
       <c r="D33" t="s">
-        <v>143</v>
+        <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
-        <v>154</v>
+        <v>117</v>
       </c>
       <c r="D34" t="s">
-        <v>144</v>
+        <v>107</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -3078,13 +2900,13 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>252</v>
+        <v>197</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>145</v>
+        <v>108</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -3097,7 +2919,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
-        <v>221</v>
+        <v>174</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -3105,29 +2927,29 @@
         <v>4</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>225</v>
+        <v>178</v>
       </c>
       <c r="C38" t="s">
         <v>4</v>
       </c>
       <c r="D38" t="s">
-        <v>146</v>
+        <v>109</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B39" s="3" t="s">
-        <v>155</v>
+        <v>118</v>
       </c>
       <c r="D39" t="s">
-        <v>101</v>
+        <v>69</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B40" s="3" t="s">
-        <v>183</v>
+        <v>137</v>
       </c>
       <c r="D40" t="s">
-        <v>180</v>
+        <v>136</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -3135,13 +2957,13 @@
         <v>4</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>226</v>
+        <v>179</v>
       </c>
       <c r="C41" t="s">
         <v>4</v>
       </c>
       <c r="D41" t="s">
-        <v>227</v>
+        <v>180</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -3175,12 +2997,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45722500-6D63-48B1-B48D-DE8F55297416}">
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -3196,7 +3018,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>160</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3204,7 +3026,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>161</v>
+        <v>124</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3212,7 +3034,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>162</v>
+        <v>125</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -3220,7 +3042,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>138</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -3231,7 +3053,7 @@
     </row>
     <row r="7" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>196</v>
+        <v>149</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -3239,21 +3061,21 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>156</v>
+        <v>119</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
       </c>
       <c r="D8" t="s">
-        <v>102</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>157</v>
+        <v>120</v>
       </c>
       <c r="D9" t="s">
-        <v>103</v>
+        <v>71</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -3261,13 +3083,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>158</v>
+        <v>121</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>104</v>
+        <v>72</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -3275,13 +3097,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>159</v>
+        <v>122</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>105</v>
+        <v>73</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -3289,13 +3111,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>242</v>
+        <v>187</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>106</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -3304,12 +3126,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView topLeftCell="B9" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -3333,7 +3155,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>185</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3341,7 +3163,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -3349,17 +3171,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>87</v>
+        <v>254</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="171.6" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>190</v>
+        <v>144</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>189</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -3367,7 +3189,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>237</v>
+        <v>183</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -3384,7 +3206,7 @@
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>251</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -3392,13 +3214,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>248</v>
+        <v>193</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>147</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -3406,13 +3228,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>238</v>
+        <v>184</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>148</v>
+        <v>111</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -3420,49 +3242,152 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>243</v>
+        <v>188</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>149</v>
+        <v>112</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>191</v>
+        <v>145</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>187</v>
+        <v>141</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>186</v>
+        <v>140</v>
       </c>
       <c r="D16" t="s">
-        <v>100</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>188</v>
+        <v>142</v>
       </c>
       <c r="D17" t="s">
-        <v>229</v>
+        <v>182</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>192</v>
+        <v>146</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="198" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6640625" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D9" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D10" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
+        <v>134</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
win11en: remove empty chapter
</commit_message>
<xml_diff>
--- a/win11_en.xlsx
+++ b/win11_en.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{43EB432D-C892-455D-B241-1F97B0DAFD7D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B2A5D0-BA5D-42AD-AA43-BA50BAF25EFF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6708" yWindow="-15096" windowWidth="8652" windowHeight="11592" tabRatio="729" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6708" yWindow="-15096" windowWidth="8652" windowHeight="11592" tabRatio="729" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,6 @@
     <sheet name="ch5" sheetId="12" r:id="rId7"/>
     <sheet name="ch6" sheetId="5" r:id="rId8"/>
     <sheet name="ch7" sheetId="8" r:id="rId9"/>
-    <sheet name="ch8" sheetId="13" r:id="rId10"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
@@ -1549,19 +1548,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87D4E1FF-6B8C-4FDC-839A-EEEE7C41D6DF}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <phoneticPr fontId="1"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF0FC8B8-3740-45D4-A5FA-75052BCDA48C}">
   <dimension ref="A1:D48"/>
@@ -3298,7 +3284,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
win11en: add 3 images
</commit_message>
<xml_diff>
--- a/win11_en.xlsx
+++ b/win11_en.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92B2A5D0-BA5D-42AD-AA43-BA50BAF25EFF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8333F8D3-0857-40B2-805E-D88D3BDF17F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6708" yWindow="-15096" windowWidth="8652" windowHeight="11592" tabRatio="729" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6708" yWindow="-15096" windowWidth="8652" windowHeight="11592" tabRatio="729" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="259">
   <si>
     <t>header1</t>
   </si>
@@ -929,10 +929,6 @@
     <t>win11en-winlic-active-notyet.png</t>
   </si>
   <si>
-    <t>Please click start button and open "Setting" application. Then click "Advanced options", and enable "Receive updates for other Microsoft products". Please check additional updates by "Chek for update" button (①). After checking it, back to the main menu of Windows Update (②)</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Click "Check for updates" button. The installations would be queued automatically &lt;span class="check"&gt;check-4&lt;/span&gt; The update of the Microsoft Defender virus database is done during this &lt;span class="check"&gt;check-5&lt;/span&gt;.</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1055,6 +1051,25 @@
   </si>
   <si>
     <t>FRESTA-TEXT-2021 Win11en chap.6</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11en-winupdate-option1.png</t>
+  </si>
+  <si>
+    <t>Please check "Chek for update" button (①). After checking it, back to the main menu of Windows Update (②)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Please clik "Windows Update" (①), then move to "Advanced Options" (②)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Please toggle "Receive updates for other Microsoft products" to ON (①), then click "Windows Update" text to return to the previous menu.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11en-winupdate-option2.png</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -2078,10 +2093,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -2089,7 +2104,7 @@
     <col min="1" max="1" width="10.6640625" customWidth="1"/>
     <col min="2" max="2" width="89.77734375" style="1" customWidth="1"/>
     <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="32.109375" style="4" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -2167,62 +2182,56 @@
         <v>221</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="C11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>223</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
-      </c>
-      <c r="D12" s="4" t="s">
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="C14" t="s">
-        <v>4</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>82</v>
-      </c>
-    </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B15" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>83</v>
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -2230,27 +2239,21 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>4</v>
-      </c>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="C17" t="s">
-        <v>4</v>
+        <v>89</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -2258,103 +2261,131 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>4</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D20" s="4" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>4</v>
-      </c>
-      <c r="B20" s="1" t="s">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>4</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>4</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>224</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="B22" s="1" t="s">
-        <v>225</v>
-      </c>
-      <c r="D22" s="4" t="s">
+      <c r="D25" s="4" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
-      <c r="B23" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="D23" s="4" t="s">
+    <row r="26" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
-      <c r="B24" s="1" t="s">
+      <c r="D26" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="D24" s="4" t="s">
+    </row>
+    <row r="27" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="D27" s="4" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B25" s="1" t="s">
+    <row r="28" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="B28" s="1" t="s">
+        <v>233</v>
+      </c>
+      <c r="D28" s="4" t="s">
         <v>232</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="B26" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>233</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B27" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>243</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B28" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B31" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D31" s="4" t="s">
         <v>240</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B32" s="1" t="s">
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -2412,7 +2443,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D4"/>
     </row>
@@ -2425,7 +2456,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -2494,7 +2525,7 @@
     </row>
     <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -2502,7 +2533,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -2513,18 +2544,18 @@
     </row>
     <row r="15" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>248</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
   </sheetData>
@@ -2579,7 +2610,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -3028,7 +3059,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -3157,7 +3188,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="171.6" x14ac:dyDescent="0.2">
@@ -3284,7 +3315,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
win11en: update Windows Update
</commit_message>
<xml_diff>
--- a/win11_en.xlsx
+++ b/win11_en.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8333F8D3-0857-40B2-805E-D88D3BDF17F3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F226E96-A176-4DDD-A0C5-DE22EE06D197}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6708" yWindow="-15096" windowWidth="8652" windowHeight="11592" tabRatio="729" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -335,9 +335,6 @@
     <t>win11en-windows-update.png</t>
   </si>
   <si>
-    <t>win11en-windows-update-option.png</t>
-  </si>
-  <si>
     <t>win11en-setting-security.png</t>
   </si>
   <si>
@@ -929,10 +926,6 @@
     <t>win11en-winlic-active-notyet.png</t>
   </si>
   <si>
-    <t>Click "Check for updates" button. The installations would be queued automatically &lt;span class="check"&gt;check-4&lt;/span&gt; The update of the Microsoft Defender virus database is done during this &lt;span class="check"&gt;check-5&lt;/span&gt;.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Open "Setting" application, and proceed to "Privacy &amp; Security". Then search "Device Encryption" menu in the right side.</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1071,6 +1064,13 @@
   <si>
     <t>win11en-winupdate-option2.png</t>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Please click "Check for updates" button. The installations would be queued automatically &lt;span class="check"&gt;check-4&lt;/span&gt; The update of the Microsoft Defender virus database is done during this &lt;span class="check"&gt;check-5&lt;/span&gt;.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11en-update-start.png</t>
   </si>
 </sst>
 </file>
@@ -1525,7 +1525,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -1533,7 +1533,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -1609,7 +1609,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="285.60000000000002" ph="1" x14ac:dyDescent="0.2">
@@ -1679,7 +1679,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s" ph="1">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C11" t="s" ph="1">
         <v>5</v>
@@ -1799,7 +1799,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s" ph="1">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C20" t="s" ph="1">
         <v>5</v>
@@ -1846,18 +1846,18 @@
     </row>
     <row r="24" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B24" s="5" t="s" ph="1">
+        <v>200</v>
+      </c>
+      <c r="C24" s="6" t="s" ph="1">
         <v>201</v>
       </c>
-      <c r="C24" s="6" t="s" ph="1">
+      <c r="D24" s="6" t="s" ph="1">
         <v>202</v>
-      </c>
-      <c r="D24" s="6" t="s" ph="1">
-        <v>203</v>
       </c>
     </row>
     <row r="25" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s" ph="1">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C25" t="s" ph="1">
         <v>5</v>
@@ -1868,13 +1868,13 @@
     </row>
     <row r="26" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B26" s="7" t="s" ph="1">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C26" s="8" t="s" ph="1">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D26" s="8" t="s" ph="1">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="27" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -1998,7 +1998,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="184.8" x14ac:dyDescent="0.2">
@@ -2006,7 +2006,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -2042,7 +2042,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -2056,13 +2056,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C10" t="s">
+        <v>201</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>208</v>
-      </c>
-      <c r="C10" t="s">
-        <v>202</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -2070,18 +2070,18 @@
         <v>4</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C11" t="s">
+        <v>201</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>210</v>
-      </c>
-      <c r="C11" t="s">
-        <v>202</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -2096,7 +2096,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B7" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -2112,7 +2112,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2136,7 +2136,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
@@ -2144,7 +2144,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -2160,42 +2160,42 @@
     </row>
     <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>214</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>215</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>218</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D10" s="4" t="s">
         <v>220</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>221</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -2203,7 +2203,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
@@ -2217,13 +2217,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>222</v>
+        <v>257</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>81</v>
+        <v>258</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -2239,21 +2239,21 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C16" t="s">
         <v>4</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -2261,13 +2261,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -2275,13 +2275,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -2289,10 +2289,10 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -2305,7 +2305,7 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -2313,79 +2313,79 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D23" s="4" t="s">
         <v>223</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>224</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="D31" s="4" t="s">
         <v>238</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
   </sheetData>
@@ -2416,7 +2416,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D1"/>
     </row>
@@ -2443,7 +2443,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D4"/>
     </row>
@@ -2456,7 +2456,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -2476,21 +2476,21 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C8" t="s">
         <v>5</v>
       </c>
       <c r="D8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -2498,34 +2498,34 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D11" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -2533,29 +2533,29 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
       </c>
       <c r="D14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -2586,7 +2586,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2594,7 +2594,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2602,7 +2602,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -2610,7 +2610,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -2618,7 +2618,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -2632,7 +2632,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -2648,12 +2648,12 @@
     </row>
     <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -2675,13 +2675,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -2689,15 +2689,15 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -2705,26 +2705,26 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D16" t="s">
         <v>154</v>
-      </c>
-      <c r="D16" t="s">
-        <v>155</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D17" t="s">
         <v>68</v>
@@ -2735,7 +2735,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -2749,18 +2749,18 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" t="s">
         <v>158</v>
-      </c>
-      <c r="C19" t="s">
-        <v>4</v>
-      </c>
-      <c r="D19" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -2768,21 +2768,21 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" t="s">
         <v>161</v>
-      </c>
-      <c r="C21" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D22" t="s">
         <v>163</v>
-      </c>
-      <c r="D22" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -2790,21 +2790,21 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
         <v>165</v>
-      </c>
-      <c r="C23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="D24" t="s">
         <v>167</v>
-      </c>
-      <c r="D24" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -2812,13 +2812,13 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -2829,7 +2829,7 @@
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
@@ -2843,13 +2843,13 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -2857,10 +2857,10 @@
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D29" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -2868,18 +2868,18 @@
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -2887,10 +2887,10 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D32" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -2898,18 +2898,18 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D33" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D34" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -2917,13 +2917,13 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
       </c>
       <c r="D35" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -2936,7 +2936,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -2944,18 +2944,18 @@
         <v>4</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C38" t="s">
         <v>4</v>
       </c>
       <c r="D38" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B39" s="3" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D39" t="s">
         <v>69</v>
@@ -2963,10 +2963,10 @@
     </row>
     <row r="40" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B40" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D40" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -2974,13 +2974,13 @@
         <v>4</v>
       </c>
       <c r="B41" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C41" t="s">
+        <v>4</v>
+      </c>
+      <c r="D41" t="s">
         <v>179</v>
-      </c>
-      <c r="C41" t="s">
-        <v>4</v>
-      </c>
-      <c r="D41" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -3035,7 +3035,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3043,7 +3043,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3051,7 +3051,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -3059,7 +3059,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -3070,7 +3070,7 @@
     </row>
     <row r="7" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -3078,7 +3078,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -3089,7 +3089,7 @@
     </row>
     <row r="9" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D9" t="s">
         <v>71</v>
@@ -3100,7 +3100,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -3114,7 +3114,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -3128,7 +3128,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -3172,7 +3172,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3188,17 +3188,17 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="171.6" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -3206,7 +3206,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -3223,7 +3223,7 @@
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -3231,13 +3231,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
       </c>
       <c r="D10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -3245,13 +3245,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
       </c>
       <c r="D11" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -3259,28 +3259,28 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D16" t="s">
         <v>68</v>
@@ -3288,15 +3288,15 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D17" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="198" x14ac:dyDescent="0.2">
@@ -3332,7 +3332,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3353,7 +3353,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -3361,18 +3361,18 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="D7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -3380,31 +3380,31 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="D9" t="s">
         <v>129</v>
-      </c>
-      <c r="D9" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="D10" t="s">
         <v>131</v>
-      </c>
-      <c r="D10" t="s">
-        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
win11en: win11ja-xxx.png -> win11en-xxx.png
</commit_message>
<xml_diff>
--- a/win11_en.xlsx
+++ b/win11_en.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{506DC67B-C2B1-49DE-821A-8D19F7519BD9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48789808-EDC6-45A6-98E5-50BF10693A09}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6708" yWindow="-15096" windowWidth="8652" windowHeight="11592" tabRatio="729" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,9 +24,6 @@
     <sheet name="ch7" sheetId="8" r:id="rId9"/>
     <sheet name="ch8" sheetId="13" r:id="rId10"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId11"/>
-  </externalReferences>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
@@ -1074,18 +1071,6 @@
     <t>fresta</t>
   </si>
   <si>
-    <t>win11ja-onedrive-indicator.png</t>
-  </si>
-  <si>
-    <t>win11ja-odrv-app.png</t>
-  </si>
-  <si>
-    <t>win11ja-odrv22-noaccount.png</t>
-  </si>
-  <si>
-    <t>win11ja-odrv22-withaccount.png</t>
-  </si>
-  <si>
     <t>OneDriveの設定ウィンドウを開いて、「バックアップ」(①)タブを表示し、「バックアップを管理」(②)ボタンを押します。</t>
     <rPh sb="9" eb="11">
       <t>セッテイ</t>
@@ -1105,9 +1090,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11ja-odrv22-backup.png</t>
-  </si>
-  <si>
     <t>バックアップ対象のフォルダを選ぶウィンドウが表示されます。ここから全ての「バックアップを停止」を実行します。</t>
     <rPh sb="6" eb="8">
       <t>タイショウ</t>
@@ -1130,9 +1112,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11ja-odrv22-backup-mgr.png</t>
-  </si>
-  <si>
     <t>1つのフォルダの「バックアップを停止」をクリックするとこのような警告が出ますが、「バックアップを停止」で進めます。</t>
     <rPh sb="16" eb="18">
       <t>テイシ</t>
@@ -1152,9 +1131,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11ja-odrv22-backup-stopwarn1.png</t>
-  </si>
-  <si>
     <t>さらにこのようなメッセージが出ます。「閉じる」で進めます。</t>
     <rPh sb="14" eb="15">
       <t>デ</t>
@@ -1168,9 +1144,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11ja-odrv22-backup-stopwarn2.png</t>
-  </si>
-  <si>
     <t>全てのフォルダのバックアップを停止すると、改めてバックアップを開始する状態になっています。各フォルダアイコンの右上のチェックを外し、全てバックアップ対象から除外します。</t>
     <rPh sb="0" eb="1">
       <t>スベ</t>
@@ -1208,9 +1181,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11ja-odrv22-backup-select.png</t>
-  </si>
-  <si>
     <t>全てのフォルダのバックアップの予定を解除すると「バックアップの開始」はグレーアウトします。右上の「X」ボタンでこのウィンドウを閉じます。</t>
     <rPh sb="0" eb="1">
       <t>スベ</t>
@@ -1233,9 +1203,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11ja-odrv22-backup-unselect.png</t>
-  </si>
-  <si>
     <t>再び「アカウント」(①)タブを表示し、「このPCのリンク解除」(②)をクリックします。</t>
     <rPh sb="0" eb="1">
       <t>フタタ</t>
@@ -1249,9 +1216,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11ja-odrv22-unlink-pc.png</t>
-  </si>
-  <si>
     <t>設定ウィンドウが閉じ、サインインを促すウィンドウが開くので、右上の「X」ボタンで閉じます。</t>
     <rPh sb="0" eb="2">
       <t>セッテイ</t>
@@ -1274,9 +1238,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11ja-odrv-close-signin.png</t>
-  </si>
-  <si>
     <t>バックアップしていたフォルダ（この例では、デスクトップ、ドキュメント、ピクチャ）に「ファイルの場所」というショートカットが出来ています。これはOneDriveリンクは維持するがフォルダのバックアップはやめた、という状態の時にOneDriveストレージの同名のフォルダを探すためのリンクです。ここで説明する手順ではリンクも解除するため無効になりますので、削除して構いません。</t>
     <rPh sb="17" eb="18">
       <t>レイ</t>
@@ -1323,9 +1284,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11ja-link-to-original-folder.png</t>
-  </si>
-  <si>
     <t>&lt;h3 id="block_autostart_2022"&gt;自動起動の抑止&lt;/h3&gt;</t>
     <rPh sb="30" eb="32">
       <t>ジドウ</t>
@@ -1391,9 +1349,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11ja-odrv22-uncheck-autostart.png</t>
-  </si>
-  <si>
     <t>&lt;h3 id="link_2022"&gt;OneDriveへのIMCアカウントの追加&lt;/h3&gt;</t>
     <rPh sb="38" eb="40">
       <t>ツイカ</t>
@@ -1466,9 +1421,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11ja-setting-acct-odrv.png</t>
-  </si>
-  <si>
     <t>MSアカウントを入力するウィンドウが開きます。IMCアカウント(@hiroshima-u.ac.jpを付加すること)とパスワードでサインインします。「すべてのアプリにサインインしたままにする」で「OK」を押さないよう注意してください。</t>
     <rPh sb="8" eb="10">
       <t>ニュウリョク</t>
@@ -1504,9 +1456,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11ja-odrv-no-optional-data.png</t>
-  </si>
-  <si>
     <t>OneDriveフォルダーに「- Hiroshima University」がついていることを確認しましょう。</t>
     <rPh sb="47" eb="49">
       <t>カクニン</t>
@@ -1514,9 +1463,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11ja-imc-odrv-dirname.png</t>
-  </si>
-  <si>
     <t>バックアップ対象のフォルダを選ぶ画面になります。ここでは&lt;strong&gt;必ずデスクトップを除外してください&lt;/strong&gt;。さもないと貴方が普通に作るデータは全てOneDrive管理下となるため、同期の異常が起きたり、一部の授業で使うOneDrive管理下で動かないアプリを使うことができなくなります。</t>
     <rPh sb="6" eb="8">
       <t>タイショウ</t>
@@ -1551,9 +1497,6 @@
     <t>ドキュメントと写真は選択してもしなくても構いません。終わったら「続ける」で進めます。</t>
   </si>
   <si>
-    <t>win11ja-odrv22-exclude-desktop.png</t>
-  </si>
-  <si>
     <t>指示に沿ってすすめていくと準備が完了します。「OneDriveフォルダを開く」をクリックします。</t>
     <rPh sb="0" eb="2">
       <t>シジ</t>
@@ -1573,9 +1516,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11ja-odrv-backup-ready.png</t>
-  </si>
-  <si>
     <t>OneDriveフォルダに「デスクトップ」というフォルダができている場合があります。このデスクトップはOneDrive側にあるフォルダに単に「デスクトップ」という名前がつけてあるだけで、皆さんのPCのデスクトップのことを指している保証はありません。</t>
     <rPh sb="34" eb="36">
       <t>バアイ</t>
@@ -1601,9 +1541,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11ja-explorer-with-desktop.png</t>
-  </si>
-  <si>
     <t>エクスプローラの左サイドメニューの「ホーム」(①)をクリックし、クイックアクセスに出ているフォルダの状況を見てみましょう。少なくとも「デスクトップ」(②)には雲マークがついていないことを確認してください。ついていた場合は、&lt;a href="#unlink_2022"&gt;リンク解除&lt;/a&gt;の手順を実施してからあらためてリンク設定を試してください。</t>
     <rPh sb="8" eb="9">
       <t>ヒダリ</t>
@@ -1705,9 +1642,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11ja-odrv24-open-setting.png</t>
-  </si>
-  <si>
     <t>OneDrive設定のウィンドウが開きます。「アカウント」(①)メニューを確認します。「接続されているアカウントがありません」と表示された場合はOneDriveリンクされていませんが、ユーザの指示なしに自動的にリンクをはじめる場合があります。&lt;a href="#unlink_2024"&gt;解除手順&lt;/a&gt;の準備として確認している場合は、&lt;a href="#block_autostart_2024"&gt;自動起動の停止&lt;/a&gt;も実施してください。</t>
     <rPh sb="44" eb="46">
       <t>セツゾク</t>
@@ -1757,9 +1691,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11ja-odrv24-noaccount.png</t>
-  </si>
-  <si>
     <t>メールアドレスが表示されていればOneDriveリンク済みです。</t>
     <rPh sb="8" eb="10">
       <t>ヒョウジ</t>
@@ -1770,9 +1701,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11ja-odrv24-withaccount.png</t>
-  </si>
-  <si>
     <t>&lt;h3 id="unlink_2024"&gt;リンク解除&lt;/h3&gt;</t>
     <rPh sb="24" eb="26">
       <t>カイジョ</t>
@@ -1812,9 +1740,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11ja-odrv24-backup.png</t>
-  </si>
-  <si>
     <t>バックアップ対象のフォルダを選ぶウィンドウが表示されます。全てのトグルスイッチをオフにします。</t>
     <rPh sb="6" eb="8">
       <t>タイショウ</t>
@@ -1831,9 +1756,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11ja-odrv24-backup-mgr.png</t>
-  </si>
-  <si>
     <t>1つのトグルをオフにするとこのような警告が出ますが、「バックアップを停止」で進めます。</t>
     <rPh sb="18" eb="20">
       <t>ケイコク</t>
@@ -1850,9 +1772,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11ja-odrv24-unlink-warning.png</t>
-  </si>
-  <si>
     <t>全てのトグルスイッチをオフにし、「変更の保存」がグレーアウトしたら、「閉じる」でこのウィンドウを閉じます。</t>
     <rPh sb="0" eb="1">
       <t>スベ</t>
@@ -1872,9 +1791,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11ja-odrv24-backup-unselect.png</t>
-  </si>
-  <si>
     <t>再び「アカウント」(①)タブを表示し、「このPCからリンクを解除する」(②)をクリックします。</t>
     <rPh sb="0" eb="1">
       <t>フタタ</t>
@@ -1888,9 +1804,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11ja-odrv24-unlink-pc.png</t>
-  </si>
-  <si>
     <t>&lt;h3 id="block_autostart_2024"&gt;自動起動の抑止&lt;/h3&gt;</t>
     <rPh sb="30" eb="32">
       <t>ジドウ</t>
@@ -1953,9 +1866,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11ja-odrv24-uncheck-autostart.png</t>
-  </si>
-  <si>
     <t>&lt;h3 id="link_2024"&gt;OneDriveへのIMCアカウントの追加&lt;/h3&gt;</t>
     <rPh sb="38" eb="40">
       <t>ツイカ</t>
@@ -1963,12 +1873,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11ja-odrv24-dir-selector.png</t>
-  </si>
-  <si>
-    <t>win11ja-odrv24-exclude-desktop.png</t>
-  </si>
-  <si>
     <t>エクスプローラの左サイドメニューの「ホーム」(①)をクリックし、クイックアクセスに出ているフォルダの状況を見てみましょう。少なくとも「デスクトップ」(②)には雲マークがついていないことを確認してください。ついていた場合は、&lt;a href="#unlink_2024"&gt;リンク解除&lt;/a&gt;の手順を実施してからあらためてリンク設定を試してください。</t>
     <rPh sb="8" eb="9">
       <t>ヒダリ</t>
@@ -2035,21 +1939,6 @@
   </si>
   <si>
     <t>FRESTA-TEXT-2024 Win11 chap.8</t>
-  </si>
-  <si>
-    <t>win11ja-odrv22-open-setting.png</t>
-  </si>
-  <si>
-    <t>win11ja-odrv-add-acct.png</t>
-  </si>
-  <si>
-    <t>win11ja-odrv22-dir-selector.png</t>
-  </si>
-  <si>
-    <t xml:space="preserve">win11ja-odrv-explorer-home.png </t>
-  </si>
-  <si>
-    <t>win11ja-odrv24-enable-autostart.png</t>
   </si>
   <si>
     <t>OneDrive status check, unlink, and link</t>
@@ -2140,6 +2029,114 @@
       <t>カクニン</t>
     </rPh>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11en-onedrive-indicator.png</t>
+  </si>
+  <si>
+    <t>win11en-odrv-app.png</t>
+  </si>
+  <si>
+    <t>win11en-odrv22-open-setting.png</t>
+  </si>
+  <si>
+    <t>win11en-odrv22-noaccount.png</t>
+  </si>
+  <si>
+    <t>win11en-odrv22-withaccount.png</t>
+  </si>
+  <si>
+    <t>win11en-odrv22-backup.png</t>
+  </si>
+  <si>
+    <t>win11en-odrv22-backup-mgr.png</t>
+  </si>
+  <si>
+    <t>win11en-odrv22-backup-stopwarn1.png</t>
+  </si>
+  <si>
+    <t>win11en-odrv22-backup-stopwarn2.png</t>
+  </si>
+  <si>
+    <t>win11en-odrv22-backup-select.png</t>
+  </si>
+  <si>
+    <t>win11en-odrv22-backup-unselect.png</t>
+  </si>
+  <si>
+    <t>win11en-odrv22-unlink-pc.png</t>
+  </si>
+  <si>
+    <t>win11en-odrv-close-signin.png</t>
+  </si>
+  <si>
+    <t>win11en-link-to-original-folder.png</t>
+  </si>
+  <si>
+    <t>win11en-odrv22-uncheck-autostart.png</t>
+  </si>
+  <si>
+    <t>win11en-setting-acct-odrv.png</t>
+  </si>
+  <si>
+    <t>win11en-odrv-add-acct.png</t>
+  </si>
+  <si>
+    <t>win11en-odrv-no-optional-data.png</t>
+  </si>
+  <si>
+    <t>win11en-imc-odrv-dirname.png</t>
+  </si>
+  <si>
+    <t>win11en-odrv22-dir-selector.png</t>
+  </si>
+  <si>
+    <t>win11en-odrv22-exclude-desktop.png</t>
+  </si>
+  <si>
+    <t>win11en-odrv-backup-ready.png</t>
+  </si>
+  <si>
+    <t>win11en-explorer-with-desktop.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">win11en-odrv-explorer-home.png </t>
+  </si>
+  <si>
+    <t>win11en-odrv24-open-setting.png</t>
+  </si>
+  <si>
+    <t>win11en-odrv24-noaccount.png</t>
+  </si>
+  <si>
+    <t>win11en-odrv24-withaccount.png</t>
+  </si>
+  <si>
+    <t>win11en-odrv24-backup.png</t>
+  </si>
+  <si>
+    <t>win11en-odrv24-backup-mgr.png</t>
+  </si>
+  <si>
+    <t>win11en-odrv24-unlink-warning.png</t>
+  </si>
+  <si>
+    <t>win11en-odrv24-backup-unselect.png</t>
+  </si>
+  <si>
+    <t>win11en-odrv24-unlink-pc.png</t>
+  </si>
+  <si>
+    <t>win11en-odrv24-uncheck-autostart.png</t>
+  </si>
+  <si>
+    <t>win11en-odrv24-dir-selector.png</t>
+  </si>
+  <si>
+    <t>win11en-odrv24-exclude-desktop.png</t>
+  </si>
+  <si>
+    <t>win11en-odrv24-enable-autostart.png</t>
   </si>
 </sst>
 </file>
@@ -2296,37 +2293,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="index"/>
-      <sheetName val="ch0"/>
-      <sheetName val="ch1"/>
-      <sheetName val="ch2"/>
-      <sheetName val="ch3"/>
-      <sheetName val="ch4"/>
-      <sheetName val="ch5"/>
-      <sheetName val="ch6"/>
-      <sheetName val="ch7"/>
-      <sheetName val="ch8"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2"/>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2727,15 +2693,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CB03C1F-8A6F-4A43-BA2E-2C62B3131330}">
   <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="D9" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="4"/>
     <col min="2" max="2" width="88.44140625" style="4" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="4"/>
+    <col min="3" max="3" width="8.88671875" style="4"/>
+    <col min="4" max="4" width="34.88671875" style="4" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -2743,7 +2711,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>335</v>
+        <v>299</v>
       </c>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
@@ -2753,7 +2721,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>336</v>
+        <v>300</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
@@ -2773,7 +2741,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>329</v>
+        <v>298</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -2787,7 +2755,7 @@
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="10"/>
       <c r="B6" s="9" t="s">
-        <v>337</v>
+        <v>301</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
@@ -2801,7 +2769,7 @@
     <row r="8" spans="1:4" ht="264" x14ac:dyDescent="0.2">
       <c r="A8" s="10"/>
       <c r="B8" s="9" t="s">
-        <v>338</v>
+        <v>302</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
@@ -2815,7 +2783,7 @@
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="10"/>
       <c r="B10" s="9" t="s">
-        <v>339</v>
+        <v>303</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
@@ -2823,7 +2791,7 @@
     <row r="11" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A11" s="10"/>
       <c r="B11" s="9" t="s">
-        <v>340</v>
+        <v>304</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
@@ -2831,27 +2799,27 @@
     <row r="12" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A12" s="10"/>
       <c r="B12" s="9" t="s">
-        <v>341</v>
+        <v>305</v>
       </c>
       <c r="C12" s="10" ph="1"/>
       <c r="D12" s="10" t="s">
-        <v>258</v>
+        <v>314</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A13" s="10"/>
       <c r="B13" s="9" t="s">
-        <v>342</v>
+        <v>306</v>
       </c>
       <c r="C13" s="10" ph="1"/>
       <c r="D13" s="10" t="s">
-        <v>259</v>
+        <v>315</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="11"/>
       <c r="B14" s="12" t="s">
-        <v>343</v>
+        <v>307</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
@@ -2859,7 +2827,7 @@
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="13"/>
       <c r="B15" s="14" t="s">
-        <v>344</v>
+        <v>308</v>
       </c>
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
@@ -2867,31 +2835,31 @@
     <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A16" s="11"/>
       <c r="B16" s="12" t="s">
-        <v>345</v>
+        <v>309</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11" t="s">
-        <v>330</v>
+        <v>316</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A17" s="11"/>
       <c r="B17" s="12" t="s">
-        <v>346</v>
+        <v>310</v>
       </c>
       <c r="C17" s="11"/>
       <c r="D17" s="11" t="s">
-        <v>260</v>
+        <v>317</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A18" s="11"/>
       <c r="B18" s="12" t="s">
-        <v>347</v>
+        <v>311</v>
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="11" t="s">
-        <v>261</v>
+        <v>318</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -2903,7 +2871,7 @@
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="13"/>
       <c r="B20" s="14" t="s">
-        <v>348</v>
+        <v>312</v>
       </c>
       <c r="C20" s="13"/>
       <c r="D20" s="13"/>
@@ -2911,7 +2879,7 @@
     <row r="21" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A21" s="11"/>
       <c r="B21" s="12" t="s">
-        <v>349</v>
+        <v>313</v>
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="11"/>
@@ -2919,71 +2887,71 @@
     <row r="22" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A22" s="11"/>
       <c r="B22" s="12" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C22" s="11"/>
       <c r="D22" s="11" t="s">
-        <v>263</v>
+        <v>319</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A23" s="11"/>
       <c r="B23" s="12" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="11" t="s">
-        <v>265</v>
+        <v>320</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A24" s="11"/>
       <c r="B24" s="12" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="11" t="s">
-        <v>267</v>
+        <v>321</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="11"/>
       <c r="B25" s="12" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="C25" s="11"/>
       <c r="D25" s="11" t="s">
-        <v>269</v>
+        <v>322</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A26" s="11"/>
       <c r="B26" s="12" t="s">
-        <v>270</v>
+        <v>262</v>
       </c>
       <c r="C26" s="11"/>
       <c r="D26" s="11" t="s">
-        <v>271</v>
+        <v>323</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A27" s="11"/>
       <c r="B27" s="12" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="C27" s="11"/>
       <c r="D27" s="11" t="s">
-        <v>273</v>
+        <v>324</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="11"/>
       <c r="B28" s="12" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="C28" s="11"/>
       <c r="D28" s="11" t="s">
-        <v>275</v>
+        <v>325</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -2991,21 +2959,21 @@
         <v>4</v>
       </c>
       <c r="B29" s="12" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="C29" s="11"/>
       <c r="D29" s="11" t="s">
-        <v>277</v>
+        <v>326</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A30" s="11"/>
       <c r="B30" s="12" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
       <c r="C30" s="11"/>
       <c r="D30" s="11" t="s">
-        <v>279</v>
+        <v>327</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -3017,7 +2985,7 @@
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="13"/>
       <c r="B32" s="14" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
       <c r="C32" s="13"/>
       <c r="D32" s="13"/>
@@ -3031,11 +2999,11 @@
     <row r="34" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A34" s="11"/>
       <c r="B34" s="12" t="s">
-        <v>281</v>
+        <v>268</v>
       </c>
       <c r="C34" s="11"/>
       <c r="D34" s="11" t="s">
-        <v>282</v>
+        <v>328</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -3047,7 +3015,7 @@
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="13"/>
       <c r="B36" s="14" t="s">
-        <v>283</v>
+        <v>269</v>
       </c>
       <c r="C36" s="13"/>
       <c r="D36" s="13"/>
@@ -3055,7 +3023,7 @@
     <row r="37" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A37" s="11"/>
       <c r="B37" s="12" t="s">
-        <v>284</v>
+        <v>270</v>
       </c>
       <c r="C37" s="11"/>
       <c r="D37" s="11"/>
@@ -3063,51 +3031,51 @@
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="11"/>
       <c r="B38" s="12" t="s">
-        <v>285</v>
+        <v>271</v>
       </c>
       <c r="C38" s="11"/>
       <c r="D38" s="11" t="s">
-        <v>286</v>
+        <v>329</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A39" s="11"/>
       <c r="B39" s="12" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="C39" s="11"/>
       <c r="D39" s="11" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A40" s="11"/>
       <c r="B40" s="12" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
       <c r="C40" s="11"/>
       <c r="D40" s="11" t="s">
-        <v>289</v>
+        <v>331</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="11"/>
       <c r="B41" s="12" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
       <c r="C41" s="11"/>
       <c r="D41" s="11" t="s">
-        <v>291</v>
+        <v>332</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A42" s="11"/>
       <c r="B42" s="12" t="s">
-        <v>292</v>
+        <v>275</v>
       </c>
       <c r="C42" s="11"/>
       <c r="D42" s="11" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -3115,47 +3083,47 @@
         <v>4</v>
       </c>
       <c r="B43" s="12" t="s">
-        <v>293</v>
+        <v>276</v>
       </c>
       <c r="C43" s="11"/>
       <c r="D43" s="11" t="s">
-        <v>294</v>
+        <v>334</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" s="11"/>
       <c r="B44" s="12" t="s">
-        <v>295</v>
+        <v>277</v>
       </c>
       <c r="C44" s="11"/>
       <c r="D44" s="11" t="s">
-        <v>296</v>
+        <v>335</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A45" s="11"/>
       <c r="B45" s="12" t="s">
-        <v>297</v>
+        <v>278</v>
       </c>
       <c r="C45" s="11"/>
       <c r="D45" s="11" t="s">
-        <v>298</v>
+        <v>336</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A46" s="11"/>
       <c r="B46" s="12" t="s">
-        <v>299</v>
+        <v>279</v>
       </c>
       <c r="C46" s="11"/>
       <c r="D46" s="11" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A47" s="11"/>
       <c r="B47" s="12" t="s">
-        <v>300</v>
+        <v>280</v>
       </c>
       <c r="C47" s="11"/>
       <c r="D47" s="11"/>
@@ -3169,7 +3137,7 @@
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A49" s="15"/>
       <c r="B49" s="16" t="s">
-        <v>301</v>
+        <v>281</v>
       </c>
       <c r="C49" s="15"/>
       <c r="D49" s="15"/>
@@ -3177,7 +3145,7 @@
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A50" s="17"/>
       <c r="B50" s="18" t="s">
-        <v>302</v>
+        <v>282</v>
       </c>
       <c r="C50" s="17"/>
       <c r="D50" s="17"/>
@@ -3185,31 +3153,31 @@
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A51" s="15"/>
       <c r="B51" s="16" t="s">
-        <v>303</v>
+        <v>283</v>
       </c>
       <c r="C51" s="15"/>
       <c r="D51" s="15" t="s">
-        <v>304</v>
+        <v>338</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A52" s="15"/>
       <c r="B52" s="16" t="s">
-        <v>305</v>
+        <v>284</v>
       </c>
       <c r="C52" s="15"/>
       <c r="D52" s="15" t="s">
-        <v>306</v>
+        <v>339</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="15"/>
       <c r="B53" s="16" t="s">
-        <v>307</v>
+        <v>285</v>
       </c>
       <c r="C53" s="15"/>
       <c r="D53" s="15" t="s">
-        <v>308</v>
+        <v>340</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -3221,7 +3189,7 @@
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="17"/>
       <c r="B55" s="18" t="s">
-        <v>309</v>
+        <v>286</v>
       </c>
       <c r="C55" s="17"/>
       <c r="D55" s="17"/>
@@ -3229,7 +3197,7 @@
     <row r="56" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A56" s="15"/>
       <c r="B56" s="16" t="s">
-        <v>310</v>
+        <v>287</v>
       </c>
       <c r="C56" s="15"/>
       <c r="D56" s="15"/>
@@ -3237,51 +3205,51 @@
     <row r="57" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A57" s="15"/>
       <c r="B57" s="16" t="s">
-        <v>311</v>
+        <v>288</v>
       </c>
       <c r="C57" s="15"/>
       <c r="D57" s="15" t="s">
-        <v>312</v>
+        <v>341</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="15"/>
       <c r="B58" s="16" t="s">
-        <v>313</v>
+        <v>289</v>
       </c>
       <c r="C58" s="15"/>
       <c r="D58" s="15" t="s">
-        <v>314</v>
+        <v>342</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="15"/>
       <c r="B59" s="16" t="s">
-        <v>315</v>
+        <v>290</v>
       </c>
       <c r="C59" s="15"/>
       <c r="D59" s="15" t="s">
-        <v>316</v>
+        <v>343</v>
       </c>
     </row>
     <row r="60" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A60" s="15"/>
       <c r="B60" s="16" t="s">
-        <v>317</v>
+        <v>291</v>
       </c>
       <c r="C60" s="15"/>
       <c r="D60" s="15" t="s">
-        <v>318</v>
+        <v>344</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A61" s="15"/>
       <c r="B61" s="16" t="s">
-        <v>319</v>
+        <v>292</v>
       </c>
       <c r="C61" s="15"/>
       <c r="D61" s="15" t="s">
-        <v>320</v>
+        <v>345</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -3289,21 +3257,21 @@
         <v>4</v>
       </c>
       <c r="B62" s="16" t="s">
-        <v>276</v>
+        <v>265</v>
       </c>
       <c r="C62" s="15"/>
       <c r="D62" s="15" t="s">
-        <v>277</v>
+        <v>326</v>
       </c>
     </row>
     <row r="63" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A63" s="15"/>
       <c r="B63" s="16" t="s">
-        <v>278</v>
+        <v>266</v>
       </c>
       <c r="C63" s="15"/>
       <c r="D63" s="15" t="s">
-        <v>279</v>
+        <v>327</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
@@ -3315,7 +3283,7 @@
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A65" s="17"/>
       <c r="B65" s="18" t="s">
-        <v>321</v>
+        <v>293</v>
       </c>
       <c r="C65" s="17"/>
       <c r="D65" s="17"/>
@@ -3329,11 +3297,11 @@
     <row r="67" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A67" s="15"/>
       <c r="B67" s="16" t="s">
-        <v>322</v>
+        <v>294</v>
       </c>
       <c r="C67" s="15"/>
       <c r="D67" s="15" t="s">
-        <v>323</v>
+        <v>346</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
@@ -3345,7 +3313,7 @@
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="17"/>
       <c r="B69" s="18" t="s">
-        <v>324</v>
+        <v>295</v>
       </c>
       <c r="C69" s="17"/>
       <c r="D69" s="17"/>
@@ -3353,7 +3321,7 @@
     <row r="70" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A70" s="15"/>
       <c r="B70" s="16" t="s">
-        <v>284</v>
+        <v>270</v>
       </c>
       <c r="C70" s="15"/>
       <c r="D70" s="15"/>
@@ -3361,51 +3329,51 @@
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" s="15"/>
       <c r="B71" s="16" t="s">
-        <v>285</v>
+        <v>271</v>
       </c>
       <c r="C71" s="15"/>
       <c r="D71" s="15" t="s">
-        <v>286</v>
+        <v>329</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A72" s="15"/>
       <c r="B72" s="16" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="C72" s="15"/>
       <c r="D72" s="15" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="15"/>
       <c r="B73" s="16" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
       <c r="C73" s="15"/>
       <c r="D73" s="15" t="s">
-        <v>289</v>
+        <v>331</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="15"/>
       <c r="B74" s="16" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
       <c r="C74" s="15"/>
       <c r="D74" s="15" t="s">
-        <v>291</v>
+        <v>332</v>
       </c>
     </row>
     <row r="75" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A75" s="15"/>
       <c r="B75" s="16" t="s">
-        <v>292</v>
+        <v>275</v>
       </c>
       <c r="C75" s="15"/>
       <c r="D75" s="15" t="s">
-        <v>325</v>
+        <v>347</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -3413,51 +3381,51 @@
         <v>4</v>
       </c>
       <c r="B76" s="16" t="s">
-        <v>293</v>
+        <v>276</v>
       </c>
       <c r="C76" s="15"/>
       <c r="D76" s="15" t="s">
-        <v>326</v>
+        <v>348</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A77" s="15"/>
       <c r="B77" s="16" t="s">
-        <v>295</v>
+        <v>277</v>
       </c>
       <c r="C77" s="15"/>
       <c r="D77" s="15" t="s">
-        <v>296</v>
+        <v>335</v>
       </c>
     </row>
     <row r="78" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A78" s="15"/>
       <c r="B78" s="16" t="s">
-        <v>297</v>
+        <v>278</v>
       </c>
       <c r="C78" s="15"/>
       <c r="D78" s="15" t="s">
-        <v>298</v>
+        <v>336</v>
       </c>
     </row>
     <row r="79" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A79" s="15"/>
       <c r="B79" s="16" t="s">
-        <v>327</v>
+        <v>296</v>
       </c>
       <c r="C79" s="15"/>
       <c r="D79" s="15" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
     </row>
     <row r="80" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A80" s="15"/>
       <c r="B80" s="16" t="s">
-        <v>328</v>
+        <v>297</v>
       </c>
       <c r="C80" s="15"/>
       <c r="D80" s="15" t="s">
-        <v>334</v>
+        <v>349</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
win11en: add more images
</commit_message>
<xml_diff>
--- a/win11_en.xlsx
+++ b/win11_en.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48789808-EDC6-45A6-98E5-50BF10693A09}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{808113EA-383E-4ED1-BFAB-52D0A175264E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6708" yWindow="-15096" windowWidth="8652" windowHeight="11592" tabRatio="729" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="350">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="351">
   <si>
     <t>header1</t>
   </si>
@@ -2031,9 +2031,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11en-onedrive-indicator.png</t>
-  </si>
-  <si>
     <t>win11en-odrv-app.png</t>
   </si>
   <si>
@@ -2137,6 +2134,14 @@
   </si>
   <si>
     <t>win11en-odrv24-enable-autostart.png</t>
+  </si>
+  <si>
+    <t>win11en-odrv-indicator.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11en-odrv-add-acct.png</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -2691,10 +2696,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CB03C1F-8A6F-4A43-BA2E-2C62B3131330}">
-  <dimension ref="A1:D80"/>
+  <dimension ref="A1:D79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="D9" sqref="D1:D1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -2803,7 +2808,7 @@
       </c>
       <c r="C12" s="10" ph="1"/>
       <c r="D12" s="10" t="s">
-        <v>314</v>
+        <v>349</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -2813,7 +2818,7 @@
       </c>
       <c r="C13" s="10" ph="1"/>
       <c r="D13" s="10" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -2839,7 +2844,7 @@
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -2849,7 +2854,7 @@
       </c>
       <c r="C17" s="11"/>
       <c r="D17" s="11" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -2859,7 +2864,7 @@
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="11" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -2891,7 +2896,7 @@
       </c>
       <c r="C22" s="11"/>
       <c r="D22" s="11" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -2901,7 +2906,7 @@
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="11" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -2911,7 +2916,7 @@
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="11" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -2921,7 +2926,7 @@
       </c>
       <c r="C25" s="11"/>
       <c r="D25" s="11" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -2931,7 +2936,7 @@
       </c>
       <c r="C26" s="11"/>
       <c r="D26" s="11" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -2941,7 +2946,7 @@
       </c>
       <c r="C27" s="11"/>
       <c r="D27" s="11" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -2951,7 +2956,7 @@
       </c>
       <c r="C28" s="11"/>
       <c r="D28" s="11" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -2963,7 +2968,7 @@
       </c>
       <c r="C29" s="11"/>
       <c r="D29" s="11" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -2973,7 +2978,7 @@
       </c>
       <c r="C30" s="11"/>
       <c r="D30" s="11" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -3003,7 +3008,7 @@
       </c>
       <c r="C34" s="11"/>
       <c r="D34" s="11" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -3035,7 +3040,7 @@
       </c>
       <c r="C38" s="11"/>
       <c r="D38" s="11" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -3045,7 +3050,7 @@
       </c>
       <c r="C39" s="11"/>
       <c r="D39" s="11" t="s">
-        <v>330</v>
+        <v>350</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -3055,7 +3060,7 @@
       </c>
       <c r="C40" s="11"/>
       <c r="D40" s="11" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -3065,7 +3070,7 @@
       </c>
       <c r="C41" s="11"/>
       <c r="D41" s="11" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -3075,7 +3080,7 @@
       </c>
       <c r="C42" s="11"/>
       <c r="D42" s="11" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -3087,7 +3092,7 @@
       </c>
       <c r="C43" s="11"/>
       <c r="D43" s="11" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -3097,73 +3102,73 @@
       </c>
       <c r="C44" s="11"/>
       <c r="D44" s="11" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A45" s="11"/>
       <c r="B45" s="12" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C45" s="11"/>
       <c r="D45" s="11" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A46" s="11"/>
       <c r="B46" s="12" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C46" s="11"/>
-      <c r="D46" s="11" t="s">
+      <c r="D46" s="11"/>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" s="10"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="10"/>
+      <c r="D47" s="10"/>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" s="15"/>
+      <c r="B48" s="16" t="s">
+        <v>281</v>
+      </c>
+      <c r="C48" s="15"/>
+      <c r="D48" s="15"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" s="17"/>
+      <c r="B49" s="18" t="s">
+        <v>282</v>
+      </c>
+      <c r="C49" s="17"/>
+      <c r="D49" s="17"/>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" s="15"/>
+      <c r="B50" s="16" t="s">
+        <v>283</v>
+      </c>
+      <c r="C50" s="15"/>
+      <c r="D50" s="15" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A47" s="11"/>
-      <c r="B47" s="12" t="s">
-        <v>280</v>
-      </c>
-      <c r="C47" s="11"/>
-      <c r="D47" s="11"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A48" s="10"/>
-      <c r="B48" s="9"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="10"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" s="15"/>
-      <c r="B49" s="16" t="s">
-        <v>281</v>
-      </c>
-      <c r="C49" s="15"/>
-      <c r="D49" s="15"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A50" s="17"/>
-      <c r="B50" s="18" t="s">
-        <v>282</v>
-      </c>
-      <c r="C50" s="17"/>
-      <c r="D50" s="17"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A51" s="15"/>
       <c r="B51" s="16" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C51" s="15"/>
       <c r="D51" s="15" t="s">
         <v>338</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="15"/>
       <c r="B52" s="16" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="C52" s="15"/>
       <c r="D52" s="15" t="s">
@@ -3172,40 +3177,40 @@
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A53" s="15"/>
-      <c r="B53" s="16" t="s">
-        <v>285</v>
-      </c>
+      <c r="B53" s="16"/>
       <c r="C53" s="15"/>
-      <c r="D53" s="15" t="s">
-        <v>340</v>
-      </c>
+      <c r="D53" s="15"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" s="15"/>
-      <c r="B54" s="16"/>
-      <c r="C54" s="15"/>
-      <c r="D54" s="15"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A55" s="17"/>
-      <c r="B55" s="18" t="s">
+      <c r="A54" s="17"/>
+      <c r="B54" s="18" t="s">
         <v>286</v>
       </c>
-      <c r="C55" s="17"/>
-      <c r="D55" s="17"/>
+      <c r="C54" s="17"/>
+      <c r="D54" s="17"/>
+    </row>
+    <row r="55" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="A55" s="15"/>
+      <c r="B55" s="16" t="s">
+        <v>287</v>
+      </c>
+      <c r="C55" s="15"/>
+      <c r="D55" s="15"/>
     </row>
     <row r="56" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A56" s="15"/>
       <c r="B56" s="16" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C56" s="15"/>
-      <c r="D56" s="15"/>
-    </row>
-    <row r="57" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+      <c r="D56" s="15" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A57" s="15"/>
       <c r="B57" s="16" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C57" s="15"/>
       <c r="D57" s="15" t="s">
@@ -3215,27 +3220,27 @@
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A58" s="15"/>
       <c r="B58" s="16" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C58" s="15"/>
       <c r="D58" s="15" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A59" s="15"/>
       <c r="B59" s="16" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C59" s="15"/>
       <c r="D59" s="15" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="15"/>
       <c r="B60" s="16" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C60" s="15"/>
       <c r="D60" s="15" t="s">
@@ -3243,103 +3248,103 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="15"/>
+      <c r="A61" s="15" t="s">
+        <v>4</v>
+      </c>
       <c r="B61" s="16" t="s">
-        <v>292</v>
+        <v>265</v>
       </c>
       <c r="C61" s="15"/>
       <c r="D61" s="15" t="s">
-        <v>345</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A62" s="15" t="s">
-        <v>4</v>
-      </c>
+        <v>325</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+      <c r="A62" s="15"/>
       <c r="B62" s="16" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="C62" s="15"/>
       <c r="D62" s="15" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="15"/>
-      <c r="B63" s="16" t="s">
-        <v>266</v>
-      </c>
+      <c r="B63" s="16"/>
       <c r="C63" s="15"/>
-      <c r="D63" s="15" t="s">
-        <v>327</v>
-      </c>
+      <c r="D63" s="15"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A64" s="15"/>
-      <c r="B64" s="16"/>
-      <c r="C64" s="15"/>
-      <c r="D64" s="15"/>
+      <c r="A64" s="17"/>
+      <c r="B64" s="18" t="s">
+        <v>293</v>
+      </c>
+      <c r="C64" s="17"/>
+      <c r="D64" s="17"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A65" s="17"/>
-      <c r="B65" s="18" t="s">
-        <v>293</v>
-      </c>
-      <c r="C65" s="17"/>
-      <c r="D65" s="17"/>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="15"/>
+      <c r="B65" s="16"/>
+      <c r="C65" s="15"/>
+      <c r="D65" s="15"/>
+    </row>
+    <row r="66" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A66" s="15"/>
-      <c r="B66" s="16"/>
+      <c r="B66" s="16" t="s">
+        <v>294</v>
+      </c>
       <c r="C66" s="15"/>
-      <c r="D66" s="15"/>
-    </row>
-    <row r="67" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="D66" s="15" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="15"/>
-      <c r="B67" s="16" t="s">
-        <v>294</v>
-      </c>
+      <c r="B67" s="16"/>
       <c r="C67" s="15"/>
-      <c r="D67" s="15" t="s">
-        <v>346</v>
-      </c>
+      <c r="D67" s="15"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="15"/>
-      <c r="B68" s="16"/>
-      <c r="C68" s="15"/>
-      <c r="D68" s="15"/>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A69" s="17"/>
-      <c r="B69" s="18" t="s">
+      <c r="A68" s="17"/>
+      <c r="B68" s="18" t="s">
         <v>295</v>
       </c>
-      <c r="C69" s="17"/>
-      <c r="D69" s="17"/>
-    </row>
-    <row r="70" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="C68" s="17"/>
+      <c r="D68" s="17"/>
+    </row>
+    <row r="69" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="A69" s="15"/>
+      <c r="B69" s="16" t="s">
+        <v>270</v>
+      </c>
+      <c r="C69" s="15"/>
+      <c r="D69" s="15"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="15"/>
       <c r="B70" s="16" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C70" s="15"/>
-      <c r="D70" s="15"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D70" s="15" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A71" s="15"/>
       <c r="B71" s="16" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="C71" s="15"/>
       <c r="D71" s="15" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A72" s="15"/>
       <c r="B72" s="16" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C72" s="15"/>
       <c r="D72" s="15" t="s">
@@ -3349,27 +3354,29 @@
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="15"/>
       <c r="B73" s="16" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="C73" s="15"/>
       <c r="D73" s="15" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A74" s="15"/>
       <c r="B74" s="16" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C74" s="15"/>
       <c r="D74" s="15" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
-      <c r="A75" s="15"/>
+        <v>346</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A75" s="15" t="s">
+        <v>4</v>
+      </c>
       <c r="B75" s="16" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="C75" s="15"/>
       <c r="D75" s="15" t="s">
@@ -3377,55 +3384,43 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A76" s="15" t="s">
-        <v>4</v>
-      </c>
+      <c r="A76" s="15"/>
       <c r="B76" s="16" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C76" s="15"/>
       <c r="D76" s="15" t="s">
-        <v>348</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.2">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A77" s="15"/>
       <c r="B77" s="16" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="C77" s="15"/>
       <c r="D77" s="15" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A78" s="15"/>
       <c r="B78" s="16" t="s">
-        <v>278</v>
+        <v>296</v>
       </c>
       <c r="C78" s="15"/>
       <c r="D78" s="15" t="s">
         <v>336</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A79" s="15"/>
       <c r="B79" s="16" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="C79" s="15"/>
       <c r="D79" s="15" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A80" s="15"/>
-      <c r="B80" s="16" t="s">
-        <v>297</v>
-      </c>
-      <c r="C80" s="15"/>
-      <c r="D80" s="15" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
win11en: add missing images
</commit_message>
<xml_diff>
--- a/win11_en.xlsx
+++ b/win11_en.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{808113EA-383E-4ED1-BFAB-52D0A175264E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14052024-7D3C-458C-9CA0-06584DAF8AAC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6708" yWindow="-15096" windowWidth="8652" windowHeight="11592" tabRatio="729" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2698,8 +2698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CB03C1F-8A6F-4A43-BA2E-2C62B3131330}">
   <dimension ref="A1:D79"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
win11en: fix check number
</commit_message>
<xml_diff>
--- a/win11_en.xlsx
+++ b/win11_en.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta\fresta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3194697-3229-4D66-8736-362E0E727A16}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4454EED-49EF-4725-ABA0-79765882CF20}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6708" yWindow="-15096" windowWidth="8652" windowHeight="11592" tabRatio="729" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -579,10 +579,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>You would be able to check the messages addressed to your email address assigned by Hiroshima University.&lt;span class="check"&gt;check-11&lt;span&gt;&lt;/span&gt;&lt;/span&gt;</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Set up Windows Update so that your Windows11 will keep updated. And set up anti-virus software, Microsoft Defender, to be updated automatically.</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -619,11 +615,6 @@
   <si>
     <t>Input Hirodai ID(your student number) to the "User Name" box, and input your Hirodai password to the "Password" box.
  (*) This login form may be skipped. This is a normal behavier, so please go on.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Confirm that you can see "Dashboard" similar to this pic.&lt;span class="check"&gt;check-8&lt;/span&gt;
-</t>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>moodle-dashboard-en.svg</t>
@@ -650,10 +641,6 @@
   </si>
   <si>
     <t>moodle-mfa-imc.svg</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Click "Practice setting up MFA use of IMC accounts" below, and follow instruction to setup MFA. See PDF documents for details.&lt;span class="check"&gt;check-9&lt;/span&gt;</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -719,20 +706,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">Here, you can register courses or view your grades. Notifications from your courses or school will be listed in &amp;quot;Message&amp;quot;.&lt;span class="check"&gt;check-13&lt;/span&gt;
-  </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>win10-6-11a.svg</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">Click "Practice setting up MFA use of Hirodai ID" below, and follow instruction to setup MFA. See PDF documents for details.&lt;span class="check"&gt;check-10&lt;/span&gt;
-</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>moodle-checklist.svg</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -745,26 +722,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">Look carefully at &amp;quot;About&amp;quot; page.
-&amp;quot;Edition&amp;quot; entry under &amp;quot;Windows Specifications&amp;quot; tells you what kind of Windows your PC is running. In this case, your PC is running &amp;quot;Windows 11&amp;quot;. And &amp;quot;Version&amp;quot; entry gives you the detailed version number of your Windows11.&lt;span class="check"&gt;check-1&lt;span&gt;&lt;/span&gt;
-&lt;/span&gt;
-&amp;quot;System type&amp;quot; entry under &amp;quot;Device Specifications&amp;quot; tells you that your PC is running &amp;quot;64-bit operating system&amp;quot;. It means your OS can handle 64-binary-digit data.&lt;span class="check"&gt;check-2&lt;span&gt;&lt;/span&gt;
-&lt;/span&gt;
-&amp;quot;Installed RAM&amp;quot; entry tells you the capacity of the main memory in your PC. The larger the size of RAM your PC have, the more data your PC can store or the greater multi-tasking ability your PC gets.
-  </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Please click "Scan options", and choose "Full scan", then click "Scan now".&lt;span c&lt;span class="check"&gt;check-5&lt;/span&gt;lass="check"&gt;check-5&lt;/span&gt;&lt;span class="check"&gt;check-6&lt;/span&gt;</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Click "accept". You can read the license agreement from "File &gt; Account" menu in later.&lt;span class="check"&gt;check-12&lt;/span&gt;</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>If the button is changed as "disconnect", the connection with the WiFi in Hiroshima University succeeded.&lt;span class="check"&gt;check-14&lt;/span&gt;
-When you change your password, the cached password should be cleared. Please right-click the icon of "HU-CUP" icon, and choose "forget" menu to clear it.</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1054,10 +1012,6 @@
   </si>
   <si>
     <t>win11en-winupdate-option2.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Please click "Check for updates" button. The installations would be queued automatically &lt;span class="check"&gt;check-4&lt;/span&gt; The update of the Microsoft Defender virus database is done during this &lt;span class="check"&gt;check-5&lt;/span&gt;.</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1441,6 +1395,60 @@
   </si>
   <si>
     <t>fresta_en</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Please click "Scan options", and choose "Full scan", then click "Scan now".
+&lt;span class="check"&gt;check-4&lt;/span&gt;
+&lt;span class="check"&gt;check-5&lt;/span&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Look carefully at &amp;quot;About&amp;quot; page.
+&amp;quot;Edition&amp;quot; entry under &amp;quot;Windows Specifications&amp;quot; tells you what kind of Windows your PC is running. In this case, your PC is running &amp;quot;Windows 11&amp;quot;. And &amp;quot;Version&amp;quot; entry gives you the detailed version number of your Windows11.&lt;span class="check"&gt;check-1&lt;span&gt;&lt;/span&gt;
+&lt;/span&gt;
+&amp;quot;Installed RAM&amp;quot; entry tells you the capacity of the main memory in your PC. The larger the size of RAM your PC have, the more data your PC can store or the greater multi-tasking ability your PC gets.
+  </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Please click "Check for updates" button. The installations would be queued automatically 
+&lt;span class="check"&gt;check-4&lt;/span&gt;
+ The update of the Microsoft Defender virus database is done during this 
+&lt;span class="check"&gt;check-5&lt;/span&gt;.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Confirm that you can see "Dashboard" similar to this pic.
+&lt;span class="check"&gt;check-7&lt;/span&gt;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Click "Practice setting up MFA use of IMC accounts" below, and follow instruction to setup MFA. See PDF documents for details.
+&lt;span class="check"&gt;check-8&lt;/span&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Click "Practice setting up MFA use of Hirodai ID" below, and follow instruction to setup MFA. See PDF documents for details.&lt;span class="check"&gt;check-9&lt;/span&gt;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>You would be able to check the messages addressed to your email address assigned by Hiroshima University.
+&lt;span class="check"&gt;check-10&lt;/span&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Here, you can register courses or view your grades. Notifications from your courses or school will be listed in &amp;quot;Message&amp;quot;.
+&lt;span class="check"&gt;check-12&lt;/span&gt;
+  </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>If the button is changed as "disconnect", the connection with the WiFi in Hiroshima University succeeded.
+&lt;span class="check"&gt;check-13&lt;/span&gt;
+When you change your password, the cached password should be cleared. Please right-click the icon of "HU-CUP" icon, and choose "forget" menu to clear it.</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1998,7 +2006,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -2006,7 +2014,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="C5" t="s">
         <v>4</v>
@@ -2040,8 +2048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CB03C1F-8A6F-4A43-BA2E-2C62B3131330}">
   <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A36" workbookViewId="0">
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -2058,7 +2066,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
@@ -2068,7 +2076,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>360</v>
+        <v>351</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
@@ -2078,7 +2086,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>361</v>
+        <v>352</v>
       </c>
       <c r="C3" s="10"/>
       <c r="D3" s="10"/>
@@ -2088,7 +2096,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="C4" s="10"/>
       <c r="D4" s="10"/>
@@ -2102,7 +2110,7 @@
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="10"/>
       <c r="B6" s="9" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="C6" s="10"/>
       <c r="D6" s="10"/>
@@ -2116,7 +2124,7 @@
     <row r="8" spans="1:4" ht="237.6" x14ac:dyDescent="0.2">
       <c r="A8" s="10"/>
       <c r="B8" s="9" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="10"/>
@@ -2130,7 +2138,7 @@
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="10"/>
       <c r="B10" s="9" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="10"/>
@@ -2138,7 +2146,7 @@
     <row r="11" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A11" s="10"/>
       <c r="B11" s="9" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="10"/>
@@ -2146,27 +2154,27 @@
     <row r="12" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A12" s="10"/>
       <c r="B12" s="9" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="C12" s="10" ph="1"/>
       <c r="D12" s="10" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A13" s="10"/>
       <c r="B13" s="9" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="C13" s="10" ph="1"/>
       <c r="D13" s="10" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="11"/>
       <c r="B14" s="12" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
@@ -2174,7 +2182,7 @@
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="13"/>
       <c r="B15" s="14" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="C15" s="13"/>
       <c r="D15" s="13"/>
@@ -2182,31 +2190,31 @@
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="11"/>
       <c r="B16" s="12" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="C16" s="11"/>
       <c r="D16" s="11" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A17" s="11"/>
       <c r="B17" s="12" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="C17" s="11"/>
       <c r="D17" s="11" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A18" s="11"/>
       <c r="B18" s="12" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="C18" s="11"/>
       <c r="D18" s="11" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -2218,7 +2226,7 @@
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="13"/>
       <c r="B20" s="14" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="C20" s="13"/>
       <c r="D20" s="13"/>
@@ -2226,17 +2234,17 @@
     <row r="21" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A21" s="11"/>
       <c r="B21" s="12" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="C21" s="11"/>
       <c r="D21" s="11" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A22" s="11"/>
       <c r="B22" s="12" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="C22" s="11"/>
       <c r="D22" s="11"/>
@@ -2244,71 +2252,71 @@
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="11"/>
       <c r="B23" s="12" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="C23" s="11"/>
       <c r="D23" s="11" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="11"/>
       <c r="B24" s="12" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="C24" s="11"/>
       <c r="D24" s="11" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A25" s="11"/>
       <c r="B25" s="12" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="C25" s="11"/>
       <c r="D25" s="11" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="11"/>
       <c r="B26" s="12" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="C26" s="11"/>
       <c r="D26" s="11" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A27" s="11"/>
       <c r="B27" s="12" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="C27" s="11"/>
       <c r="D27" s="11" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A28" s="11"/>
       <c r="B28" s="12" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="C28" s="11"/>
       <c r="D28" s="11" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="11"/>
       <c r="B29" s="12" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="C29" s="11"/>
       <c r="D29" s="11" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -2316,27 +2324,27 @@
         <v>4</v>
       </c>
       <c r="B30" s="12" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="C30" s="11"/>
       <c r="D30" s="11" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A31" s="11"/>
       <c r="B31" s="12" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="C31" s="11"/>
       <c r="D31" s="11" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="11"/>
       <c r="B32" s="12" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="C32" s="11"/>
       <c r="D32" s="11"/>
@@ -2350,7 +2358,7 @@
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="13"/>
       <c r="B34" s="14" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="C34" s="13"/>
       <c r="D34" s="13"/>
@@ -2358,7 +2366,7 @@
     <row r="35" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A35" s="11"/>
       <c r="B35" s="12" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="C35" s="11"/>
       <c r="D35" s="11"/>
@@ -2366,91 +2374,91 @@
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="11"/>
       <c r="B36" s="12" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="C36" s="11"/>
       <c r="D36" s="11" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A37" s="11"/>
       <c r="B37" s="12" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="C37" s="11"/>
       <c r="D37" s="11" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="11"/>
       <c r="B38" s="12" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="C38" s="11"/>
       <c r="D38" s="11" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="11"/>
       <c r="B39" s="12" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="C39" s="11"/>
       <c r="D39" s="11" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="A40" s="11"/>
       <c r="B40" s="12" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="C40" s="11"/>
       <c r="D40" s="11" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="11"/>
       <c r="B41" s="12" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="C41" s="11"/>
       <c r="D41" s="11" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="11"/>
       <c r="B42" s="12" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="C42" s="11"/>
       <c r="D42" s="11" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A43" s="11"/>
       <c r="B43" s="12" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="C43" s="11"/>
       <c r="D43" s="11" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A44" s="11"/>
       <c r="B44" s="12" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="C44" s="11"/>
       <c r="D44" s="11" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -2462,7 +2470,7 @@
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="15"/>
       <c r="B46" s="16" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
       <c r="C46" s="15"/>
       <c r="D46" s="15"/>
@@ -2470,7 +2478,7 @@
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="17"/>
       <c r="B47" s="18" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="C47" s="17"/>
       <c r="D47" s="17"/>
@@ -2478,31 +2486,31 @@
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="15"/>
       <c r="B48" s="16" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="C48" s="15"/>
       <c r="D48" s="15" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A49" s="15"/>
       <c r="B49" s="16" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="C49" s="15"/>
       <c r="D49" s="15" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A50" s="15"/>
       <c r="B50" s="16" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
       <c r="C50" s="15"/>
       <c r="D50" s="15" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -2514,7 +2522,7 @@
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="17"/>
       <c r="B52" s="18" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="C52" s="17"/>
       <c r="D52" s="17"/>
@@ -2522,17 +2530,17 @@
     <row r="53" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A53" s="15"/>
       <c r="B53" s="16" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="C53" s="15"/>
       <c r="D53" s="15" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A54" s="15"/>
       <c r="B54" s="16" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="C54" s="15"/>
       <c r="D54" s="15"/>
@@ -2540,61 +2548,61 @@
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="15"/>
       <c r="B55" s="16" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="C55" s="15"/>
       <c r="D55" s="15" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="15"/>
       <c r="B56" s="16" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="C56" s="15"/>
       <c r="D56" s="15" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A57" s="15"/>
       <c r="B57" s="16" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="C57" s="15"/>
       <c r="D57" s="15" t="s">
-        <v>358</v>
+        <v>349</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A58" s="15"/>
       <c r="B58" s="16" t="s">
-        <v>355</v>
+        <v>346</v>
       </c>
       <c r="C58" s="15"/>
       <c r="D58" s="15" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="15"/>
       <c r="B59" s="16" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="C59" s="15"/>
       <c r="D59" s="15" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="15"/>
       <c r="B60" s="16" t="s">
-        <v>356</v>
+        <v>347</v>
       </c>
       <c r="C60" s="15"/>
       <c r="D60" s="15" t="s">
-        <v>357</v>
+        <v>348</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -2602,27 +2610,27 @@
         <v>4</v>
       </c>
       <c r="B61" s="16" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="C61" s="15"/>
       <c r="D61" s="15" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A62" s="15"/>
       <c r="B62" s="20" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="C62" s="15"/>
       <c r="D62" s="15" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="15"/>
       <c r="B63" s="16" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="C63" s="15"/>
       <c r="D63" s="15"/>
@@ -2636,7 +2644,7 @@
     <row r="65" spans="1:4" s="24" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="22"/>
       <c r="B65" s="23" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
       <c r="C65" s="22"/>
       <c r="D65" s="22"/>
@@ -2644,7 +2652,7 @@
     <row r="66" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A66" s="15"/>
       <c r="B66" s="16" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="C66" s="15"/>
       <c r="D66" s="22"/>
@@ -2652,41 +2660,41 @@
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="15"/>
       <c r="B67" s="16" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="C67" s="15"/>
       <c r="D67" s="15" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A68" s="15"/>
       <c r="B68" s="16" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="C68" s="15"/>
       <c r="D68" s="15" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="15"/>
       <c r="B69" s="16" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="C69" s="15"/>
       <c r="D69" s="15" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="15"/>
       <c r="B70" s="16" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="C70" s="15"/>
       <c r="D70" s="15" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -2694,49 +2702,49 @@
         <v>4</v>
       </c>
       <c r="B71" s="16" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="C71" s="15"/>
       <c r="D71" s="15" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A72" s="15"/>
       <c r="B72" s="16" t="s">
-        <v>359</v>
+        <v>350</v>
       </c>
       <c r="C72" s="15"/>
       <c r="D72" s="15" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="15"/>
       <c r="B73" s="4" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="C73" s="15"/>
       <c r="D73" s="15" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="15"/>
       <c r="B74" s="4" t="s">
-        <v>352</v>
+        <v>343</v>
       </c>
       <c r="C74" s="15"/>
       <c r="D74" s="15" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B75" s="4" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="D75" s="15" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
     </row>
   </sheetData>
@@ -2792,7 +2800,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="285.60000000000002" ph="1" x14ac:dyDescent="0.2">
@@ -2862,7 +2870,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s" ph="1">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="C11" t="s" ph="1">
         <v>5</v>
@@ -2982,7 +2990,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s" ph="1">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="C20" t="s" ph="1">
         <v>5</v>
@@ -3029,18 +3037,18 @@
     </row>
     <row r="24" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B24" s="5" t="s" ph="1">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="C24" s="6" t="s" ph="1">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="D24" s="6" t="s" ph="1">
-        <v>201</v>
+        <v>193</v>
       </c>
     </row>
     <row r="25" spans="1:4" ph="1" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s" ph="1">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="C25" t="s" ph="1">
         <v>5</v>
@@ -3051,13 +3059,13 @@
     </row>
     <row r="26" spans="1:4" ht="40.799999999999997" ph="1" x14ac:dyDescent="0.2">
       <c r="B26" s="7" t="s" ph="1">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="C26" s="8" t="s" ph="1">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="D26" s="8" t="s" ph="1">
-        <v>204</v>
+        <v>196</v>
       </c>
     </row>
     <row r="27" spans="1:4" ph="1" x14ac:dyDescent="0.2">
@@ -3140,8 +3148,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -3181,7 +3189,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="184.8" x14ac:dyDescent="0.2">
@@ -3189,7 +3197,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -3220,12 +3228,12 @@
         <v>76</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="237.6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="158.4" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>183</v>
+        <v>354</v>
       </c>
       <c r="C9" t="s">
         <v>5</v>
@@ -3239,13 +3247,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="C10" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -3253,18 +3261,18 @@
         <v>4</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
       <c r="C11" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
     </row>
   </sheetData>
@@ -3278,8 +3286,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView topLeftCell="B22" workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+    <sheetView topLeftCell="B13" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -3295,7 +3303,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3319,7 +3327,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
@@ -3327,7 +3335,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -3343,56 +3351,56 @@
     </row>
     <row r="8" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>213</v>
+        <v>205</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>218</v>
+        <v>210</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>254</v>
+        <v>355</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -3439,12 +3447,12 @@
         <v>82</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>184</v>
+        <v>353</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -3474,7 +3482,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -3482,79 +3490,79 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>220</v>
+        <v>212</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>222</v>
+        <v>214</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>221</v>
+        <v>213</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>223</v>
+        <v>215</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>224</v>
+        <v>216</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>225</v>
+        <v>217</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>228</v>
+        <v>220</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>229</v>
+        <v>221</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>237</v>
+        <v>229</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
     </row>
   </sheetData>
@@ -3612,7 +3620,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="D4"/>
     </row>
@@ -3625,7 +3633,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -3694,7 +3702,7 @@
     </row>
     <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -3702,7 +3710,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -3713,18 +3721,18 @@
     </row>
     <row r="15" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
     </row>
   </sheetData>
@@ -3738,8 +3746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D68"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B46" sqref="B46"/>
+    <sheetView topLeftCell="A24" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -3755,7 +3763,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3779,7 +3787,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -3801,7 +3809,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="C7" t="s">
         <v>4</v>
@@ -3817,12 +3825,12 @@
     </row>
     <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -3844,13 +3852,13 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
       <c r="D12" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -3858,7 +3866,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="D13" t="s">
         <v>100</v>
@@ -3866,7 +3874,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -3874,26 +3882,26 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="C15" t="s">
         <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D16" t="s">
         <v>152</v>
-      </c>
-      <c r="D16" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D17" t="s">
         <v>68</v>
@@ -3904,7 +3912,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -3918,18 +3926,18 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>156</v>
+        <v>356</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
       </c>
       <c r="D19" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -3937,43 +3945,43 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C21" t="s">
         <v>4</v>
       </c>
       <c r="D21" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="D22" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" t="s">
         <v>161</v>
-      </c>
-      <c r="D22" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>4</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="C23" t="s">
-        <v>4</v>
-      </c>
-      <c r="D23" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="D24" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -3981,13 +3989,13 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>179</v>
+        <v>358</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
       </c>
       <c r="D25" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -3998,7 +4006,7 @@
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C27" t="s">
         <v>4</v>
@@ -4012,13 +4020,13 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C28" t="s">
         <v>4</v>
       </c>
       <c r="D28" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -4026,7 +4034,7 @@
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="D29" t="s">
         <v>125</v>
@@ -4037,7 +4045,7 @@
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="D30" t="s">
         <v>101</v>
@@ -4062,12 +4070,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>145</v>
+        <v>359</v>
       </c>
       <c r="D33" t="s">
         <v>104</v>
@@ -4086,7 +4094,7 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
@@ -4105,7 +4113,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -4113,7 +4121,7 @@
         <v>4</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C38" t="s">
         <v>4</v>
@@ -4138,18 +4146,18 @@
         <v>134</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>4</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>177</v>
+        <v>360</v>
       </c>
       <c r="C41" t="s">
         <v>4</v>
       </c>
       <c r="D41" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -4188,7 +4196,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -4228,7 +4236,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -4239,7 +4247,7 @@
     </row>
     <row r="7" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -4297,7 +4305,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>185</v>
+        <v>178</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -4316,8 +4324,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView topLeftCell="B7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -4357,7 +4365,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="171.6" x14ac:dyDescent="0.2">
@@ -4375,7 +4383,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="C8" t="s">
         <v>4</v>
@@ -4392,7 +4400,7 @@
         <v>5</v>
       </c>
       <c r="D9" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -4400,7 +4408,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="C10" t="s">
         <v>4</v>
@@ -4414,7 +4422,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="C11" t="s">
         <v>4</v>
@@ -4428,7 +4436,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>186</v>
+        <v>361</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
@@ -4460,7 +4468,7 @@
         <v>140</v>
       </c>
       <c r="D17" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
win11_en.xlsx: ASCII space is required at the end of image pathname?
</commit_message>
<xml_diff>
--- a/win11_en.xlsx
+++ b/win11_en.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta2025\fresta-github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D634B35A-0952-4437-9281-6AFB654D39C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C40446EC-2D1E-492F-A1A6-40A98D45DEB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="17496" windowHeight="10296" tabRatio="729" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="17496" windowHeight="10296" tabRatio="729" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -853,16 +853,10 @@
     <t xml:space="preserve">win11en-setting-bitlocker-incomplete.png </t>
   </si>
   <si>
-    <t>win11en-open-ctrlpanel.png</t>
-  </si>
-  <si>
     <t>① Click "Start Button" on the task bar ② Type "control panel" to the search form ③ Open "Control Panel".</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">win11en-ctrl-syssec-bitlocker-mgr.png </t>
-  </si>
-  <si>
     <t>Windows11 Pro has "BitLocker Device Encryption", Windows11 Home may have "Device Encryption". Click the one your PC has.</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -897,9 +891,6 @@
   <si>
     <t>win11en-printer-select.png</t>
     <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11en-bitlocker-backup-print.png</t>
   </si>
   <si>
     <t>FRESTA-TEXT-2024 Win11en chap.3</t>
@@ -1399,103 +1390,117 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>win11-en-part1-00.00.24.161.png</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.01.14.930.png</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.01.16.930.png</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.01.49.930.png</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.01.54.930.png</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.02.12.930.png</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.02.27.930.png</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.02.54.930.png</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.03.34.930.png</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.03.39.930.png</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.03.51.930.png</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.03.57.930.png</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.04.16.930.png</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.04.34.930.png</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.04.49.930.png</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.05.22.930.png</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.05.35.930.png</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.05.56.930.png</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.06.03.930.png</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.06.10.930.png</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.06.33.930.png</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.06.51.930.png</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.07.23.930.png</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.07.34.930.png</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.07.40.930.png</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.07.51.930.png</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.08.06.930.png</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.08.13.930.png</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.08.18.930.png</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.08.21.930.png</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.08.36.930.png</t>
+  </si>
+  <si>
+    <t>win11en-bitlocker-backup-print.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">win11en-ctrl-syssec-bitlocker-mgr.png </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11-en-part1-00.00.19.649.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>win11-en-part1-00.00.15.245.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.00.19.649.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.00.24.161.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.01.14.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.01.16.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.01.49.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.01.54.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.02.12.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.02.27.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.02.54.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.03.34.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.03.39.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.03.51.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.03.57.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.04.16.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.04.34.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.04.49.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.05.22.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.05.35.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.05.56.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.06.03.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.06.10.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.06.33.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.06.51.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.07.23.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.07.34.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.07.40.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.07.51.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.08.06.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.08.13.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.08.18.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.08.21.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.08.36.930.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">win11en-open-ctrlpanel.png </t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -2075,7 +2080,7 @@
         <v>6</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="C1" s="9"/>
       <c r="D1" s="9"/>
@@ -2085,7 +2090,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C2" s="9"/>
       <c r="D2" s="9"/>
@@ -2095,7 +2100,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C3" s="9"/>
       <c r="D3" s="9"/>
@@ -2105,7 +2110,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="C4" s="9"/>
       <c r="D4" s="9"/>
@@ -2119,7 +2124,7 @@
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="9"/>
       <c r="B6" s="8" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="C6" s="9"/>
       <c r="D6" s="9"/>
@@ -2133,7 +2138,7 @@
     <row r="8" spans="1:4" ht="237.6" x14ac:dyDescent="0.2">
       <c r="A8" s="9"/>
       <c r="B8" s="8" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C8" s="9"/>
       <c r="D8" s="9"/>
@@ -2147,7 +2152,7 @@
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="9"/>
       <c r="B10" s="8" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
@@ -2155,7 +2160,7 @@
     <row r="11" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
       <c r="B11" s="8" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="9"/>
@@ -2163,27 +2168,27 @@
     <row r="12" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A12" s="9"/>
       <c r="B12" s="8" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="C12" s="9" ph="1"/>
       <c r="D12" s="9" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A13" s="9"/>
       <c r="B13" s="8" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
       <c r="C13" s="9" ph="1"/>
       <c r="D13" s="9" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="10"/>
       <c r="B14" s="11" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="10"/>
@@ -2191,7 +2196,7 @@
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="12"/>
       <c r="B15" s="13" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
@@ -2199,31 +2204,31 @@
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="10"/>
       <c r="B16" s="11" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="10" t="s">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A17" s="10"/>
       <c r="B17" s="11" t="s">
-        <v>245</v>
+        <v>242</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="10" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A18" s="10"/>
       <c r="B18" s="11" t="s">
-        <v>246</v>
+        <v>243</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="10" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -2235,7 +2240,7 @@
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="12"/>
       <c r="B20" s="13" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="C20" s="12"/>
       <c r="D20" s="12"/>
@@ -2243,17 +2248,17 @@
     <row r="21" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A21" s="10"/>
       <c r="B21" s="11" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C21" s="10"/>
       <c r="D21" s="10" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A22" s="10"/>
       <c r="B22" s="11" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C22" s="10"/>
       <c r="D22" s="10"/>
@@ -2261,71 +2266,71 @@
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="10"/>
       <c r="B23" s="11" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C23" s="10"/>
       <c r="D23" s="10" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="10"/>
       <c r="B24" s="11" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C24" s="10"/>
       <c r="D24" s="10" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A25" s="10"/>
       <c r="B25" s="11" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="10" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="10"/>
       <c r="B26" s="11" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C26" s="10"/>
       <c r="D26" s="10" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A27" s="10"/>
       <c r="B27" s="11" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C27" s="10"/>
       <c r="D27" s="10" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A28" s="10"/>
       <c r="B28" s="11" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C28" s="10"/>
       <c r="D28" s="10" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" s="10"/>
       <c r="B29" s="11" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C29" s="10"/>
       <c r="D29" s="10" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -2333,27 +2338,27 @@
         <v>4</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C30" s="10"/>
       <c r="D30" s="10" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A31" s="10"/>
       <c r="B31" s="11" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C31" s="10"/>
       <c r="D31" s="10" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A32" s="10"/>
       <c r="B32" s="11" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C32" s="10"/>
       <c r="D32" s="10"/>
@@ -2367,7 +2372,7 @@
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A34" s="12"/>
       <c r="B34" s="13" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C34" s="12"/>
       <c r="D34" s="12"/>
@@ -2375,7 +2380,7 @@
     <row r="35" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A35" s="10"/>
       <c r="B35" s="11" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C35" s="10"/>
       <c r="D35" s="10"/>
@@ -2383,91 +2388,91 @@
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A36" s="10"/>
       <c r="B36" s="11" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C36" s="10"/>
       <c r="D36" s="10" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A37" s="10"/>
       <c r="B37" s="11" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C37" s="10"/>
       <c r="D37" s="10" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A38" s="10"/>
       <c r="B38" s="11" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C38" s="10"/>
       <c r="D38" s="10" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A39" s="10"/>
       <c r="B39" s="11" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C39" s="10"/>
       <c r="D39" s="10" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="66" x14ac:dyDescent="0.2">
       <c r="A40" s="10"/>
       <c r="B40" s="11" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C40" s="10"/>
       <c r="D40" s="10" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" s="10"/>
       <c r="B41" s="11" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C41" s="10"/>
       <c r="D41" s="10" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A42" s="10"/>
       <c r="B42" s="11" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C42" s="10"/>
       <c r="D42" s="10" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A43" s="10"/>
       <c r="B43" s="11" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C43" s="10"/>
       <c r="D43" s="10" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A44" s="10"/>
       <c r="B44" s="11" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C44" s="10"/>
       <c r="D44" s="10" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -2479,7 +2484,7 @@
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="14"/>
       <c r="B46" s="15" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C46" s="14"/>
       <c r="D46" s="14"/>
@@ -2487,7 +2492,7 @@
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A47" s="16"/>
       <c r="B47" s="17" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C47" s="16"/>
       <c r="D47" s="16"/>
@@ -2495,31 +2500,31 @@
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A48" s="14"/>
       <c r="B48" s="15" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C48" s="14"/>
       <c r="D48" s="14" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A49" s="14"/>
       <c r="B49" s="15" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C49" s="14"/>
       <c r="D49" s="14" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="50" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A50" s="14"/>
       <c r="B50" s="15" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C50" s="14"/>
       <c r="D50" s="14" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -2531,7 +2536,7 @@
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A52" s="16"/>
       <c r="B52" s="17" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C52" s="16"/>
       <c r="D52" s="16"/>
@@ -2539,17 +2544,17 @@
     <row r="53" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A53" s="14"/>
       <c r="B53" s="15" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C53" s="14"/>
       <c r="D53" s="14" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="54" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A54" s="14"/>
       <c r="B54" s="15" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C54" s="14"/>
       <c r="D54" s="14"/>
@@ -2557,61 +2562,61 @@
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A55" s="14"/>
       <c r="B55" s="15" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C55" s="14"/>
       <c r="D55" s="14" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A56" s="14"/>
       <c r="B56" s="15" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C56" s="14"/>
       <c r="D56" s="14" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="57" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A57" s="14"/>
       <c r="B57" s="15" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C57" s="14"/>
       <c r="D57" s="14" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="58" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A58" s="14"/>
       <c r="B58" s="15" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C58" s="14"/>
       <c r="D58" s="14" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A59" s="14"/>
       <c r="B59" s="15" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C59" s="14"/>
       <c r="D59" s="14" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A60" s="14"/>
       <c r="B60" s="15" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C60" s="14"/>
       <c r="D60" s="14" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
     </row>
     <row r="61" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -2619,27 +2624,27 @@
         <v>4</v>
       </c>
       <c r="B61" s="15" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C61" s="14"/>
       <c r="D61" s="14" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="62" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A62" s="14"/>
       <c r="B62" s="19" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C62" s="14"/>
       <c r="D62" s="14" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A63" s="14"/>
       <c r="B63" s="15" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C63" s="14"/>
       <c r="D63" s="14"/>
@@ -2653,7 +2658,7 @@
     <row r="65" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A65" s="21"/>
       <c r="B65" s="22" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C65" s="21"/>
       <c r="D65" s="21"/>
@@ -2661,7 +2666,7 @@
     <row r="66" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A66" s="14"/>
       <c r="B66" s="15" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C66" s="14"/>
       <c r="D66" s="21"/>
@@ -2669,41 +2674,41 @@
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A67" s="14"/>
       <c r="B67" s="15" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C67" s="14"/>
       <c r="D67" s="14" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A68" s="14"/>
       <c r="B68" s="15" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C68" s="14"/>
       <c r="D68" s="14" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A69" s="14"/>
       <c r="B69" s="15" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C69" s="14"/>
       <c r="D69" s="14" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="14"/>
       <c r="B70" s="15" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C70" s="14"/>
       <c r="D70" s="14" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="71" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -2711,49 +2716,49 @@
         <v>4</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C71" s="14"/>
       <c r="D71" s="14" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="72" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A72" s="14"/>
       <c r="B72" s="15" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C72" s="14"/>
       <c r="D72" s="14" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A73" s="14"/>
       <c r="B73" s="3" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C73" s="14"/>
       <c r="D73" s="14" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A74" s="14"/>
       <c r="B74" s="3" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C74" s="14"/>
       <c r="D74" s="14" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B75" s="3" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="D75" s="14" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -3157,8 +3162,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:D39"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -3206,7 +3211,7 @@
         <v>4</v>
       </c>
       <c r="D6" s="9" t="s" ph="1">
-        <v>350</v>
+        <v>347</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="97.2" customHeight="1" x14ac:dyDescent="0.2">
@@ -3217,7 +3222,7 @@
         <v>19</v>
       </c>
       <c r="D7" s="3" t="s" ph="1">
-        <v>351</v>
+        <v>382</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3225,7 +3230,7 @@
         <v>19</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>352</v>
+        <v>381</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -3236,7 +3241,7 @@
         <v>19</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>353</v>
+        <v>348</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -3247,7 +3252,7 @@
         <v>19</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>354</v>
+        <v>349</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -3258,7 +3263,7 @@
         <v>19</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>355</v>
+        <v>350</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -3266,7 +3271,7 @@
         <v>19</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>356</v>
+        <v>351</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -3274,7 +3279,7 @@
         <v>19</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>357</v>
+        <v>352</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -3282,7 +3287,7 @@
         <v>19</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -3290,7 +3295,7 @@
         <v>19</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>359</v>
+        <v>354</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -3298,7 +3303,7 @@
         <v>19</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>360</v>
+        <v>355</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.2">
@@ -3306,7 +3311,7 @@
         <v>19</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>361</v>
+        <v>356</v>
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.2">
@@ -3314,7 +3319,7 @@
         <v>19</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>362</v>
+        <v>357</v>
       </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.2">
@@ -3322,7 +3327,7 @@
         <v>19</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>363</v>
+        <v>358</v>
       </c>
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.2">
@@ -3330,7 +3335,7 @@
         <v>19</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>364</v>
+        <v>359</v>
       </c>
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.2">
@@ -3338,7 +3343,7 @@
         <v>19</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>365</v>
+        <v>360</v>
       </c>
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.2">
@@ -3346,7 +3351,7 @@
         <v>19</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>366</v>
+        <v>361</v>
       </c>
     </row>
     <row r="23" spans="3:4" x14ac:dyDescent="0.2">
@@ -3354,7 +3359,7 @@
         <v>19</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>367</v>
+        <v>362</v>
       </c>
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.2">
@@ -3362,7 +3367,7 @@
         <v>19</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>368</v>
+        <v>363</v>
       </c>
     </row>
     <row r="25" spans="3:4" x14ac:dyDescent="0.2">
@@ -3370,7 +3375,7 @@
         <v>19</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>369</v>
+        <v>364</v>
       </c>
     </row>
     <row r="26" spans="3:4" x14ac:dyDescent="0.2">
@@ -3378,7 +3383,7 @@
         <v>19</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>370</v>
+        <v>365</v>
       </c>
     </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.2">
@@ -3386,7 +3391,7 @@
         <v>19</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.2">
@@ -3394,7 +3399,7 @@
         <v>19</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>372</v>
+        <v>367</v>
       </c>
     </row>
     <row r="29" spans="3:4" x14ac:dyDescent="0.2">
@@ -3402,7 +3407,7 @@
         <v>19</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>373</v>
+        <v>368</v>
       </c>
     </row>
     <row r="30" spans="3:4" x14ac:dyDescent="0.2">
@@ -3410,7 +3415,7 @@
         <v>19</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>374</v>
+        <v>369</v>
       </c>
     </row>
     <row r="31" spans="3:4" x14ac:dyDescent="0.2">
@@ -3418,7 +3423,7 @@
         <v>19</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>375</v>
+        <v>370</v>
       </c>
     </row>
     <row r="32" spans="3:4" x14ac:dyDescent="0.2">
@@ -3426,7 +3431,7 @@
         <v>19</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>376</v>
+        <v>371</v>
       </c>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.2">
@@ -3434,7 +3439,7 @@
         <v>19</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.2">
@@ -3442,7 +3447,7 @@
         <v>19</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>378</v>
+        <v>373</v>
       </c>
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.2">
@@ -3450,7 +3455,7 @@
         <v>19</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>379</v>
+        <v>374</v>
       </c>
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.2">
@@ -3458,7 +3463,7 @@
         <v>19</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>380</v>
+        <v>375</v>
       </c>
     </row>
     <row r="37" spans="3:4" x14ac:dyDescent="0.2">
@@ -3466,7 +3471,7 @@
         <v>19</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.2">
@@ -3474,7 +3479,7 @@
         <v>19</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>382</v>
+        <v>377</v>
       </c>
     </row>
     <row r="39" spans="3:4" x14ac:dyDescent="0.2">
@@ -3482,7 +3487,7 @@
         <v>19</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>383</v>
+        <v>378</v>
       </c>
     </row>
   </sheetData>
@@ -3496,8 +3501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="B23" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -3585,18 +3590,18 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
@@ -3604,13 +3609,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="C13" t="s">
         <v>4</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -3662,7 +3667,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C18" t="s">
         <v>4</v>
@@ -3692,7 +3697,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -3716,7 +3721,7 @@
     </row>
     <row r="24" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>204</v>
@@ -3732,47 +3737,47 @@
     </row>
     <row r="26" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>207</v>
+        <v>383</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>209</v>
+        <v>380</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>219</v>
+        <v>379</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D30" s="3" t="s">
         <v>215</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -3830,7 +3835,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D4"/>
     </row>
@@ -3843,7 +3848,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C6" t="s">
         <v>4</v>
@@ -3912,7 +3917,7 @@
     </row>
     <row r="13" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -3920,7 +3925,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C14" t="s">
         <v>4</v>
@@ -3931,18 +3936,18 @@
     </row>
     <row r="15" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
   </sheetData>
@@ -3997,7 +4002,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -4136,7 +4141,7 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="C19" t="s">
         <v>4</v>
@@ -4177,7 +4182,7 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C23" t="s">
         <v>4</v>
@@ -4199,7 +4204,7 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C25" t="s">
         <v>4</v>
@@ -4285,7 +4290,7 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="D33" t="s">
         <v>99</v>
@@ -4304,7 +4309,7 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C35" t="s">
         <v>4</v>
@@ -4361,7 +4366,7 @@
         <v>4</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C41" t="s">
         <v>4</v>
@@ -4446,7 +4451,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -4575,7 +4580,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="171.6" x14ac:dyDescent="0.2">
@@ -4646,7 +4651,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
win11_en.xlsx: chapter 1, append U+0020 to all PNG pathnames
</commit_message>
<xml_diff>
--- a/win11_en.xlsx
+++ b/win11_en.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta2025\fresta-github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C40446EC-2D1E-492F-A1A6-40A98D45DEB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9973AFFE-F222-4558-A29B-5DBE245E01BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="17496" windowHeight="10296" tabRatio="729" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="17496" windowHeight="10296" tabRatio="729" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -1390,99 +1390,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11-en-part1-00.00.24.161.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.01.14.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.01.16.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.01.49.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.01.54.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.02.12.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.02.27.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.02.54.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.03.34.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.03.39.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.03.51.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.03.57.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.04.16.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.04.34.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.04.49.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.05.22.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.05.35.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.05.56.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.06.03.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.06.10.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.06.33.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.06.51.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.07.23.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.07.34.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.07.40.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.07.51.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.08.06.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.08.13.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.08.18.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.08.21.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.08.36.930.png</t>
-  </si>
-  <si>
     <t>win11en-bitlocker-backup-print.png</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1491,15 +1398,139 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>win11-en-part1-00.00.19.649.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11-en-part1-00.00.15.245.png</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t xml:space="preserve">win11en-open-ctrlpanel.png </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">win11-en-part1-00.00.15.245.png </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">win11-en-part1-00.00.19.649.png </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">win11-en-part1-00.00.24.161.png </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">win11-en-part1-00.01.14.930.png </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">win11-en-part1-00.01.16.930.png </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">win11-en-part1-00.01.49.930.png </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">win11-en-part1-00.01.54.930.png </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">win11-en-part1-00.02.12.930.png </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">win11-en-part1-00.02.27.930.png </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">win11-en-part1-00.02.54.930.png </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">win11-en-part1-00.03.34.930.png </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">win11-en-part1-00.03.39.930.png </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">win11-en-part1-00.03.51.930.png </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">win11-en-part1-00.03.57.930.png </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">win11-en-part1-00.04.16.930.png </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">win11-en-part1-00.04.34.930.png </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">win11-en-part1-00.04.49.930.png </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">win11-en-part1-00.05.22.930.png </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">win11-en-part1-00.05.35.930.png </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">win11-en-part1-00.05.56.930.png </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">win11-en-part1-00.06.03.930.png </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">win11-en-part1-00.06.10.930.png </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">win11-en-part1-00.06.33.930.png </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">win11-en-part1-00.06.51.930.png </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">win11-en-part1-00.07.23.930.png </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">win11-en-part1-00.07.34.930.png </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">win11-en-part1-00.07.40.930.png </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">win11-en-part1-00.07.51.930.png </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">win11-en-part1-00.08.06.930.png </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">win11-en-part1-00.08.13.930.png </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">win11-en-part1-00.08.18.930.png </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">win11-en-part1-00.08.21.930.png </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">win11-en-part1-00.08.36.930.png </t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -2772,7 +2803,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF0FC8B8-3740-45D4-A5FA-75052BCDA48C}">
   <dimension ref="A1:D48"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A8" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
@@ -3162,8 +3193,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -3222,7 +3253,7 @@
         <v>19</v>
       </c>
       <c r="D7" s="3" t="s" ph="1">
-        <v>382</v>
+        <v>351</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
@@ -3230,7 +3261,7 @@
         <v>19</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>381</v>
+        <v>352</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -3241,7 +3272,7 @@
         <v>19</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>348</v>
+        <v>353</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -3252,7 +3283,7 @@
         <v>19</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>349</v>
+        <v>354</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -3263,7 +3294,7 @@
         <v>19</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>350</v>
+        <v>355</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -3271,7 +3302,7 @@
         <v>19</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>351</v>
+        <v>356</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -3279,7 +3310,7 @@
         <v>19</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>352</v>
+        <v>357</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -3287,7 +3318,7 @@
         <v>19</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>353</v>
+        <v>358</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -3295,7 +3326,7 @@
         <v>19</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>354</v>
+        <v>359</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -3303,7 +3334,7 @@
         <v>19</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>355</v>
+        <v>360</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.2">
@@ -3311,7 +3342,7 @@
         <v>19</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>356</v>
+        <v>361</v>
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.2">
@@ -3319,7 +3350,7 @@
         <v>19</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>357</v>
+        <v>362</v>
       </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.2">
@@ -3327,7 +3358,7 @@
         <v>19</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>358</v>
+        <v>363</v>
       </c>
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.2">
@@ -3335,7 +3366,7 @@
         <v>19</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>359</v>
+        <v>364</v>
       </c>
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.2">
@@ -3343,7 +3374,7 @@
         <v>19</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>360</v>
+        <v>365</v>
       </c>
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.2">
@@ -3351,7 +3382,7 @@
         <v>19</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>361</v>
+        <v>366</v>
       </c>
     </row>
     <row r="23" spans="3:4" x14ac:dyDescent="0.2">
@@ -3359,7 +3390,7 @@
         <v>19</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>362</v>
+        <v>367</v>
       </c>
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.2">
@@ -3367,7 +3398,7 @@
         <v>19</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>363</v>
+        <v>368</v>
       </c>
     </row>
     <row r="25" spans="3:4" x14ac:dyDescent="0.2">
@@ -3375,7 +3406,7 @@
         <v>19</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>364</v>
+        <v>369</v>
       </c>
     </row>
     <row r="26" spans="3:4" x14ac:dyDescent="0.2">
@@ -3383,7 +3414,7 @@
         <v>19</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>365</v>
+        <v>370</v>
       </c>
     </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.2">
@@ -3391,7 +3422,7 @@
         <v>19</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.2">
@@ -3399,7 +3430,7 @@
         <v>19</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>367</v>
+        <v>372</v>
       </c>
     </row>
     <row r="29" spans="3:4" x14ac:dyDescent="0.2">
@@ -3407,7 +3438,7 @@
         <v>19</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>368</v>
+        <v>373</v>
       </c>
     </row>
     <row r="30" spans="3:4" x14ac:dyDescent="0.2">
@@ -3415,7 +3446,7 @@
         <v>19</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>369</v>
+        <v>374</v>
       </c>
     </row>
     <row r="31" spans="3:4" x14ac:dyDescent="0.2">
@@ -3423,7 +3454,7 @@
         <v>19</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>370</v>
+        <v>375</v>
       </c>
     </row>
     <row r="32" spans="3:4" x14ac:dyDescent="0.2">
@@ -3431,7 +3462,7 @@
         <v>19</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>371</v>
+        <v>376</v>
       </c>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.2">
@@ -3439,7 +3470,7 @@
         <v>19</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>372</v>
+        <v>377</v>
       </c>
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.2">
@@ -3447,7 +3478,7 @@
         <v>19</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>373</v>
+        <v>378</v>
       </c>
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.2">
@@ -3455,7 +3486,7 @@
         <v>19</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>374</v>
+        <v>379</v>
       </c>
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.2">
@@ -3463,7 +3494,7 @@
         <v>19</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>375</v>
+        <v>380</v>
       </c>
     </row>
     <row r="37" spans="3:4" x14ac:dyDescent="0.2">
@@ -3471,7 +3502,7 @@
         <v>19</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>376</v>
+        <v>381</v>
       </c>
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.2">
@@ -3479,7 +3510,7 @@
         <v>19</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>377</v>
+        <v>382</v>
       </c>
     </row>
     <row r="39" spans="3:4" x14ac:dyDescent="0.2">
@@ -3487,7 +3518,7 @@
         <v>19</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>378</v>
+        <v>383</v>
       </c>
     </row>
   </sheetData>
@@ -3501,8 +3532,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B23" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView topLeftCell="B23" workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -3740,7 +3771,7 @@
         <v>207</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>383</v>
+        <v>350</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -3748,7 +3779,7 @@
         <v>208</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>380</v>
+        <v>349</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -3756,7 +3787,7 @@
         <v>211</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>379</v>
+        <v>348</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
win11_en.xlsx: try to embed a YouTube link in chapter 1
</commit_message>
<xml_diff>
--- a/win11_en.xlsx
+++ b/win11_en.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta2025\fresta-github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9973AFFE-F222-4558-A29B-5DBE245E01BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{681557C8-5A59-4A61-8509-AFE2A53FC07F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="17496" windowHeight="10296" tabRatio="729" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="12260" tabRatio="729" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="385">
   <si>
     <t>header1</t>
   </si>
@@ -1531,6 +1531,10 @@
   </si>
   <si>
     <t xml:space="preserve">win11-en-part1-00.08.36.930.png </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>This is a movie of the procedure described in this chapter.</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -3191,10 +3195,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D39"/>
+  <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D41" sqref="D41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -3237,53 +3241,34 @@
         <v>191</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="9" t="s" ph="1">
+    <row r="8" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="D8" s="9" t="s" ph="1">
         <v>347</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="97.2" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" s="3" t="s" ph="1">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C8" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="97.2" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="3" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>4</v>
-      </c>
+      <c r="D9" s="3" t="s" ph="1">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C10" s="9" t="s">
         <v>19</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -3294,23 +3279,29 @@
         <v>19</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>4</v>
+      </c>
       <c r="C12" s="9" t="s">
         <v>19</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
       <c r="C13" s="9" t="s">
         <v>19</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -3318,7 +3309,7 @@
         <v>19</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -3326,7 +3317,7 @@
         <v>19</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -3334,7 +3325,7 @@
         <v>19</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.2">
@@ -3342,7 +3333,7 @@
         <v>19</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.2">
@@ -3350,7 +3341,7 @@
         <v>19</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.2">
@@ -3358,7 +3349,7 @@
         <v>19</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.2">
@@ -3366,7 +3357,7 @@
         <v>19</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.2">
@@ -3374,7 +3365,7 @@
         <v>19</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.2">
@@ -3382,7 +3373,7 @@
         <v>19</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="23" spans="3:4" x14ac:dyDescent="0.2">
@@ -3390,7 +3381,7 @@
         <v>19</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.2">
@@ -3398,7 +3389,7 @@
         <v>19</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="25" spans="3:4" x14ac:dyDescent="0.2">
@@ -3406,7 +3397,7 @@
         <v>19</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="26" spans="3:4" x14ac:dyDescent="0.2">
@@ -3414,7 +3405,7 @@
         <v>19</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.2">
@@ -3422,7 +3413,7 @@
         <v>19</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.2">
@@ -3430,7 +3421,7 @@
         <v>19</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="29" spans="3:4" x14ac:dyDescent="0.2">
@@ -3438,7 +3429,7 @@
         <v>19</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="30" spans="3:4" x14ac:dyDescent="0.2">
@@ -3446,7 +3437,7 @@
         <v>19</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="31" spans="3:4" x14ac:dyDescent="0.2">
@@ -3454,7 +3445,7 @@
         <v>19</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="32" spans="3:4" x14ac:dyDescent="0.2">
@@ -3462,7 +3453,7 @@
         <v>19</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.2">
@@ -3470,7 +3461,7 @@
         <v>19</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.2">
@@ -3478,7 +3469,7 @@
         <v>19</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.2">
@@ -3486,7 +3477,7 @@
         <v>19</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.2">
@@ -3494,7 +3485,7 @@
         <v>19</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
     </row>
     <row r="37" spans="3:4" x14ac:dyDescent="0.2">
@@ -3502,7 +3493,7 @@
         <v>19</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.2">
@@ -3510,7 +3501,7 @@
         <v>19</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="39" spans="3:4" x14ac:dyDescent="0.2">
@@ -3518,6 +3509,22 @@
         <v>19</v>
       </c>
       <c r="D39" s="3" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="40" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C40" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="41" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C41" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D41" s="3" t="s">
         <v>383</v>
       </c>
     </row>

</xml_diff>

<commit_message>
win11_en.xlsx: chapter 1, revert 86f1cf7b6feeb040fb223be3edefefaedb7d6774
</commit_message>
<xml_diff>
--- a/win11_en.xlsx
+++ b/win11_en.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta2025\fresta-github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18670A6B-860C-4CFD-A813-5A63E8EB1EC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9E71B88-2D19-4E89-8DED-27F2A3C6EFB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="12260" tabRatio="729" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1394,147 +1394,147 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>win11-en-part1-00.00.19.649.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11-en-part1-00.00.15.245.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t xml:space="preserve">win11en-open-ctrlpanel.png </t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t xml:space="preserve">win11-en-part1-00.00.15.245.png </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">win11-en-part1-00.00.19.649.png </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">win11-en-part1-00.00.24.161.png </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">win11-en-part1-00.01.14.930.png </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">win11-en-part1-00.01.16.930.png </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">win11-en-part1-00.01.49.930.png </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">win11-en-part1-00.01.54.930.png </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">win11-en-part1-00.02.12.930.png </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">win11-en-part1-00.02.27.930.png </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">win11-en-part1-00.02.54.930.png </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">win11-en-part1-00.03.34.930.png </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">win11-en-part1-00.03.39.930.png </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">win11-en-part1-00.03.51.930.png </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">win11-en-part1-00.03.57.930.png </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">win11-en-part1-00.04.16.930.png </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">win11-en-part1-00.04.34.930.png </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">win11-en-part1-00.04.49.930.png </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">win11-en-part1-00.05.22.930.png </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">win11-en-part1-00.05.35.930.png </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">win11-en-part1-00.05.56.930.png </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">win11-en-part1-00.06.03.930.png </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">win11-en-part1-00.06.10.930.png </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">win11-en-part1-00.06.33.930.png </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">win11-en-part1-00.06.51.930.png </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">win11-en-part1-00.07.23.930.png </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">win11-en-part1-00.07.34.930.png </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">win11-en-part1-00.07.40.930.png </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">win11-en-part1-00.07.51.930.png </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">win11-en-part1-00.08.06.930.png </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">win11-en-part1-00.08.13.930.png </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">win11-en-part1-00.08.18.930.png </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">win11-en-part1-00.08.21.930.png </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">win11-en-part1-00.08.36.930.png </t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>This is a movie of the procedure described in this chapter.</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>raw:&lt;iframe width="100%" height="315" src="https://www.youtube.com/embed/kz1XpJ6mQTg?list=PLjGYIiYIuSrDEjw795bCCO9RHIpHIYWea" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen=""&gt;&lt;/iframe&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11-en-part1-00.00.24.161.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11-en-part1-00.01.14.930.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11-en-part1-00.01.16.930.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11-en-part1-00.01.49.930.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11-en-part1-00.01.54.930.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11-en-part1-00.02.12.930.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11-en-part1-00.02.27.930.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11-en-part1-00.02.54.930.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11-en-part1-00.03.34.930.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11-en-part1-00.03.39.930.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11-en-part1-00.03.51.930.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11-en-part1-00.03.57.930.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11-en-part1-00.04.16.930.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11-en-part1-00.04.34.930.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11-en-part1-00.04.49.930.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11-en-part1-00.05.22.930.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11-en-part1-00.05.35.930.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11-en-part1-00.05.56.930.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11-en-part1-00.06.03.930.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11-en-part1-00.06.10.930.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11-en-part1-00.06.33.930.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11-en-part1-00.06.51.930.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11-en-part1-00.07.23.930.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11-en-part1-00.07.34.930.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11-en-part1-00.07.40.930.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11-en-part1-00.07.51.930.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11-en-part1-00.08.06.930.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11-en-part1-00.08.13.930.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11-en-part1-00.08.18.930.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11-en-part1-00.08.21.930.png</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11-en-part1-00.08.36.930.png</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -3198,8 +3198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="D41" sqref="D41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -3247,10 +3247,10 @@
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>383</v>
+        <v>352</v>
       </c>
       <c r="D8" s="24" t="s" ph="1">
-        <v>384</v>
+        <v>353</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="97.2" customHeight="1" x14ac:dyDescent="0.2">
@@ -3269,7 +3269,7 @@
         <v>19</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -3280,7 +3280,7 @@
         <v>19</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -3291,7 +3291,7 @@
         <v>19</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -3302,7 +3302,7 @@
         <v>19</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -3310,7 +3310,7 @@
         <v>19</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>355</v>
+        <v>357</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -3318,7 +3318,7 @@
         <v>19</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -3326,7 +3326,7 @@
         <v>19</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.2">
@@ -3334,7 +3334,7 @@
         <v>19</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.2">
@@ -3342,7 +3342,7 @@
         <v>19</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.2">
@@ -3350,7 +3350,7 @@
         <v>19</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.2">
@@ -3358,7 +3358,7 @@
         <v>19</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.2">
@@ -3366,7 +3366,7 @@
         <v>19</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.2">
@@ -3374,7 +3374,7 @@
         <v>19</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
     </row>
     <row r="23" spans="3:4" x14ac:dyDescent="0.2">
@@ -3382,7 +3382,7 @@
         <v>19</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.2">
@@ -3390,7 +3390,7 @@
         <v>19</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
     </row>
     <row r="25" spans="3:4" x14ac:dyDescent="0.2">
@@ -3398,7 +3398,7 @@
         <v>19</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
     </row>
     <row r="26" spans="3:4" x14ac:dyDescent="0.2">
@@ -3406,7 +3406,7 @@
         <v>19</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
     </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.2">
@@ -3414,7 +3414,7 @@
         <v>19</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.2">
@@ -3422,7 +3422,7 @@
         <v>19</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
     </row>
     <row r="29" spans="3:4" x14ac:dyDescent="0.2">
@@ -3430,7 +3430,7 @@
         <v>19</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
     </row>
     <row r="30" spans="3:4" x14ac:dyDescent="0.2">
@@ -3438,7 +3438,7 @@
         <v>19</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
     </row>
     <row r="31" spans="3:4" x14ac:dyDescent="0.2">
@@ -3446,7 +3446,7 @@
         <v>19</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
     </row>
     <row r="32" spans="3:4" x14ac:dyDescent="0.2">
@@ -3454,7 +3454,7 @@
         <v>19</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>373</v>
+        <v>375</v>
       </c>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.2">
@@ -3462,7 +3462,7 @@
         <v>19</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.2">
@@ -3470,7 +3470,7 @@
         <v>19</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.2">
@@ -3478,7 +3478,7 @@
         <v>19</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.2">
@@ -3486,7 +3486,7 @@
         <v>19</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
     </row>
     <row r="37" spans="3:4" x14ac:dyDescent="0.2">
@@ -3494,7 +3494,7 @@
         <v>19</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.2">
@@ -3502,7 +3502,7 @@
         <v>19</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
     </row>
     <row r="39" spans="3:4" x14ac:dyDescent="0.2">
@@ -3510,7 +3510,7 @@
         <v>19</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
     </row>
     <row r="40" spans="3:4" x14ac:dyDescent="0.2">
@@ -3518,7 +3518,7 @@
         <v>19</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
     </row>
     <row r="41" spans="3:4" x14ac:dyDescent="0.2">
@@ -3526,7 +3526,7 @@
         <v>19</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>382</v>
+        <v>384</v>
       </c>
     </row>
   </sheetData>
@@ -3779,7 +3779,7 @@
         <v>207</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
win11_en.xlsx: fix chapter 2
</commit_message>
<xml_diff>
--- a/win11_en.xlsx
+++ b/win11_en.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta2025\fresta-github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94593FDF-A7B0-4382-9525-4FDADD301843}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E57D2C5-CED2-4EDE-9097-4323BA262364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="12260" tabRatio="729" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12300" tabRatio="729" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -1297,12 +1297,12 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.6328125" customWidth="1"/>
+    <col min="2" max="2" width="100.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6328125" customWidth="1"/>
+    <col min="4" max="4" width="20.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -1329,7 +1329,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="66" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="65" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1343,7 +1343,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="52" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1368,17 +1368,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EFCA2B8-55C7-4AC3-9E13-35156DBD8BC5}">
   <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="88.44140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="3"/>
-    <col min="4" max="4" width="34.88671875" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="1" width="10.90625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="88.453125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="8.90625" style="3"/>
+    <col min="4" max="4" width="34.90625" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="8.90625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -1433,7 +1433,7 @@
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="19.5" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="2" t="s">
         <v>280</v>
@@ -1895,12 +1895,12 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="64.5546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="29.44140625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="10.6328125" customWidth="1"/>
+    <col min="2" max="2" width="64.54296875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="10.6328125" customWidth="1"/>
+    <col min="4" max="4" width="29.453125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -1940,7 +1940,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="97.2" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="97.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -1954,7 +1954,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="19.5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -2236,18 +2236,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="89.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="32.109375" style="3" customWidth="1"/>
+    <col min="1" max="1" width="10.6328125" customWidth="1"/>
+    <col min="2" max="2" width="89.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6328125" customWidth="1"/>
+    <col min="4" max="4" width="32.08984375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -2282,23 +2282,15 @@
         <v>259</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2" t="s">
+    <row r="7" spans="1:4" ht="19.5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>280</v>
       </c>
-      <c r="D6" s="4" t="s" ph="1">
+      <c r="D7" s="4" t="s" ph="1">
         <v>246</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C7" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -2306,7 +2298,7 @@
         <v>9</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -2314,7 +2306,7 @@
         <v>9</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -2322,7 +2314,7 @@
         <v>9</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -2330,7 +2322,7 @@
         <v>9</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -2338,18 +2330,15 @@
         <v>9</v>
       </c>
       <c r="D12" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -2360,7 +2349,7 @@
         <v>9</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -2371,26 +2360,26 @@
         <v>9</v>
       </c>
       <c r="D15" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="3" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C16" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" s="3" t="s">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="3" t="s">
         <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -2401,7 +2390,7 @@
         <v>9</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -2412,7 +2401,7 @@
         <v>9</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -2423,7 +2412,7 @@
         <v>9</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -2434,7 +2423,7 @@
         <v>9</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -2445,15 +2434,18 @@
         <v>9</v>
       </c>
       <c r="D22" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>4</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="3" t="s">
         <v>62</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C23" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -2461,7 +2453,7 @@
         <v>9</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -2469,7 +2461,7 @@
         <v>9</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -2477,7 +2469,7 @@
         <v>9</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -2485,7 +2477,7 @@
         <v>9</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -2493,7 +2485,7 @@
         <v>9</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -2501,7 +2493,7 @@
         <v>9</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -2509,7 +2501,7 @@
         <v>9</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -2517,7 +2509,7 @@
         <v>9</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -2525,7 +2517,7 @@
         <v>9</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.2">
@@ -2533,7 +2525,7 @@
         <v>9</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.2">
@@ -2541,6 +2533,14 @@
         <v>9</v>
       </c>
       <c r="D34" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="35" spans="3:4" x14ac:dyDescent="0.2">
+      <c r="C35" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>74</v>
       </c>
     </row>
@@ -2559,12 +2559,12 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="66.5546875" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="10.6328125" customWidth="1"/>
+    <col min="2" max="2" width="66.54296875" customWidth="1"/>
+    <col min="3" max="3" width="10.6328125" customWidth="1"/>
+    <col min="4" max="4" width="20.6328125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -2614,7 +2614,7 @@
       <c r="B6" s="1"/>
       <c r="D6"/>
     </row>
-    <row r="7" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="19.5" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
         <v>280</v>
       </c>
@@ -3039,12 +3039,12 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="76.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.6328125" customWidth="1"/>
+    <col min="2" max="2" width="76.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6328125" customWidth="1"/>
+    <col min="4" max="4" width="20.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -3090,7 +3090,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="19.5" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
         <v>280</v>
       </c>
@@ -3452,7 +3452,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" ht="19.5" x14ac:dyDescent="0.2">
       <c r="C45" s="4" t="s">
         <v>9</v>
       </c>
@@ -3495,10 +3495,10 @@
         <v>163</v>
       </c>
     </row>
-    <row r="61" spans="3:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+    <row r="61" spans="3:4" ht="19.5" x14ac:dyDescent="0.2">
       <c r="D61" ph="1"/>
     </row>
-    <row r="68" spans="4:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+    <row r="68" spans="4:4" ht="19.5" x14ac:dyDescent="0.2">
       <c r="D68" ph="1"/>
     </row>
   </sheetData>
@@ -3516,12 +3516,12 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.6328125" customWidth="1"/>
     <col min="2" max="2" width="81" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="3" max="3" width="10.6328125" customWidth="1"/>
+    <col min="4" max="4" width="20.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -3565,7 +3565,7 @@
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1"/>
     </row>
-    <row r="8" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="19.5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -3707,12 +3707,12 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.6328125" customWidth="1"/>
+    <col min="2" max="2" width="100.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6328125" customWidth="1"/>
+    <col min="4" max="4" width="20.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -3747,7 +3747,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="19.5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -3913,12 +3913,12 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" customWidth="1"/>
-    <col min="2" max="2" width="100.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="10.6328125" customWidth="1"/>
+    <col min="2" max="2" width="100.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.6328125" customWidth="1"/>
+    <col min="4" max="4" width="20.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -3953,7 +3953,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="19.5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>4</v>
       </c>
@@ -4182,13 +4182,13 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="3"/>
-    <col min="2" max="2" width="88.44140625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="3"/>
-    <col min="4" max="4" width="34.88671875" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="3"/>
+    <col min="1" max="1" width="8.90625" style="3"/>
+    <col min="2" max="2" width="88.453125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="8.90625" style="3"/>
+    <col min="4" max="4" width="34.90625" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="8.90625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -4243,7 +4243,7 @@
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="19.5" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="2" t="s">
         <v>280</v>

</xml_diff>

<commit_message>
win11_en.xlsx: update chapter 1
</commit_message>
<xml_diff>
--- a/win11_en.xlsx
+++ b/win11_en.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta2025\fresta-github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E57D2C5-CED2-4EDE-9097-4323BA262364}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{518B33D0-7784-4F2A-B674-67CF1EF75792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12300" tabRatio="729" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12300" tabRatio="729" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="308">
   <si>
     <t>header1</t>
   </si>
@@ -90,9 +90,6 @@
     <t>win11-en-part1-00.00.15.245.png</t>
   </si>
   <si>
-    <t>win11-en-part1-00.00.19.649.png</t>
-  </si>
-  <si>
     <t>win11-en-part1-00.00.24.161.png</t>
   </si>
   <si>
@@ -159,9 +156,6 @@
     <t>win11-en-part1-00.06.51.930.png</t>
   </si>
   <si>
-    <t>win11-en-part1-00.07.23.930.png</t>
-  </si>
-  <si>
     <t>win11-en-part1-00.07.34.930.png</t>
   </si>
   <si>
@@ -174,9 +168,6 @@
     <t>win11-en-part1-00.08.06.930.png</t>
   </si>
   <si>
-    <t>win11-en-part1-00.08.13.930.png</t>
-  </si>
-  <si>
     <t>win11-en-part1-00.08.18.930.png</t>
   </si>
   <si>
@@ -921,6 +912,126 @@
   </si>
   <si>
     <t>This is a movie of the procedure described in this chapter.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Choose preferred language.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Choose the location to specify the preferred language culture.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Connect to available network</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Check "Connect automatically" to reconnect smoothly.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Fill account &amp; password (if your network requests) and click "OK".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Click "Connect".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Installer starts its first update.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Read the end user license agreement carefully and accept it.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Skip the naming of your PC.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Installer starts its second update.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Sign-in to prepare a Microsoft account to initialize this PC.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Choose "&lt;strong&gt;Create one!&lt;/strong&gt;"</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Choose "&lt;strong&gt;Get a new email address&lt;/strong&gt;"</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Give a new email address string, and press "Next".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Give a password to new email address, uncheck the promotions to your email address</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Fill your first and last names.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Fill your region and birthday.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Fill alternative email address (to be used for recovery)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Skip a face or fingerprint authentication configuration.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Start a creation of a PIN code.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Fill PIN code twice.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Configure your privacy setting. Disable all switches.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Choose "Set up as a new PC".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Skip extra components.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Skip the linking of your phone and PC.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Skip the shaping of the photos in your phone and Microsoft account.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Decline the promotion of Microsoft 365 service.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Ditto.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Choose "Next".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>You would launch on the desktop environment by new Microsoft account.</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1326,7 +1437,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -1386,7 +1497,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -1396,7 +1507,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -1416,7 +1527,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -1436,11 +1547,11 @@
     <row r="7" spans="1:4" ht="19.5" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="2" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="s" ph="1">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -1450,7 +1561,7 @@
         <v>9</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -1460,7 +1571,7 @@
         <v>9</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -1470,7 +1581,7 @@
         <v>9</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1480,7 +1591,7 @@
         <v>9</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -1490,7 +1601,7 @@
         <v>9</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -1500,7 +1611,7 @@
         <v>9</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -1510,7 +1621,7 @@
         <v>9</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -1889,10 +2000,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -1908,7 +2019,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -1916,7 +2027,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1932,7 +2043,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -1948,16 +2059,19 @@
     </row>
     <row r="8" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D8" s="4" t="s" ph="1">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="19.5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>4</v>
       </c>
+      <c r="B9" s="2" t="s">
+        <v>278</v>
+      </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
@@ -1966,8 +2080,8 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>4</v>
+      <c r="B10" s="2" t="s">
+        <v>279</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
@@ -1977,8 +2091,8 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>4</v>
+      <c r="B11" s="2" t="s">
+        <v>280</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
@@ -1988,6 +2102,9 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="2" t="s">
+        <v>281</v>
+      </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
@@ -1996,6 +2113,9 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B13" s="2" t="s">
+        <v>282</v>
+      </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
@@ -2004,6 +2124,9 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B14" s="2" t="s">
+        <v>283</v>
+      </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
@@ -2012,6 +2135,9 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="2" t="s">
+        <v>284</v>
+      </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
@@ -2020,6 +2146,9 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B16" s="2" t="s">
+        <v>285</v>
+      </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
@@ -2027,7 +2156,10 @@
         <v>21</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B17" s="2" t="s">
+        <v>286</v>
+      </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
@@ -2035,7 +2167,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B18" s="2" t="s">
+        <v>287</v>
+      </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
@@ -2043,7 +2178,10 @@
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B19" s="2" t="s">
+        <v>288</v>
+      </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
       </c>
@@ -2051,7 +2189,10 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B20" s="2" t="s">
+        <v>289</v>
+      </c>
       <c r="C20" s="4" t="s">
         <v>9</v>
       </c>
@@ -2059,7 +2200,10 @@
         <v>25</v>
       </c>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B21" s="2" t="s">
+        <v>290</v>
+      </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
       </c>
@@ -2067,7 +2211,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B22" s="2" t="s">
+        <v>291</v>
+      </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
       </c>
@@ -2075,7 +2222,10 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="B23" s="2" t="s">
+        <v>292</v>
+      </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
       </c>
@@ -2083,7 +2233,10 @@
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B24" s="2" t="s">
+        <v>293</v>
+      </c>
       <c r="C24" s="4" t="s">
         <v>9</v>
       </c>
@@ -2091,7 +2244,10 @@
         <v>29</v>
       </c>
     </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B25" s="2" t="s">
+        <v>294</v>
+      </c>
       <c r="C25" s="4" t="s">
         <v>9</v>
       </c>
@@ -2099,7 +2255,10 @@
         <v>30</v>
       </c>
     </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B26" s="2" t="s">
+        <v>295</v>
+      </c>
       <c r="C26" s="4" t="s">
         <v>9</v>
       </c>
@@ -2107,7 +2266,10 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B27" s="2" t="s">
+        <v>296</v>
+      </c>
       <c r="C27" s="4" t="s">
         <v>9</v>
       </c>
@@ -2115,7 +2277,10 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B28" s="2" t="s">
+        <v>297</v>
+      </c>
       <c r="C28" s="4" t="s">
         <v>9</v>
       </c>
@@ -2123,7 +2288,10 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B29" s="2" t="s">
+        <v>298</v>
+      </c>
       <c r="C29" s="4" t="s">
         <v>9</v>
       </c>
@@ -2131,7 +2299,10 @@
         <v>34</v>
       </c>
     </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B30" s="2" t="s">
+        <v>299</v>
+      </c>
       <c r="C30" s="4" t="s">
         <v>9</v>
       </c>
@@ -2139,7 +2310,10 @@
         <v>35</v>
       </c>
     </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B31" s="2" t="s">
+        <v>300</v>
+      </c>
       <c r="C31" s="4" t="s">
         <v>9</v>
       </c>
@@ -2147,7 +2321,10 @@
         <v>36</v>
       </c>
     </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B32" s="2" t="s">
+        <v>301</v>
+      </c>
       <c r="C32" s="4" t="s">
         <v>9</v>
       </c>
@@ -2155,7 +2332,10 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B33" s="2" t="s">
+        <v>302</v>
+      </c>
       <c r="C33" s="4" t="s">
         <v>9</v>
       </c>
@@ -2163,7 +2343,10 @@
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B34" s="2" t="s">
+        <v>303</v>
+      </c>
       <c r="C34" s="4" t="s">
         <v>9</v>
       </c>
@@ -2171,7 +2354,10 @@
         <v>39</v>
       </c>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B35" s="2" t="s">
+        <v>304</v>
+      </c>
       <c r="C35" s="4" t="s">
         <v>9</v>
       </c>
@@ -2179,7 +2365,10 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B36" s="2" t="s">
+        <v>305</v>
+      </c>
       <c r="C36" s="4" t="s">
         <v>9</v>
       </c>
@@ -2187,7 +2376,10 @@
         <v>41</v>
       </c>
     </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B37" s="2" t="s">
+        <v>306</v>
+      </c>
       <c r="C37" s="4" t="s">
         <v>9</v>
       </c>
@@ -2195,36 +2387,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B38" s="2" t="s">
+        <v>307</v>
+      </c>
       <c r="C38" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>43</v>
-      </c>
-    </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C39" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C40" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="41" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C41" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D41" s="3" t="s">
-        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -2238,7 +2409,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
@@ -2255,7 +2426,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2263,7 +2434,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2279,7 +2450,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="19.5" x14ac:dyDescent="0.2">
@@ -2287,10 +2458,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D7" s="4" t="s" ph="1">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -2298,7 +2469,7 @@
         <v>9</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -2306,7 +2477,7 @@
         <v>9</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -2314,7 +2485,7 @@
         <v>9</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -2322,7 +2493,7 @@
         <v>9</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -2330,7 +2501,7 @@
         <v>9</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -2338,7 +2509,7 @@
         <v>9</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -2349,7 +2520,7 @@
         <v>9</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -2360,7 +2531,7 @@
         <v>9</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -2371,7 +2542,7 @@
         <v>9</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -2379,7 +2550,7 @@
         <v>9</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -2390,7 +2561,7 @@
         <v>9</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -2401,7 +2572,7 @@
         <v>9</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -2412,7 +2583,7 @@
         <v>9</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -2423,7 +2594,7 @@
         <v>9</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -2434,7 +2605,7 @@
         <v>9</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -2445,7 +2616,7 @@
         <v>9</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -2453,7 +2624,7 @@
         <v>9</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -2461,7 +2632,7 @@
         <v>9</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -2469,7 +2640,7 @@
         <v>9</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -2477,7 +2648,7 @@
         <v>9</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -2485,7 +2656,7 @@
         <v>9</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -2493,7 +2664,7 @@
         <v>9</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -2501,7 +2672,7 @@
         <v>9</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -2509,7 +2680,7 @@
         <v>9</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -2517,7 +2688,7 @@
         <v>9</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.2">
@@ -2525,7 +2696,7 @@
         <v>9</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.2">
@@ -2533,7 +2704,7 @@
         <v>9</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.2">
@@ -2541,7 +2712,7 @@
         <v>9</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2572,7 +2743,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="D1"/>
     </row>
@@ -2581,7 +2752,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="D2"/>
     </row>
@@ -2599,7 +2770,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="D4"/>
     </row>
@@ -2616,10 +2787,10 @@
     </row>
     <row r="7" spans="1:4" ht="19.5" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D7" s="4" t="s" ph="1">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -2631,7 +2802,7 @@
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -2640,7 +2811,7 @@
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -2652,7 +2823,7 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -2661,7 +2832,7 @@
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -2670,7 +2841,7 @@
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -2679,7 +2850,7 @@
         <v>9</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -2691,7 +2862,7 @@
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -2700,7 +2871,7 @@
         <v>9</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -2709,7 +2880,7 @@
         <v>9</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.2">
@@ -2717,7 +2888,7 @@
         <v>9</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.2">
@@ -2725,7 +2896,7 @@
         <v>9</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.2">
@@ -2733,7 +2904,7 @@
         <v>9</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.2">
@@ -2741,7 +2912,7 @@
         <v>9</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.2">
@@ -2749,7 +2920,7 @@
         <v>9</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.2">
@@ -2757,7 +2928,7 @@
         <v>9</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="23" spans="3:4" x14ac:dyDescent="0.2">
@@ -2765,7 +2936,7 @@
         <v>9</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.2">
@@ -2773,7 +2944,7 @@
         <v>9</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="3:4" x14ac:dyDescent="0.2">
@@ -2781,7 +2952,7 @@
         <v>9</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="3:4" x14ac:dyDescent="0.2">
@@ -2789,7 +2960,7 @@
         <v>9</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.2">
@@ -2797,7 +2968,7 @@
         <v>9</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.2">
@@ -2805,7 +2976,7 @@
         <v>9</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="3:4" x14ac:dyDescent="0.2">
@@ -2813,7 +2984,7 @@
         <v>9</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
     </row>
     <row r="30" spans="3:4" x14ac:dyDescent="0.2">
@@ -2821,7 +2992,7 @@
         <v>9</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="3:4" x14ac:dyDescent="0.2">
@@ -2829,7 +3000,7 @@
         <v>9</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
     </row>
     <row r="32" spans="3:4" x14ac:dyDescent="0.2">
@@ -2837,7 +3008,7 @@
         <v>9</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.2">
@@ -2845,7 +3016,7 @@
         <v>9</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.2">
@@ -2853,7 +3024,7 @@
         <v>9</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.2">
@@ -2861,7 +3032,7 @@
         <v>9</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.2">
@@ -2869,7 +3040,7 @@
         <v>9</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="37" spans="3:4" x14ac:dyDescent="0.2">
@@ -2877,7 +3048,7 @@
         <v>9</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.2">
@@ -2885,7 +3056,7 @@
         <v>9</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="39" spans="3:4" x14ac:dyDescent="0.2">
@@ -2893,7 +3064,7 @@
         <v>9</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="40" spans="3:4" x14ac:dyDescent="0.2">
@@ -2901,7 +3072,7 @@
         <v>9</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
     </row>
     <row r="41" spans="3:4" x14ac:dyDescent="0.2">
@@ -2909,7 +3080,7 @@
         <v>9</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="42" spans="3:4" x14ac:dyDescent="0.2">
@@ -2917,7 +3088,7 @@
         <v>9</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="43" spans="3:4" x14ac:dyDescent="0.2">
@@ -2925,7 +3096,7 @@
         <v>9</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="44" spans="3:4" x14ac:dyDescent="0.2">
@@ -2933,7 +3104,7 @@
         <v>9</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="45" spans="3:4" x14ac:dyDescent="0.2">
@@ -2941,7 +3112,7 @@
         <v>9</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="46" spans="3:4" x14ac:dyDescent="0.2">
@@ -2949,7 +3120,7 @@
         <v>9</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="47" spans="3:4" x14ac:dyDescent="0.2">
@@ -2957,7 +3128,7 @@
         <v>9</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="48" spans="3:4" x14ac:dyDescent="0.2">
@@ -2965,7 +3136,7 @@
         <v>9</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="49" spans="3:4" x14ac:dyDescent="0.2">
@@ -2973,7 +3144,7 @@
         <v>9</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
     </row>
     <row r="50" spans="3:4" x14ac:dyDescent="0.2">
@@ -2981,7 +3152,7 @@
         <v>9</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
     </row>
     <row r="51" spans="3:4" x14ac:dyDescent="0.2">
@@ -2989,7 +3160,7 @@
         <v>9</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
     </row>
     <row r="52" spans="3:4" x14ac:dyDescent="0.2">
@@ -2997,7 +3168,7 @@
         <v>9</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
     </row>
     <row r="53" spans="3:4" x14ac:dyDescent="0.2">
@@ -3005,7 +3176,7 @@
         <v>9</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="54" spans="3:4" x14ac:dyDescent="0.2">
@@ -3013,7 +3184,7 @@
         <v>9</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="55" spans="3:4" x14ac:dyDescent="0.2">
@@ -3021,7 +3192,7 @@
         <v>9</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -3052,7 +3223,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3076,7 +3247,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -3092,10 +3263,10 @@
     </row>
     <row r="8" spans="1:4" ht="19.5" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D8" s="4" t="s" ph="1">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -3103,7 +3274,7 @@
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -3111,7 +3282,7 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -3122,7 +3293,7 @@
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -3133,7 +3304,7 @@
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -3144,7 +3315,7 @@
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -3152,7 +3323,7 @@
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -3163,7 +3334,7 @@
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -3171,7 +3342,7 @@
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -3179,7 +3350,7 @@
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -3190,7 +3361,7 @@
         <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -3201,7 +3372,7 @@
         <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -3209,7 +3380,7 @@
         <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -3220,7 +3391,7 @@
         <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -3228,7 +3399,7 @@
         <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -3239,7 +3410,7 @@
         <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -3247,7 +3418,7 @@
         <v>9</v>
       </c>
       <c r="D24" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -3258,7 +3429,7 @@
         <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -3266,7 +3437,7 @@
         <v>9</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -3277,7 +3448,7 @@
         <v>9</v>
       </c>
       <c r="D27" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -3288,7 +3459,7 @@
         <v>9</v>
       </c>
       <c r="D28" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -3299,7 +3470,7 @@
         <v>9</v>
       </c>
       <c r="D29" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -3310,7 +3481,7 @@
         <v>9</v>
       </c>
       <c r="D30" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -3318,7 +3489,7 @@
         <v>9</v>
       </c>
       <c r="D31" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -3329,7 +3500,7 @@
         <v>9</v>
       </c>
       <c r="D32" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -3340,7 +3511,7 @@
         <v>9</v>
       </c>
       <c r="D33" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -3348,7 +3519,7 @@
         <v>9</v>
       </c>
       <c r="D34" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -3359,7 +3530,7 @@
         <v>9</v>
       </c>
       <c r="D35" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -3370,7 +3541,7 @@
         <v>9</v>
       </c>
       <c r="D36" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -3378,7 +3549,7 @@
         <v>9</v>
       </c>
       <c r="D37" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -3390,7 +3561,7 @@
         <v>9</v>
       </c>
       <c r="D38" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -3399,7 +3570,7 @@
         <v>9</v>
       </c>
       <c r="D39" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -3408,7 +3579,7 @@
         <v>9</v>
       </c>
       <c r="D40" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -3419,7 +3590,7 @@
         <v>9</v>
       </c>
       <c r="D41" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -3427,7 +3598,7 @@
         <v>9</v>
       </c>
       <c r="D42" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -3438,7 +3609,7 @@
         <v>9</v>
       </c>
       <c r="D43" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -3449,7 +3620,7 @@
         <v>9</v>
       </c>
       <c r="D44" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="19.5" x14ac:dyDescent="0.2">
@@ -3457,7 +3628,7 @@
         <v>9</v>
       </c>
       <c r="D45" t="s" ph="1">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -3468,7 +3639,7 @@
         <v>9</v>
       </c>
       <c r="D46" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -3476,7 +3647,7 @@
         <v>9</v>
       </c>
       <c r="D47" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -3484,7 +3655,7 @@
         <v>9</v>
       </c>
       <c r="D48" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="49" spans="3:4" x14ac:dyDescent="0.2">
@@ -3492,7 +3663,7 @@
         <v>9</v>
       </c>
       <c r="D49" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="61" spans="3:4" ht="19.5" x14ac:dyDescent="0.2">
@@ -3529,7 +3700,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3537,7 +3708,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3553,7 +3724,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -3570,10 +3741,10 @@
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D8" s="4" t="s" ph="1">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -3582,7 +3753,7 @@
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -3594,7 +3765,7 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -3606,7 +3777,7 @@
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -3618,7 +3789,7 @@
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -3626,7 +3797,7 @@
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -3634,7 +3805,7 @@
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -3642,7 +3813,7 @@
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -3650,7 +3821,7 @@
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.2">
@@ -3658,7 +3829,7 @@
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.2">
@@ -3666,7 +3837,7 @@
         <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.2">
@@ -3674,7 +3845,7 @@
         <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.2">
@@ -3682,7 +3853,7 @@
         <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.2">
@@ -3690,7 +3861,7 @@
         <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
   </sheetData>
@@ -3720,7 +3891,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3728,7 +3899,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3744,7 +3915,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="19.5" x14ac:dyDescent="0.2">
@@ -3752,10 +3923,10 @@
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D8" s="4" t="s" ph="1">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -3766,7 +3937,7 @@
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -3777,7 +3948,7 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -3788,7 +3959,7 @@
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -3799,7 +3970,7 @@
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -3807,7 +3978,7 @@
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -3815,7 +3986,7 @@
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -3823,7 +3994,7 @@
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -3831,7 +4002,7 @@
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.2">
@@ -3839,7 +4010,7 @@
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.2">
@@ -3847,7 +4018,7 @@
         <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.2">
@@ -3855,7 +4026,7 @@
         <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.2">
@@ -3863,7 +4034,7 @@
         <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.2">
@@ -3871,7 +4042,7 @@
         <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.2">
@@ -3879,7 +4050,7 @@
         <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="23" spans="3:4" x14ac:dyDescent="0.2">
@@ -3887,7 +4058,7 @@
         <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.2">
@@ -3895,7 +4066,7 @@
         <v>9</v>
       </c>
       <c r="D24" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -3923,10 +4094,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3934,7 +4105,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3950,7 +4121,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="19.5" x14ac:dyDescent="0.2">
@@ -3958,10 +4129,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="D7" s="4" t="s" ph="1">
-        <v>251</v>
+        <v>248</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -3969,7 +4140,7 @@
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -3980,7 +4151,7 @@
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -3988,7 +4159,7 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -3996,7 +4167,7 @@
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -4004,7 +4175,7 @@
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -4012,7 +4183,7 @@
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -4020,7 +4191,7 @@
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -4028,7 +4199,7 @@
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -4036,7 +4207,7 @@
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.2">
@@ -4044,7 +4215,7 @@
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.2">
@@ -4052,7 +4223,7 @@
         <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.2">
@@ -4060,7 +4231,7 @@
         <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.2">
@@ -4068,7 +4239,7 @@
         <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.2">
@@ -4076,7 +4247,7 @@
         <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.2">
@@ -4084,7 +4255,7 @@
         <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="23" spans="3:4" x14ac:dyDescent="0.2">
@@ -4092,7 +4263,7 @@
         <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.2">
@@ -4100,7 +4271,7 @@
         <v>9</v>
       </c>
       <c r="D24" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="25" spans="3:4" x14ac:dyDescent="0.2">
@@ -4108,7 +4279,7 @@
         <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="26" spans="3:4" x14ac:dyDescent="0.2">
@@ -4116,7 +4287,7 @@
         <v>9</v>
       </c>
       <c r="D26" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.2">
@@ -4124,7 +4295,7 @@
         <v>9</v>
       </c>
       <c r="D27" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.2">
@@ -4132,7 +4303,7 @@
         <v>9</v>
       </c>
       <c r="D28" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="29" spans="3:4" x14ac:dyDescent="0.2">
@@ -4140,7 +4311,7 @@
         <v>9</v>
       </c>
       <c r="D29" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
     <row r="30" spans="3:4" x14ac:dyDescent="0.2">
@@ -4148,7 +4319,7 @@
         <v>9</v>
       </c>
       <c r="D30" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="31" spans="3:4" x14ac:dyDescent="0.2">
@@ -4156,7 +4327,7 @@
         <v>9</v>
       </c>
       <c r="D31" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="32" spans="3:4" x14ac:dyDescent="0.2">
@@ -4164,7 +4335,7 @@
         <v>9</v>
       </c>
       <c r="D32" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
   </sheetData>
@@ -4196,7 +4367,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -4206,7 +4377,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -4226,7 +4397,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -4246,11 +4417,11 @@
     <row r="7" spans="1:4" ht="19.5" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="2" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="s" ph="1">
-        <v>252</v>
+        <v>249</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -4260,7 +4431,7 @@
         <v>9</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -4270,7 +4441,7 @@
         <v>9</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -4280,7 +4451,7 @@
         <v>9</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -4290,7 +4461,7 @@
         <v>9</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -4300,7 +4471,7 @@
         <v>9</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -4310,7 +4481,7 @@
         <v>9</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -4320,7 +4491,7 @@
         <v>9</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -4330,7 +4501,7 @@
         <v>9</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -4340,7 +4511,7 @@
         <v>9</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -4350,7 +4521,7 @@
         <v>9</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -4360,7 +4531,7 @@
         <v>9</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -4370,7 +4541,7 @@
         <v>9</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -4380,7 +4551,7 @@
         <v>9</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -4390,7 +4561,7 @@
         <v>9</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -4400,7 +4571,7 @@
         <v>9</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -4410,7 +4581,7 @@
         <v>9</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -4420,7 +4591,7 @@
         <v>9</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -4430,7 +4601,7 @@
         <v>9</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -4440,7 +4611,7 @@
         <v>9</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -4450,7 +4621,7 @@
         <v>9</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
win11_en.xlsx: updated to use new screenshots.
</commit_message>
<xml_diff>
--- a/win11_en.xlsx
+++ b/win11_en.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta2025\fresta-github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{518B33D0-7784-4F2A-B674-67CF1EF75792}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE068D6-5FF6-4A3D-9F30-D7ECA02114FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12300" tabRatio="729" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" tabRatio="729" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="481">
   <si>
     <t>header1</t>
   </si>
@@ -1034,12 +1034,752 @@
     <t>You would launch on the desktop environment by new Microsoft account.</t>
     <phoneticPr fontId="1"/>
   </si>
+  <si>
+    <t>Open "Start menu" from "田" on the taskbar (or "田" key).</t>
+    <rPh sb="24" eb="25">
+      <t>タ</t>
+    </rPh>
+    <rPh sb="47" eb="48">
+      <t>タ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>Click "Settings" app from gear icon ("</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>⚙</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>")</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Search "license" in Settings app, and proceed to "Activation settings".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Expand "Activation state", and confirm your operating system is activated.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Click "Manage providers" in the right side menu.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Search "virus" and proceed to "Virus &amp; threat protection".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Confirm the provider of the anti-virus software. In this case, "Microsoft Defender" (Windows Defender) is used. The "Laptop PC Check List" would ask it in later, take note of the name of anti-virus software.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Search "user" and proceed to "Other users".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Click "Add account".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Proceed to "I don't have…".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Proceed to "Add a user without…".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Set your account name (with alphabets and digits, upto 12 characters), and password.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Set secret answers to three questions (for the case of the loss of your password), and click "Next".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>You can find new local account. Click "v" to expand the extra menu.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Click "Change account type".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>You would get a window to change the account type. Click "Standard User".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Select "Administrator".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Click "OK".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>You would find that new local account becomes an administrator.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Open Start menu, and click the current account icon at the lower left corner, to expand sub menu.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Expand "…" menu near of "Sign out". Confirm new local account is listed.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Click "Sign out".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Default account at the login panel is the account for the previous session.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Change to new local account, and login.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Login process of new local account takes some time.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Configure your privacy setting. Again, disable all switches.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Now you got the assess of the desktop of new local account.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Open Start menu.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Open "Settings" app.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Search "spec" and proceed to "Windows specifications".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Detailed information of your operating system is displayed. The "Laptop PC Check List" would ask it in later, take not of the edition &amp; version.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Detailed information of your hardware is displayed in previous section.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Search "start" and proceed to "Start settings".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>You would get a panel looking like this.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Disable "Show account-related notifications" switch. This notification tries to make you change your local account to a Microsoft account.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Search "cmd" and choose "Command Prompt".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Proceed to "Run as administrator".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Allow "Do you want to allow this app…" by "Yes".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Type a command &lt;tt&gt;manage-bde.exe -protectors -get C:&lt;/tt&gt;, then press "Enter" key.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>You would get the BitLocker encryption key information. Take record of ID and password, to prepare the loss of the storage access in some accidents. The "Laptop PC Check List" would ask "have you checked BitLocker key?" you don't have to answer the password, but you should confirm "I have recorded the password". Taking a photo of this windows is sufficient. After the recording of ID &amp; password, close this command prompt window.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Open Settings app.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Search "update" and proceed to "Windows Update settings".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>You would get the menu looking like this. Do not press "Download &amp; install all" yet.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Proceed to "Advanced options".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Enable "Receive updates for…" and "Notify me…".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Proceed to "Optional updates".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>In this example, no optional updates, but if you find something useful, check them to include the update.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Return to the Windows Update top menu, and click "Download &amp; install all". If it is grayed-out, check each "Download &amp; install" for each updates.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>If all updates are applied, clicking "Check for updates" makes you returned to "You're up to date" indication.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Click "Scan options".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Check "Full scan".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Click "Scan now".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Minimize the anti-virus software window, and click "Edge" icon (a web browser) on the desktop.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>If your web browser shows some web content, proceed to &lt;a href="#config-start-page"&gt;configuration of web browser start page&lt;/a&gt;.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Proceed to "Start without your data".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Uncheck "Bring over your data…" and click "Confirm and continue".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Uncheck "Make your Microsoft experience…" and click "Confirm and continue"</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Click "Next".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Click "Finish".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h3 id="config-start-page"&gt;Configure the start page of your web browser&lt;/h3&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>Click the gear icon "</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>⚙</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>" on the upper right of the web content area.</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>You would get the menu looking like this.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Choose the preferred language. Sometimes your computer is localized based on IP address and the preferred language is different from the setting in the initialization.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Scroll down the menu, and disable "Show weather".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Disable "background".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Disable all switches under "Quick links &amp; search".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Disable "Show content", "Show widgets", and "Show feed".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h3 id="bookmark-momiji"&gt;Bookmark "Momiji" website&lt;/h3&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Search "hirodai momiji" from web search engine.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Visit "momiji.hiroshima-u.ac.jp".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>After launching "momiji.hiroshima-u.ac.jp", bookmark it by clicking "☆" button.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Search "hirodai momiji" in web search engine, and launch "momiji.hiroshima-u.ac.jp".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Click "Hirodai Moodle" button.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>You would launch an intermediate web page before Hirodai Moodle (this page is used for the announcement of the downtime etc). Click "Hirodai Moodle" icon.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Click "Login with Hirodai ID".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Fill your student ID (starting with uppercase alphabet and followed by digits), and password, click "Login".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Your web browsers suggests you to save your password, decline it.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>"Hirodai Moodle" is a website of online course system: distributes the materials for lectures, receives the submissions from students.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Back to "momiji" top page, and click "Login to My MOMIJI".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>If your session to Hirodai Moodle is cached, you would not be asked for Hirodai ID and password. "My Momiji" is a web site of the syllabus, registration of the lectures, and evaluations of the lectures.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Back to "momiji" top page, and click "Web Mail".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>It would guide you to a page titled "Microsoft 365 Portal". This is not "Microsoft 365 Portal" itself, it is a page describing about "Microsoft 365 Portal". Click "Microsoft 365 Portal" button on it.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">Fill your IMC account, starting with lowecase alphabet and followed by digits, plus "@hiroshima-u.ac.jp". </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Fill your password.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>"Stay signed in" should be declined either.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>"Sign in to Microsoft Edge" should be declined either.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>You launched Microsoft 365 web page. Expand the 3x3 dots menu on the upper left corner.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>You can find "Outlook" icon in submenu.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Click "Outlook" icon.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Your mailbox would be shown. The mail contacts from university office would come to this mailbox.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Back to the desktop, and open Start menu.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>If they are not installed, no App would be displayed. If Microsoft Office is not found, install it in below.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h2 id="install-microsoft-office"&gt;Install Microsoft Office&lt;/h2&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Open "Microsoft 365" of your account.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Click "Install and more" at the upper right area to expand the menu.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Proceed "Install Microsoft 365 apps".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Click "Install Office" under "Office apps &amp; devices".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>The installer would be downloaded.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Click "…" of the web browser to expand its menu.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Proceed to "Downloads".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>The list of downloaded items would be displayed. Click "folder" icon of the office installer.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>A window for downloaded items folder would be displayed.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Close (or minimize) other window, and start the installer by double-click.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>The installer starts and download the applications.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Click "Close" to finish the installation</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h2 id="hirodai-moodle"&gt;Hirodai Moodle&lt;/h2&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h2 id="my-momiji"&gt;My Momiji&lt;/h2&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h2 id="microsoft-365"&gt;Web Mail / Microsoft 365&lt;/h2&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Search "excel" or "word" or "powerpoint". If such Microsoft Office applications are already installed, some App would be returned. If you found them, proceed to next chapter.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Search "Excel" (or "Word" or "PowerPoint") from Start menu.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Choose "Run" to start it.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>In this example, "Excel" has started.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>What a while, or click "Sign in" on the top menu, "welcome" dialogue would be shown. Click "Continue" to sign in.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Fill IMC account (starting with lowercase alphabet, followed by digits, plus "@hiroshima-u.ac.jp"), and click "Next".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Fill your password, and click "Next".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Uncheck "Allow my organization…" and proceed by "No, this app only".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>You would receive such dialogue. Do not click blue button.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Acceot the license agreement.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>"Sign in" is changed to your name.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Clicking the name on the top menu would show the account information.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Search "OneDrive" in Start menu, and run it.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Fill your IMC account (starting with lowercase alphabet, followed by digits, plus "@hiroshima-u.ac.jp")</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Uncheck "Allow my organization…" and click "No, this app only".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Proceed by "Next".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;strong&gt;Do not click blue button here&lt;/strong&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Proceed by "Later".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Click "Open my OneDrive folder".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Click "Home" in shortcut in the left side panel.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Confirm that Documents folder has a "cloud" icon, but Desktop does not have.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Exclude "Pictures" and "Desktop" (include "Desktop"), then click "Start backup". If you include "Desktop", you would have serious trouble to copy the OneDrive storage to your local storage when you would graduate our university and lose the access with OneDrive.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Open Start menu</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Search "teams" in Start menu. If Microsoft Teams app is already installed, proceed to next chapter.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>If no app is found, install "Microsoft Teams" app.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Start Microsoft Edge (or other web browser).</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Search "hiroshima university media center".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Visit "www.media.hiroshima-u.ac.jp"</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>You would launch on the web site of IMC (information media center).</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Scroll to "Microsoft Teams" link.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>This is a web page of IMC to describe how to use Microsoft Teams.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Proceed to "How to use it".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Scroll to "Use the desktop app".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Follow the link to Microsoft site for Microsoft Teams desktop.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Download the installer from Microsoft.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Expand "…" menu of the web browser.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Choose "Downloads".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Find the installer of Microsoft Teams in the downloaded items list.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Click the folder icon.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>You would get the window of the downloaded item.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Close (or minimize) other windows, start the installer.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Installation would start.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Microsoft Teams app would start automatically.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Choose the account corresponding to your student ID.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Allow the access to the camera.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Disallow the access to the location info.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Click "…" icon at the left of your account icon.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>A configuration menu would be expanded.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Choose "Settings".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Choose "Devices".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Allow the access to the mic.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Click "Make a test call".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>The test call would start immediately.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Click "Share" button.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Choose "Window" menu to select the window to be shared.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Choose a window for sharing.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Shared window would have red enclosing box, and the duplicated window is shown in Teams app.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>The test call would terminate automatically, and the available and tested devices would be listed.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Click the "radiowave" icon on the taskbar.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Confirm the "radiowave" icon is active.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Click "&gt;" at the right of "radiowave" icon.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>You would find the list of available WiFi stations.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Choose "HU-CUP", and check "Connect automatically", then proceed to "Connect".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Fill your IMC accunt (starting with lowercase alphabet, followed by digits, plus "@hiroshima-u.ac.jp") and password, and click "OK".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Click "Connect" as far as you are in the campus of our university.</t>
+    <phoneticPr fontId="1"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1058,6 +1798,12 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="ＭＳ Ｐゴシック"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Segoe UI Symbol"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -1479,8 +2225,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EFCA2B8-55C7-4AC3-9E13-35156DBD8BC5}">
   <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -1556,7 +2302,9 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
-      <c r="B8" s="5"/>
+      <c r="B8" s="5" t="s">
+        <v>474</v>
+      </c>
       <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
@@ -1566,7 +2314,9 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
+      <c r="B9" s="5" t="s">
+        <v>475</v>
+      </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
@@ -1576,7 +2326,9 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
+      <c r="B10" s="5" t="s">
+        <v>476</v>
+      </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
@@ -1586,7 +2338,9 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
-      <c r="B11" s="5"/>
+      <c r="B11" s="5" t="s">
+        <v>477</v>
+      </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
@@ -1596,7 +2350,9 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
-      <c r="B12" s="5"/>
+      <c r="B12" s="5" t="s">
+        <v>478</v>
+      </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
@@ -1604,9 +2360,11 @@
         <v>239</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
-      <c r="B13" s="5"/>
+      <c r="B13" s="5" t="s">
+        <v>479</v>
+      </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
@@ -1616,7 +2374,9 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
-      <c r="B14" s="5"/>
+      <c r="B14" s="5" t="s">
+        <v>480</v>
+      </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
@@ -2002,7 +2762,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
@@ -2409,8 +3169,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="B22" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -2465,6 +3225,9 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
+        <v>308</v>
+      </c>
       <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
@@ -2472,7 +3235,10 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="B9" s="1" t="s">
+        <v>309</v>
+      </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
@@ -2481,6 +3247,9 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
+        <v>310</v>
+      </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
@@ -2489,6 +3258,9 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
+        <v>311</v>
+      </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
@@ -2497,6 +3269,9 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
+        <v>313</v>
+      </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
@@ -2505,6 +3280,9 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
+        <v>312</v>
+      </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
@@ -2512,9 +3290,12 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>4</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>314</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
@@ -2527,6 +3308,9 @@
       <c r="A15" t="s">
         <v>4</v>
       </c>
+      <c r="B15" s="1" t="s">
+        <v>315</v>
+      </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
@@ -2538,6 +3322,9 @@
       <c r="A16" t="s">
         <v>4</v>
       </c>
+      <c r="B16" s="1" t="s">
+        <v>316</v>
+      </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
@@ -2546,6 +3333,9 @@
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
+        <v>317</v>
+      </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
@@ -2557,6 +3347,9 @@
       <c r="A18" t="s">
         <v>4</v>
       </c>
+      <c r="B18" s="1" t="s">
+        <v>318</v>
+      </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
@@ -2568,6 +3361,9 @@
       <c r="A19" t="s">
         <v>4</v>
       </c>
+      <c r="B19" s="1" t="s">
+        <v>319</v>
+      </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
       </c>
@@ -2579,6 +3375,9 @@
       <c r="A20" t="s">
         <v>4</v>
       </c>
+      <c r="B20" s="1" t="s">
+        <v>320</v>
+      </c>
       <c r="C20" s="4" t="s">
         <v>9</v>
       </c>
@@ -2590,6 +3389,9 @@
       <c r="A21" t="s">
         <v>4</v>
       </c>
+      <c r="B21" s="1" t="s">
+        <v>321</v>
+      </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
       </c>
@@ -2601,6 +3403,9 @@
       <c r="A22" t="s">
         <v>4</v>
       </c>
+      <c r="B22" s="1" t="s">
+        <v>322</v>
+      </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
       </c>
@@ -2612,6 +3417,9 @@
       <c r="A23" t="s">
         <v>4</v>
       </c>
+      <c r="B23" s="1" t="s">
+        <v>323</v>
+      </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
       </c>
@@ -2620,6 +3428,9 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
+        <v>324</v>
+      </c>
       <c r="C24" s="4" t="s">
         <v>9</v>
       </c>
@@ -2636,6 +3447,9 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
+        <v>325</v>
+      </c>
       <c r="C26" s="4" t="s">
         <v>9</v>
       </c>
@@ -2644,6 +3458,9 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
+        <v>326</v>
+      </c>
       <c r="C27" s="4" t="s">
         <v>9</v>
       </c>
@@ -2652,6 +3469,9 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B28" s="1" t="s">
+        <v>327</v>
+      </c>
       <c r="C28" s="4" t="s">
         <v>9</v>
       </c>
@@ -2660,6 +3480,9 @@
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B29" s="1" t="s">
+        <v>328</v>
+      </c>
       <c r="C29" s="4" t="s">
         <v>9</v>
       </c>
@@ -2668,6 +3491,9 @@
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B30" s="1" t="s">
+        <v>329</v>
+      </c>
       <c r="C30" s="4" t="s">
         <v>9</v>
       </c>
@@ -2676,6 +3502,9 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B31" s="1" t="s">
+        <v>330</v>
+      </c>
       <c r="C31" s="4" t="s">
         <v>9</v>
       </c>
@@ -2684,6 +3513,9 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B32" s="1" t="s">
+        <v>331</v>
+      </c>
       <c r="C32" s="4" t="s">
         <v>9</v>
       </c>
@@ -2691,7 +3523,10 @@
         <v>68</v>
       </c>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B33" s="1" t="s">
+        <v>332</v>
+      </c>
       <c r="C33" s="4" t="s">
         <v>9</v>
       </c>
@@ -2699,7 +3534,10 @@
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B34" s="1" t="s">
+        <v>333</v>
+      </c>
       <c r="C34" s="4" t="s">
         <v>9</v>
       </c>
@@ -2707,7 +3545,10 @@
         <v>70</v>
       </c>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B35" s="1" t="s">
+        <v>334</v>
+      </c>
       <c r="C35" s="4" t="s">
         <v>9</v>
       </c>
@@ -2724,10 +3565,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D3AC582-7A6D-4EA0-8C12-75B8749BA9E2}">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:D59"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A46" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B60" sqref="B60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -2797,7 +3638,9 @@
       <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>336</v>
+      </c>
       <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
@@ -2806,7 +3649,9 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>337</v>
+      </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
@@ -2814,11 +3659,13 @@
         <v>73</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>338</v>
+      </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
@@ -2827,7 +3674,9 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>339</v>
+      </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
@@ -2836,7 +3685,9 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>340</v>
+      </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
@@ -2845,7 +3696,9 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B13" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>341</v>
+      </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
@@ -2853,11 +3706,13 @@
         <v>77</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>4</v>
       </c>
-      <c r="B14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>342</v>
+      </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
@@ -2866,7 +3721,9 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B15" s="1"/>
+      <c r="B15" s="1" t="s">
+        <v>335</v>
+      </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
@@ -2875,7 +3732,9 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B16" s="1"/>
+      <c r="B16" s="1" t="s">
+        <v>343</v>
+      </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
@@ -2883,7 +3742,10 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
+        <v>344</v>
+      </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
@@ -2891,7 +3753,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
@@ -2899,7 +3761,10 @@
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
+        <v>345</v>
+      </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
       </c>
@@ -2907,7 +3772,10 @@
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>346</v>
+      </c>
       <c r="C20" s="4" t="s">
         <v>9</v>
       </c>
@@ -2915,7 +3783,10 @@
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:4" ht="78" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>347</v>
+      </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
       </c>
@@ -2923,7 +3794,10 @@
         <v>85</v>
       </c>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
+        <v>348</v>
+      </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
       </c>
@@ -2931,7 +3805,10 @@
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>349</v>
+      </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
       </c>
@@ -2939,7 +3816,10 @@
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
+        <v>350</v>
+      </c>
       <c r="C24" s="4" t="s">
         <v>9</v>
       </c>
@@ -2947,7 +3827,10 @@
         <v>88</v>
       </c>
     </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
+        <v>351</v>
+      </c>
       <c r="C25" s="4" t="s">
         <v>9</v>
       </c>
@@ -2955,7 +3838,10 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
+        <v>352</v>
+      </c>
       <c r="C26" s="4" t="s">
         <v>9</v>
       </c>
@@ -2963,7 +3849,10 @@
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
+        <v>353</v>
+      </c>
       <c r="C27" s="4" t="s">
         <v>9</v>
       </c>
@@ -2971,7 +3860,10 @@
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="B28" s="1" t="s">
+        <v>354</v>
+      </c>
       <c r="C28" s="4" t="s">
         <v>9</v>
       </c>
@@ -2979,7 +3871,10 @@
         <v>92</v>
       </c>
     </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="B29" s="1" t="s">
+        <v>355</v>
+      </c>
       <c r="C29" s="4" t="s">
         <v>9</v>
       </c>
@@ -2987,7 +3882,10 @@
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="B30" s="1" t="s">
+        <v>356</v>
+      </c>
       <c r="C30" s="4" t="s">
         <v>9</v>
       </c>
@@ -2995,7 +3893,10 @@
         <v>94</v>
       </c>
     </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B31" s="1" t="s">
+        <v>313</v>
+      </c>
       <c r="C31" s="4" t="s">
         <v>9</v>
       </c>
@@ -3003,7 +3904,10 @@
         <v>95</v>
       </c>
     </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B32" s="1" t="s">
+        <v>357</v>
+      </c>
       <c r="C32" s="4" t="s">
         <v>9</v>
       </c>
@@ -3011,7 +3915,10 @@
         <v>96</v>
       </c>
     </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B33" s="1" t="s">
+        <v>358</v>
+      </c>
       <c r="C33" s="4" t="s">
         <v>9</v>
       </c>
@@ -3019,7 +3926,10 @@
         <v>97</v>
       </c>
     </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B34" s="1" t="s">
+        <v>359</v>
+      </c>
       <c r="C34" s="4" t="s">
         <v>9</v>
       </c>
@@ -3027,7 +3937,10 @@
         <v>98</v>
       </c>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="B35" s="1" t="s">
+        <v>360</v>
+      </c>
       <c r="C35" s="4" t="s">
         <v>9</v>
       </c>
@@ -3035,7 +3948,10 @@
         <v>99</v>
       </c>
     </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="B36" s="1" t="s">
+        <v>361</v>
+      </c>
       <c r="C36" s="4" t="s">
         <v>9</v>
       </c>
@@ -3043,7 +3959,10 @@
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B37" s="1" t="s">
+        <v>362</v>
+      </c>
       <c r="C37" s="4" t="s">
         <v>9</v>
       </c>
@@ -3051,7 +3970,10 @@
         <v>101</v>
       </c>
     </row>
-    <row r="38" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B38" s="1" t="s">
+        <v>363</v>
+      </c>
       <c r="C38" s="4" t="s">
         <v>9</v>
       </c>
@@ -3059,7 +3981,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="39" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C39" s="4" t="s">
         <v>9</v>
       </c>
@@ -3067,7 +3989,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="40" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C40" s="4" t="s">
         <v>9</v>
       </c>
@@ -3075,7 +3997,10 @@
         <v>104</v>
       </c>
     </row>
-    <row r="41" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="B41" s="1" t="s">
+        <v>364</v>
+      </c>
       <c r="C41" s="4" t="s">
         <v>9</v>
       </c>
@@ -3083,7 +4008,10 @@
         <v>105</v>
       </c>
     </row>
-    <row r="42" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B42" s="1" t="s">
+        <v>365</v>
+      </c>
       <c r="C42" s="4" t="s">
         <v>9</v>
       </c>
@@ -3091,7 +4019,10 @@
         <v>106</v>
       </c>
     </row>
-    <row r="43" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B43" s="1" t="s">
+        <v>366</v>
+      </c>
       <c r="C43" s="4" t="s">
         <v>9</v>
       </c>
@@ -3099,99 +4030,145 @@
         <v>107</v>
       </c>
     </row>
-    <row r="44" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C44" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D44" s="3" t="s">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B44" s="1"/>
+      <c r="C44" s="4"/>
+    </row>
+    <row r="45" spans="2:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="B45" s="1" t="s">
+        <v>367</v>
+      </c>
+      <c r="C45" s="4"/>
+    </row>
+    <row r="46" spans="2:4" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="B46" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D46" s="3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="45" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C45" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D45" s="3" t="s">
+    <row r="47" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B47" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D47" s="3" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="46" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C46" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D46" s="3" t="s">
+    <row r="48" spans="2:4" ht="39" x14ac:dyDescent="0.2">
+      <c r="B48" s="1" t="s">
+        <v>370</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D48" s="3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="47" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C47" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D47" s="3" t="s">
+    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B49" s="1" t="s">
+        <v>371</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D49" s="3" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="48" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C48" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D48" s="3" t="s">
+    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B50" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D50" s="3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C49" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D49" s="3" t="s">
+    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B51" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D51" s="3" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="50" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C50" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D50" s="3" t="s">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B52" s="1" t="s">
+        <v>373</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D52" s="3" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C51" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D51" s="3" t="s">
+    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B54" t="s">
+        <v>375</v>
+      </c>
+      <c r="C54" s="4"/>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B55" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D55" s="3" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C52" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D52" s="3" t="s">
+    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C56" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D56" s="3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="53" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C53" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D53" s="3" t="s">
+    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="C57" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D57" s="3" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="54" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C54" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D54" s="3" t="s">
+    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B58" s="1" t="s">
+        <v>377</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D58" s="3" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="55" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C55" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D55" s="3" t="s">
+    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B59" t="s">
+        <v>378</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D59" s="3" t="s">
         <v>119</v>
       </c>
     </row>
@@ -3204,10 +4181,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:D68"/>
+  <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A37" zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -3270,6 +4247,9 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>379</v>
+      </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
@@ -3278,327 +4258,359 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="C10" s="4"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
+        <v>413</v>
+      </c>
+      <c r="C11" s="4"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
+        <v>380</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>4</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" t="s">
+    <row r="13" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>381</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D12" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>382</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="C13" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D13" t="s">
+    <row r="15" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>383</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C14" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D14" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
+        <v>384</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D15" t="s">
+    <row r="17" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>385</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C16" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D16" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="C19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C17" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" t="s">
+    <row r="21" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>387</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D21" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D18" t="s">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C22" s="4"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>415</v>
+      </c>
+      <c r="C23" s="4"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>4</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>4</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" t="s">
+    <row r="25" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C20" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" t="s">
+    <row r="26" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D26" t="s">
         <v>131</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C22" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D22" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>4</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D23" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C24" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D25" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C26" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>4</v>
       </c>
+      <c r="B27" s="1" t="s">
+        <v>391</v>
+      </c>
       <c r="C27" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D27" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>4</v>
+      <c r="B28" s="1" t="s">
+        <v>384</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D28" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>4</v>
       </c>
+      <c r="B29" s="1" t="s">
+        <v>392</v>
+      </c>
       <c r="C29" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D29" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>4</v>
+      <c r="B30" s="1" t="s">
+        <v>393</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D30" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>4</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>394</v>
+      </c>
       <c r="C31" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D31" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>4</v>
+      <c r="B32" s="1" t="s">
+        <v>395</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D32" t="s">
-        <v>143</v>
+      <c r="D32" s="3" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>4</v>
       </c>
+      <c r="B33" s="1" t="s">
+        <v>396</v>
+      </c>
       <c r="C33" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D33" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>397</v>
+      </c>
       <c r="C34" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D34" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>4</v>
-      </c>
-      <c r="C35" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D35" t="s">
-        <v>146</v>
-      </c>
+      <c r="C35" s="4"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>4</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D36" t="s">
-        <v>147</v>
-      </c>
+      <c r="B36" s="1" t="s">
+        <v>400</v>
+      </c>
+      <c r="C36" s="4"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>4</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>398</v>
+      </c>
       <c r="C37" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D37" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>4</v>
       </c>
-      <c r="B38" s="2"/>
+      <c r="B38" s="1" t="s">
+        <v>416</v>
+      </c>
       <c r="C38" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D38" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B39" s="2"/>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="B39" s="1" t="s">
+        <v>399</v>
+      </c>
       <c r="C39" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D39" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B40" s="2"/>
+      <c r="A40" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>401</v>
+      </c>
       <c r="C40" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D40" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>4</v>
       </c>
+      <c r="B41" s="1" t="s">
+        <v>402</v>
+      </c>
       <c r="C41" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D41" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B42" s="1" t="s">
+        <v>403</v>
+      </c>
       <c r="C42" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D42" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -3609,68 +4621,174 @@
         <v>9</v>
       </c>
       <c r="D43" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>4</v>
       </c>
+      <c r="B44" s="1" t="s">
+        <v>404</v>
+      </c>
       <c r="C44" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D44" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" ht="19.5" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B45" s="1" t="s">
+        <v>405</v>
+      </c>
       <c r="C45" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D45" t="s" ph="1">
-        <v>156</v>
+      <c r="D45" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>4</v>
       </c>
+      <c r="B46" s="2" t="s">
+        <v>406</v>
+      </c>
       <c r="C46" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D46" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B47" s="2" t="s">
+        <v>407</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D47" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B48" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D48" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>4</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>409</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D49" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B50" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D50" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>4</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D51" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>4</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D52" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="19.5" x14ac:dyDescent="0.2">
+      <c r="C53" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D53" t="s" ph="1">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>4</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D54" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C47" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D47" t="s">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B55" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D55" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C48" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D48" t="s">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C56" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D56" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="49" spans="3:4" x14ac:dyDescent="0.2">
-      <c r="C49" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D49" t="s">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B57" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D57" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="61" spans="3:4" ht="19.5" x14ac:dyDescent="0.2">
-      <c r="D61" ph="1"/>
-    </row>
-    <row r="68" spans="4:4" ht="19.5" x14ac:dyDescent="0.2">
-      <c r="D68" ph="1"/>
+    <row r="69" spans="4:4" ht="19.5" x14ac:dyDescent="0.2">
+      <c r="D69" ph="1"/>
+    </row>
+    <row r="76" spans="4:4" ht="19.5" x14ac:dyDescent="0.2">
+      <c r="D76" ph="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -3683,8 +4801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45722500-6D63-48B1-B48D-DE8F55297416}">
   <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A7" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -3748,7 +4866,9 @@
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>417</v>
+      </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
@@ -3760,7 +4880,9 @@
       <c r="A10" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>418</v>
+      </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
@@ -3772,7 +4894,9 @@
       <c r="A11" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>419</v>
+      </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
@@ -3784,7 +4908,6 @@
       <c r="A12" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="1"/>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
@@ -3792,7 +4915,10 @@
         <v>164</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
+        <v>420</v>
+      </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
@@ -3800,7 +4926,10 @@
         <v>165</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
+        <v>421</v>
+      </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
@@ -3809,6 +4938,9 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
+        <v>422</v>
+      </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
@@ -3817,6 +4949,9 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
+        <v>424</v>
+      </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
@@ -3824,7 +4959,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
@@ -3832,7 +4967,10 @@
         <v>169</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
+        <v>423</v>
+      </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
@@ -3840,7 +4978,10 @@
         <v>170</v>
       </c>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
+        <v>425</v>
+      </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
       </c>
@@ -3848,7 +4989,10 @@
         <v>171</v>
       </c>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>426</v>
+      </c>
       <c r="C20" s="4" t="s">
         <v>9</v>
       </c>
@@ -3856,7 +5000,10 @@
         <v>172</v>
       </c>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>427</v>
+      </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
       </c>
@@ -3874,8 +5021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="A9" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -3933,6 +5080,9 @@
       <c r="A9" t="s">
         <v>4</v>
       </c>
+      <c r="B9" s="1" t="s">
+        <v>335</v>
+      </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
@@ -3944,6 +5094,9 @@
       <c r="A10" t="s">
         <v>4</v>
       </c>
+      <c r="B10" s="1" t="s">
+        <v>428</v>
+      </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
@@ -3955,6 +5108,9 @@
       <c r="A11" t="s">
         <v>4</v>
       </c>
+      <c r="B11" s="1" t="s">
+        <v>429</v>
+      </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
@@ -3966,6 +5122,9 @@
       <c r="A12" t="s">
         <v>4</v>
       </c>
+      <c r="B12" s="1" t="s">
+        <v>391</v>
+      </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
@@ -3974,6 +5133,9 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
+        <v>430</v>
+      </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
@@ -3982,6 +5144,9 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
+        <v>431</v>
+      </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
@@ -3990,6 +5155,9 @@
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
+        <v>432</v>
+      </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
@@ -3997,7 +5165,10 @@
         <v>180</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="39" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
+        <v>437</v>
+      </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
@@ -4005,7 +5176,10 @@
         <v>181</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
+        <v>431</v>
+      </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
@@ -4013,7 +5187,10 @@
         <v>182</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
+        <v>431</v>
+      </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
@@ -4021,7 +5198,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C19" s="4" t="s">
         <v>9</v>
       </c>
@@ -4029,7 +5206,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C20" s="4" t="s">
         <v>9</v>
       </c>
@@ -4037,7 +5214,10 @@
         <v>185</v>
       </c>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>433</v>
+      </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
       </c>
@@ -4045,7 +5225,10 @@
         <v>186</v>
       </c>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
+        <v>434</v>
+      </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
       </c>
@@ -4053,7 +5236,10 @@
         <v>187</v>
       </c>
     </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>435</v>
+      </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
       </c>
@@ -4061,7 +5247,10 @@
         <v>188</v>
       </c>
     </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
+        <v>436</v>
+      </c>
       <c r="C24" s="4" t="s">
         <v>9</v>
       </c>
@@ -4080,8 +5269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A13" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -4136,6 +5325,9 @@
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
+        <v>438</v>
+      </c>
       <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
@@ -4147,6 +5339,9 @@
       <c r="A9" t="s">
         <v>4</v>
       </c>
+      <c r="B9" s="1" t="s">
+        <v>439</v>
+      </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
@@ -4155,6 +5350,9 @@
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
+        <v>440</v>
+      </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
@@ -4163,6 +5361,9 @@
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
+        <v>441</v>
+      </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
@@ -4179,6 +5380,9 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
+        <v>442</v>
+      </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
@@ -4187,6 +5391,9 @@
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
+        <v>443</v>
+      </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
@@ -4203,6 +5410,9 @@
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
+        <v>444</v>
+      </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
@@ -4210,7 +5420,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
@@ -4218,7 +5428,10 @@
         <v>199</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
+        <v>445</v>
+      </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
@@ -4226,7 +5439,10 @@
         <v>200</v>
       </c>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
+        <v>446</v>
+      </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
       </c>
@@ -4234,7 +5450,10 @@
         <v>201</v>
       </c>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>447</v>
+      </c>
       <c r="C20" s="4" t="s">
         <v>9</v>
       </c>
@@ -4242,7 +5461,10 @@
         <v>202</v>
       </c>
     </row>
-    <row r="21" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>448</v>
+      </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
       </c>
@@ -4250,7 +5472,10 @@
         <v>203</v>
       </c>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B22" s="1" t="s">
+        <v>449</v>
+      </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
       </c>
@@ -4258,7 +5483,10 @@
         <v>204</v>
       </c>
     </row>
-    <row r="23" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>450</v>
+      </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
       </c>
@@ -4266,7 +5494,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="C24" s="4" t="s">
         <v>9</v>
       </c>
@@ -4274,7 +5502,10 @@
         <v>206</v>
       </c>
     </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
+        <v>451</v>
+      </c>
       <c r="C25" s="4" t="s">
         <v>9</v>
       </c>
@@ -4282,7 +5513,10 @@
         <v>207</v>
       </c>
     </row>
-    <row r="26" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B26" s="1" t="s">
+        <v>452</v>
+      </c>
       <c r="C26" s="4" t="s">
         <v>9</v>
       </c>
@@ -4290,7 +5524,10 @@
         <v>208</v>
       </c>
     </row>
-    <row r="27" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B27" s="1" t="s">
+        <v>453</v>
+      </c>
       <c r="C27" s="4" t="s">
         <v>9</v>
       </c>
@@ -4298,7 +5535,10 @@
         <v>209</v>
       </c>
     </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B28" s="1" t="s">
+        <v>454</v>
+      </c>
       <c r="C28" s="4" t="s">
         <v>9</v>
       </c>
@@ -4306,7 +5546,10 @@
         <v>210</v>
       </c>
     </row>
-    <row r="29" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B29" s="1" t="s">
+        <v>455</v>
+      </c>
       <c r="C29" s="4" t="s">
         <v>9</v>
       </c>
@@ -4314,7 +5557,10 @@
         <v>211</v>
       </c>
     </row>
-    <row r="30" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B30" s="1" t="s">
+        <v>456</v>
+      </c>
       <c r="C30" s="4" t="s">
         <v>9</v>
       </c>
@@ -4322,7 +5568,10 @@
         <v>212</v>
       </c>
     </row>
-    <row r="31" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B31" s="1" t="s">
+        <v>457</v>
+      </c>
       <c r="C31" s="4" t="s">
         <v>9</v>
       </c>
@@ -4330,7 +5579,10 @@
         <v>213</v>
       </c>
     </row>
-    <row r="32" spans="3:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B32" s="1" t="s">
+        <v>458</v>
+      </c>
       <c r="C32" s="4" t="s">
         <v>9</v>
       </c>
@@ -4349,8 +5601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CB03C1F-8A6F-4A43-BA2E-2C62B3131330}">
   <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A9" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -4426,7 +5678,9 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
-      <c r="B8" s="5"/>
+      <c r="B8" s="5" t="s">
+        <v>459</v>
+      </c>
       <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
@@ -4436,7 +5690,9 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
-      <c r="B9" s="5"/>
+      <c r="B9" s="5" t="s">
+        <v>391</v>
+      </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
@@ -4456,7 +5712,9 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
-      <c r="B11" s="5"/>
+      <c r="B11" s="5" t="s">
+        <v>423</v>
+      </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
@@ -4466,7 +5724,6 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
-      <c r="B12" s="5"/>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
@@ -4476,7 +5733,9 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
-      <c r="B13" s="5"/>
+      <c r="B13" s="5" t="s">
+        <v>460</v>
+      </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
@@ -4486,7 +5745,9 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
-      <c r="B14" s="5"/>
+      <c r="B14" s="5" t="s">
+        <v>461</v>
+      </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
@@ -4496,7 +5757,9 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
-      <c r="B15" s="5"/>
+      <c r="B15" s="3" t="s">
+        <v>462</v>
+      </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
@@ -4506,7 +5769,9 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
-      <c r="B16" s="5"/>
+      <c r="B16" s="5" t="s">
+        <v>463</v>
+      </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
@@ -4516,7 +5781,9 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
-      <c r="B17" s="5"/>
+      <c r="B17" s="5" t="s">
+        <v>464</v>
+      </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
@@ -4526,7 +5793,9 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
-      <c r="B18" s="5"/>
+      <c r="B18" s="5" t="s">
+        <v>465</v>
+      </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
@@ -4546,7 +5815,9 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
-      <c r="B20" s="5"/>
+      <c r="B20" s="5" t="s">
+        <v>466</v>
+      </c>
       <c r="C20" s="4" t="s">
         <v>9</v>
       </c>
@@ -4556,7 +5827,9 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
-      <c r="B21" s="5"/>
+      <c r="B21" s="5" t="s">
+        <v>467</v>
+      </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
       </c>
@@ -4566,7 +5839,9 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
-      <c r="B22" s="5"/>
+      <c r="B22" s="5" t="s">
+        <v>468</v>
+      </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
       </c>
@@ -4576,7 +5851,9 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
-      <c r="B23" s="5"/>
+      <c r="B23" s="5" t="s">
+        <v>469</v>
+      </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
       </c>
@@ -4586,7 +5863,9 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
-      <c r="B24" s="5"/>
+      <c r="B24" s="5" t="s">
+        <v>470</v>
+      </c>
       <c r="C24" s="4" t="s">
         <v>9</v>
       </c>
@@ -4596,7 +5875,9 @@
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
-      <c r="B25" s="5"/>
+      <c r="B25" s="5" t="s">
+        <v>471</v>
+      </c>
       <c r="C25" s="4" t="s">
         <v>9</v>
       </c>
@@ -4606,7 +5887,9 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
-      <c r="B26" s="5"/>
+      <c r="B26" s="5" t="s">
+        <v>472</v>
+      </c>
       <c r="C26" s="4" t="s">
         <v>9</v>
       </c>
@@ -4616,7 +5899,9 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
-      <c r="B27" s="5"/>
+      <c r="B27" s="5" t="s">
+        <v>473</v>
+      </c>
       <c r="C27" s="4" t="s">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
win11_en.xlsx: fix incorrect mapping between note & image (wip, until ch3)
</commit_message>
<xml_diff>
--- a/win11_en.xlsx
+++ b/win11_en.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta2025\fresta-github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BE068D6-5FF6-4A3D-9F30-D7ECA02114FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F5CAF5-EB92-4502-A2E7-D951FCA831AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" tabRatio="729" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" tabRatio="729" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="830" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="478">
   <si>
     <t>header1</t>
   </si>
@@ -357,9 +357,6 @@
     <t>win11-en-part3-00.04.59.726.png</t>
   </si>
   <si>
-    <t>win11-en-part3-00.05.00.726.png</t>
-  </si>
-  <si>
     <t>win11-en-part3-00.05.02.726.png</t>
   </si>
   <si>
@@ -391,12 +388,6 @@
   </si>
   <si>
     <t>win11-en-part3-00.06.29.124.png</t>
-  </si>
-  <si>
-    <t>win11-en-part3-00.06.30.124.png</t>
-  </si>
-  <si>
-    <t>win11-en-part3-00.06.33.124.png</t>
   </si>
   <si>
     <t>win11-en-part3-00.06.35.124.png</t>
@@ -2183,7 +2174,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -2225,7 +2216,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EFCA2B8-55C7-4AC3-9E13-35156DBD8BC5}">
   <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -2243,7 +2234,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -2253,7 +2244,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -2273,7 +2264,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>270</v>
+        <v>267</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -2293,95 +2284,95 @@
     <row r="7" spans="1:4" ht="19.5" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="s" ph="1">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="5" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="5" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="5" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="5" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="5" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="5" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>240</v>
+        <v>237</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="5" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -2779,7 +2770,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2787,7 +2778,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2803,7 +2794,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -2819,10 +2810,10 @@
     </row>
     <row r="8" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D8" s="4" t="s" ph="1">
-        <v>242</v>
+        <v>239</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="19.5" x14ac:dyDescent="0.2">
@@ -2830,7 +2821,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
@@ -2841,7 +2832,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
@@ -2852,7 +2843,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
@@ -2863,7 +2854,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
@@ -2874,7 +2865,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
-        <v>282</v>
+        <v>279</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
@@ -2885,7 +2876,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
@@ -2896,7 +2887,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
@@ -2907,7 +2898,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
-        <v>285</v>
+        <v>282</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
@@ -2918,7 +2909,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
-        <v>286</v>
+        <v>283</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
@@ -2929,7 +2920,7 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
@@ -2940,7 +2931,7 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
-        <v>288</v>
+        <v>285</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
@@ -2951,7 +2942,7 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>9</v>
@@ -2962,7 +2953,7 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
@@ -2973,7 +2964,7 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
@@ -2984,7 +2975,7 @@
     </row>
     <row r="23" spans="2:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B23" s="2" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
@@ -2995,7 +2986,7 @@
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
-        <v>293</v>
+        <v>290</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>9</v>
@@ -3006,7 +2997,7 @@
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
-        <v>294</v>
+        <v>291</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>9</v>
@@ -3017,7 +3008,7 @@
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
-        <v>295</v>
+        <v>292</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>9</v>
@@ -3028,7 +3019,7 @@
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>9</v>
@@ -3039,7 +3030,7 @@
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>9</v>
@@ -3050,7 +3041,7 @@
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>9</v>
@@ -3061,7 +3052,7 @@
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>9</v>
@@ -3072,7 +3063,7 @@
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B31" s="2" t="s">
-        <v>300</v>
+        <v>297</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>9</v>
@@ -3083,7 +3074,7 @@
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B32" s="2" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>9</v>
@@ -3094,7 +3085,7 @@
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>9</v>
@@ -3105,7 +3096,7 @@
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" s="2" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>9</v>
@@ -3116,7 +3107,7 @@
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" s="2" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>9</v>
@@ -3127,7 +3118,7 @@
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="2" t="s">
-        <v>305</v>
+        <v>302</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>9</v>
@@ -3138,7 +3129,7 @@
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B37" s="2" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>9</v>
@@ -3149,7 +3140,7 @@
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" s="2" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>9</v>
@@ -3186,7 +3177,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3194,7 +3185,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3210,7 +3201,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>256</v>
+        <v>253</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="19.5" x14ac:dyDescent="0.2">
@@ -3218,15 +3209,15 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D7" s="4" t="s" ph="1">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>308</v>
+        <v>305</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>9</v>
@@ -3237,7 +3228,7 @@
     </row>
     <row r="9" spans="1:4" ht="16.5" x14ac:dyDescent="0.45">
       <c r="B9" s="1" t="s">
-        <v>309</v>
+        <v>306</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
@@ -3248,7 +3239,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>310</v>
+        <v>307</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
@@ -3259,7 +3250,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
@@ -3270,7 +3261,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
@@ -3281,7 +3272,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
@@ -3295,7 +3286,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
@@ -3309,7 +3300,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>315</v>
+        <v>312</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
@@ -3323,7 +3314,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
@@ -3334,7 +3325,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
@@ -3348,7 +3339,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
@@ -3362,7 +3353,7 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
@@ -3376,7 +3367,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>9</v>
@@ -3390,7 +3381,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
@@ -3404,7 +3395,7 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
@@ -3418,7 +3409,7 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
@@ -3429,7 +3420,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>9</v>
@@ -3448,7 +3439,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>9</v>
@@ -3459,7 +3450,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>9</v>
@@ -3470,7 +3461,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>9</v>
@@ -3481,7 +3472,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>9</v>
@@ -3492,7 +3483,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>9</v>
@@ -3503,7 +3494,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>9</v>
@@ -3514,7 +3505,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>9</v>
@@ -3525,7 +3516,7 @@
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>332</v>
+        <v>329</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>9</v>
@@ -3536,7 +3527,7 @@
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
-        <v>333</v>
+        <v>330</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>9</v>
@@ -3547,7 +3538,7 @@
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>9</v>
@@ -3565,10 +3556,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D3AC582-7A6D-4EA0-8C12-75B8749BA9E2}">
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -3584,7 +3575,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="D1"/>
     </row>
@@ -3593,7 +3584,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="D2"/>
     </row>
@@ -3611,7 +3602,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>259</v>
+        <v>256</v>
       </c>
       <c r="D4"/>
     </row>
@@ -3628,10 +3619,10 @@
     </row>
     <row r="7" spans="1:4" ht="19.5" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D7" s="4" t="s" ph="1">
-        <v>244</v>
+        <v>241</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -3639,7 +3630,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>9</v>
@@ -3650,7 +3641,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
@@ -3664,7 +3655,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
@@ -3675,7 +3666,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>339</v>
+        <v>336</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
@@ -3686,7 +3677,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
@@ -3697,7 +3688,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
@@ -3711,7 +3702,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
@@ -3722,7 +3713,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
@@ -3733,7 +3724,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
@@ -3744,7 +3735,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
@@ -3763,7 +3754,7 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
@@ -3774,7 +3765,7 @@
     </row>
     <row r="20" spans="2:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>9</v>
@@ -3785,7 +3776,7 @@
     </row>
     <row r="21" spans="2:4" ht="78" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
@@ -3796,7 +3787,7 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
@@ -3807,7 +3798,7 @@
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>349</v>
+        <v>346</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
@@ -3818,7 +3809,7 @@
     </row>
     <row r="24" spans="2:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>350</v>
+        <v>347</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>9</v>
@@ -3829,7 +3820,7 @@
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>351</v>
+        <v>348</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>9</v>
@@ -3840,7 +3831,7 @@
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>352</v>
+        <v>349</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>9</v>
@@ -3851,7 +3842,7 @@
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>353</v>
+        <v>350</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>9</v>
@@ -3862,7 +3853,7 @@
     </row>
     <row r="28" spans="2:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
-        <v>354</v>
+        <v>351</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>9</v>
@@ -3873,7 +3864,7 @@
     </row>
     <row r="29" spans="2:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
-        <v>355</v>
+        <v>352</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>9</v>
@@ -3884,7 +3875,7 @@
     </row>
     <row r="30" spans="2:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>9</v>
@@ -3895,7 +3886,7 @@
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>9</v>
@@ -3906,7 +3897,7 @@
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>9</v>
@@ -3917,7 +3908,7 @@
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>9</v>
@@ -3928,7 +3919,7 @@
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>9</v>
@@ -3939,7 +3930,7 @@
     </row>
     <row r="35" spans="2:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>9</v>
@@ -3950,7 +3941,7 @@
     </row>
     <row r="36" spans="2:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>9</v>
@@ -3961,7 +3952,7 @@
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>9</v>
@@ -3972,7 +3963,7 @@
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>9</v>
@@ -3981,7 +3972,10 @@
         <v>102</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="B39" s="1" t="s">
+        <v>361</v>
+      </c>
       <c r="C39" s="4" t="s">
         <v>9</v>
       </c>
@@ -3990,6 +3984,9 @@
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B40" s="1" t="s">
+        <v>362</v>
+      </c>
       <c r="C40" s="4" t="s">
         <v>9</v>
       </c>
@@ -3997,9 +3994,9 @@
         <v>104</v>
       </c>
     </row>
-    <row r="41" spans="2:4" ht="26" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>9</v>
@@ -4009,40 +4006,40 @@
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="1"/>
+      <c r="C42" s="4"/>
+    </row>
+    <row r="43" spans="2:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="B43" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="C43" s="4"/>
+    </row>
+    <row r="44" spans="2:4" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="B44" s="1" t="s">
         <v>365</v>
       </c>
-      <c r="C42" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D42" s="3" t="s">
+      <c r="C44" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D44" s="3" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B43" s="1" t="s">
+    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B45" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="C43" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D43" s="3" t="s">
+      <c r="C45" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D45" s="3" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B44" s="1"/>
-      <c r="C44" s="4"/>
-    </row>
-    <row r="45" spans="2:4" ht="26" x14ac:dyDescent="0.2">
-      <c r="B45" s="1" t="s">
+    <row r="46" spans="2:4" ht="39" x14ac:dyDescent="0.2">
+      <c r="B46" s="1" t="s">
         <v>367</v>
-      </c>
-      <c r="C45" s="4"/>
-    </row>
-    <row r="46" spans="2:4" ht="16.5" x14ac:dyDescent="0.45">
-      <c r="B46" s="1" t="s">
-        <v>368</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>9</v>
@@ -4053,7 +4050,7 @@
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>9</v>
@@ -4062,9 +4059,9 @@
         <v>109</v>
       </c>
     </row>
-    <row r="48" spans="2:4" ht="39" x14ac:dyDescent="0.2">
+    <row r="48" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B48" s="1" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>9</v>
@@ -4086,7 +4083,7 @@
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B50" s="1" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>9</v>
@@ -4096,9 +4093,6 @@
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B51" s="1" t="s">
-        <v>374</v>
-      </c>
       <c r="C51" s="4" t="s">
         <v>9</v>
       </c>
@@ -4106,26 +4100,26 @@
         <v>113</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B52" s="1" t="s">
+    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B53" t="s">
+        <v>372</v>
+      </c>
+      <c r="C53" s="4"/>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B54" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="C52" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D52" s="3" t="s">
+      <c r="C54" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D54" s="3" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B54" t="s">
-        <v>375</v>
-      </c>
-      <c r="C54" s="4"/>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B55" s="1" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>9</v>
@@ -4135,41 +4129,14 @@
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B56" t="s">
+        <v>375</v>
+      </c>
       <c r="C56" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>116</v>
-      </c>
-    </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C57" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D57" s="3" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B58" s="1" t="s">
-        <v>377</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D58" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B59" t="s">
-        <v>378</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D59" s="3" t="s">
-        <v>119</v>
       </c>
     </row>
   </sheetData>
@@ -4200,7 +4167,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -4224,7 +4191,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>275</v>
+        <v>272</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -4240,21 +4207,21 @@
     </row>
     <row r="8" spans="1:4" ht="19.5" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D8" s="4" t="s" ph="1">
-        <v>245</v>
+        <v>242</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -4262,19 +4229,19 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4282,13 +4249,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -4296,13 +4263,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>382</v>
+        <v>379</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4310,24 +4277,24 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>383</v>
+        <v>380</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4335,13 +4302,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -4349,30 +4316,30 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="C19" s="4"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -4380,7 +4347,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="C23" s="4"/>
     </row>
@@ -4389,13 +4356,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D24" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -4403,24 +4370,24 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D26" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -4428,24 +4395,24 @@
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D27" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
-        <v>384</v>
+        <v>381</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D28" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -4453,24 +4420,24 @@
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D29" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D30" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -4478,24 +4445,24 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D31" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -4503,13 +4470,13 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D33" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4517,13 +4484,13 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>397</v>
+        <v>394</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D34" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -4531,7 +4498,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
-        <v>400</v>
+        <v>397</v>
       </c>
       <c r="C36" s="4"/>
     </row>
@@ -4540,13 +4507,13 @@
         <v>4</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>398</v>
+        <v>395</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D37" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4554,24 +4521,24 @@
         <v>4</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D38" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>399</v>
+        <v>396</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D39" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -4579,13 +4546,13 @@
         <v>4</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D40" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -4593,24 +4560,24 @@
         <v>4</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D41" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D42" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -4621,7 +4588,7 @@
         <v>9</v>
       </c>
       <c r="D43" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -4629,24 +4596,24 @@
         <v>4</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D44" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D45" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -4654,35 +4621,35 @@
         <v>4</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D46" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B47" s="2" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D47" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B48" s="2" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D48" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -4690,24 +4657,24 @@
         <v>4</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D49" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B50" s="1" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D50" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -4718,7 +4685,7 @@
         <v>9</v>
       </c>
       <c r="D51" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
@@ -4726,13 +4693,13 @@
         <v>4</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>345</v>
+        <v>342</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D52" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="19.5" x14ac:dyDescent="0.2">
@@ -4740,7 +4707,7 @@
         <v>9</v>
       </c>
       <c r="D53" t="s" ph="1">
-        <v>156</v>
+        <v>153</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -4751,18 +4718,18 @@
         <v>9</v>
       </c>
       <c r="D54" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B55" s="1" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D55" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -4770,18 +4737,18 @@
         <v>9</v>
       </c>
       <c r="D56" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B57" s="1" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D57" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="69" spans="4:4" ht="19.5" x14ac:dyDescent="0.2">
@@ -4818,7 +4785,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -4826,7 +4793,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -4842,7 +4809,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -4859,21 +4826,21 @@
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D8" s="4" t="s" ph="1">
-        <v>246</v>
+        <v>243</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -4881,13 +4848,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -4895,13 +4862,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -4912,51 +4879,51 @@
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
@@ -4964,51 +4931,51 @@
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -5038,7 +5005,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5046,7 +5013,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -5062,7 +5029,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>273</v>
+        <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="19.5" x14ac:dyDescent="0.2">
@@ -5070,10 +5037,10 @@
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D8" s="4" t="s" ph="1">
-        <v>247</v>
+        <v>244</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -5081,13 +5048,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -5095,13 +5062,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -5109,13 +5076,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -5123,79 +5090,79 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
@@ -5203,7 +5170,7 @@
         <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
@@ -5211,51 +5178,51 @@
         <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D24" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
   </sheetData>
@@ -5283,10 +5250,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>267</v>
+        <v>264</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5294,7 +5261,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -5310,7 +5277,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>272</v>
+        <v>269</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="19.5" x14ac:dyDescent="0.2">
@@ -5318,21 +5285,21 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="D7" s="4" t="s" ph="1">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -5340,35 +5307,35 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -5376,29 +5343,29 @@
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -5406,18 +5373,18 @@
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
@@ -5425,73 +5392,73 @@
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
@@ -5499,95 +5466,95 @@
         <v>9</v>
       </c>
       <c r="D24" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D26" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D27" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D28" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D29" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D30" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D31" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D32" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
     </row>
   </sheetData>
@@ -5619,7 +5586,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -5629,7 +5596,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -5649,7 +5616,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -5669,35 +5636,35 @@
     <row r="7" spans="1:4" ht="19.5" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="2" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="s" ph="1">
-        <v>249</v>
+        <v>246</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="5" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="5" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -5707,19 +5674,19 @@
         <v>9</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="5" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -5728,79 +5695,79 @@
         <v>9</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="5" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="5" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="3" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="5" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="5" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="5" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -5810,103 +5777,103 @@
         <v>9</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="5" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="5" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
       <c r="B22" s="5" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
       <c r="B23" s="5" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
       <c r="B24" s="5" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
       <c r="B25" s="5" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
       <c r="B26" s="5" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
       <c r="B27" s="5" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
win11_en.xlsx: fix the correspondings between notes & images
</commit_message>
<xml_diff>
--- a/win11_en.xlsx
+++ b/win11_en.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta2025\fresta-github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1F5CAF5-EB92-4502-A2E7-D951FCA831AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0555572-3251-477E-B1AE-BB54A2EA2F4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" tabRatio="729" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" tabRatio="729" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="465">
   <si>
     <t>header1</t>
   </si>
@@ -291,9 +291,6 @@
     <t>win11-en-part3-00.01.33.000.png</t>
   </si>
   <si>
-    <t>win11-en-part3-00.01.34.000.png</t>
-  </si>
-  <si>
     <t>win11-en-part3-00.01.36.000.png</t>
   </si>
   <si>
@@ -474,9 +471,6 @@
     <t>win11-en-part4-00.04.15.407.png</t>
   </si>
   <si>
-    <t>win11-en-part4-00.04.20.407.png</t>
-  </si>
-  <si>
     <t>win11-en-part4-00.04.24.407.png</t>
   </si>
   <si>
@@ -498,24 +492,12 @@
     <t>win11-en-part4-00.04.58.407.png</t>
   </si>
   <si>
-    <t>win11-en-part4-00.05.04.407.png</t>
-  </si>
-  <si>
     <t>win11-en-part4-00.05.05.407.png</t>
   </si>
   <si>
-    <t>win11-en-part4-00.05.09.407.png</t>
-  </si>
-  <si>
-    <t>win11-en-part4-00.05.10.407.png</t>
-  </si>
-  <si>
     <t>win11-en-part4-00.05.12.407.png</t>
   </si>
   <si>
-    <t>win11-en-part4-00.05.19.407.png</t>
-  </si>
-  <si>
     <t>win11-en-part4-00.05.22.407.png</t>
   </si>
   <si>
@@ -528,9 +510,6 @@
     <t>win11-en-part5-00.00.17.623.png</t>
   </si>
   <si>
-    <t>win11-en-part5-00.00.18.623.png</t>
-  </si>
-  <si>
     <t>win11-en-part5-00.00.20.623.png</t>
   </si>
   <si>
@@ -543,9 +522,6 @@
     <t>win11-en-part5-00.00.56.623.png</t>
   </si>
   <si>
-    <t>win11-en-part5-00.01.00.623.png</t>
-  </si>
-  <si>
     <t>win11-en-part5-00.01.00.902.png</t>
   </si>
   <si>
@@ -591,9 +567,6 @@
     <t>win11-en-part6-00.01.19.000.png</t>
   </si>
   <si>
-    <t>win11-en-part6-00.01.23.000.png</t>
-  </si>
-  <si>
     <t>win11-en-part6-00.01.24.000.png</t>
   </si>
   <si>
@@ -618,24 +591,15 @@
     <t>win11-en-part7-00.00.40.000.png</t>
   </si>
   <si>
-    <t>win11-en-part7-00.00.44.000.png</t>
-  </si>
-  <si>
     <t>win11-en-part7-00.01.02.000.png</t>
   </si>
   <si>
     <t>win11-en-part7-00.01.03.000.png</t>
   </si>
   <si>
-    <t>win11-en-part7-00.01.04.000.png</t>
-  </si>
-  <si>
     <t>win11-en-part7-00.01.19.000.png</t>
   </si>
   <si>
-    <t>win11-en-part7-00.01.20.000.png</t>
-  </si>
-  <si>
     <t>win11-en-part7-00.01.40.000.png</t>
   </si>
   <si>
@@ -687,15 +651,9 @@
     <t>win11-en-part8-00.00.11.000.png</t>
   </si>
   <si>
-    <t>win11-en-part8-00.00.22.000.png</t>
-  </si>
-  <si>
     <t>win11-en-part8-00.00.24.000.png</t>
   </si>
   <si>
-    <t>win11-en-part8-00.00.36.000.png</t>
-  </si>
-  <si>
     <t>win11-en-part8-00.00.37.000.png</t>
   </si>
   <si>
@@ -712,9 +670,6 @@
   </si>
   <si>
     <t>win11-en-part8-00.01.01.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part8-00.01.05.000.png</t>
   </si>
   <si>
     <t>win11-en-part8-00.01.07.000.png</t>
@@ -1205,10 +1160,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Type a command &lt;tt&gt;manage-bde.exe -protectors -get C:&lt;/tt&gt;, then press "Enter" key.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>You would get the BitLocker encryption key information. Take record of ID and password, to prepare the loss of the storage access in some accidents. The "Laptop PC Check List" would ask "have you checked BitLocker key?" you don't have to answer the password, but you should confirm "I have recorded the password". Taking a photo of this windows is sufficient. After the recording of ID &amp; password, close this command prompt window.</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1763,6 +1714,18 @@
   </si>
   <si>
     <t>Click "Connect" as far as you are in the campus of our university.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Type a command &lt;span&gt;&lt;strong&gt;manage-bde.exe -protectors -get C:&lt;/strong&gt;&lt;/span&gt;, then press "Enter" key.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Confirm the language is changed.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Downloading starts.</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -2174,7 +2137,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="65" x14ac:dyDescent="0.2">
@@ -2216,7 +2179,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EFCA2B8-55C7-4AC3-9E13-35156DBD8BC5}">
   <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -2234,7 +2197,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -2244,7 +2207,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>249</v>
+        <v>234</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -2264,7 +2227,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>267</v>
+        <v>252</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -2284,95 +2247,95 @@
     <row r="7" spans="1:4" ht="19.5" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="2" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="s" ph="1">
-        <v>247</v>
+        <v>232</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="5" t="s">
-        <v>471</v>
+        <v>455</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>232</v>
+        <v>217</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="5" t="s">
-        <v>472</v>
+        <v>456</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>233</v>
+        <v>218</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="5" t="s">
-        <v>473</v>
+        <v>457</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>234</v>
+        <v>219</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="5" t="s">
-        <v>474</v>
+        <v>458</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>235</v>
+        <v>220</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="5" t="s">
-        <v>475</v>
+        <v>459</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>236</v>
+        <v>221</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="5" t="s">
-        <v>476</v>
+        <v>460</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>237</v>
+        <v>222</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="5" t="s">
-        <v>477</v>
+        <v>461</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>238</v>
+        <v>223</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -2770,7 +2733,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>252</v>
+        <v>237</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -2778,7 +2741,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>251</v>
+        <v>236</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -2794,7 +2757,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>250</v>
+        <v>235</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -2810,10 +2773,10 @@
     </row>
     <row r="8" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="D8" s="4" t="s" ph="1">
-        <v>239</v>
+        <v>224</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="19.5" x14ac:dyDescent="0.2">
@@ -2821,7 +2784,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
@@ -2832,7 +2795,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
@@ -2843,7 +2806,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
@@ -2854,7 +2817,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
-        <v>278</v>
+        <v>263</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
@@ -2865,7 +2828,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
@@ -2876,7 +2839,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
@@ -2887,7 +2850,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
@@ -2898,7 +2861,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
@@ -2909,7 +2872,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
@@ -2920,7 +2883,7 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
@@ -2931,7 +2894,7 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
-        <v>285</v>
+        <v>270</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
@@ -2942,7 +2905,7 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
-        <v>286</v>
+        <v>271</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>9</v>
@@ -2953,7 +2916,7 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
@@ -2964,7 +2927,7 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
@@ -2975,7 +2938,7 @@
     </row>
     <row r="23" spans="2:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B23" s="2" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
@@ -2986,7 +2949,7 @@
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>9</v>
@@ -2997,7 +2960,7 @@
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>9</v>
@@ -3008,7 +2971,7 @@
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>9</v>
@@ -3019,7 +2982,7 @@
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
-        <v>293</v>
+        <v>278</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>9</v>
@@ -3030,7 +2993,7 @@
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
-        <v>294</v>
+        <v>279</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>9</v>
@@ -3041,7 +3004,7 @@
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
-        <v>295</v>
+        <v>280</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>9</v>
@@ -3052,7 +3015,7 @@
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
-        <v>296</v>
+        <v>281</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>9</v>
@@ -3063,7 +3026,7 @@
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B31" s="2" t="s">
-        <v>297</v>
+        <v>282</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>9</v>
@@ -3074,7 +3037,7 @@
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B32" s="2" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>9</v>
@@ -3085,7 +3048,7 @@
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">
-        <v>299</v>
+        <v>284</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>9</v>
@@ -3096,7 +3059,7 @@
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" s="2" t="s">
-        <v>300</v>
+        <v>285</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>9</v>
@@ -3107,7 +3070,7 @@
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" s="2" t="s">
-        <v>301</v>
+        <v>286</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>9</v>
@@ -3118,7 +3081,7 @@
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="2" t="s">
-        <v>302</v>
+        <v>287</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>9</v>
@@ -3129,7 +3092,7 @@
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B37" s="2" t="s">
-        <v>303</v>
+        <v>288</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>9</v>
@@ -3140,7 +3103,7 @@
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" s="2" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>9</v>
@@ -3177,7 +3140,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>255</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3185,7 +3148,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>254</v>
+        <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3201,7 +3164,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="19.5" x14ac:dyDescent="0.2">
@@ -3209,15 +3172,15 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="D7" s="4" t="s" ph="1">
-        <v>240</v>
+        <v>225</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>305</v>
+        <v>290</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>9</v>
@@ -3228,7 +3191,7 @@
     </row>
     <row r="9" spans="1:4" ht="16.5" x14ac:dyDescent="0.45">
       <c r="B9" s="1" t="s">
-        <v>306</v>
+        <v>291</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
@@ -3239,7 +3202,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
@@ -3250,7 +3213,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>308</v>
+        <v>293</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
@@ -3261,7 +3224,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>310</v>
+        <v>295</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
@@ -3272,7 +3235,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>309</v>
+        <v>294</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
@@ -3286,7 +3249,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>311</v>
+        <v>296</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
@@ -3300,7 +3263,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>312</v>
+        <v>297</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
@@ -3314,7 +3277,7 @@
         <v>4</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>313</v>
+        <v>298</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
@@ -3325,7 +3288,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>314</v>
+        <v>299</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
@@ -3339,7 +3302,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>315</v>
+        <v>300</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
@@ -3353,7 +3316,7 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>316</v>
+        <v>301</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
@@ -3367,7 +3330,7 @@
         <v>4</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>317</v>
+        <v>302</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>9</v>
@@ -3381,7 +3344,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>318</v>
+        <v>303</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
@@ -3395,7 +3358,7 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>319</v>
+        <v>304</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
@@ -3409,7 +3372,7 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>320</v>
+        <v>305</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
@@ -3420,7 +3383,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>321</v>
+        <v>306</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>9</v>
@@ -3439,7 +3402,7 @@
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>322</v>
+        <v>307</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>9</v>
@@ -3450,7 +3413,7 @@
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>323</v>
+        <v>308</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>9</v>
@@ -3461,7 +3424,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
-        <v>324</v>
+        <v>309</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>9</v>
@@ -3472,7 +3435,7 @@
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
-        <v>325</v>
+        <v>310</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>9</v>
@@ -3483,7 +3446,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>326</v>
+        <v>311</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>9</v>
@@ -3494,7 +3457,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>327</v>
+        <v>312</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>9</v>
@@ -3505,7 +3468,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
-        <v>328</v>
+        <v>313</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>9</v>
@@ -3516,7 +3479,7 @@
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>9</v>
@@ -3527,7 +3490,7 @@
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
-        <v>330</v>
+        <v>315</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>9</v>
@@ -3538,7 +3501,7 @@
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
-        <v>331</v>
+        <v>316</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>9</v>
@@ -3556,10 +3519,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D3AC582-7A6D-4EA0-8C12-75B8749BA9E2}">
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51"/>
+    <sheetView topLeftCell="A45" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -3575,7 +3538,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>258</v>
+        <v>243</v>
       </c>
       <c r="D1"/>
     </row>
@@ -3584,7 +3547,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>257</v>
+        <v>242</v>
       </c>
       <c r="D2"/>
     </row>
@@ -3602,7 +3565,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>256</v>
+        <v>241</v>
       </c>
       <c r="D4"/>
     </row>
@@ -3619,10 +3582,10 @@
     </row>
     <row r="7" spans="1:4" ht="19.5" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="D7" s="4" t="s" ph="1">
-        <v>241</v>
+        <v>226</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -3630,7 +3593,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>9</v>
@@ -3641,7 +3604,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>334</v>
+        <v>319</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
@@ -3655,7 +3618,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>335</v>
+        <v>320</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
@@ -3666,7 +3629,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>336</v>
+        <v>321</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
@@ -3677,7 +3640,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>337</v>
+        <v>322</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
@@ -3688,7 +3651,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>338</v>
+        <v>323</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
@@ -3702,7 +3665,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>339</v>
+        <v>324</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
@@ -3713,7 +3676,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>332</v>
+        <v>317</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
@@ -3724,7 +3687,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
@@ -3735,7 +3698,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
@@ -3745,6 +3708,9 @@
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
+        <v>327</v>
+      </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
@@ -3752,9 +3718,9 @@
         <v>82</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>342</v>
+        <v>462</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
@@ -3763,9 +3729,9 @@
         <v>83</v>
       </c>
     </row>
-    <row r="20" spans="2:4" ht="26" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:4" ht="78" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>343</v>
+        <v>328</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>9</v>
@@ -3774,9 +3740,9 @@
         <v>84</v>
       </c>
     </row>
-    <row r="21" spans="2:4" ht="78" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>344</v>
+        <v>329</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
@@ -3787,7 +3753,7 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>345</v>
+        <v>330</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
@@ -3796,9 +3762,9 @@
         <v>86</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>346</v>
+        <v>331</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
@@ -3807,9 +3773,9 @@
         <v>87</v>
       </c>
     </row>
-    <row r="24" spans="2:4" ht="26" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>347</v>
+        <v>332</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>9</v>
@@ -3820,7 +3786,7 @@
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>9</v>
@@ -3831,7 +3797,7 @@
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>9</v>
@@ -3840,9 +3806,9 @@
         <v>90</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>350</v>
+        <v>335</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>9</v>
@@ -3853,7 +3819,7 @@
     </row>
     <row r="28" spans="2:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
-        <v>351</v>
+        <v>336</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>9</v>
@@ -3864,7 +3830,7 @@
     </row>
     <row r="29" spans="2:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>9</v>
@@ -3873,9 +3839,9 @@
         <v>93</v>
       </c>
     </row>
-    <row r="30" spans="2:4" ht="26" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>353</v>
+        <v>295</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>9</v>
@@ -3886,7 +3852,7 @@
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>310</v>
+        <v>338</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>9</v>
@@ -3897,7 +3863,7 @@
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
-        <v>354</v>
+        <v>339</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>9</v>
@@ -3908,7 +3874,7 @@
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>355</v>
+        <v>340</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>9</v>
@@ -3917,9 +3883,9 @@
         <v>97</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
-        <v>356</v>
+        <v>341</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>9</v>
@@ -3930,7 +3896,7 @@
     </row>
     <row r="35" spans="2:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
-        <v>357</v>
+        <v>342</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>9</v>
@@ -3939,9 +3905,9 @@
         <v>99</v>
       </c>
     </row>
-    <row r="36" spans="2:4" ht="26" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
-        <v>358</v>
+        <v>343</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>9</v>
@@ -3952,7 +3918,7 @@
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
-        <v>359</v>
+        <v>344</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>9</v>
@@ -3961,9 +3927,9 @@
         <v>101</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
-        <v>360</v>
+        <v>345</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>9</v>
@@ -3972,9 +3938,9 @@
         <v>102</v>
       </c>
     </row>
-    <row r="39" spans="2:4" ht="26" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>361</v>
+        <v>346</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>9</v>
@@ -3985,7 +3951,7 @@
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
-        <v>362</v>
+        <v>347</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>9</v>
@@ -3995,29 +3961,29 @@
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B41" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D41" s="3" t="s">
+      <c r="B41" s="1"/>
+      <c r="C41" s="4"/>
+    </row>
+    <row r="42" spans="2:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="B42" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="C42" s="4"/>
+    </row>
+    <row r="43" spans="2:4" ht="16.5" x14ac:dyDescent="0.45">
+      <c r="B43" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D43" s="3" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B42" s="1"/>
-      <c r="C42" s="4"/>
-    </row>
-    <row r="43" spans="2:4" ht="26" x14ac:dyDescent="0.2">
-      <c r="B43" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="C43" s="4"/>
-    </row>
-    <row r="44" spans="2:4" ht="16.5" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
-        <v>365</v>
+        <v>350</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>9</v>
@@ -4026,9 +3992,9 @@
         <v>106</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="2:4" ht="39" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
-        <v>366</v>
+        <v>351</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>9</v>
@@ -4037,9 +4003,9 @@
         <v>107</v>
       </c>
     </row>
-    <row r="46" spans="2:4" ht="39" x14ac:dyDescent="0.2">
+    <row r="46" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s">
-        <v>367</v>
+        <v>463</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>9</v>
@@ -4050,7 +4016,7 @@
     </row>
     <row r="47" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
-        <v>368</v>
+        <v>352</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>9</v>
@@ -4061,7 +4027,7 @@
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B48" s="1" t="s">
-        <v>369</v>
+        <v>353</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>9</v>
@@ -4072,7 +4038,7 @@
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B49" s="1" t="s">
-        <v>371</v>
+        <v>355</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>9</v>
@@ -4083,7 +4049,7 @@
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B50" s="1" t="s">
-        <v>370</v>
+        <v>354</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>9</v>
@@ -4092,23 +4058,26 @@
         <v>112</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="C51" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D51" s="3" t="s">
+    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B52" t="s">
+        <v>356</v>
+      </c>
+      <c r="C52" s="4"/>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B53" s="1" t="s">
+        <v>357</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D53" s="3" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B53" t="s">
-        <v>372</v>
-      </c>
-      <c r="C53" s="4"/>
     </row>
     <row r="54" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B54" s="1" t="s">
-        <v>373</v>
+        <v>358</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>9</v>
@@ -4118,25 +4087,14 @@
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B55" s="1" t="s">
-        <v>374</v>
+      <c r="B55" t="s">
+        <v>359</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>115</v>
-      </c>
-    </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B56" t="s">
-        <v>375</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -4150,8 +4108,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView topLeftCell="A39" zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
+      <selection activeCell="A52" sqref="A52:XFD52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -4167,7 +4125,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -4191,7 +4149,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>272</v>
+        <v>257</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -4207,21 +4165,21 @@
     </row>
     <row r="8" spans="1:4" ht="19.5" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="D8" s="4" t="s" ph="1">
-        <v>242</v>
+        <v>227</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>376</v>
+        <v>360</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -4229,19 +4187,19 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>410</v>
+        <v>394</v>
       </c>
       <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>377</v>
+        <v>361</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4249,13 +4207,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>378</v>
+        <v>362</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -4263,13 +4221,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>379</v>
+        <v>363</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4277,24 +4235,24 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>380</v>
+        <v>364</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>381</v>
+        <v>365</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4302,13 +4260,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>382</v>
+        <v>366</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -4316,30 +4274,30 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>411</v>
+        <v>395</v>
       </c>
       <c r="C19" s="4"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>383</v>
+        <v>367</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>384</v>
+        <v>368</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -4347,7 +4305,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>412</v>
+        <v>396</v>
       </c>
       <c r="C23" s="4"/>
     </row>
@@ -4356,13 +4314,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>385</v>
+        <v>369</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D24" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="39" x14ac:dyDescent="0.2">
@@ -4370,24 +4328,24 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>386</v>
+        <v>370</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>387</v>
+        <v>371</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D26" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -4395,24 +4353,24 @@
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>388</v>
+        <v>372</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D27" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
-        <v>381</v>
+        <v>365</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D28" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -4420,24 +4378,24 @@
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>389</v>
+        <v>373</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D29" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>390</v>
+        <v>374</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D30" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -4445,24 +4403,24 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>391</v>
+        <v>375</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
-        <v>392</v>
+        <v>376</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -4470,13 +4428,13 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>393</v>
+        <v>377</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4484,13 +4442,13 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>394</v>
+        <v>378</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D34" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -4498,7 +4456,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
-        <v>397</v>
+        <v>381</v>
       </c>
       <c r="C36" s="4"/>
     </row>
@@ -4507,13 +4465,13 @@
         <v>4</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>395</v>
+        <v>379</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D37" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="26" x14ac:dyDescent="0.2">
@@ -4521,24 +4479,24 @@
         <v>4</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D38" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>396</v>
+        <v>380</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D39" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -4546,13 +4504,13 @@
         <v>4</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D40" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -4560,201 +4518,155 @@
         <v>4</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>399</v>
+        <v>383</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D41" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
-        <v>400</v>
+        <v>384</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D42" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>4</v>
       </c>
+      <c r="B43" s="1" t="s">
+        <v>385</v>
+      </c>
       <c r="C43" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D43" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B44" s="1" t="s">
+        <v>386</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D44" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>4</v>
       </c>
-      <c r="B44" s="1" t="s">
-        <v>401</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D44" t="s">
+      <c r="B45" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D45" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B45" s="1" t="s">
-        <v>402</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D45" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B46" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D46" t="s">
         <v>145</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>4</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D46" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B47" s="2" t="s">
-        <v>404</v>
+        <v>389</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D47" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>4</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D48" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B48" s="2" t="s">
-        <v>405</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D48" t="s">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B49" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D49" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A49" t="s">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>4</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>406</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D49" t="s">
+      <c r="B50" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D50" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B50" s="1" t="s">
-        <v>407</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D50" t="s">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B51" s="1" t="s">
+        <v>392</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D51" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A51" t="s">
-        <v>4</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D51" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B52" s="1" t="s">
+        <v>393</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D52" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A52" t="s">
-        <v>4</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="C52" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D52" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="19.5" x14ac:dyDescent="0.2">
-      <c r="C53" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D53" t="s" ph="1">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A54" t="s">
-        <v>4</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D54" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B55" s="1" t="s">
-        <v>408</v>
-      </c>
-      <c r="C55" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D55" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C56" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D56" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B57" s="1" t="s">
-        <v>409</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D57" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="69" spans="4:4" ht="19.5" x14ac:dyDescent="0.2">
-      <c r="D69" ph="1"/>
-    </row>
-    <row r="76" spans="4:4" ht="19.5" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" ht="19.5" x14ac:dyDescent="0.2">
+      <c r="D64" ph="1"/>
+    </row>
+    <row r="71" spans="4:4" ht="19.5" x14ac:dyDescent="0.2">
+      <c r="D71" ph="1"/>
+    </row>
+    <row r="76" spans="4:4" x14ac:dyDescent="0.2">
       <c r="D76" ph="1"/>
     </row>
   </sheetData>
@@ -4766,10 +4678,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45722500-6D63-48B1-B48D-DE8F55297416}">
-  <dimension ref="A1:D21"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="A16" sqref="A16:XFD16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -4785,7 +4697,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -4793,7 +4705,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>260</v>
+        <v>245</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -4809,7 +4721,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>271</v>
+        <v>256</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -4826,21 +4738,21 @@
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="D8" s="4" t="s" ph="1">
-        <v>243</v>
+        <v>228</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>414</v>
+        <v>398</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -4848,13 +4760,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>415</v>
+        <v>399</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -4862,120 +4774,101 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>416</v>
+        <v>400</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>4</v>
+        <v>154</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
+        <v>401</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>161</v>
+        <v>155</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>417</v>
+        <v>402</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>418</v>
+        <v>403</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>163</v>
+        <v>157</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>419</v>
+        <v>405</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>421</v>
+        <v>404</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
+        <v>406</v>
+      </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>420</v>
+        <v>407</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>422</v>
+        <v>408</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B20" s="1" t="s">
-        <v>423</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D20" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B21" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D21" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>
@@ -4986,10 +4879,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView topLeftCell="A9" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24"/>
+      <selection activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -5005,7 +4898,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5013,7 +4906,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -5029,7 +4922,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>270</v>
+        <v>255</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="19.5" x14ac:dyDescent="0.2">
@@ -5037,10 +4930,10 @@
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="D8" s="4" t="s" ph="1">
-        <v>244</v>
+        <v>229</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -5048,13 +4941,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>332</v>
+        <v>317</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -5062,13 +4955,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>425</v>
+        <v>409</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -5076,13 +4969,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>426</v>
+        <v>410</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -5090,139 +4983,134 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>388</v>
+        <v>372</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>427</v>
+        <v>411</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>428</v>
+        <v>412</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>429</v>
+        <v>413</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="39" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>434</v>
+        <v>418</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>428</v>
+        <v>412</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>428</v>
+        <v>412</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
+        <v>412</v>
+      </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>414</v>
+      </c>
       <c r="C20" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>430</v>
+        <v>415</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>431</v>
+        <v>416</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>432</v>
+        <v>417</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B24" s="1" t="s">
-        <v>433</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D24" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -5234,10 +5122,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView topLeftCell="A4" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -5250,10 +5138,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>264</v>
+        <v>249</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>265</v>
+        <v>250</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5261,7 +5149,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>261</v>
+        <v>246</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -5277,7 +5165,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>269</v>
+        <v>254</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="19.5" x14ac:dyDescent="0.2">
@@ -5285,21 +5173,21 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="D7" s="4" t="s" ph="1">
-        <v>245</v>
+        <v>230</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>435</v>
+        <v>419</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -5307,254 +5195,233 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>436</v>
+        <v>420</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>437</v>
+        <v>421</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>438</v>
+        <v>422</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
+        <v>423</v>
+      </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>439</v>
+        <v>424</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>440</v>
+        <v>425</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
+        <v>426</v>
+      </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>441</v>
+        <v>427</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
+        <v>428</v>
+      </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>442</v>
+        <v>429</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>443</v>
+        <v>430</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>444</v>
+        <v>431</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>445</v>
+        <v>464</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>446</v>
+        <v>432</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>447</v>
+        <v>433</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
+        <v>434</v>
+      </c>
       <c r="C24" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D24" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>448</v>
+        <v>435</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>449</v>
+        <v>436</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D26" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>450</v>
+        <v>437</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D27" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
-        <v>451</v>
+        <v>438</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D28" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
-        <v>452</v>
+        <v>439</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D29" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B30" s="1" t="s">
-        <v>453</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D30" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B31" s="1" t="s">
-        <v>454</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D31" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B32" s="1" t="s">
-        <v>455</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D32" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -5566,10 +5433,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CB03C1F-8A6F-4A43-BA2E-2C62B3131330}">
-  <dimension ref="A1:D75"/>
+  <dimension ref="A1:D72"/>
   <sheetViews>
     <sheetView topLeftCell="A9" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="A17" sqref="A17:XFD17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -5586,7 +5453,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -5596,7 +5463,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>266</v>
+        <v>251</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -5616,7 +5483,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>268</v>
+        <v>253</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -5636,245 +5503,236 @@
     <row r="7" spans="1:4" ht="19.5" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="2" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="s" ph="1">
-        <v>246</v>
+        <v>231</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="5" t="s">
-        <v>456</v>
+        <v>440</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="5" t="s">
-        <v>388</v>
+        <v>372</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
-      <c r="B10" s="5"/>
+      <c r="B10" s="5" t="s">
+        <v>404</v>
+      </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="5" t="s">
-        <v>420</v>
+        <v>441</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
+      <c r="B12" s="5" t="s">
+        <v>442</v>
+      </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
-      <c r="B13" s="5" t="s">
-        <v>457</v>
+      <c r="B13" s="3" t="s">
+        <v>443</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="5" t="s">
-        <v>458</v>
+        <v>444</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
-      <c r="B15" s="3" t="s">
-        <v>459</v>
+      <c r="B15" s="5" t="s">
+        <v>445</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="5" t="s">
-        <v>460</v>
+        <v>446</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="5" t="s">
-        <v>461</v>
+        <v>447</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="5" t="s">
-        <v>462</v>
+        <v>448</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
-      <c r="B19" s="5"/>
+      <c r="B19" s="5" t="s">
+        <v>449</v>
+      </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="5" t="s">
-        <v>463</v>
+        <v>450</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="5" t="s">
-        <v>464</v>
+        <v>451</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
       <c r="B22" s="5" t="s">
-        <v>465</v>
+        <v>452</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
       <c r="B23" s="5" t="s">
-        <v>466</v>
+        <v>453</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
       <c r="B24" s="5" t="s">
-        <v>467</v>
+        <v>454</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
-      <c r="B25" s="5" t="s">
-        <v>468</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>229</v>
-      </c>
+      <c r="B25" s="5"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
-      <c r="B26" s="5" t="s">
-        <v>469</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>230</v>
-      </c>
+      <c r="B26" s="5"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="4"/>
-      <c r="B27" s="5" t="s">
-        <v>470</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D27" s="4" t="s">
-        <v>231</v>
-      </c>
+      <c r="A27" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B27" s="5"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
@@ -5889,9 +5747,7 @@
       <c r="D29" s="4"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A30" s="4"/>
       <c r="B30" s="5"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -6059,7 +5915,9 @@
       <c r="D57" s="4"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="4"/>
+      <c r="A58" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="B58" s="5"/>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
@@ -6077,9 +5935,7 @@
       <c r="D60" s="4"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A61" s="4"/>
       <c r="B61" s="5"/>
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
@@ -6121,7 +5977,9 @@
       <c r="D67" s="4"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="4"/>
+      <c r="A68" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="B68" s="5"/>
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
@@ -6134,36 +5992,16 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="4"/>
-      <c r="B70" s="5"/>
       <c r="C70" s="4"/>
       <c r="D70" s="4"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B71" s="5"/>
+      <c r="A71" s="4"/>
       <c r="C71" s="4"/>
       <c r="D71" s="4"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="4"/>
-      <c r="B72" s="5"/>
-      <c r="C72" s="4"/>
       <c r="D72" s="4"/>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="4"/>
-      <c r="C73" s="4"/>
-      <c r="D73" s="4"/>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="4"/>
-      <c r="C74" s="4"/>
-      <c r="D74" s="4"/>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D75" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
win11_en.xlsx: add MFA PDFs.
</commit_message>
<xml_diff>
--- a/win11_en.xlsx
+++ b/win11_en.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta2025\fresta-github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC15651C-923C-4D5F-8316-41D190D4091D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71871504-840A-4958-AAF2-D292B78B8A2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" tabRatio="729" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" tabRatio="729" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="464">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="470">
   <si>
     <t>header1</t>
   </si>
@@ -1723,6 +1723,30 @@
   </si>
   <si>
     <t>&lt;h3 id="config-edge-first"&gt;Configure Microsoft Edge&lt;/h3&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h2 id="mfa-hirodai-id"&gt;Configure Multi-Factor Authentication for Hirodai ID&lt;/h2&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h2 id="mfa-imc-account"&gt;Configure Multi-Factor Authentication for IMC Account&lt;/h2&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>raw:&lt;iframe width="100%" height="100%" style="aspect-ratio: 1000 / 1414" src="https://www.media.hiroshima-u.ac.jp/wp-content/uploads/2023/03/mfa-easymanual-20230327-en_HIRODAIID.pdf"&gt;&lt;/iframe&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>raw:&lt;iframe width="100%" height="100%" style="aspect-ratio: 1000 / 1414" src="https://www.media.hiroshima-u.ac.jp/wp-content/uploads/2025/02/mfa-easymanual-20250225-en_IMCaccount.pdf"&gt;&lt;/iframe&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>This PDF intructs how to configure MFA for Hirodai ID. This is required for the access from out of the campus network.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>This PDF intructs how to configure MFA for IMC account. This is required for the access from out of the campus network.</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -2174,10 +2198,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EFCA2B8-55C7-4AC3-9E13-35156DBD8BC5}">
-  <dimension ref="A1:D75"/>
+  <dimension ref="A1:D72"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="13" x14ac:dyDescent="0.2"/>
@@ -2342,34 +2366,39 @@
       <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16" s="4"/>
-      <c r="B16" s="5"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="4"/>
-      <c r="B17" s="5"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="4"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
+      <c r="B16" s="2" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="B17" s="2" t="s">
+        <v>468</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="3" customFormat="1" ht="13" customHeight="1" ph="1" x14ac:dyDescent="0.2">
+      <c r="B18" s="2"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="4"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A20" s="4"/>
-      <c r="B20" s="5"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
+      <c r="B19" s="2" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="26" x14ac:dyDescent="0.2">
+      <c r="B20" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>467</v>
+      </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
@@ -2408,7 +2437,9 @@
       <c r="D26" s="4"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A27" s="4"/>
+      <c r="A27" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="B27" s="5"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
@@ -2426,9 +2457,7 @@
       <c r="D29" s="4"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A30" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A30" s="4"/>
       <c r="B30" s="5"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -2596,7 +2625,9 @@
       <c r="D57" s="4"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A58" s="4"/>
+      <c r="A58" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="B58" s="5"/>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
@@ -2614,9 +2645,7 @@
       <c r="D60" s="4"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A61" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A61" s="4"/>
       <c r="B61" s="5"/>
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
@@ -2658,7 +2687,9 @@
       <c r="D67" s="4"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A68" s="4"/>
+      <c r="A68" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="B68" s="5"/>
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
@@ -2671,36 +2702,16 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" s="4"/>
-      <c r="B70" s="5"/>
       <c r="C70" s="4"/>
       <c r="D70" s="4"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A71" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B71" s="5"/>
+      <c r="A71" s="4"/>
       <c r="C71" s="4"/>
       <c r="D71" s="4"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A72" s="4"/>
-      <c r="B72" s="5"/>
-      <c r="C72" s="4"/>
       <c r="D72" s="4"/>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A73" s="4"/>
-      <c r="C73" s="4"/>
-      <c r="D73" s="4"/>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A74" s="4"/>
-      <c r="C74" s="4"/>
-      <c r="D74" s="4"/>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D75" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -3518,8 +3529,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D3AC582-7A6D-4EA0-8C12-75B8749BA9E2}">
   <dimension ref="A1:D56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B36" sqref="B36"/>
+    <sheetView topLeftCell="A49" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B58" sqref="B58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
win11_en.xlsx: fix section list
</commit_message>
<xml_diff>
--- a/win11_en.xlsx
+++ b/win11_en.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta2025\fresta-github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{041BD149-7C9C-41C1-8D5A-8243C34843F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D62D0C2-A023-4F2B-99A3-331F7DE60176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" tabRatio="729" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" tabRatio="729" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="484">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="487">
   <si>
     <t>header1</t>
   </si>
@@ -1443,10 +1443,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Search "excel" or "word" or "powerpoint". If such Microsoft Office applications are already installed, some App would be returned. If you found them, proceed to next chapter.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Search "Excel" (or "Word" or "PowerPoint") from Start menu.</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -1532,10 +1528,6 @@
   </si>
   <si>
     <t>Open Start menu</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Search "teams" in Start menu. If Microsoft Teams app is already installed, proceed to next chapter.</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1761,17 +1753,6 @@
   </si>
   <si>
     <t>&lt;h2 id="sign-in"&gt;Sign-in with new local account&lt;/h2&gt;</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve">This chapter show how to create new local account to be used as a student. The free-charged Microsoft account created for the initializatin has limited storage online. Using it as stable account would fill the storage immediately, and you would have the difficulty to distinguish it with the student account. Using new local account would be safer.
-&lt;ul&gt;
-&lt;li&gt;&lt;a href="#check-activation"&gt;Check the license of Windows&lt;/a&gt;&lt;/li&gt;
-&lt;li&gt;&lt;a href="#check-anti-virus"&gt;Check anti-virus software&lt;/a&gt;&lt;/li&gt;
-&lt;li&gt;&lt;a href="#add-local-account"Add a local account&lt;/a&gt;&lt;/li&gt;
-&lt;li&gt;&lt;a href="#sign-in"&gt;Sign-in with new local account&lt;/a&gt;&lt;/li&gt;
-&lt;/ul&gt;
-</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1827,6 +1808,42 @@
   </si>
   <si>
     <t>This chapter describes how to configure OneDrive online strage service.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>This chapter describes how to configure Microsoft Teams.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>&lt;h2 id="hu-cup"&gt;Configure your PC to connect to the campus network "HU-CUP" automatically.&lt;/h2&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>This chapter describes how to configure your PC to connect to the campus network "HU-CUP", and configure the multi-factor authentication. If you initialize your PC in the campus, the configuration for HU-CUP would be already done, proceed to &lt;a href="#mfa-hirodai-id"&gt;the MFA settings&lt;/a&gt;.
+&lt;ul&gt;
+&lt;li&gt;&lt;a href="#hu-cup"&gt;Configure your PC to connect to the campus network "HU-CUP" automatically.&lt;/a&gt;&lt;/li&gt;
+&lt;li&gt;&lt;a href="#mfa-hirodai-id"&gt;Configure MFA for Hirodai ID.&lt;/a&gt;&lt;/li&gt;
+&lt;li&gt;&lt;a href="#mfa-imc-account"&gt;Configure MFA for IMC account.&lt;/a&gt;&lt;/li&gt;
+&lt;/ul&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t xml:space="preserve">This chapter show how to create new local account to be used as a student. The free-charged Microsoft account created for the initializatin has limited storage online. Using it as stable account would fill the storage immediately, and you would have the difficulty to distinguish it with the student account. Using new local account would be safer.
+&lt;ul&gt;
+&lt;li&gt;&lt;a href="#check-activation"&gt;Check the license of Windows&lt;/a&gt;&lt;/li&gt;
+&lt;li&gt;&lt;a href="#check-anti-virus"&gt;Check anti-virus software&lt;/a&gt;&lt;/li&gt;
+&lt;li&gt;&lt;a href="#add-local-account"&gt;Add a local account&lt;/a&gt;&lt;/li&gt;
+&lt;li&gt;&lt;a href="#sign-in"&gt;Sign-in with new local account&lt;/a&gt;&lt;/li&gt;
+&lt;/ul&gt;
+</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Search "excel" or "word" or "powerpoint". If such Microsoft Office applications are already installed, some App would be returned. If you find them, proceed to &lt;a href="ch5.html"&gt;the next chapter&lt;/a&gt;.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Search "teams" in Start menu. If Microsoft Teams app is already installed, proceed to &lt;a href="ch9.html"&gt;the next chapter&lt;/a&gt;.</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -2278,10 +2295,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EFCA2B8-55C7-4AC3-9E13-35156DBD8BC5}">
-  <dimension ref="A1:D72"/>
+  <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2345,158 +2362,162 @@
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:4" ht="21" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" ht="121.5" x14ac:dyDescent="0.15">
       <c r="A7" s="4"/>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="5" t="s">
+        <v>483</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.15">
+      <c r="A8" s="4"/>
+      <c r="B8" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4" t="s" ph="1">
+      <c r="C8" s="4"/>
+      <c r="D8" s="4" t="s" ph="1">
         <v>230</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8" s="4"/>
-      <c r="B8" s="5" t="s">
-        <v>451</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" ht="21" x14ac:dyDescent="0.15">
       <c r="A9" s="4"/>
-      <c r="B9" s="5" t="s">
-        <v>452</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B9" s="2"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4" ph="1"/>
+    </row>
+    <row r="10" spans="1:4" ht="21" x14ac:dyDescent="0.15">
       <c r="A10" s="4"/>
-      <c r="B10" s="5" t="s">
-        <v>453</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>217</v>
-      </c>
+      <c r="B10" s="2" t="s">
+        <v>482</v>
+      </c>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4" ph="1"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="4"/>
       <c r="B11" s="5" t="s">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="4"/>
       <c r="B12" s="5" t="s">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="27" x14ac:dyDescent="0.15">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="4"/>
       <c r="B13" s="5" t="s">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="4"/>
       <c r="B14" s="5" t="s">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="4"/>
-      <c r="B15" s="5"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="B16" s="2" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="27" x14ac:dyDescent="0.15">
-      <c r="B17" s="2" t="s">
-        <v>466</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="3" customFormat="1" ht="12.95" customHeight="1" ph="1" x14ac:dyDescent="0.15">
-      <c r="B18" s="2"/>
+      <c r="B15" s="5" t="s">
+        <v>453</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="27" x14ac:dyDescent="0.15">
+      <c r="A16" s="4"/>
+      <c r="B16" s="5" t="s">
+        <v>454</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A17" s="4"/>
+      <c r="B17" s="5" t="s">
+        <v>455</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A18" s="4"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B19" s="2" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="B20" s="2" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D20" s="3" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="3" customFormat="1" ht="12.95" customHeight="1" ph="1" x14ac:dyDescent="0.15">
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="B22" s="2" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="27" x14ac:dyDescent="0.15">
+      <c r="B23" s="2" t="s">
         <v>465</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A21" s="4"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A22" s="4"/>
-      <c r="B22" s="5"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A23" s="4"/>
-      <c r="B23" s="5"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
+      <c r="C23" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>463</v>
+      </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" s="4"/>
@@ -2517,9 +2538,7 @@
       <c r="D26" s="4"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A27" s="4"/>
       <c r="B27" s="5"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
@@ -2537,7 +2556,9 @@
       <c r="D29" s="4"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A30" s="4"/>
+      <c r="A30" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="B30" s="5"/>
       <c r="C30" s="4"/>
       <c r="D30" s="4"/>
@@ -2705,9 +2726,7 @@
       <c r="D57" s="4"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A58" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A58" s="4"/>
       <c r="B58" s="5"/>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
@@ -2725,7 +2744,9 @@
       <c r="D60" s="4"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A61" s="4"/>
+      <c r="A61" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="B61" s="5"/>
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
@@ -2767,9 +2788,7 @@
       <c r="D67" s="4"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A68" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A68" s="4"/>
       <c r="B68" s="5"/>
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
@@ -2782,16 +2801,36 @@
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A70" s="4"/>
+      <c r="B70" s="5"/>
       <c r="C70" s="4"/>
       <c r="D70" s="4"/>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A71" s="4"/>
+      <c r="A71" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B71" s="5"/>
       <c r="C71" s="4"/>
       <c r="D71" s="4"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A72" s="4"/>
+      <c r="B72" s="5"/>
+      <c r="C72" s="4"/>
       <c r="D72" s="4"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A73" s="4"/>
+      <c r="C73" s="4"/>
+      <c r="D73" s="4"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A74" s="4"/>
+      <c r="C74" s="4"/>
+      <c r="D74" s="4"/>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D75" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>
@@ -2858,7 +2897,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>468</v>
+        <v>466</v>
       </c>
       <c r="D7" s="3" ph="1"/>
     </row>
@@ -3214,7 +3253,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -3260,7 +3299,7 @@
     </row>
     <row r="6" spans="1:4" ht="189" x14ac:dyDescent="0.15">
       <c r="B6" s="1" t="s">
-        <v>473</v>
+        <v>484</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="21" x14ac:dyDescent="0.15">
@@ -3305,7 +3344,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B12" s="2" t="s">
-        <v>469</v>
+        <v>467</v>
       </c>
       <c r="C12" s="4"/>
     </row>
@@ -3336,7 +3375,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B16" s="2" t="s">
-        <v>470</v>
+        <v>468</v>
       </c>
       <c r="C16" s="4"/>
     </row>
@@ -3381,7 +3420,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B21" s="2" t="s">
-        <v>471</v>
+        <v>469</v>
       </c>
       <c r="C21" s="4"/>
     </row>
@@ -3546,7 +3585,7 @@
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B35" s="2" t="s">
-        <v>472</v>
+        <v>470</v>
       </c>
       <c r="C35" s="4"/>
     </row>
@@ -3649,7 +3688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D3AC582-7A6D-4EA0-8C12-75B8749BA9E2}">
   <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -3706,7 +3745,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="D6"/>
     </row>
@@ -3739,7 +3778,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B10" s="1" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10"/>
@@ -3787,7 +3826,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B15" s="1" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15"/>
@@ -3835,7 +3874,7 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B20" s="1" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20"/>
@@ -3886,7 +3925,7 @@
     </row>
     <row r="25" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="B25" s="1" t="s">
-        <v>458</v>
+        <v>456</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>9</v>
@@ -3913,7 +3952,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B28" s="1" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28"/>
@@ -4023,7 +4062,7 @@
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B39" s="1" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="C39" s="4"/>
     </row>
@@ -4077,7 +4116,7 @@
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B45" s="1" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="C45" s="4"/>
     </row>
@@ -4094,7 +4133,7 @@
     </row>
     <row r="47" spans="2:4" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B47" s="1" t="s">
-        <v>461</v>
+        <v>459</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>9</v>
@@ -4192,7 +4231,7 @@
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B57" s="1" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>9</v>
@@ -4295,8 +4334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A30" zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4350,7 +4389,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.15">
@@ -4664,12 +4703,12 @@
         <v>134</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="27" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:4" ht="40.5" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>4</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>393</v>
+        <v>485</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>9</v>
@@ -4922,7 +4961,7 @@
     </row>
     <row r="7" spans="1:4" ht="67.5" x14ac:dyDescent="0.15">
       <c r="B7" s="1" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.15">
@@ -4938,7 +4977,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B9" s="1" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
@@ -4952,7 +4991,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
@@ -4966,7 +5005,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
@@ -4977,7 +5016,7 @@
     </row>
     <row r="12" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="B12" s="1" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
@@ -4988,7 +5027,7 @@
     </row>
     <row r="13" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="B13" s="1" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
@@ -4999,7 +5038,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B14" s="1" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
@@ -5010,7 +5049,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B15" s="1" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
@@ -5021,7 +5060,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B16" s="1" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
@@ -5032,7 +5071,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B17" s="1" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
@@ -5043,7 +5082,7 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B18" s="1" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
@@ -5054,7 +5093,7 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B19" s="1" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
@@ -5119,7 +5158,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B7" s="1" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.15">
@@ -5152,7 +5191,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
@@ -5166,7 +5205,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
@@ -5191,7 +5230,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B13" s="1" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
@@ -5202,7 +5241,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B14" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
@@ -5213,7 +5252,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B15" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
@@ -5224,7 +5263,7 @@
     </row>
     <row r="16" spans="1:4" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B16" s="1" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
@@ -5235,7 +5274,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B17" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
@@ -5246,7 +5285,7 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B18" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
@@ -5257,7 +5296,7 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B19" s="1" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
@@ -5268,7 +5307,7 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B20" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>9</v>
@@ -5279,7 +5318,7 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B21" s="1" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
@@ -5290,7 +5329,7 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B22" s="1" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
@@ -5301,7 +5340,7 @@
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B23" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
@@ -5321,8 +5360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -5378,7 +5417,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B8" s="1" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>9</v>
@@ -5387,12 +5426,12 @@
         <v>176</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>416</v>
+        <v>486</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
@@ -5403,7 +5442,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B10" s="1" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
@@ -5414,7 +5453,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B11" s="1" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
@@ -5425,7 +5464,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B12" s="1" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
@@ -5436,7 +5475,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B13" s="1" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
@@ -5447,7 +5486,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B14" s="1" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
@@ -5458,7 +5497,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B15" s="1" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
@@ -5469,7 +5508,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B16" s="1" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
@@ -5480,7 +5519,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B17" s="1" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
@@ -5491,7 +5530,7 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B18" s="1" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
@@ -5502,7 +5541,7 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B19" s="1" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
@@ -5513,7 +5552,7 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B20" s="1" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>9</v>
@@ -5524,7 +5563,7 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B21" s="1" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
@@ -5535,7 +5574,7 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B22" s="1" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
@@ -5546,7 +5585,7 @@
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B23" s="1" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
@@ -5557,7 +5596,7 @@
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B24" s="1" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>9</v>
@@ -5568,7 +5607,7 @@
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B25" s="1" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>9</v>
@@ -5579,7 +5618,7 @@
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B26" s="1" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>9</v>
@@ -5590,7 +5629,7 @@
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B27" s="1" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>9</v>
@@ -5601,7 +5640,7 @@
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B28" s="1" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>9</v>
@@ -5612,7 +5651,7 @@
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B29" s="1" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>9</v>
@@ -5630,10 +5669,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CB03C1F-8A6F-4A43-BA2E-2C62B3131330}">
-  <dimension ref="A1:D72"/>
+  <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView topLeftCell="A9" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:XFD17"/>
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -5697,225 +5736,227 @@
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:4" ht="21" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="4"/>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="5" t="s">
+        <v>481</v>
+      </c>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.15">
+      <c r="A8" s="4"/>
+      <c r="B8" s="2" t="s">
         <v>257</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4" t="s" ph="1">
+      <c r="C8" s="4"/>
+      <c r="D8" s="4" t="s" ph="1">
         <v>229</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A8" s="4"/>
-      <c r="B8" s="5" t="s">
-        <v>436</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="4"/>
       <c r="B9" s="5" t="s">
-        <v>368</v>
+        <v>434</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="4"/>
       <c r="B10" s="5" t="s">
-        <v>400</v>
+        <v>368</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="4"/>
       <c r="B11" s="5" t="s">
-        <v>437</v>
+        <v>399</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="4"/>
       <c r="B12" s="5" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="4"/>
-      <c r="B13" s="3" t="s">
-        <v>439</v>
+      <c r="B13" s="5" t="s">
+        <v>436</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="4"/>
-      <c r="B14" s="5" t="s">
-        <v>440</v>
+      <c r="B14" s="3" t="s">
+        <v>437</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="4"/>
       <c r="B15" s="5" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="4"/>
       <c r="B16" s="5" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="4"/>
       <c r="B17" s="5" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="4"/>
       <c r="B18" s="5" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="4"/>
       <c r="B19" s="5" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="4"/>
       <c r="B20" s="5" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" s="4"/>
       <c r="B21" s="5" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" s="4"/>
       <c r="B22" s="5" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" s="4"/>
       <c r="B23" s="5" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" s="4"/>
       <c r="B24" s="5" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" s="4"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
+      <c r="B25" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>214</v>
+      </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A26" s="4"/>
@@ -5924,15 +5965,15 @@
       <c r="D26" s="4"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A27" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A27" s="4"/>
       <c r="B27" s="5"/>
       <c r="C27" s="4"/>
       <c r="D27" s="4"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A28" s="4"/>
+      <c r="A28" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="B28" s="5"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
@@ -6112,15 +6153,15 @@
       <c r="D57" s="4"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A58" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A58" s="4"/>
       <c r="B58" s="5"/>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A59" s="4"/>
+      <c r="A59" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="B59" s="5"/>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
@@ -6174,21 +6215,22 @@
       <c r="D67" s="4"/>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A68" s="4" t="s">
-        <v>4</v>
-      </c>
+      <c r="A68" s="4"/>
       <c r="B68" s="5"/>
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.15">
-      <c r="A69" s="4"/>
+      <c r="A69" s="4" t="s">
+        <v>4</v>
+      </c>
       <c r="B69" s="5"/>
       <c r="C69" s="4"/>
       <c r="D69" s="4"/>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A70" s="4"/>
+      <c r="B70" s="5"/>
       <c r="C70" s="4"/>
       <c r="D70" s="4"/>
     </row>
@@ -6198,7 +6240,12 @@
       <c r="D71" s="4"/>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="A72" s="4"/>
+      <c r="C72" s="4"/>
       <c r="D72" s="4"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.15">
+      <c r="D73" s="4"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1"/>

</xml_diff>

<commit_message>
win11_en: use low-quality JPEG at ch9 (test)
</commit_message>
<xml_diff>
--- a/win11_en.xlsx
+++ b/win11_en.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta2025\fresta-github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D62D0C2-A023-4F2B-99A3-331F7DE60176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6197AA7C-D96B-46EF-86B4-AB1F07984EB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" tabRatio="729" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -688,27 +688,6 @@
   </si>
   <si>
     <t>win11-en-part8-00.01.58.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part9-00.00.06.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part9-00.00.07.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part9-00.00.12.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part9-00.00.13.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part9-00.00.17.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part9-00.00.33.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part9-00.00.41.000.png</t>
   </si>
   <si>
     <t>raw:&lt;iframe width="100%" height="315" src="https://www.youtube.com/embed/2Ojmvtgy35Y?list=PLjGYIiYIuSrByd_Llk0LaHf1-ZJzhU4fQ" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen=""&gt;&lt;/iframe&gt;</t>
@@ -1845,6 +1824,27 @@
   <si>
     <t>Search "teams" in Start menu. If Microsoft Teams app is already installed, proceed to &lt;a href="ch9.html"&gt;the next chapter&lt;/a&gt;.</t>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>win11-en-part9-00.00.06.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part9-00.00.07.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part9-00.00.12.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part9-00.00.13.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part9-00.00.17.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part9-00.00.33.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part9-00.00.41.000.jpg</t>
   </si>
 </sst>
 </file>
@@ -2255,7 +2255,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="67.5" x14ac:dyDescent="0.15">
@@ -2297,8 +2297,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EFCA2B8-55C7-4AC3-9E13-35156DBD8BC5}">
   <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView tabSelected="1" topLeftCell="B9" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2315,7 +2315,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -2325,7 +2325,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -2345,7 +2345,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -2365,7 +2365,7 @@
     <row r="7" spans="1:4" ht="121.5" x14ac:dyDescent="0.15">
       <c r="A7" s="4"/>
       <c r="B7" s="5" t="s">
-        <v>483</v>
+        <v>476</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -2373,11 +2373,11 @@
     <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.15">
       <c r="A8" s="4"/>
       <c r="B8" s="2" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4" t="s" ph="1">
-        <v>230</v>
+        <v>223</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="21" x14ac:dyDescent="0.15">
@@ -2389,7 +2389,7 @@
     <row r="10" spans="1:4" ht="21" x14ac:dyDescent="0.15">
       <c r="A10" s="4"/>
       <c r="B10" s="2" t="s">
-        <v>482</v>
+        <v>475</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4" ph="1"/>
@@ -2397,85 +2397,85 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="4"/>
       <c r="B11" s="5" t="s">
-        <v>449</v>
+        <v>442</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>215</v>
+        <v>480</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="4"/>
       <c r="B12" s="5" t="s">
-        <v>450</v>
+        <v>443</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>216</v>
+        <v>481</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="4"/>
       <c r="B13" s="5" t="s">
-        <v>451</v>
+        <v>444</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>217</v>
+        <v>482</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="4"/>
       <c r="B14" s="5" t="s">
-        <v>452</v>
+        <v>445</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>218</v>
+        <v>483</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="4"/>
       <c r="B15" s="5" t="s">
-        <v>453</v>
+        <v>446</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>219</v>
+        <v>484</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="A16" s="4"/>
       <c r="B16" s="5" t="s">
-        <v>454</v>
+        <v>447</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>220</v>
+        <v>485</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="4"/>
       <c r="B17" s="5" t="s">
-        <v>455</v>
+        <v>448</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>221</v>
+        <v>486</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
@@ -2486,18 +2486,18 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B19" s="2" t="s">
-        <v>460</v>
+        <v>453</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="B20" s="2" t="s">
-        <v>464</v>
+        <v>457</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>462</v>
+        <v>455</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="3" customFormat="1" ht="12.95" customHeight="1" ph="1" x14ac:dyDescent="0.15">
@@ -2505,18 +2505,18 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B22" s="2" t="s">
-        <v>461</v>
+        <v>454</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="B23" s="2" t="s">
-        <v>465</v>
+        <v>458</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>463</v>
+        <v>456</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
@@ -2860,7 +2860,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
@@ -2868,7 +2868,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
@@ -2884,7 +2884,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
@@ -2897,16 +2897,16 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>466</v>
+        <v>459</v>
       </c>
       <c r="D7" s="3" ph="1"/>
     </row>
     <row r="8" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="2" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="D8" s="4" t="s" ph="1">
-        <v>222</v>
+        <v>215</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="21" x14ac:dyDescent="0.15">
@@ -2914,7 +2914,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
@@ -2925,7 +2925,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B10" s="2" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
@@ -2936,7 +2936,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B11" s="2" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
@@ -2947,7 +2947,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B12" s="2" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
@@ -2958,7 +2958,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B13" s="2" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
@@ -2969,7 +2969,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B14" s="2" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
@@ -2980,7 +2980,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B15" s="2" t="s">
-        <v>264</v>
+        <v>257</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
@@ -2991,7 +2991,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B16" s="2" t="s">
-        <v>265</v>
+        <v>258</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
@@ -3002,7 +3002,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B17" s="2" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
@@ -3013,7 +3013,7 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B18" s="2" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
@@ -3024,7 +3024,7 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B19" s="2" t="s">
-        <v>268</v>
+        <v>261</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
@@ -3035,7 +3035,7 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B20" s="2" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>9</v>
@@ -3046,7 +3046,7 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B21" s="2" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
@@ -3057,7 +3057,7 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B22" s="2" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
@@ -3068,7 +3068,7 @@
     </row>
     <row r="23" spans="2:4" ht="27" x14ac:dyDescent="0.15">
       <c r="B23" s="2" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
@@ -3079,7 +3079,7 @@
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B24" s="2" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>9</v>
@@ -3090,7 +3090,7 @@
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B25" s="2" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>9</v>
@@ -3101,7 +3101,7 @@
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B26" s="2" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>9</v>
@@ -3112,7 +3112,7 @@
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B27" s="2" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>9</v>
@@ -3123,7 +3123,7 @@
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B28" s="2" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>9</v>
@@ -3134,7 +3134,7 @@
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B29" s="2" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>9</v>
@@ -3145,7 +3145,7 @@
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B30" s="2" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>9</v>
@@ -3156,7 +3156,7 @@
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B31" s="2" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>9</v>
@@ -3167,7 +3167,7 @@
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B32" s="2" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>9</v>
@@ -3178,7 +3178,7 @@
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B33" s="2" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>9</v>
@@ -3189,7 +3189,7 @@
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B34" s="2" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>9</v>
@@ -3200,7 +3200,7 @@
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B35" s="2" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>9</v>
@@ -3211,7 +3211,7 @@
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B36" s="2" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>9</v>
@@ -3222,7 +3222,7 @@
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B37" s="2" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>9</v>
@@ -3233,7 +3233,7 @@
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B38" s="2" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>9</v>
@@ -3270,7 +3270,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>238</v>
+        <v>231</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
@@ -3278,7 +3278,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>237</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
@@ -3294,12 +3294,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>236</v>
+        <v>229</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="189" x14ac:dyDescent="0.15">
       <c r="B6" s="1" t="s">
-        <v>484</v>
+        <v>477</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="21" x14ac:dyDescent="0.15">
@@ -3307,10 +3307,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="D7" s="4" t="s" ph="1">
-        <v>223</v>
+        <v>216</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.15">
@@ -3319,7 +3319,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B9" s="1" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
@@ -3330,7 +3330,7 @@
     </row>
     <row r="10" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
@@ -3344,13 +3344,13 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B12" s="2" t="s">
-        <v>467</v>
+        <v>460</v>
       </c>
       <c r="C12" s="4"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B13" s="1" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
@@ -3361,7 +3361,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B14" s="1" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
@@ -3375,13 +3375,13 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B16" s="2" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="C16" s="4"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B17" s="1" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
@@ -3392,7 +3392,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B18" s="1" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
@@ -3406,7 +3406,7 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>294</v>
+        <v>287</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
@@ -3420,7 +3420,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B21" s="2" t="s">
-        <v>469</v>
+        <v>462</v>
       </c>
       <c r="C21" s="4"/>
     </row>
@@ -3429,7 +3429,7 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>295</v>
+        <v>288</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
@@ -3443,7 +3443,7 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>296</v>
+        <v>289</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
@@ -3454,7 +3454,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B24" s="1" t="s">
-        <v>297</v>
+        <v>290</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>9</v>
@@ -3468,7 +3468,7 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>9</v>
@@ -3482,7 +3482,7 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>299</v>
+        <v>292</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>9</v>
@@ -3496,7 +3496,7 @@
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>300</v>
+        <v>293</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>9</v>
@@ -3510,7 +3510,7 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>301</v>
+        <v>294</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>9</v>
@@ -3524,7 +3524,7 @@
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>302</v>
+        <v>295</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>9</v>
@@ -3538,7 +3538,7 @@
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>303</v>
+        <v>296</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>9</v>
@@ -3549,7 +3549,7 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B31" s="1" t="s">
-        <v>304</v>
+        <v>297</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>9</v>
@@ -3560,7 +3560,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B32" s="1" t="s">
-        <v>305</v>
+        <v>298</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>9</v>
@@ -3571,7 +3571,7 @@
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B33" s="1" t="s">
-        <v>306</v>
+        <v>299</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>9</v>
@@ -3585,13 +3585,13 @@
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B35" s="2" t="s">
-        <v>470</v>
+        <v>463</v>
       </c>
       <c r="C35" s="4"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B36" s="1" t="s">
-        <v>307</v>
+        <v>300</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>9</v>
@@ -3602,7 +3602,7 @@
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B37" s="1" t="s">
-        <v>308</v>
+        <v>301</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>9</v>
@@ -3613,7 +3613,7 @@
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B38" s="1" t="s">
-        <v>309</v>
+        <v>302</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>9</v>
@@ -3624,7 +3624,7 @@
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B39" s="1" t="s">
-        <v>310</v>
+        <v>303</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>9</v>
@@ -3635,7 +3635,7 @@
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B40" s="1" t="s">
-        <v>311</v>
+        <v>304</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>9</v>
@@ -3646,7 +3646,7 @@
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B41" s="1" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>9</v>
@@ -3657,7 +3657,7 @@
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B42" s="1" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>9</v>
@@ -3668,7 +3668,7 @@
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B43" s="1" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>9</v>
@@ -3705,7 +3705,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>241</v>
+        <v>234</v>
       </c>
       <c r="D1"/>
     </row>
@@ -3714,7 +3714,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>240</v>
+        <v>233</v>
       </c>
       <c r="D2"/>
     </row>
@@ -3732,7 +3732,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>239</v>
+        <v>232</v>
       </c>
       <c r="D4"/>
     </row>
@@ -3745,16 +3745,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>477</v>
+        <v>470</v>
       </c>
       <c r="D6"/>
     </row>
     <row r="7" spans="1:4" ht="21" x14ac:dyDescent="0.15">
       <c r="B7" s="2" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="D7" s="4" t="s" ph="1">
-        <v>224</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
@@ -3762,7 +3762,7 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>316</v>
+        <v>309</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>9</v>
@@ -3778,14 +3778,14 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B10" s="1" t="s">
-        <v>471</v>
+        <v>464</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B11" s="1" t="s">
-        <v>317</v>
+        <v>310</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
@@ -3799,7 +3799,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
@@ -3810,7 +3810,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B13" s="1" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
@@ -3826,14 +3826,14 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B15" s="1" t="s">
-        <v>472</v>
+        <v>465</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B16" s="1" t="s">
-        <v>320</v>
+        <v>313</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
@@ -3844,7 +3844,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B17" s="1" t="s">
-        <v>321</v>
+        <v>314</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
@@ -3858,7 +3858,7 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
@@ -3874,14 +3874,14 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B20" s="1" t="s">
-        <v>473</v>
+        <v>466</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B21" s="1" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
@@ -3892,7 +3892,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B22" s="1" t="s">
-        <v>323</v>
+        <v>316</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
@@ -3903,7 +3903,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B23" s="1" t="s">
-        <v>324</v>
+        <v>317</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
@@ -3914,7 +3914,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B24" s="1" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>9</v>
@@ -3925,7 +3925,7 @@
     </row>
     <row r="25" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="B25" s="1" t="s">
-        <v>456</v>
+        <v>449</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>9</v>
@@ -3936,7 +3936,7 @@
     </row>
     <row r="26" spans="1:4" ht="81" x14ac:dyDescent="0.15">
       <c r="B26" s="1" t="s">
-        <v>326</v>
+        <v>319</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>9</v>
@@ -3952,14 +3952,14 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B28" s="1" t="s">
-        <v>474</v>
+        <v>467</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B29" s="1" t="s">
-        <v>327</v>
+        <v>320</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>9</v>
@@ -3970,7 +3970,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B30" s="1" t="s">
-        <v>328</v>
+        <v>321</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>9</v>
@@ -3981,7 +3981,7 @@
     </row>
     <row r="31" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="B31" s="1" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>9</v>
@@ -3992,7 +3992,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B32" s="1" t="s">
-        <v>330</v>
+        <v>323</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>9</v>
@@ -4003,7 +4003,7 @@
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B33" s="1" t="s">
-        <v>331</v>
+        <v>324</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>9</v>
@@ -4014,7 +4014,7 @@
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B34" s="1" t="s">
-        <v>332</v>
+        <v>325</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>9</v>
@@ -4025,7 +4025,7 @@
     </row>
     <row r="35" spans="2:4" ht="27" x14ac:dyDescent="0.15">
       <c r="B35" s="1" t="s">
-        <v>333</v>
+        <v>326</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>9</v>
@@ -4036,7 +4036,7 @@
     </row>
     <row r="36" spans="2:4" ht="27" x14ac:dyDescent="0.15">
       <c r="B36" s="1" t="s">
-        <v>334</v>
+        <v>327</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>9</v>
@@ -4047,7 +4047,7 @@
     </row>
     <row r="37" spans="2:4" ht="27" x14ac:dyDescent="0.15">
       <c r="B37" s="1" t="s">
-        <v>335</v>
+        <v>328</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>9</v>
@@ -4062,13 +4062,13 @@
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B39" s="1" t="s">
-        <v>475</v>
+        <v>468</v>
       </c>
       <c r="C39" s="4"/>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B40" s="1" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>9</v>
@@ -4079,7 +4079,7 @@
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B41" s="1" t="s">
-        <v>336</v>
+        <v>329</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>9</v>
@@ -4090,7 +4090,7 @@
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B42" s="1" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>9</v>
@@ -4101,7 +4101,7 @@
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B43" s="1" t="s">
-        <v>338</v>
+        <v>331</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>9</v>
@@ -4116,13 +4116,13 @@
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B45" s="1" t="s">
-        <v>476</v>
+        <v>469</v>
       </c>
       <c r="C45" s="4"/>
     </row>
     <row r="46" spans="2:4" ht="27" x14ac:dyDescent="0.15">
       <c r="B46" s="1" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>9</v>
@@ -4133,7 +4133,7 @@
     </row>
     <row r="47" spans="2:4" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B47" s="1" t="s">
-        <v>459</v>
+        <v>452</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>9</v>
@@ -4144,7 +4144,7 @@
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B48" s="1" t="s">
-        <v>340</v>
+        <v>333</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>9</v>
@@ -4155,7 +4155,7 @@
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B49" s="1" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>9</v>
@@ -4166,7 +4166,7 @@
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B50" s="1" t="s">
-        <v>342</v>
+        <v>335</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>9</v>
@@ -4177,7 +4177,7 @@
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B51" s="1" t="s">
-        <v>343</v>
+        <v>336</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>9</v>
@@ -4192,13 +4192,13 @@
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B53" s="1" t="s">
-        <v>344</v>
+        <v>337</v>
       </c>
       <c r="C53" s="4"/>
     </row>
     <row r="54" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B54" s="1" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>9</v>
@@ -4209,7 +4209,7 @@
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B55" s="1" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>9</v>
@@ -4220,7 +4220,7 @@
     </row>
     <row r="56" spans="2:4" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B56" s="1" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>9</v>
@@ -4231,7 +4231,7 @@
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B57" s="1" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>9</v>
@@ -4242,7 +4242,7 @@
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B58" s="1" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>9</v>
@@ -4253,7 +4253,7 @@
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B59" s="1" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>9</v>
@@ -4264,7 +4264,7 @@
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B60" s="1" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>9</v>
@@ -4275,7 +4275,7 @@
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B61" s="1" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>9</v>
@@ -4286,13 +4286,13 @@
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B63" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="C63" s="4"/>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B64" s="1" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>9</v>
@@ -4303,7 +4303,7 @@
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B65" s="1" t="s">
-        <v>354</v>
+        <v>347</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>9</v>
@@ -4314,7 +4314,7 @@
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B66" t="s">
-        <v>355</v>
+        <v>348</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>9</v>
@@ -4351,7 +4351,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
@@ -4375,7 +4375,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
@@ -4389,20 +4389,20 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>478</v>
+        <v>471</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.15">
       <c r="B8" s="2" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="D8" s="4" t="s" ph="1">
-        <v>225</v>
+        <v>218</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B9" s="1" t="s">
-        <v>356</v>
+        <v>349</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
@@ -4416,13 +4416,13 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B11" s="1" t="s">
-        <v>390</v>
+        <v>383</v>
       </c>
       <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B12" s="1" t="s">
-        <v>357</v>
+        <v>350</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
@@ -4436,7 +4436,7 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
@@ -4450,7 +4450,7 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
@@ -4464,7 +4464,7 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
@@ -4475,7 +4475,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B16" s="1" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
@@ -4489,7 +4489,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
@@ -4503,13 +4503,13 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B19" s="1" t="s">
-        <v>391</v>
+        <v>384</v>
       </c>
       <c r="C19" s="4"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B20" s="1" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>9</v>
@@ -4520,7 +4520,7 @@
     </row>
     <row r="21" spans="1:4" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B21" s="1" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
@@ -4534,7 +4534,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B23" s="1" t="s">
-        <v>392</v>
+        <v>385</v>
       </c>
       <c r="C23" s="4"/>
     </row>
@@ -4543,7 +4543,7 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>9</v>
@@ -4557,7 +4557,7 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>366</v>
+        <v>359</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>9</v>
@@ -4568,7 +4568,7 @@
     </row>
     <row r="26" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="B26" s="1" t="s">
-        <v>367</v>
+        <v>360</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>9</v>
@@ -4582,7 +4582,7 @@
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>9</v>
@@ -4593,7 +4593,7 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B28" s="1" t="s">
-        <v>361</v>
+        <v>354</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>9</v>
@@ -4607,7 +4607,7 @@
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>369</v>
+        <v>362</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>9</v>
@@ -4618,7 +4618,7 @@
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B30" s="1" t="s">
-        <v>370</v>
+        <v>363</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>9</v>
@@ -4632,7 +4632,7 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>371</v>
+        <v>364</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>9</v>
@@ -4643,7 +4643,7 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B32" s="1" t="s">
-        <v>372</v>
+        <v>365</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>9</v>
@@ -4657,7 +4657,7 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>373</v>
+        <v>366</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>9</v>
@@ -4671,7 +4671,7 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>9</v>
@@ -4685,7 +4685,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B36" s="1" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="C36" s="4"/>
     </row>
@@ -4694,7 +4694,7 @@
         <v>4</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>9</v>
@@ -4708,7 +4708,7 @@
         <v>4</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>485</v>
+        <v>478</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>9</v>
@@ -4719,7 +4719,7 @@
     </row>
     <row r="39" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="B39" s="1" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>9</v>
@@ -4733,7 +4733,7 @@
         <v>4</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>9</v>
@@ -4747,7 +4747,7 @@
         <v>4</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>9</v>
@@ -4758,7 +4758,7 @@
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B42" s="1" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>9</v>
@@ -4772,7 +4772,7 @@
         <v>4</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>9</v>
@@ -4783,7 +4783,7 @@
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B44" s="1" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>9</v>
@@ -4797,7 +4797,7 @@
         <v>4</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>9</v>
@@ -4808,7 +4808,7 @@
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B46" s="2" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>9</v>
@@ -4819,7 +4819,7 @@
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B47" s="2" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>9</v>
@@ -4833,7 +4833,7 @@
         <v>4</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>9</v>
@@ -4844,7 +4844,7 @@
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B49" s="1" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>9</v>
@@ -4858,7 +4858,7 @@
         <v>4</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>325</v>
+        <v>318</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>9</v>
@@ -4869,7 +4869,7 @@
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B51" s="1" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>9</v>
@@ -4880,7 +4880,7 @@
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B52" s="1" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>9</v>
@@ -4926,7 +4926,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
@@ -4934,7 +4934,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
@@ -4950,7 +4950,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
@@ -4961,7 +4961,7 @@
     </row>
     <row r="7" spans="1:4" ht="67.5" x14ac:dyDescent="0.15">
       <c r="B7" s="1" t="s">
-        <v>479</v>
+        <v>472</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.15">
@@ -4969,15 +4969,15 @@
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="D8" s="4" t="s" ph="1">
-        <v>226</v>
+        <v>219</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B9" s="1" t="s">
-        <v>393</v>
+        <v>386</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
@@ -4991,7 +4991,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>394</v>
+        <v>387</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
@@ -5005,7 +5005,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>395</v>
+        <v>388</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
@@ -5016,7 +5016,7 @@
     </row>
     <row r="12" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="B12" s="1" t="s">
-        <v>396</v>
+        <v>389</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
@@ -5027,7 +5027,7 @@
     </row>
     <row r="13" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="B13" s="1" t="s">
-        <v>397</v>
+        <v>390</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
@@ -5038,7 +5038,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B14" s="1" t="s">
-        <v>398</v>
+        <v>391</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
@@ -5049,7 +5049,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B15" s="1" t="s">
-        <v>400</v>
+        <v>393</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
@@ -5060,7 +5060,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B16" s="1" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
@@ -5071,7 +5071,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B17" s="1" t="s">
-        <v>401</v>
+        <v>394</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
@@ -5082,7 +5082,7 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B18" s="1" t="s">
-        <v>402</v>
+        <v>395</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
@@ -5093,7 +5093,7 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B19" s="1" t="s">
-        <v>403</v>
+        <v>396</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
@@ -5129,7 +5129,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
@@ -5137,7 +5137,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
@@ -5153,12 +5153,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B7" s="1" t="s">
-        <v>480</v>
+        <v>473</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.15">
@@ -5166,10 +5166,10 @@
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="D8" s="4" t="s" ph="1">
-        <v>227</v>
+        <v>220</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
@@ -5177,7 +5177,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
@@ -5191,7 +5191,7 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>404</v>
+        <v>397</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
@@ -5205,7 +5205,7 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>405</v>
+        <v>398</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
@@ -5219,7 +5219,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
@@ -5230,7 +5230,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B13" s="1" t="s">
-        <v>406</v>
+        <v>399</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
@@ -5241,7 +5241,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B14" s="1" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
@@ -5252,7 +5252,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B15" s="1" t="s">
-        <v>408</v>
+        <v>401</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
@@ -5263,7 +5263,7 @@
     </row>
     <row r="16" spans="1:4" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B16" s="1" t="s">
-        <v>413</v>
+        <v>406</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
@@ -5274,7 +5274,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B17" s="1" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
@@ -5285,7 +5285,7 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B18" s="1" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
@@ -5296,7 +5296,7 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B19" s="1" t="s">
-        <v>407</v>
+        <v>400</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
@@ -5307,7 +5307,7 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B20" s="1" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>9</v>
@@ -5318,7 +5318,7 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B21" s="1" t="s">
-        <v>410</v>
+        <v>403</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
@@ -5329,7 +5329,7 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B22" s="1" t="s">
-        <v>411</v>
+        <v>404</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
@@ -5340,7 +5340,7 @@
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B23" s="1" t="s">
-        <v>412</v>
+        <v>405</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
@@ -5374,10 +5374,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
@@ -5385,7 +5385,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
@@ -5401,7 +5401,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="21" x14ac:dyDescent="0.15">
@@ -5409,15 +5409,15 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="D7" s="4" t="s" ph="1">
-        <v>228</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B8" s="1" t="s">
-        <v>414</v>
+        <v>407</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>9</v>
@@ -5431,7 +5431,7 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>486</v>
+        <v>479</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
@@ -5442,7 +5442,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B10" s="1" t="s">
-        <v>415</v>
+        <v>408</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
@@ -5453,7 +5453,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B11" s="1" t="s">
-        <v>416</v>
+        <v>409</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
@@ -5464,7 +5464,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B12" s="1" t="s">
-        <v>417</v>
+        <v>410</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
@@ -5475,7 +5475,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B13" s="1" t="s">
-        <v>418</v>
+        <v>411</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
@@ -5486,7 +5486,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B14" s="1" t="s">
-        <v>419</v>
+        <v>412</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
@@ -5497,7 +5497,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B15" s="1" t="s">
-        <v>420</v>
+        <v>413</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
@@ -5508,7 +5508,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B16" s="1" t="s">
-        <v>421</v>
+        <v>414</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
@@ -5519,7 +5519,7 @@
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B17" s="1" t="s">
-        <v>422</v>
+        <v>415</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
@@ -5530,7 +5530,7 @@
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B18" s="1" t="s">
-        <v>423</v>
+        <v>416</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
@@ -5541,7 +5541,7 @@
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B19" s="1" t="s">
-        <v>424</v>
+        <v>417</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
@@ -5552,7 +5552,7 @@
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B20" s="1" t="s">
-        <v>425</v>
+        <v>418</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>9</v>
@@ -5563,7 +5563,7 @@
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B21" s="1" t="s">
-        <v>458</v>
+        <v>451</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
@@ -5574,7 +5574,7 @@
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B22" s="1" t="s">
-        <v>426</v>
+        <v>419</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
@@ -5585,7 +5585,7 @@
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B23" s="1" t="s">
-        <v>427</v>
+        <v>420</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
@@ -5596,7 +5596,7 @@
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B24" s="1" t="s">
-        <v>428</v>
+        <v>421</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>9</v>
@@ -5607,7 +5607,7 @@
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B25" s="1" t="s">
-        <v>429</v>
+        <v>422</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>9</v>
@@ -5618,7 +5618,7 @@
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B26" s="1" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>9</v>
@@ -5629,7 +5629,7 @@
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B27" s="1" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>9</v>
@@ -5640,7 +5640,7 @@
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B28" s="1" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>9</v>
@@ -5651,7 +5651,7 @@
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B29" s="1" t="s">
-        <v>433</v>
+        <v>426</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>9</v>
@@ -5689,7 +5689,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -5699,7 +5699,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -5719,7 +5719,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -5739,7 +5739,7 @@
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="4"/>
       <c r="B7" s="5" t="s">
-        <v>481</v>
+        <v>474</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -5747,17 +5747,17 @@
     <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.15">
       <c r="A8" s="4"/>
       <c r="B8" s="2" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4" t="s" ph="1">
-        <v>229</v>
+        <v>222</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="4"/>
       <c r="B9" s="5" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
@@ -5769,7 +5769,7 @@
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="4"/>
       <c r="B10" s="5" t="s">
-        <v>368</v>
+        <v>361</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
@@ -5781,7 +5781,7 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="4"/>
       <c r="B11" s="5" t="s">
-        <v>399</v>
+        <v>392</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
@@ -5793,7 +5793,7 @@
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="4"/>
       <c r="B12" s="5" t="s">
-        <v>435</v>
+        <v>428</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
@@ -5805,7 +5805,7 @@
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="4"/>
       <c r="B13" s="5" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
@@ -5817,7 +5817,7 @@
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="4"/>
       <c r="B14" s="3" t="s">
-        <v>437</v>
+        <v>430</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
@@ -5829,7 +5829,7 @@
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="4"/>
       <c r="B15" s="5" t="s">
-        <v>438</v>
+        <v>431</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
@@ -5841,7 +5841,7 @@
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="4"/>
       <c r="B16" s="5" t="s">
-        <v>439</v>
+        <v>432</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
@@ -5853,7 +5853,7 @@
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="4"/>
       <c r="B17" s="5" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
@@ -5865,7 +5865,7 @@
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="4"/>
       <c r="B18" s="5" t="s">
-        <v>441</v>
+        <v>434</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
@@ -5877,7 +5877,7 @@
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="4"/>
       <c r="B19" s="5" t="s">
-        <v>442</v>
+        <v>435</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
@@ -5889,7 +5889,7 @@
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="4"/>
       <c r="B20" s="5" t="s">
-        <v>443</v>
+        <v>436</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>9</v>
@@ -5901,7 +5901,7 @@
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" s="4"/>
       <c r="B21" s="5" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
@@ -5913,7 +5913,7 @@
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" s="4"/>
       <c r="B22" s="5" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
@@ -5925,7 +5925,7 @@
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" s="4"/>
       <c r="B23" s="5" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
@@ -5937,7 +5937,7 @@
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" s="4"/>
       <c r="B24" s="5" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>9</v>
@@ -5949,7 +5949,7 @@
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" s="4"/>
       <c r="B25" s="5" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
win11_en.xlsx: replace all new screenshot by low-quality 30% JPEGs
</commit_message>
<xml_diff>
--- a/win11_en.xlsx
+++ b/win11_en.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta2025\fresta-github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6197AA7C-D96B-46EF-86B4-AB1F07984EB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B508261-59A6-4D49-926F-E91955D20D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" tabRatio="729" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="21840" windowHeight="13020" tabRatio="729" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -85,609 +85,6 @@
   <si>
     <t>fresta_en</t>
     <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>win11-en-part1-00.00.15.245.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.00.24.161.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.01.14.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.01.16.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.01.49.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.01.54.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.02.12.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.02.27.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.02.54.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.03.34.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.03.39.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.03.51.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.03.57.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.04.16.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.04.34.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.04.49.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.05.22.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.05.35.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.05.56.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.06.03.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.06.10.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.06.33.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.06.51.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.07.34.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.07.40.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.07.51.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.08.06.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.08.18.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.08.21.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part1-00.08.36.930.png</t>
-  </si>
-  <si>
-    <t>win11-en-part2-00.00.08.642.png</t>
-  </si>
-  <si>
-    <t>win11-en-part2-00.00.10.642.png</t>
-  </si>
-  <si>
-    <t>win11-en-part2-00.00.24.642.png</t>
-  </si>
-  <si>
-    <t>win11-en-part2-00.00.31.642.png</t>
-  </si>
-  <si>
-    <t>win11-en-part2-00.00.45.025.png</t>
-  </si>
-  <si>
-    <t>win11-en-part2-00.01.02.302.png</t>
-  </si>
-  <si>
-    <t>win11-en-part2-00.01.08.481.png</t>
-  </si>
-  <si>
-    <t>win11-en-part2-00.01.30.044.png</t>
-  </si>
-  <si>
-    <t>win11-en-part2-00.01.35.789.png</t>
-  </si>
-  <si>
-    <t>win11-en-part2-00.01.46.015.png</t>
-  </si>
-  <si>
-    <t>win11-en-part2-00.01.53.560.png</t>
-  </si>
-  <si>
-    <t>win11-en-part2-00.02.18.560.png</t>
-  </si>
-  <si>
-    <t>win11-en-part2-00.02.39.875.png</t>
-  </si>
-  <si>
-    <t>win11-en-part2-00.02.53.875.png</t>
-  </si>
-  <si>
-    <t>win11-en-part2-00.02.58.755.png</t>
-  </si>
-  <si>
-    <t>win11-en-part2-00.03.04.755.png</t>
-  </si>
-  <si>
-    <t>win11-en-part2-00.03.09.755.png</t>
-  </si>
-  <si>
-    <t>win11-en-part2-00.03.14.755.png</t>
-  </si>
-  <si>
-    <t>win11-en-part2-00.03.26.755.png</t>
-  </si>
-  <si>
-    <t>win11-en-part2-00.03.40.755.png</t>
-  </si>
-  <si>
-    <t>win11-en-part2-00.03.48.755.png</t>
-  </si>
-  <si>
-    <t>win11-en-part2-00.03.55.755.png</t>
-  </si>
-  <si>
-    <t>win11-en-part2-00.04.10.755.png</t>
-  </si>
-  <si>
-    <t>win11-en-part2-00.04.16.755.png</t>
-  </si>
-  <si>
-    <t>win11-en-part2-00.04.37.755.png</t>
-  </si>
-  <si>
-    <t>win11-en-part2-00.04.58.601.png</t>
-  </si>
-  <si>
-    <t>win11-en-part2-00.05.02.601.png</t>
-  </si>
-  <si>
-    <t>win11-en-part3-00.00.10.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part3-00.00.22.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part3-00.00.28.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part3-00.00.40.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part3-00.00.55.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part3-00.00.59.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part3-00.01.08.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part3-00.01.27.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part3-00.01.28.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part3-00.01.33.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part3-00.01.36.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part3-00.01.57.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part3-00.01.58.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part3-00.02.22.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part3-00.02.34.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part3-00.02.43.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part3-00.02.45.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part3-00.02.54.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part3-00.02.59.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part3-00.03.00.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part3-00.03.10.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part3-00.03.35.553.png</t>
-  </si>
-  <si>
-    <t>win11-en-part3-00.03.42.553.png</t>
-  </si>
-  <si>
-    <t>win11-en-part3-00.03.56.553.png</t>
-  </si>
-  <si>
-    <t>win11-en-part3-00.04.05.553.png</t>
-  </si>
-  <si>
-    <t>win11-en-part3-00.04.10.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part3-00.04.36.726.png</t>
-  </si>
-  <si>
-    <t>win11-en-part3-00.04.47.726.png</t>
-  </si>
-  <si>
-    <t>win11-en-part3-00.04.58.726.png</t>
-  </si>
-  <si>
-    <t>win11-en-part3-00.04.59.726.png</t>
-  </si>
-  <si>
-    <t>win11-en-part3-00.05.02.726.png</t>
-  </si>
-  <si>
-    <t>win11-en-part3-00.05.07.726.png</t>
-  </si>
-  <si>
-    <t>win11-en-part3-00.05.16.726.png</t>
-  </si>
-  <si>
-    <t>win11-en-part3-00.05.21.726.png</t>
-  </si>
-  <si>
-    <t>win11-en-part3-00.05.30.726.png</t>
-  </si>
-  <si>
-    <t>win11-en-part3-00.05.38.726.png</t>
-  </si>
-  <si>
-    <t>win11-en-part3-00.05.45.726.png</t>
-  </si>
-  <si>
-    <t>win11-en-part3-00.05.51.726.png</t>
-  </si>
-  <si>
-    <t>win11-en-part3-00.05.57.124.png</t>
-  </si>
-  <si>
-    <t>win11-en-part3-00.06.06.124.png</t>
-  </si>
-  <si>
-    <t>win11-en-part3-00.06.29.124.png</t>
-  </si>
-  <si>
-    <t>win11-en-part3-00.06.35.124.png</t>
-  </si>
-  <si>
-    <t>win11-en-part3-00.06.55.124.png</t>
-  </si>
-  <si>
-    <t>win11-en-part4-00.00.14.059.png</t>
-  </si>
-  <si>
-    <t>win11-en-part4-00.00.36.059.png</t>
-  </si>
-  <si>
-    <t>win11-en-part4-00.00.41.059.png</t>
-  </si>
-  <si>
-    <t>win11-en-part4-00.00.47.059.png</t>
-  </si>
-  <si>
-    <t>win11-en-part4-00.01.09.407.png</t>
-  </si>
-  <si>
-    <t>win11-en-part4-00.01.12.407.png</t>
-  </si>
-  <si>
-    <t>win11-en-part4-00.01.32.407.png</t>
-  </si>
-  <si>
-    <t>win11-en-part4-00.01.40.407.png</t>
-  </si>
-  <si>
-    <t>win11-en-part4-00.01.46.407.png</t>
-  </si>
-  <si>
-    <t>win11-en-part4-00.02.06.407.png</t>
-  </si>
-  <si>
-    <t>win11-en-part4-00.02.19.407.png</t>
-  </si>
-  <si>
-    <t>win11-en-part4-00.02.42.407.png</t>
-  </si>
-  <si>
-    <t>win11-en-part4-00.02.56.407.png</t>
-  </si>
-  <si>
-    <t>win11-en-part4-00.02.58.407.png</t>
-  </si>
-  <si>
-    <t>win11-en-part4-00.03.03.407.png</t>
-  </si>
-  <si>
-    <t>win11-en-part4-00.03.08.407.png</t>
-  </si>
-  <si>
-    <t>win11-en-part4-00.03.17.407.png</t>
-  </si>
-  <si>
-    <t>win11-en-part4-00.03.19.407.png</t>
-  </si>
-  <si>
-    <t>win11-en-part4-00.03.23.407.png</t>
-  </si>
-  <si>
-    <t>win11-en-part4-00.03.36.407.png</t>
-  </si>
-  <si>
-    <t>win11-en-part4-00.03.50.407.png</t>
-  </si>
-  <si>
-    <t>win11-en-part4-00.03.51.407.png</t>
-  </si>
-  <si>
-    <t>win11-en-part4-00.03.58.407.png</t>
-  </si>
-  <si>
-    <t>win11-en-part4-00.04.10.407.png</t>
-  </si>
-  <si>
-    <t>win11-en-part4-00.04.14.407.png</t>
-  </si>
-  <si>
-    <t>win11-en-part4-00.04.15.407.png</t>
-  </si>
-  <si>
-    <t>win11-en-part4-00.04.24.407.png</t>
-  </si>
-  <si>
-    <t>win11-en-part4-00.04.29.407.png</t>
-  </si>
-  <si>
-    <t>win11-en-part4-00.04.37.407.png</t>
-  </si>
-  <si>
-    <t>win11-en-part4-00.04.42.407.png</t>
-  </si>
-  <si>
-    <t>win11-en-part4-00.04.47.407.png</t>
-  </si>
-  <si>
-    <t>win11-en-part4-00.04.51.407.png</t>
-  </si>
-  <si>
-    <t>win11-en-part4-00.04.58.407.png</t>
-  </si>
-  <si>
-    <t>win11-en-part4-00.05.05.407.png</t>
-  </si>
-  <si>
-    <t>win11-en-part4-00.05.12.407.png</t>
-  </si>
-  <si>
-    <t>win11-en-part4-00.05.22.407.png</t>
-  </si>
-  <si>
-    <t>win11-en-part5-00.00.08.623.png</t>
-  </si>
-  <si>
-    <t>win11-en-part5-00.00.14.623.png</t>
-  </si>
-  <si>
-    <t>win11-en-part5-00.00.17.623.png</t>
-  </si>
-  <si>
-    <t>win11-en-part5-00.00.20.623.png</t>
-  </si>
-  <si>
-    <t>win11-en-part5-00.00.34.623.png</t>
-  </si>
-  <si>
-    <t>win11-en-part5-00.00.50.623.png</t>
-  </si>
-  <si>
-    <t>win11-en-part5-00.00.56.623.png</t>
-  </si>
-  <si>
-    <t>win11-en-part5-00.01.00.902.png</t>
-  </si>
-  <si>
-    <t>win11-en-part5-00.01.10.902.png</t>
-  </si>
-  <si>
-    <t>win11-en-part5-00.01.11.902.png</t>
-  </si>
-  <si>
-    <t>win11-en-part5-00.01.21.902.png</t>
-  </si>
-  <si>
-    <t>win11-en-part6-00.00.07.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part6-00.00.11.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part6-00.00.17.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part6-00.00.30.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part6-00.00.37.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part6-00.00.46.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part6-00.00.55.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part6-00.01.06.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part6-00.01.09.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part6-00.01.14.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part6-00.01.19.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part6-00.01.24.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part6-00.01.30.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part6-00.01.38.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part6-00.01.48.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part7-00.00.10.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part7-00.00.14.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part7-00.00.32.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part7-00.00.40.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part7-00.01.02.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part7-00.01.03.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part7-00.01.19.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part7-00.01.40.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part7-00.01.44.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part7-00.01.50.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part7-00.01.56.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part7-00.02.02.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part7-00.02.17.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part7-00.02.21.109.png</t>
-  </si>
-  <si>
-    <t>win11-en-part7-00.02.28.109.png</t>
-  </si>
-  <si>
-    <t>win11-en-part7-00.02.30.109.png</t>
-  </si>
-  <si>
-    <t>win11-en-part7-00.02.32.109.png</t>
-  </si>
-  <si>
-    <t>win11-en-part7-00.02.37.109.png</t>
-  </si>
-  <si>
-    <t>win11-en-part7-00.02.41.109.png</t>
-  </si>
-  <si>
-    <t>win11-en-part7-00.02.46.109.png</t>
-  </si>
-  <si>
-    <t>win11-en-part7-00.02.54.109.png</t>
-  </si>
-  <si>
-    <t>win11-en-part7-00.03.00.109.png</t>
-  </si>
-  <si>
-    <t>win11-en-part8-00.00.08.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part8-00.00.11.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part8-00.00.24.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part8-00.00.37.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part8-00.00.42.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part8-00.00.52.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part8-00.00.53.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part8-00.00.58.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part8-00.01.01.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part8-00.01.07.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part8-00.01.15.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part8-00.01.28.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part8-00.01.33.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part8-00.01.38.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part8-00.01.48.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part8-00.01.53.000.png</t>
-  </si>
-  <si>
-    <t>win11-en-part8-00.01.58.000.png</t>
   </si>
   <si>
     <t>raw:&lt;iframe width="100%" height="315" src="https://www.youtube.com/embed/2Ojmvtgy35Y?list=PLjGYIiYIuSrByd_Llk0LaHf1-ZJzhU4fQ" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen=""&gt;&lt;/iframe&gt;</t>
@@ -1845,6 +1242,609 @@
   </si>
   <si>
     <t>win11-en-part9-00.00.41.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part8-00.00.08.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part8-00.00.11.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part8-00.00.24.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part8-00.00.37.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part8-00.00.42.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part8-00.00.52.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part8-00.00.53.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part8-00.00.58.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part8-00.01.01.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part8-00.01.07.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part8-00.01.15.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part8-00.01.28.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part8-00.01.33.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part8-00.01.38.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part8-00.01.48.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part8-00.01.53.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part8-00.01.58.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part7-00.00.10.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part7-00.00.14.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part7-00.00.32.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part7-00.00.40.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part7-00.01.02.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part7-00.01.03.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part7-00.01.19.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part7-00.01.40.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part7-00.01.44.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part7-00.01.50.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part7-00.01.56.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part7-00.02.02.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part7-00.02.17.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part7-00.02.21.109.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part7-00.02.28.109.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part7-00.02.30.109.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part7-00.02.32.109.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part7-00.02.37.109.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part7-00.02.41.109.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part7-00.02.46.109.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part7-00.02.54.109.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part7-00.03.00.109.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part6-00.00.07.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part6-00.00.11.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part6-00.00.17.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part6-00.00.30.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part6-00.00.37.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part6-00.00.46.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part6-00.00.55.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part6-00.01.06.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part6-00.01.09.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part6-00.01.14.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part6-00.01.19.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part6-00.01.24.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part6-00.01.30.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part6-00.01.38.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part6-00.01.48.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part5-00.00.08.623.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part5-00.00.14.623.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part5-00.00.17.623.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part5-00.00.20.623.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part5-00.00.34.623.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part5-00.00.50.623.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part5-00.00.56.623.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part5-00.01.00.902.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part5-00.01.10.902.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part5-00.01.11.902.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part5-00.01.21.902.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part4-00.00.14.059.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part4-00.00.36.059.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part4-00.00.41.059.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part4-00.00.47.059.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part4-00.01.09.407.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part4-00.01.12.407.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part4-00.01.32.407.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part4-00.01.40.407.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part4-00.01.46.407.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part4-00.02.06.407.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part4-00.02.19.407.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part4-00.02.42.407.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part4-00.02.56.407.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part4-00.02.58.407.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part4-00.03.03.407.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part4-00.03.08.407.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part4-00.03.17.407.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part4-00.03.19.407.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part4-00.03.23.407.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part4-00.03.36.407.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part4-00.03.50.407.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part4-00.03.51.407.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part4-00.03.58.407.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part4-00.04.10.407.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part4-00.04.14.407.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part4-00.04.15.407.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part4-00.04.24.407.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part4-00.04.29.407.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part4-00.04.37.407.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part4-00.04.42.407.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part4-00.04.47.407.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part4-00.04.51.407.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part4-00.04.58.407.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part4-00.05.05.407.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part4-00.05.12.407.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part4-00.05.22.407.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part3-00.00.10.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part3-00.00.22.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part3-00.00.28.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part3-00.00.40.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part3-00.00.55.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part3-00.00.59.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part3-00.01.08.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part3-00.01.27.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part3-00.01.28.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part3-00.01.33.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part3-00.01.36.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part3-00.01.57.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part3-00.01.58.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part3-00.02.22.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part3-00.02.34.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part3-00.02.43.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part3-00.02.45.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part3-00.02.54.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part3-00.02.59.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part3-00.03.00.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part3-00.03.10.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part3-00.03.35.553.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part3-00.03.42.553.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part3-00.03.56.553.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part3-00.04.05.553.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part3-00.04.10.000.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part3-00.04.36.726.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part3-00.04.47.726.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part3-00.04.58.726.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part3-00.04.59.726.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part3-00.05.02.726.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part3-00.05.07.726.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part3-00.05.16.726.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part3-00.05.21.726.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part3-00.05.30.726.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part3-00.05.38.726.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part3-00.05.45.726.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part3-00.05.51.726.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part3-00.05.57.124.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part3-00.06.06.124.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part3-00.06.29.124.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part3-00.06.35.124.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part3-00.06.55.124.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part2-00.00.08.642.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part2-00.00.10.642.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part2-00.00.24.642.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part2-00.00.31.642.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part2-00.00.45.025.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part2-00.01.02.302.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part2-00.01.08.481.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part2-00.01.30.044.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part2-00.01.35.789.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part2-00.01.46.015.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part2-00.01.53.560.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part2-00.02.18.560.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part2-00.02.39.875.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part2-00.02.53.875.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part2-00.02.58.755.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part2-00.03.04.755.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part2-00.03.09.755.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part2-00.03.14.755.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part2-00.03.26.755.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part2-00.03.40.755.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part2-00.03.48.755.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part2-00.03.55.755.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part2-00.04.10.755.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part2-00.04.16.755.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part2-00.04.37.755.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part2-00.04.58.601.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part2-00.05.02.601.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.00.15.245.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.00.24.161.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.01.14.930.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.01.16.930.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.01.49.930.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.01.54.930.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.02.12.930.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.02.27.930.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.02.54.930.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.03.34.930.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.03.39.930.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.03.51.930.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.03.57.930.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.04.16.930.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.04.34.930.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.04.49.930.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.05.22.930.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.05.35.930.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.05.56.930.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.06.03.930.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.06.10.930.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.06.33.930.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.06.51.930.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.07.34.930.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.07.40.930.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.07.51.930.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.08.06.930.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.08.18.930.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.08.21.930.jpg</t>
+  </si>
+  <si>
+    <t>win11-en-part1-00.08.36.930.jpg</t>
   </si>
 </sst>
 </file>
@@ -2255,7 +2255,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>249</v>
+        <v>48</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="67.5" x14ac:dyDescent="0.15">
@@ -2297,7 +2297,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EFCA2B8-55C7-4AC3-9E13-35156DBD8BC5}">
   <dimension ref="A1:D75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B9" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView topLeftCell="B9" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
@@ -2315,7 +2315,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>224</v>
+        <v>23</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -2325,7 +2325,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>225</v>
+        <v>24</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -2345,7 +2345,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>243</v>
+        <v>42</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -2365,7 +2365,7 @@
     <row r="7" spans="1:4" ht="121.5" x14ac:dyDescent="0.15">
       <c r="A7" s="4"/>
       <c r="B7" s="5" t="s">
-        <v>476</v>
+        <v>275</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -2373,11 +2373,11 @@
     <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.15">
       <c r="A8" s="4"/>
       <c r="B8" s="2" t="s">
-        <v>250</v>
+        <v>49</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4" t="s" ph="1">
-        <v>223</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="21" x14ac:dyDescent="0.15">
@@ -2389,7 +2389,7 @@
     <row r="10" spans="1:4" ht="21" x14ac:dyDescent="0.15">
       <c r="A10" s="4"/>
       <c r="B10" s="2" t="s">
-        <v>475</v>
+        <v>274</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4" ph="1"/>
@@ -2397,85 +2397,85 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="4"/>
       <c r="B11" s="5" t="s">
-        <v>442</v>
+        <v>241</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>480</v>
+        <v>279</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="4"/>
       <c r="B12" s="5" t="s">
-        <v>443</v>
+        <v>242</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>481</v>
+        <v>280</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="4"/>
       <c r="B13" s="5" t="s">
-        <v>444</v>
+        <v>243</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>482</v>
+        <v>281</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="4"/>
       <c r="B14" s="5" t="s">
-        <v>445</v>
+        <v>244</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>483</v>
+        <v>282</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="4"/>
       <c r="B15" s="5" t="s">
-        <v>446</v>
+        <v>245</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>484</v>
+        <v>283</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="A16" s="4"/>
       <c r="B16" s="5" t="s">
-        <v>447</v>
+        <v>246</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>485</v>
+        <v>284</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="4"/>
       <c r="B17" s="5" t="s">
-        <v>448</v>
+        <v>247</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>486</v>
+        <v>285</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
@@ -2486,18 +2486,18 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B19" s="2" t="s">
-        <v>453</v>
+        <v>252</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="B20" s="2" t="s">
-        <v>457</v>
+        <v>256</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>455</v>
+        <v>254</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="3" customFormat="1" ht="12.95" customHeight="1" ph="1" x14ac:dyDescent="0.15">
@@ -2505,18 +2505,18 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B22" s="2" t="s">
-        <v>454</v>
+        <v>253</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="B23" s="2" t="s">
-        <v>458</v>
+        <v>257</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>456</v>
+        <v>255</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
@@ -2843,8 +2843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9:D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2860,7 +2860,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>228</v>
+        <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
@@ -2868,7 +2868,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>227</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
@@ -2884,7 +2884,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>226</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
@@ -2897,16 +2897,16 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>459</v>
+        <v>258</v>
       </c>
       <c r="D7" s="3" ph="1"/>
     </row>
     <row r="8" spans="1:4" ht="20.45" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B8" s="2" t="s">
-        <v>250</v>
+        <v>49</v>
       </c>
       <c r="D8" s="4" t="s" ph="1">
-        <v>215</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="21" x14ac:dyDescent="0.15">
@@ -2914,332 +2914,332 @@
         <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>251</v>
+        <v>50</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="3" t="s" ph="1">
-        <v>14</v>
+        <v>457</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B10" s="2" t="s">
-        <v>252</v>
+        <v>51</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>15</v>
+        <v>458</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B11" s="2" t="s">
-        <v>253</v>
+        <v>52</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>16</v>
+        <v>459</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B12" s="2" t="s">
-        <v>254</v>
+        <v>53</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>17</v>
+        <v>460</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B13" s="2" t="s">
-        <v>255</v>
+        <v>54</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>18</v>
+        <v>461</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B14" s="2" t="s">
-        <v>256</v>
+        <v>55</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>19</v>
+        <v>462</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B15" s="2" t="s">
-        <v>257</v>
+        <v>56</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>20</v>
+        <v>463</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B16" s="2" t="s">
-        <v>258</v>
+        <v>57</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>21</v>
+        <v>464</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B17" s="2" t="s">
-        <v>259</v>
+        <v>58</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>22</v>
+        <v>465</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B18" s="2" t="s">
-        <v>260</v>
+        <v>59</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>23</v>
+        <v>466</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B19" s="2" t="s">
-        <v>261</v>
+        <v>60</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>24</v>
+        <v>467</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B20" s="2" t="s">
-        <v>262</v>
+        <v>61</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>25</v>
+        <v>468</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B21" s="2" t="s">
-        <v>263</v>
+        <v>62</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>26</v>
+        <v>469</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B22" s="2" t="s">
-        <v>264</v>
+        <v>63</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>27</v>
+        <v>470</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="27" x14ac:dyDescent="0.15">
       <c r="B23" s="2" t="s">
-        <v>265</v>
+        <v>64</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>28</v>
+        <v>471</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B24" s="2" t="s">
-        <v>266</v>
+        <v>65</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>29</v>
+        <v>472</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B25" s="2" t="s">
-        <v>267</v>
+        <v>66</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>30</v>
+        <v>473</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B26" s="2" t="s">
-        <v>268</v>
+        <v>67</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>31</v>
+        <v>474</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B27" s="2" t="s">
-        <v>269</v>
+        <v>68</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>32</v>
+        <v>475</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B28" s="2" t="s">
-        <v>270</v>
+        <v>69</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>33</v>
+        <v>476</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B29" s="2" t="s">
-        <v>271</v>
+        <v>70</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>34</v>
+        <v>477</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B30" s="2" t="s">
-        <v>272</v>
+        <v>71</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>35</v>
+        <v>478</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B31" s="2" t="s">
-        <v>273</v>
+        <v>72</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>36</v>
+        <v>479</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B32" s="2" t="s">
-        <v>274</v>
+        <v>73</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>37</v>
+        <v>480</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B33" s="2" t="s">
-        <v>275</v>
+        <v>74</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>38</v>
+        <v>481</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B34" s="2" t="s">
-        <v>276</v>
+        <v>75</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>39</v>
+        <v>482</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B35" s="2" t="s">
-        <v>277</v>
+        <v>76</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>40</v>
+        <v>483</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B36" s="2" t="s">
-        <v>278</v>
+        <v>77</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>41</v>
+        <v>484</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B37" s="2" t="s">
-        <v>279</v>
+        <v>78</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>42</v>
+        <v>485</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B38" s="2" t="s">
-        <v>280</v>
+        <v>79</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>43</v>
+        <v>486</v>
       </c>
     </row>
   </sheetData>
@@ -3253,8 +3253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="C7" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9:D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3270,7 +3270,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>231</v>
+        <v>30</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
@@ -3278,7 +3278,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>230</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
@@ -3294,12 +3294,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>229</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="189" x14ac:dyDescent="0.15">
       <c r="B6" s="1" t="s">
-        <v>477</v>
+        <v>276</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="21" x14ac:dyDescent="0.15">
@@ -3307,10 +3307,10 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>250</v>
+        <v>49</v>
       </c>
       <c r="D7" s="4" t="s" ph="1">
-        <v>216</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.15">
@@ -3319,24 +3319,24 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B9" s="1" t="s">
-        <v>281</v>
+        <v>80</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>44</v>
+        <v>430</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B10" s="1" t="s">
-        <v>282</v>
+        <v>81</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>45</v>
+        <v>431</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
@@ -3344,30 +3344,30 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B12" s="2" t="s">
-        <v>460</v>
+        <v>259</v>
       </c>
       <c r="C12" s="4"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B13" s="1" t="s">
-        <v>283</v>
+        <v>82</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>46</v>
+        <v>432</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B14" s="1" t="s">
-        <v>284</v>
+        <v>83</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>47</v>
+        <v>433</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
@@ -3375,30 +3375,30 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B16" s="2" t="s">
-        <v>461</v>
+        <v>260</v>
       </c>
       <c r="C16" s="4"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B17" s="1" t="s">
-        <v>286</v>
+        <v>85</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>48</v>
+        <v>434</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B18" s="1" t="s">
-        <v>285</v>
+        <v>84</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>49</v>
+        <v>435</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="27" x14ac:dyDescent="0.15">
@@ -3406,13 +3406,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>287</v>
+        <v>86</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>50</v>
+        <v>436</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
@@ -3420,7 +3420,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B21" s="2" t="s">
-        <v>462</v>
+        <v>261</v>
       </c>
       <c r="C21" s="4"/>
     </row>
@@ -3429,13 +3429,13 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>288</v>
+        <v>87</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>51</v>
+        <v>437</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
@@ -3443,24 +3443,24 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>289</v>
+        <v>88</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>52</v>
+        <v>438</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B24" s="1" t="s">
-        <v>290</v>
+        <v>89</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>53</v>
+        <v>439</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
@@ -3468,13 +3468,13 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>291</v>
+        <v>90</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>54</v>
+        <v>440</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">
@@ -3482,13 +3482,13 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>292</v>
+        <v>91</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>55</v>
+        <v>441</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
@@ -3496,13 +3496,13 @@
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>293</v>
+        <v>92</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>56</v>
+        <v>442</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
@@ -3510,13 +3510,13 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>294</v>
+        <v>93</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>57</v>
+        <v>443</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
@@ -3524,13 +3524,13 @@
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>295</v>
+        <v>94</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>58</v>
+        <v>444</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
@@ -3538,46 +3538,46 @@
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>296</v>
+        <v>95</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>59</v>
+        <v>445</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B31" s="1" t="s">
-        <v>297</v>
+        <v>96</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>60</v>
+        <v>446</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B32" s="1" t="s">
-        <v>298</v>
+        <v>97</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>61</v>
+        <v>447</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B33" s="1" t="s">
-        <v>299</v>
+        <v>98</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>62</v>
+        <v>448</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.15">
@@ -3585,96 +3585,96 @@
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B35" s="2" t="s">
-        <v>463</v>
+        <v>262</v>
       </c>
       <c r="C35" s="4"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B36" s="1" t="s">
-        <v>300</v>
+        <v>99</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>63</v>
+        <v>449</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B37" s="1" t="s">
-        <v>301</v>
+        <v>100</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>64</v>
+        <v>450</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B38" s="1" t="s">
-        <v>302</v>
+        <v>101</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>65</v>
+        <v>451</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B39" s="1" t="s">
-        <v>303</v>
+        <v>102</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>66</v>
+        <v>452</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B40" s="1" t="s">
-        <v>304</v>
+        <v>103</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>67</v>
+        <v>453</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B41" s="1" t="s">
-        <v>305</v>
+        <v>104</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>68</v>
+        <v>454</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B42" s="1" t="s">
-        <v>306</v>
+        <v>105</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>69</v>
+        <v>455</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B43" s="1" t="s">
-        <v>307</v>
+        <v>106</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>70</v>
+        <v>456</v>
       </c>
     </row>
   </sheetData>
@@ -3688,8 +3688,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D3AC582-7A6D-4EA0-8C12-75B8749BA9E2}">
   <dimension ref="A1:D66"/>
   <sheetViews>
-    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="C7" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8:D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3705,7 +3705,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>234</v>
+        <v>33</v>
       </c>
       <c r="D1"/>
     </row>
@@ -3714,7 +3714,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>233</v>
+        <v>32</v>
       </c>
       <c r="D2"/>
     </row>
@@ -3732,7 +3732,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>232</v>
+        <v>31</v>
       </c>
       <c r="D4"/>
     </row>
@@ -3745,16 +3745,16 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>470</v>
+        <v>269</v>
       </c>
       <c r="D6"/>
     </row>
     <row r="7" spans="1:4" ht="21" x14ac:dyDescent="0.15">
       <c r="B7" s="2" t="s">
-        <v>250</v>
+        <v>49</v>
       </c>
       <c r="D7" s="4" t="s" ph="1">
-        <v>217</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
@@ -3762,13 +3762,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>309</v>
+        <v>108</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>71</v>
+        <v>387</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
@@ -3778,20 +3778,20 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B10" s="1" t="s">
-        <v>464</v>
+        <v>263</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B11" s="1" t="s">
-        <v>310</v>
+        <v>109</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>72</v>
+        <v>388</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="27" x14ac:dyDescent="0.15">
@@ -3799,24 +3799,24 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>311</v>
+        <v>110</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>73</v>
+        <v>389</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B13" s="1" t="s">
-        <v>312</v>
+        <v>111</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>74</v>
+        <v>390</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
@@ -3826,31 +3826,31 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B15" s="1" t="s">
-        <v>465</v>
+        <v>264</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B16" s="1" t="s">
-        <v>313</v>
+        <v>112</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>75</v>
+        <v>391</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B17" s="1" t="s">
-        <v>314</v>
+        <v>113</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>76</v>
+        <v>392</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="27" x14ac:dyDescent="0.15">
@@ -3858,13 +3858,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>315</v>
+        <v>114</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>77</v>
+        <v>393</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3874,75 +3874,75 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B20" s="1" t="s">
-        <v>466</v>
+        <v>265</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B21" s="1" t="s">
-        <v>308</v>
+        <v>107</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>78</v>
+        <v>394</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B22" s="1" t="s">
-        <v>316</v>
+        <v>115</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>79</v>
+        <v>395</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B23" s="1" t="s">
-        <v>317</v>
+        <v>116</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>80</v>
+        <v>396</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B24" s="1" t="s">
-        <v>318</v>
+        <v>117</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>81</v>
+        <v>397</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="B25" s="1" t="s">
-        <v>449</v>
+        <v>248</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>82</v>
+        <v>398</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="81" x14ac:dyDescent="0.15">
       <c r="B26" s="1" t="s">
-        <v>319</v>
+        <v>118</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>83</v>
+        <v>399</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
@@ -3952,108 +3952,108 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B28" s="1" t="s">
-        <v>467</v>
+        <v>266</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B29" s="1" t="s">
-        <v>320</v>
+        <v>119</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>84</v>
+        <v>400</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B30" s="1" t="s">
-        <v>321</v>
+        <v>120</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>85</v>
+        <v>401</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="B31" s="1" t="s">
-        <v>322</v>
+        <v>121</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>86</v>
+        <v>402</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B32" s="1" t="s">
-        <v>323</v>
+        <v>122</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>87</v>
+        <v>403</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B33" s="1" t="s">
-        <v>324</v>
+        <v>123</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>88</v>
+        <v>404</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B34" s="1" t="s">
-        <v>325</v>
+        <v>124</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>89</v>
+        <v>405</v>
       </c>
     </row>
     <row r="35" spans="2:4" ht="27" x14ac:dyDescent="0.15">
       <c r="B35" s="1" t="s">
-        <v>326</v>
+        <v>125</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>90</v>
+        <v>406</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="27" x14ac:dyDescent="0.15">
       <c r="B36" s="1" t="s">
-        <v>327</v>
+        <v>126</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>91</v>
+        <v>407</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="27" x14ac:dyDescent="0.15">
       <c r="B37" s="1" t="s">
-        <v>328</v>
+        <v>127</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>92</v>
+        <v>408</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.15">
@@ -4062,52 +4062,52 @@
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B39" s="1" t="s">
-        <v>468</v>
+        <v>267</v>
       </c>
       <c r="C39" s="4"/>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B40" s="1" t="s">
-        <v>286</v>
+        <v>85</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>93</v>
+        <v>409</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B41" s="1" t="s">
-        <v>329</v>
+        <v>128</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>94</v>
+        <v>410</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B42" s="1" t="s">
-        <v>330</v>
+        <v>129</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>95</v>
+        <v>411</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B43" s="1" t="s">
-        <v>331</v>
+        <v>130</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>96</v>
+        <v>412</v>
       </c>
     </row>
     <row r="44" spans="2:4" x14ac:dyDescent="0.15">
@@ -4116,74 +4116,74 @@
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B45" s="1" t="s">
-        <v>469</v>
+        <v>268</v>
       </c>
       <c r="C45" s="4"/>
     </row>
     <row r="46" spans="2:4" ht="27" x14ac:dyDescent="0.15">
       <c r="B46" s="1" t="s">
-        <v>332</v>
+        <v>131</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>97</v>
+        <v>413</v>
       </c>
     </row>
     <row r="47" spans="2:4" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B47" s="1" t="s">
-        <v>452</v>
+        <v>251</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>98</v>
+        <v>414</v>
       </c>
     </row>
     <row r="48" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B48" s="1" t="s">
-        <v>333</v>
+        <v>132</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>99</v>
+        <v>415</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B49" s="1" t="s">
-        <v>334</v>
+        <v>133</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>100</v>
+        <v>416</v>
       </c>
     </row>
     <row r="50" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B50" s="1" t="s">
-        <v>335</v>
+        <v>134</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>101</v>
+        <v>417</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B51" s="1" t="s">
-        <v>336</v>
+        <v>135</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>102</v>
+        <v>418</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.15">
@@ -4192,135 +4192,135 @@
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B53" s="1" t="s">
-        <v>337</v>
+        <v>136</v>
       </c>
       <c r="C53" s="4"/>
     </row>
     <row r="54" spans="2:4" ht="16.5" x14ac:dyDescent="0.3">
       <c r="B54" s="1" t="s">
-        <v>338</v>
+        <v>137</v>
       </c>
       <c r="C54" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>103</v>
+        <v>419</v>
       </c>
     </row>
     <row r="55" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B55" s="1" t="s">
-        <v>339</v>
+        <v>138</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>104</v>
+        <v>420</v>
       </c>
     </row>
     <row r="56" spans="2:4" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B56" s="1" t="s">
-        <v>340</v>
+        <v>139</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>105</v>
+        <v>421</v>
       </c>
     </row>
     <row r="57" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B57" s="1" t="s">
-        <v>450</v>
+        <v>249</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>106</v>
+        <v>422</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B58" s="1" t="s">
-        <v>341</v>
+        <v>140</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>107</v>
+        <v>423</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B59" s="1" t="s">
-        <v>342</v>
+        <v>141</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>108</v>
+        <v>424</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B60" s="1" t="s">
-        <v>344</v>
+        <v>143</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>109</v>
+        <v>425</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B61" s="1" t="s">
-        <v>343</v>
+        <v>142</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>110</v>
+        <v>426</v>
       </c>
     </row>
     <row r="63" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B63" t="s">
-        <v>345</v>
+        <v>144</v>
       </c>
       <c r="C63" s="4"/>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B64" s="1" t="s">
-        <v>346</v>
+        <v>145</v>
       </c>
       <c r="C64" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D64" s="3" t="s">
-        <v>111</v>
+        <v>427</v>
       </c>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B65" s="1" t="s">
-        <v>347</v>
+        <v>146</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>112</v>
+        <v>428</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B66" t="s">
-        <v>348</v>
+        <v>147</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>113</v>
+        <v>429</v>
       </c>
     </row>
   </sheetData>
@@ -4334,8 +4334,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D76"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+    <sheetView topLeftCell="B44" zoomScale="166" zoomScaleNormal="166" workbookViewId="0">
+      <selection activeCell="D52" sqref="D9:D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4351,7 +4351,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>235</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
@@ -4375,7 +4375,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>248</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.15">
@@ -4389,26 +4389,26 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>471</v>
+        <v>270</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.15">
       <c r="B8" s="2" t="s">
-        <v>250</v>
+        <v>49</v>
       </c>
       <c r="D8" s="4" t="s" ph="1">
-        <v>218</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B9" s="1" t="s">
-        <v>349</v>
+        <v>148</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>114</v>
+        <v>351</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
@@ -4416,19 +4416,19 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B11" s="1" t="s">
-        <v>383</v>
+        <v>182</v>
       </c>
       <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B12" s="1" t="s">
-        <v>350</v>
+        <v>149</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>115</v>
+        <v>352</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="27" x14ac:dyDescent="0.15">
@@ -4436,13 +4436,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>351</v>
+        <v>150</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>116</v>
+        <v>353</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
@@ -4450,13 +4450,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>352</v>
+        <v>151</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>117</v>
+        <v>354</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="27" x14ac:dyDescent="0.15">
@@ -4464,24 +4464,24 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>353</v>
+        <v>152</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>118</v>
+        <v>355</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B16" s="1" t="s">
-        <v>354</v>
+        <v>153</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>119</v>
+        <v>356</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="27" x14ac:dyDescent="0.15">
@@ -4489,13 +4489,13 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>355</v>
+        <v>154</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>120</v>
+        <v>357</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
@@ -4503,30 +4503,30 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B19" s="1" t="s">
-        <v>384</v>
+        <v>183</v>
       </c>
       <c r="C19" s="4"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B20" s="1" t="s">
-        <v>356</v>
+        <v>155</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>121</v>
+        <v>358</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B21" s="1" t="s">
-        <v>357</v>
+        <v>156</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>122</v>
+        <v>359</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
@@ -4534,7 +4534,7 @@
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B23" s="1" t="s">
-        <v>385</v>
+        <v>184</v>
       </c>
       <c r="C23" s="4"/>
     </row>
@@ -4543,13 +4543,13 @@
         <v>4</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>358</v>
+        <v>157</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D24" t="s">
-        <v>123</v>
+        <v>360</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="40.5" x14ac:dyDescent="0.15">
@@ -4557,24 +4557,24 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>359</v>
+        <v>158</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>124</v>
+        <v>361</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="B26" s="1" t="s">
-        <v>360</v>
+        <v>159</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D26" t="s">
-        <v>125</v>
+        <v>362</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.15">
@@ -4582,24 +4582,24 @@
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>361</v>
+        <v>160</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D27" t="s">
-        <v>126</v>
+        <v>363</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B28" s="1" t="s">
-        <v>354</v>
+        <v>153</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D28" t="s">
-        <v>127</v>
+        <v>364</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.15">
@@ -4607,24 +4607,24 @@
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>362</v>
+        <v>161</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D29" t="s">
-        <v>128</v>
+        <v>365</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B30" s="1" t="s">
-        <v>363</v>
+        <v>162</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D30" t="s">
-        <v>129</v>
+        <v>366</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.15">
@@ -4632,24 +4632,24 @@
         <v>4</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>364</v>
+        <v>163</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D31" t="s">
-        <v>130</v>
+        <v>367</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B32" s="1" t="s">
-        <v>365</v>
+        <v>164</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>131</v>
+        <v>368</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.15">
@@ -4657,13 +4657,13 @@
         <v>4</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>366</v>
+        <v>165</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D33" t="s">
-        <v>132</v>
+        <v>369</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="27" x14ac:dyDescent="0.15">
@@ -4671,13 +4671,13 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>367</v>
+        <v>166</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D34" t="s">
-        <v>133</v>
+        <v>370</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.15">
@@ -4685,7 +4685,7 @@
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B36" s="1" t="s">
-        <v>370</v>
+        <v>169</v>
       </c>
       <c r="C36" s="4"/>
     </row>
@@ -4694,13 +4694,13 @@
         <v>4</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>368</v>
+        <v>167</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D37" t="s">
-        <v>134</v>
+        <v>371</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="40.5" x14ac:dyDescent="0.15">
@@ -4708,24 +4708,24 @@
         <v>4</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>478</v>
+        <v>277</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D38" t="s">
-        <v>135</v>
+        <v>372</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="B39" s="1" t="s">
-        <v>369</v>
+        <v>168</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D39" t="s">
-        <v>136</v>
+        <v>373</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.15">
@@ -4733,13 +4733,13 @@
         <v>4</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>371</v>
+        <v>170</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D40" t="s">
-        <v>137</v>
+        <v>374</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.15">
@@ -4747,24 +4747,24 @@
         <v>4</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>372</v>
+        <v>171</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D41" t="s">
-        <v>138</v>
+        <v>375</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B42" s="1" t="s">
-        <v>373</v>
+        <v>172</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D42" t="s">
-        <v>139</v>
+        <v>376</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.15">
@@ -4772,24 +4772,24 @@
         <v>4</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>374</v>
+        <v>173</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D43" t="s">
-        <v>140</v>
+        <v>377</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B44" s="1" t="s">
-        <v>375</v>
+        <v>174</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D44" t="s">
-        <v>141</v>
+        <v>378</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.15">
@@ -4797,35 +4797,35 @@
         <v>4</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>376</v>
+        <v>175</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D45" t="s">
-        <v>142</v>
+        <v>379</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B46" s="2" t="s">
-        <v>377</v>
+        <v>176</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D46" t="s">
-        <v>143</v>
+        <v>380</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B47" s="2" t="s">
-        <v>378</v>
+        <v>177</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D47" t="s">
-        <v>144</v>
+        <v>381</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.15">
@@ -4833,24 +4833,24 @@
         <v>4</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>379</v>
+        <v>178</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D48" t="s">
-        <v>145</v>
+        <v>382</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B49" s="1" t="s">
-        <v>380</v>
+        <v>179</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D49" t="s">
-        <v>146</v>
+        <v>383</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.15">
@@ -4858,35 +4858,35 @@
         <v>4</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>318</v>
+        <v>117</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D50" t="s">
-        <v>147</v>
+        <v>384</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B51" s="1" t="s">
-        <v>381</v>
+        <v>180</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D51" t="s">
-        <v>148</v>
+        <v>385</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B52" s="1" t="s">
-        <v>382</v>
+        <v>181</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D52" t="s">
-        <v>149</v>
+        <v>386</v>
       </c>
     </row>
     <row r="64" spans="1:4" ht="21" x14ac:dyDescent="0.15">
@@ -4909,8 +4909,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45722500-6D63-48B1-B48D-DE8F55297416}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView topLeftCell="B4" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9:D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4926,7 +4926,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>236</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
@@ -4934,7 +4934,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>236</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
@@ -4950,7 +4950,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>247</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.15">
@@ -4961,7 +4961,7 @@
     </row>
     <row r="7" spans="1:4" ht="67.5" x14ac:dyDescent="0.15">
       <c r="B7" s="1" t="s">
-        <v>472</v>
+        <v>271</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.15">
@@ -4969,21 +4969,21 @@
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>250</v>
+        <v>49</v>
       </c>
       <c r="D8" s="4" t="s" ph="1">
-        <v>219</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B9" s="1" t="s">
-        <v>386</v>
+        <v>185</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>150</v>
+        <v>340</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
@@ -4991,13 +4991,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>387</v>
+        <v>186</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>151</v>
+        <v>341</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
@@ -5005,101 +5005,101 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>388</v>
+        <v>187</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>152</v>
+        <v>342</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="B12" s="1" t="s">
-        <v>389</v>
+        <v>188</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>153</v>
+        <v>343</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="27" x14ac:dyDescent="0.15">
       <c r="B13" s="1" t="s">
-        <v>390</v>
+        <v>189</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>154</v>
+        <v>344</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B14" s="1" t="s">
-        <v>391</v>
+        <v>190</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>155</v>
+        <v>345</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B15" s="1" t="s">
-        <v>393</v>
+        <v>192</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>156</v>
+        <v>346</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B16" s="1" t="s">
-        <v>392</v>
+        <v>191</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>157</v>
+        <v>347</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B17" s="1" t="s">
-        <v>394</v>
+        <v>193</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>158</v>
+        <v>348</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B18" s="1" t="s">
-        <v>395</v>
+        <v>194</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>159</v>
+        <v>349</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B19" s="1" t="s">
-        <v>396</v>
+        <v>195</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>160</v>
+        <v>350</v>
       </c>
     </row>
   </sheetData>
@@ -5112,8 +5112,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="B1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9:D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -5129,7 +5129,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>239</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
@@ -5137,7 +5137,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>238</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
@@ -5153,12 +5153,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>246</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B7" s="1" t="s">
-        <v>473</v>
+        <v>272</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.15">
@@ -5166,10 +5166,10 @@
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>250</v>
+        <v>49</v>
       </c>
       <c r="D8" s="4" t="s" ph="1">
-        <v>220</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
@@ -5177,13 +5177,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>308</v>
+        <v>107</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>161</v>
+        <v>325</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
@@ -5191,13 +5191,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>397</v>
+        <v>196</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>162</v>
+        <v>326</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
@@ -5205,13 +5205,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>398</v>
+        <v>197</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>163</v>
+        <v>327</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
@@ -5219,134 +5219,134 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>361</v>
+        <v>160</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>164</v>
+        <v>328</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B13" s="1" t="s">
-        <v>399</v>
+        <v>198</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>165</v>
+        <v>329</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B14" s="1" t="s">
-        <v>400</v>
+        <v>199</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>166</v>
+        <v>330</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B15" s="1" t="s">
-        <v>401</v>
+        <v>200</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>167</v>
+        <v>331</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B16" s="1" t="s">
-        <v>406</v>
+        <v>205</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>168</v>
+        <v>332</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B17" s="1" t="s">
-        <v>400</v>
+        <v>199</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>169</v>
+        <v>333</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B18" s="1" t="s">
-        <v>400</v>
+        <v>199</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>170</v>
+        <v>334</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B19" s="1" t="s">
-        <v>400</v>
+        <v>199</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>171</v>
+        <v>335</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B20" s="1" t="s">
-        <v>402</v>
+        <v>201</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>172</v>
+        <v>336</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B21" s="1" t="s">
-        <v>403</v>
+        <v>202</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>173</v>
+        <v>337</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B22" s="1" t="s">
-        <v>404</v>
+        <v>203</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>174</v>
+        <v>338</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B23" s="1" t="s">
-        <v>405</v>
+        <v>204</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>175</v>
+        <v>339</v>
       </c>
     </row>
   </sheetData>
@@ -5360,8 +5360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E8" sqref="D8:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -5374,10 +5374,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>240</v>
+        <v>39</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>241</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.15">
@@ -5385,7 +5385,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>237</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.15">
@@ -5401,7 +5401,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>245</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="21" x14ac:dyDescent="0.15">
@@ -5409,21 +5409,21 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>250</v>
+        <v>49</v>
       </c>
       <c r="D7" s="4" t="s" ph="1">
-        <v>221</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B8" s="1" t="s">
-        <v>407</v>
+        <v>206</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>176</v>
+        <v>303</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="27" x14ac:dyDescent="0.15">
@@ -5431,233 +5431,233 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>479</v>
+        <v>278</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>177</v>
+        <v>304</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B10" s="1" t="s">
-        <v>408</v>
+        <v>207</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>178</v>
+        <v>305</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B11" s="1" t="s">
-        <v>409</v>
+        <v>208</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>179</v>
+        <v>306</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B12" s="1" t="s">
-        <v>410</v>
+        <v>209</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>180</v>
+        <v>307</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B13" s="1" t="s">
-        <v>411</v>
+        <v>210</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>181</v>
+        <v>308</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B14" s="1" t="s">
-        <v>412</v>
+        <v>211</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>182</v>
+        <v>309</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B15" s="1" t="s">
-        <v>413</v>
+        <v>212</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>183</v>
+        <v>310</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="B16" s="1" t="s">
-        <v>414</v>
+        <v>213</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>184</v>
+        <v>311</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B17" s="1" t="s">
-        <v>415</v>
+        <v>214</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>185</v>
+        <v>312</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B18" s="1" t="s">
-        <v>416</v>
+        <v>215</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>186</v>
+        <v>313</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B19" s="1" t="s">
-        <v>417</v>
+        <v>216</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>187</v>
+        <v>314</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B20" s="1" t="s">
-        <v>418</v>
+        <v>217</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>188</v>
+        <v>315</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B21" s="1" t="s">
-        <v>451</v>
+        <v>250</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>189</v>
+        <v>316</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B22" s="1" t="s">
-        <v>419</v>
+        <v>218</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>190</v>
+        <v>317</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B23" s="1" t="s">
-        <v>420</v>
+        <v>219</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>191</v>
+        <v>318</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B24" s="1" t="s">
-        <v>421</v>
+        <v>220</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D24" t="s">
-        <v>192</v>
+        <v>319</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B25" s="1" t="s">
-        <v>422</v>
+        <v>221</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>193</v>
+        <v>320</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B26" s="1" t="s">
-        <v>423</v>
+        <v>222</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D26" t="s">
-        <v>194</v>
+        <v>321</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B27" s="1" t="s">
-        <v>424</v>
+        <v>223</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D27" t="s">
-        <v>195</v>
+        <v>322</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B28" s="1" t="s">
-        <v>425</v>
+        <v>224</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D28" t="s">
-        <v>196</v>
+        <v>323</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.15">
       <c r="B29" s="1" t="s">
-        <v>426</v>
+        <v>225</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D29" t="s">
-        <v>197</v>
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -5671,8 +5671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CB03C1F-8A6F-4A43-BA2E-2C62B3131330}">
   <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -5689,7 +5689,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>242</v>
+        <v>41</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -5699,7 +5699,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>242</v>
+        <v>41</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -5719,7 +5719,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>244</v>
+        <v>43</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -5739,7 +5739,7 @@
     <row r="7" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A7" s="4"/>
       <c r="B7" s="5" t="s">
-        <v>474</v>
+        <v>273</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -5747,215 +5747,215 @@
     <row r="8" spans="1:4" ht="21" x14ac:dyDescent="0.15">
       <c r="A8" s="4"/>
       <c r="B8" s="2" t="s">
-        <v>250</v>
+        <v>49</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4" t="s" ph="1">
-        <v>222</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A9" s="4"/>
       <c r="B9" s="5" t="s">
-        <v>427</v>
+        <v>226</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>198</v>
+        <v>286</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A10" s="4"/>
       <c r="B10" s="5" t="s">
-        <v>361</v>
+        <v>160</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>199</v>
+        <v>287</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A11" s="4"/>
       <c r="B11" s="5" t="s">
-        <v>392</v>
+        <v>191</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>200</v>
+        <v>288</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A12" s="4"/>
       <c r="B12" s="5" t="s">
-        <v>428</v>
+        <v>227</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>201</v>
+        <v>289</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A13" s="4"/>
       <c r="B13" s="5" t="s">
-        <v>429</v>
+        <v>228</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>202</v>
+        <v>290</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A14" s="4"/>
       <c r="B14" s="3" t="s">
-        <v>430</v>
+        <v>229</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>203</v>
+        <v>291</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A15" s="4"/>
       <c r="B15" s="5" t="s">
-        <v>431</v>
+        <v>230</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>204</v>
+        <v>292</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A16" s="4"/>
       <c r="B16" s="5" t="s">
-        <v>432</v>
+        <v>231</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>205</v>
+        <v>293</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A17" s="4"/>
       <c r="B17" s="5" t="s">
-        <v>433</v>
+        <v>232</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>206</v>
+        <v>294</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A18" s="4"/>
       <c r="B18" s="5" t="s">
-        <v>434</v>
+        <v>233</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>207</v>
+        <v>295</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A19" s="4"/>
       <c r="B19" s="5" t="s">
-        <v>435</v>
+        <v>234</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>208</v>
+        <v>296</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A20" s="4"/>
       <c r="B20" s="5" t="s">
-        <v>436</v>
+        <v>235</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>209</v>
+        <v>297</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A21" s="4"/>
       <c r="B21" s="5" t="s">
-        <v>437</v>
+        <v>236</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>210</v>
+        <v>298</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A22" s="4"/>
       <c r="B22" s="5" t="s">
-        <v>438</v>
+        <v>237</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>211</v>
+        <v>299</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A23" s="4"/>
       <c r="B23" s="5" t="s">
-        <v>439</v>
+        <v>238</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>212</v>
+        <v>300</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A24" s="4"/>
       <c r="B24" s="5" t="s">
-        <v>440</v>
+        <v>239</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>213</v>
+        <v>301</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.15">
       <c r="A25" s="4"/>
       <c r="B25" s="5" t="s">
-        <v>441</v>
+        <v>240</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>214</v>
+        <v>302</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.15">

</xml_diff>

<commit_message>
win11_en.xlsx: refer (1) (2) etc for the entries with corresponding images have such
</commit_message>
<xml_diff>
--- a/win11_en.xlsx
+++ b/win11_en.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta2025\fresta-github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B347B4-7823-404E-B5E7-BA2F2A381D93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BFE0356-28DA-44D9-BC03-B537D9FAACA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="16663" windowHeight="10457" tabRatio="729" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="17496" windowHeight="10296" tabRatio="729" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="818" uniqueCount="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="815" uniqueCount="491">
   <si>
     <t>header1</t>
   </si>
@@ -215,22 +215,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Choose preferred language.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Choose the location to specify the preferred language culture.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Connect to available network</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Check "Connect automatically" to reconnect smoothly.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Fill account &amp; password (if your network requests) and click "OK".</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -303,10 +287,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Choose "Set up as a new PC".</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Skip extra components.</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -335,61 +315,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Open "Start menu" from "田" on the taskbar (or "田" key).</t>
-    <rPh sb="24" eb="25">
-      <t>タ</t>
-    </rPh>
-    <rPh sb="47" eb="48">
-      <t>タ</t>
-    </rPh>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <r>
-      <t>Click "Settings" app from gear icon ("</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI Symbol"/>
-        <family val="2"/>
-      </rPr>
-      <t>⚙</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="ＭＳ Ｐゴシック"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>")</t>
-    </r>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Search "license" in Settings app, and proceed to "Activation settings".</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Expand "Activation state", and confirm your operating system is activated.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Click "Manage providers" in the right side menu.</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Search "virus" and proceed to "Virus &amp; threat protection".</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Search "user" and proceed to "Other users".</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Click "Add account".</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -410,14 +339,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>You can find new local account. Click "v" to expand the extra menu.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Click "Change account type".</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>You would get a window to change the account type. Click "Standard User".</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -426,22 +347,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Click "OK".</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>You would find that new local account becomes an administrator.</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Open Start menu, and click the current account icon at the lower left corner, to expand sub menu.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Expand "…" menu near of "Sign out". Confirm new local account is listed.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Click "Sign out".</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -470,22 +379,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Open "Settings" app.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Search "spec" and proceed to "Windows specifications".</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Detailed information of your hardware is displayed in previous section.</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Search "start" and proceed to "Start settings".</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>You would get a panel looking like this.</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -494,10 +391,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Search "cmd" and choose "Command Prompt".</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Proceed to "Run as administrator".</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -506,14 +399,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Open Settings app.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Search "update" and proceed to "Windows Update settings".</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>You would get the menu looking like this. Do not press "Download &amp; install all" yet.</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -547,14 +432,6 @@
   </si>
   <si>
     <t>Minimize the anti-virus software window, and click "Edge" icon (a web browser) on the desktop.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Uncheck "Bring over your data…" and click "Confirm and continue".</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Uncheck "Make your Microsoft experience…" and click "Confirm and continue"</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -695,10 +572,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>You can find "Outlook" icon in submenu.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Click "Outlook" icon.</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -719,14 +592,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Click "Install and more" at the upper right area to expand the menu.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Proceed "Install Microsoft 365 apps".</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Click "Install Office" under "Office apps &amp; devices".</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -735,10 +600,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Click "…" of the web browser to expand its menu.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Proceed to "Downloads".</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -775,22 +636,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Search "Excel" (or "Word" or "PowerPoint") from Start menu.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Choose "Run" to start it.</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>In this example, "Excel" has started.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>What a while, or click "Sign in" on the top menu, "welcome" dialogue would be shown. Click "Continue" to sign in.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Fill IMC account (starting with lowercase alphabet, followed by digits, plus "@hiroshima-u.ac.jp"), and click "Next".</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -819,18 +668,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Search "OneDrive" in Start menu, and run it.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Fill your IMC account (starting with lowercase alphabet, followed by digits, plus "@hiroshima-u.ac.jp")</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Uncheck "Allow my organization…" and click "No, this app only".</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Proceed by "Next".</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -855,18 +696,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Exclude "Pictures" and "Desktop" (include "Desktop"), then click "Start backup". If you include "Desktop", you would have serious trouble to copy the OneDrive storage to your local storage when you would graduate our university and lose the access with OneDrive.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Open Start menu</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>If no app is found, install "Microsoft Teams" app.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Start Microsoft Edge (or other web browser).</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -904,14 +737,6 @@
   </si>
   <si>
     <t>Download the installer from Microsoft.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Expand "…" menu of the web browser.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Choose "Downloads".</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1271,9 +1096,6 @@
     <t>win11-en-part7-00.02.28.109.jpg</t>
   </si>
   <si>
-    <t>win11-en-part7-00.02.30.109.jpg</t>
-  </si>
-  <si>
     <t>win11-en-part7-00.02.32.109.jpg</t>
   </si>
   <si>
@@ -1797,14 +1619,6 @@
   </si>
   <si>
     <t>FRESTA-TEXT-2025 Win11 chap.7</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Search "excel" or "word" or "powerpoint". If such Microsoft Office applications are already installed, some App would be returned. If you find them, proceed to &lt;a href="ch4.html"&gt;the next chapter&lt;/a&gt;.</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>Search "teams" in Start menu. If Microsoft Teams app is already installed, proceed to &lt;a href="ch7.html"&gt;the next chapter&lt;/a&gt;.</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1871,6 +1685,197 @@
   </si>
   <si>
     <t>If you expand your course, you would find Laptop PC Check List which ask you about the status of your PC. During this initialization or after the initialization, you should submit the check result.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Choose preferred language (1) and proceed (2).</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Choose the location (1) to specify the preferred language culture, and proceed (2).</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Check "Connect automatically" to reconnect smoothly (1), then proceed.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Connect to available network. In this example, the campus network is used, but if you are out of campus, choose appropriate network which you can use.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Choose "Set up as a new PC" (1) and proceed (2).</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Open "Start menu" from "田" on the taskbar (or "田" key) (1).</t>
+    <rPh sb="24" eb="25">
+      <t>タ</t>
+    </rPh>
+    <rPh sb="47" eb="48">
+      <t>タ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <r>
+      <t>Click "Settings" app from gear icon ("</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Symbol"/>
+        <family val="2"/>
+      </rPr>
+      <t>⚙</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="ＭＳ Ｐゴシック"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>") (2).</t>
+    </r>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Search "license" in Settings app (1), and proceed to "Activation settings" (2).</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Check the row of "Activation state" by clicking "v" (1), and confirm your operating system is activated (2).</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Search "virus" (1) and proceed to "Virus &amp; threat protection" (2).</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Search "user" (1) and proceed to "Other users" (2).</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>You can find new local account. Click "v" to expand the extra menu (1).</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Click "Change account type" at the "Account options" row.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Confirm the account type is changed to "Administrator" (1), then click "OK" (2).</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Open Start menu (1), and click the current account icon at the lower left corner (2), to expand sub menu.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Expand "…" menu near of "Sign out" (1). Confirm new local account is listed.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Open Start menu (1), and open "Settings" app (2).</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Search "start" (1), and proceed to "Start settings" (2).</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Search "spec" (1) in Setting app, and proceed to "Windows specifications" (2).</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Search "cmd" in Start menu (1), and choose "Command Prompt" (2).</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Open Start menu (1), and open Settings app (2).</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Search "update" (1), and proceed to "Windows Update settings" (2).</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Search "virus" in Setting app (1), and proceed to "Virus &amp; threat protection" (2).</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Uncheck "Bring over your data…" (1) and click "Confirm and continue" (2).</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Uncheck "Make your Microsoft experience…" (1) and click "Confirm and continue" (2)</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>In the submenu expanded by 3x3 dots menu (1), you can find "Outlook" icon (2) in submenu.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Expanding Start menu (1), search "excel" or "word" or "powerpoint" in Start menu panel (2). If such Microsoft Office applications are already installed, some App would be returned (3). If you find them, proceed to &lt;a href="ch4.html"&gt;the next chapter&lt;/a&gt;.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>You would find "Install and more" at the upper right area.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Click "Install and more" (1) and proceed "Install Microsoft 365 apps" (2).</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Click "…" of the web browser (1) to expand its submenu (2).</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>After the confirmation that the publisher of this app is Microsoft, allow "Do you want to allow this app…" by "Yes".</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Open Start menu (1), then search "Excel" (or "Word" or "PowerPoint") from Start menu. You would find the application (3). Even if your PC was sold without Microsoft Office, you ought to have installed it in &lt;a href="ch3.html"&gt;the previous chapter&lt;/a&gt;.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>In this example, when "Excel" has started, the user has not activated your Microsoft Office, or signed-in by an account with the license.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Wait a while, or click "Sign in" on the top menu, "welcome" dialogue would be shown. Click "Continue" to sign in.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>After opening Start menu (1), search "OneDrive" in Start menu (2), and open it (3).</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Uncheck "Allow my organization…" (1), and click "No, this app only" (2).</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Exclude "Pictures" and "Desktop" (1), (leave "Documents" as included), then click "Start backup" (2). If you include "Desktop", you would have serious trouble to copy the OneDrive storage to your local storage when you would graduate our university and lose the access with OneDrive.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>After opening Start menu (1), search "teams" in Start menu (2). If Microsoft Teams app is already installed and found like this, proceed to &lt;a href="ch7.html"&gt;the next chapter&lt;/a&gt;.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>If no app is found like this, install "Microsoft Teams" app as described in below.</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Expand "…" menu (1) of the web browser, proceed to "Downloads" (2).</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Uncheck "Allow my organization…" (1) and proceed by "No, this app only" (2).</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -2392,7 +2397,7 @@
     <row r="7" spans="1:4" ht="119.6" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="5" t="s">
-        <v>260</v>
+        <v>223</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -2416,7 +2421,7 @@
     <row r="10" spans="1:4" ht="19.75" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="2" t="s">
-        <v>259</v>
+        <v>222</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4" ph="1"/>
@@ -2424,85 +2429,85 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="5" t="s">
-        <v>230</v>
+        <v>193</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>262</v>
+        <v>225</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="5" t="s">
-        <v>231</v>
+        <v>194</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>263</v>
+        <v>226</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="5" t="s">
-        <v>232</v>
+        <v>195</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>264</v>
+        <v>227</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="5" t="s">
-        <v>233</v>
+        <v>196</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>265</v>
+        <v>228</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="5" t="s">
-        <v>234</v>
+        <v>197</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>266</v>
+        <v>229</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.6" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="5" t="s">
-        <v>235</v>
+        <v>198</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>267</v>
+        <v>230</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39.9" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="5" t="s">
-        <v>486</v>
+        <v>446</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>268</v>
+        <v>231</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -2513,18 +2518,18 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>240</v>
+        <v>203</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="53.15" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>487</v>
+        <v>447</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>242</v>
+        <v>205</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="3" customFormat="1" ht="12.9" customHeight="1" ph="1" x14ac:dyDescent="0.25">
@@ -2532,18 +2537,18 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>241</v>
+        <v>204</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="53.15" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>488</v>
+        <v>448</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>243</v>
+        <v>206</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
@@ -2870,8 +2875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D38"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="136" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="13.3" x14ac:dyDescent="0.25"/>
@@ -2911,7 +2916,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>470</v>
+        <v>432</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -2924,7 +2929,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>471</v>
+        <v>433</v>
       </c>
       <c r="D7" s="3" ph="1"/>
     </row>
@@ -2941,332 +2946,332 @@
         <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>46</v>
+        <v>450</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="3" t="s" ph="1">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="26.6" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>47</v>
+        <v>451</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="39.9" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
-        <v>48</v>
+        <v>453</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>441</v>
+        <v>403</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>49</v>
+        <v>452</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>442</v>
+        <v>404</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>443</v>
+        <v>405</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="2" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>444</v>
+        <v>406</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>445</v>
+        <v>407</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>446</v>
+        <v>408</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>447</v>
+        <v>409</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>448</v>
+        <v>410</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>449</v>
+        <v>411</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>450</v>
+        <v>412</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>451</v>
+        <v>413</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>452</v>
+        <v>414</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="26.6" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>453</v>
+        <v>415</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>454</v>
+        <v>416</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>455</v>
+        <v>417</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>456</v>
+        <v>418</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>457</v>
+        <v>419</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>458</v>
+        <v>420</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>459</v>
+        <v>421</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B30" s="2" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>460</v>
+        <v>422</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B31" s="2" t="s">
-        <v>68</v>
+        <v>454</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>461</v>
+        <v>423</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B32" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>462</v>
+        <v>424</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>463</v>
+        <v>425</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" s="2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>464</v>
+        <v>426</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>465</v>
+        <v>427</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>466</v>
+        <v>428</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="2" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>467</v>
+        <v>429</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" s="2" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>468</v>
+        <v>430</v>
       </c>
     </row>
   </sheetData>
@@ -3280,8 +3285,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+    <sheetView topLeftCell="A20" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="13.3" x14ac:dyDescent="0.25"/>
@@ -3326,7 +3331,7 @@
     </row>
     <row r="6" spans="1:4" ht="186" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
-        <v>261</v>
+        <v>224</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="19.75" x14ac:dyDescent="0.25">
@@ -3346,24 +3351,24 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>76</v>
+        <v>455</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>413</v>
+        <v>375</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="1" t="s">
-        <v>77</v>
+        <v>456</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>414</v>
+        <v>376</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -3371,30 +3376,30 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>244</v>
+        <v>207</v>
       </c>
       <c r="C12" s="4"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>78</v>
+        <v>457</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>415</v>
+        <v>377</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>79</v>
+        <v>458</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>416</v>
+        <v>378</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -3402,30 +3407,30 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>245</v>
+        <v>208</v>
       </c>
       <c r="C16" s="4"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>81</v>
+        <v>459</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>417</v>
+        <v>379</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>418</v>
+        <v>380</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="39.9" x14ac:dyDescent="0.25">
@@ -3433,13 +3438,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>477</v>
+        <v>437</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>419</v>
+        <v>381</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -3447,7 +3452,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>246</v>
+        <v>209</v>
       </c>
       <c r="C21" s="4"/>
     </row>
@@ -3456,13 +3461,13 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>82</v>
+        <v>460</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>420</v>
+        <v>382</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -3470,24 +3475,24 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>421</v>
+        <v>383</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>422</v>
+        <v>384</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
@@ -3495,13 +3500,13 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>423</v>
+        <v>385</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
@@ -3509,13 +3514,13 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>424</v>
+        <v>386</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
@@ -3523,13 +3528,13 @@
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>425</v>
+        <v>387</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -3537,13 +3542,13 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>88</v>
+        <v>461</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>426</v>
+        <v>388</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
@@ -3551,13 +3556,13 @@
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>89</v>
+        <v>462</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>427</v>
+        <v>389</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -3565,46 +3570,46 @@
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>428</v>
+        <v>390</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>429</v>
+        <v>391</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
-        <v>92</v>
+        <v>463</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>430</v>
+        <v>392</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>431</v>
+        <v>393</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
@@ -3612,96 +3617,96 @@
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="2" t="s">
-        <v>247</v>
+        <v>210</v>
       </c>
       <c r="C35" s="4"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>94</v>
+        <v>464</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>432</v>
+        <v>394</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>95</v>
+        <v>465</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>433</v>
+        <v>395</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
-        <v>96</v>
+        <v>80</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>434</v>
+        <v>396</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" s="1" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>435</v>
+        <v>397</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>436</v>
+        <v>398</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
-        <v>99</v>
+        <v>83</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>437</v>
+        <v>399</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
-        <v>100</v>
+        <v>84</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>438</v>
+        <v>400</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>439</v>
+        <v>401</v>
       </c>
     </row>
   </sheetData>
@@ -3715,8 +3720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D3AC582-7A6D-4EA0-8C12-75B8749BA9E2}">
   <dimension ref="A1:D67"/>
   <sheetViews>
-    <sheetView topLeftCell="A42" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3" x14ac:dyDescent="0.25"/>
@@ -3772,7 +3777,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>254</v>
+        <v>217</v>
       </c>
       <c r="D6"/>
     </row>
@@ -3789,13 +3794,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>103</v>
+        <v>466</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>370</v>
+        <v>332</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -3805,20 +3810,20 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>248</v>
+        <v>211</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>104</v>
+        <v>468</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>371</v>
+        <v>333</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="39.9" x14ac:dyDescent="0.25">
@@ -3826,24 +3831,24 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>478</v>
+        <v>438</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>372</v>
+        <v>334</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>373</v>
+        <v>335</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -3853,31 +3858,31 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>249</v>
+        <v>212</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>106</v>
+        <v>467</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>374</v>
+        <v>336</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>375</v>
+        <v>337</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="26.6" x14ac:dyDescent="0.25">
@@ -3885,13 +3890,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>108</v>
+        <v>89</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>376</v>
+        <v>338</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3901,75 +3906,75 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>250</v>
+        <v>213</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>377</v>
+        <v>339</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>109</v>
+        <v>469</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>378</v>
+        <v>340</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>110</v>
+        <v>90</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>379</v>
+        <v>341</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>111</v>
+        <v>91</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>380</v>
+        <v>342</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="26.6" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
-        <v>236</v>
+        <v>199</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>381</v>
+        <v>343</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="93" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>479</v>
+        <v>439</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>382</v>
+        <v>344</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -3979,114 +3984,114 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>251</v>
+        <v>214</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>112</v>
+        <v>470</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>383</v>
+        <v>345</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B30" s="1" t="s">
-        <v>113</v>
+        <v>471</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>384</v>
+        <v>346</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="26.6" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>114</v>
+        <v>92</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>385</v>
+        <v>347</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" s="1" t="s">
-        <v>115</v>
+        <v>93</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>386</v>
+        <v>348</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="26.6" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
-        <v>480</v>
+        <v>440</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>387</v>
+        <v>349</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="66.45" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>481</v>
+        <v>441</v>
       </c>
       <c r="C34" s="4"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
-        <v>116</v>
+        <v>94</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>388</v>
+        <v>350</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="26.6" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
-        <v>117</v>
+        <v>95</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>389</v>
+        <v>351</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="26.6" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>118</v>
+        <v>96</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>390</v>
+        <v>352</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="26.6" x14ac:dyDescent="0.25">
       <c r="B38" s="1" t="s">
-        <v>119</v>
+        <v>97</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>391</v>
+        <v>353</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
@@ -4095,52 +4100,52 @@
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
-        <v>252</v>
+        <v>215</v>
       </c>
       <c r="C40" s="4"/>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:4" ht="26.6" x14ac:dyDescent="0.25">
       <c r="B41" s="1" t="s">
-        <v>81</v>
+        <v>472</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>392</v>
+        <v>354</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B42" s="1" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>393</v>
+        <v>355</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>394</v>
+        <v>356</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="39.9" x14ac:dyDescent="0.25">
       <c r="B44" s="1" t="s">
-        <v>482</v>
+        <v>442</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>395</v>
+        <v>357</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.25">
@@ -4149,74 +4154,74 @@
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B46" s="1" t="s">
-        <v>253</v>
+        <v>216</v>
       </c>
       <c r="C46" s="4"/>
     </row>
     <row r="47" spans="2:4" ht="26.6" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>396</v>
+        <v>358</v>
       </c>
     </row>
     <row r="48" spans="2:4" ht="39.9" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
-        <v>239</v>
+        <v>202</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>397</v>
+        <v>359</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
-        <v>123</v>
+        <v>473</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>398</v>
+        <v>360</v>
       </c>
     </row>
     <row r="50" spans="2:4" ht="26.6" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
-        <v>124</v>
+        <v>474</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>399</v>
+        <v>361</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B51" s="1" t="s">
-        <v>125</v>
+        <v>101</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>400</v>
+        <v>362</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
-        <v>126</v>
+        <v>102</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>401</v>
+        <v>363</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.25">
@@ -4225,135 +4230,135 @@
     </row>
     <row r="54" spans="2:4" ht="26.6" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
-        <v>127</v>
+        <v>103</v>
       </c>
       <c r="C54" s="4"/>
     </row>
     <row r="55" spans="2:4" ht="17.149999999999999" x14ac:dyDescent="0.55000000000000004">
       <c r="B55" s="1" t="s">
-        <v>128</v>
+        <v>104</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>402</v>
+        <v>364</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B56" s="1" t="s">
-        <v>129</v>
+        <v>105</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>403</v>
+        <v>365</v>
       </c>
     </row>
     <row r="57" spans="2:4" ht="39.9" x14ac:dyDescent="0.25">
       <c r="B57" s="1" t="s">
-        <v>130</v>
+        <v>106</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>404</v>
+        <v>366</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B58" s="1" t="s">
-        <v>237</v>
+        <v>200</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>405</v>
+        <v>367</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B59" s="1" t="s">
-        <v>131</v>
+        <v>107</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>406</v>
+        <v>368</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B60" s="1" t="s">
-        <v>132</v>
+        <v>108</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>407</v>
+        <v>369</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B61" s="1" t="s">
-        <v>134</v>
+        <v>110</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>408</v>
+        <v>370</v>
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B62" s="1" t="s">
-        <v>133</v>
+        <v>109</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>409</v>
+        <v>371</v>
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B64" t="s">
-        <v>135</v>
+        <v>111</v>
       </c>
       <c r="C64" s="4"/>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B65" s="1" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>410</v>
+        <v>372</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B66" s="1" t="s">
-        <v>137</v>
+        <v>113</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>411</v>
+        <v>373</v>
       </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B67" t="s">
-        <v>138</v>
+        <v>114</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>412</v>
+        <v>374</v>
       </c>
     </row>
   </sheetData>
@@ -4367,8 +4372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D77"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A40" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="13.3" x14ac:dyDescent="0.25"/>
@@ -4408,7 +4413,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>472</v>
+        <v>434</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -4422,7 +4427,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>255</v>
+        <v>218</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="19.75" x14ac:dyDescent="0.25">
@@ -4435,13 +4440,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>139</v>
+        <v>115</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>334</v>
+        <v>296</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -4449,19 +4454,19 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>171</v>
+        <v>143</v>
       </c>
       <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>140</v>
+        <v>116</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>335</v>
+        <v>297</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.6" x14ac:dyDescent="0.25">
@@ -4469,13 +4474,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>141</v>
+        <v>117</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>336</v>
+        <v>298</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -4483,13 +4488,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>142</v>
+        <v>118</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>337</v>
+        <v>299</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.6" x14ac:dyDescent="0.25">
@@ -4497,24 +4502,24 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>143</v>
+        <v>119</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>338</v>
+        <v>300</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>339</v>
+        <v>301</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.6" x14ac:dyDescent="0.25">
@@ -4522,18 +4527,18 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>145</v>
+        <v>121</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>340</v>
+        <v>302</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="39.9" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>489</v>
+        <v>449</v>
       </c>
       <c r="C18" s="4"/>
     </row>
@@ -4542,30 +4547,30 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>172</v>
+        <v>144</v>
       </c>
       <c r="C20" s="4"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>146</v>
+        <v>122</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>341</v>
+        <v>303</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="53.15" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>483</v>
+        <v>443</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>342</v>
+        <v>304</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
@@ -4573,7 +4578,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>173</v>
+        <v>145</v>
       </c>
       <c r="C24" s="4"/>
     </row>
@@ -4582,13 +4587,13 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>147</v>
+        <v>123</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>343</v>
+        <v>305</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="39.9" x14ac:dyDescent="0.25">
@@ -4596,24 +4601,24 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>148</v>
+        <v>124</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D26" t="s">
-        <v>344</v>
+        <v>306</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.6" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>149</v>
+        <v>125</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D27" t="s">
-        <v>345</v>
+        <v>307</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -4621,24 +4626,24 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>150</v>
+        <v>126</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D28" t="s">
-        <v>346</v>
+        <v>308</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" s="1" t="s">
-        <v>144</v>
+        <v>120</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D29" t="s">
-        <v>347</v>
+        <v>309</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
@@ -4646,24 +4651,24 @@
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>151</v>
+        <v>127</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D30" t="s">
-        <v>348</v>
+        <v>310</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B31" s="1" t="s">
-        <v>152</v>
+        <v>128</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D31" t="s">
-        <v>349</v>
+        <v>311</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
@@ -4671,24 +4676,24 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>153</v>
+        <v>129</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D32" t="s">
-        <v>350</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="26.6" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
-        <v>154</v>
+        <v>475</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>351</v>
+        <v>313</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
@@ -4696,13 +4701,13 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>155</v>
+        <v>130</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D34" t="s">
-        <v>352</v>
+        <v>314</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="39.9" x14ac:dyDescent="0.25">
@@ -4710,13 +4715,13 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>484</v>
+        <v>444</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D35" t="s">
-        <v>353</v>
+        <v>315</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
@@ -4724,7 +4729,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>158</v>
+        <v>133</v>
       </c>
       <c r="C37" s="4"/>
     </row>
@@ -4733,13 +4738,13 @@
         <v>4</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>156</v>
+        <v>131</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D38" t="s">
-        <v>354</v>
+        <v>316</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="39.9" x14ac:dyDescent="0.25">
@@ -4747,24 +4752,24 @@
         <v>4</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D39" t="s">
-        <v>355</v>
+        <v>317</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="26.6" x14ac:dyDescent="0.25">
       <c r="B40" s="1" t="s">
-        <v>157</v>
+        <v>132</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D40" t="s">
-        <v>356</v>
+        <v>318</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.25">
@@ -4772,13 +4777,13 @@
         <v>4</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>159</v>
+        <v>134</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D41" t="s">
-        <v>357</v>
+        <v>319</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.25">
@@ -4786,24 +4791,24 @@
         <v>4</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>160</v>
+        <v>477</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D42" t="s">
-        <v>358</v>
+        <v>320</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B43" s="1" t="s">
-        <v>161</v>
+        <v>478</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D43" t="s">
-        <v>359</v>
+        <v>321</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
@@ -4811,24 +4816,24 @@
         <v>4</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>162</v>
+        <v>135</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D44" t="s">
-        <v>360</v>
+        <v>322</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B45" s="1" t="s">
-        <v>163</v>
+        <v>136</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D45" t="s">
-        <v>361</v>
+        <v>323</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
@@ -4836,35 +4841,35 @@
         <v>4</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>164</v>
+        <v>479</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D46" t="s">
-        <v>362</v>
+        <v>324</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B47" s="2" t="s">
-        <v>165</v>
+        <v>137</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D47" t="s">
-        <v>363</v>
+        <v>325</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B48" s="2" t="s">
-        <v>166</v>
+        <v>138</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D48" t="s">
-        <v>364</v>
+        <v>326</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -4872,60 +4877,60 @@
         <v>4</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>167</v>
+        <v>139</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D49" t="s">
-        <v>365</v>
+        <v>327</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
-        <v>168</v>
+        <v>140</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D50" t="s">
-        <v>366</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" ht="26.6" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>4</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>111</v>
+        <v>480</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D51" t="s">
-        <v>367</v>
+        <v>329</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
-        <v>169</v>
+        <v>141</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D52" t="s">
-        <v>368</v>
+        <v>330</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B53" s="1" t="s">
-        <v>170</v>
+        <v>142</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D53" t="s">
-        <v>369</v>
+        <v>331</v>
       </c>
     </row>
     <row r="65" spans="4:4" ht="19.75" x14ac:dyDescent="0.25">
@@ -4948,8 +4953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45722500-6D63-48B1-B48D-DE8F55297416}">
   <dimension ref="A1:D20"/>
   <sheetViews>
-    <sheetView topLeftCell="B11" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.3" x14ac:dyDescent="0.25"/>
@@ -5000,7 +5005,7 @@
     </row>
     <row r="7" spans="1:4" ht="79.75" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>256</v>
+        <v>219</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="19.75" x14ac:dyDescent="0.25">
@@ -5014,15 +5019,15 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="39.9" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
-        <v>174</v>
+        <v>481</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>323</v>
+        <v>285</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -5030,120 +5035,120 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>175</v>
+        <v>146</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="26.6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>176</v>
+        <v>482</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>325</v>
+        <v>287</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.6" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>177</v>
+        <v>483</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>326</v>
+        <v>288</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.6" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>178</v>
+        <v>147</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>327</v>
+        <v>289</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>179</v>
+        <v>148</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>328</v>
+        <v>290</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>181</v>
+        <v>150</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>329</v>
+        <v>291</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>180</v>
+        <v>149</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>330</v>
+        <v>292</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>182</v>
+        <v>151</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>331</v>
+        <v>293</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>183</v>
+        <v>152</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>332</v>
+        <v>294</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>184</v>
+        <v>153</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>333</v>
+        <v>295</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="39.9" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>485</v>
+        <v>445</v>
       </c>
     </row>
   </sheetData>
@@ -5157,7 +5162,7 @@
   <dimension ref="A1:D23"/>
   <sheetViews>
     <sheetView zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="13.3" x14ac:dyDescent="0.25"/>
@@ -5197,12 +5202,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>473</v>
+        <v>435</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
-        <v>257</v>
+        <v>220</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="19.75" x14ac:dyDescent="0.25">
@@ -5221,13 +5226,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>308</v>
+        <v>270</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -5235,13 +5240,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>185</v>
+        <v>484</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>309</v>
+        <v>271</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -5249,13 +5254,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>186</v>
+        <v>154</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>310</v>
+        <v>272</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -5263,134 +5268,134 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>150</v>
+        <v>126</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>311</v>
+        <v>273</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>187</v>
+        <v>485</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>312</v>
+        <v>274</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>188</v>
+        <v>155</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>313</v>
+        <v>275</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>189</v>
+        <v>156</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>314</v>
+        <v>276</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="39.9" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>194</v>
+        <v>486</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>315</v>
+        <v>277</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>188</v>
+        <v>155</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>316</v>
+        <v>278</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>188</v>
+        <v>155</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>317</v>
+        <v>279</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>188</v>
+        <v>155</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>318</v>
+        <v>280</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>190</v>
+        <v>157</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>319</v>
+        <v>281</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>191</v>
+        <v>158</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>320</v>
+        <v>282</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>192</v>
+        <v>159</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>321</v>
+        <v>283</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>193</v>
+        <v>160</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>322</v>
+        <v>284</v>
       </c>
     </row>
   </sheetData>
@@ -5402,10 +5407,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D28"/>
   <sheetViews>
-    <sheetView zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView topLeftCell="A7" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="13.3" x14ac:dyDescent="0.25"/>
@@ -5461,13 +5466,13 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
-        <v>195</v>
+        <v>161</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>286</v>
+        <v>249</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26.6" x14ac:dyDescent="0.25">
@@ -5475,233 +5480,222 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>476</v>
+        <v>487</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>287</v>
+        <v>250</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>196</v>
+        <v>488</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>288</v>
+        <v>251</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
-        <v>197</v>
+        <v>162</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>289</v>
+        <v>252</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
-        <v>198</v>
+        <v>163</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>290</v>
+        <v>253</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>199</v>
+        <v>164</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>291</v>
+        <v>254</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" s="1" t="s">
-        <v>200</v>
+        <v>165</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>292</v>
+        <v>255</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="1" t="s">
-        <v>201</v>
+        <v>166</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>293</v>
+        <v>256</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>202</v>
+        <v>167</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>294</v>
+        <v>257</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>203</v>
+        <v>168</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>295</v>
+        <v>258</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="1" t="s">
-        <v>204</v>
+        <v>169</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>296</v>
+        <v>259</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="1" t="s">
-        <v>205</v>
+        <v>170</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>297</v>
+        <v>260</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>206</v>
+        <v>171</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>298</v>
+        <v>261</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="1" t="s">
-        <v>238</v>
+        <v>201</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>299</v>
+        <v>262</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
-        <v>207</v>
+        <v>489</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>300</v>
+        <v>263</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B23" s="1" t="s">
-        <v>208</v>
+        <v>172</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>301</v>
+        <v>264</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B24" s="1" t="s">
-        <v>209</v>
+        <v>173</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D24" t="s">
-        <v>302</v>
+        <v>265</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B25" s="1" t="s">
-        <v>210</v>
+        <v>174</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>303</v>
+        <v>266</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B26" s="1" t="s">
-        <v>211</v>
+        <v>175</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D26" t="s">
-        <v>304</v>
+        <v>267</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B27" s="1" t="s">
-        <v>212</v>
+        <v>176</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D27" t="s">
-        <v>305</v>
+        <v>268</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B28" s="1" t="s">
-        <v>213</v>
+        <v>177</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D28" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" s="1" t="s">
-        <v>214</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D29" t="s">
-        <v>307</v>
+        <v>269</v>
       </c>
     </row>
   </sheetData>
@@ -5715,8 +5709,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CB03C1F-8A6F-4A43-BA2E-2C62B3131330}">
   <dimension ref="A1:D73"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.84375" defaultRowHeight="13.3" x14ac:dyDescent="0.25"/>
@@ -5763,7 +5757,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>474</v>
+        <v>436</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -5783,7 +5777,7 @@
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="4"/>
       <c r="B7" s="5" t="s">
-        <v>258</v>
+        <v>221</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -5801,205 +5795,205 @@
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="5" t="s">
-        <v>215</v>
+        <v>178</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>269</v>
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="5" t="s">
-        <v>150</v>
+        <v>126</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>270</v>
+        <v>233</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="5" t="s">
-        <v>180</v>
+        <v>490</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>271</v>
+        <v>234</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="5" t="s">
-        <v>216</v>
+        <v>179</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>272</v>
+        <v>235</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="5" t="s">
-        <v>217</v>
+        <v>180</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>273</v>
+        <v>236</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="3" t="s">
-        <v>218</v>
+        <v>181</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>274</v>
+        <v>237</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="5" t="s">
-        <v>219</v>
+        <v>182</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>275</v>
+        <v>238</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="5" t="s">
-        <v>220</v>
+        <v>183</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>276</v>
+        <v>239</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="5" t="s">
-        <v>221</v>
+        <v>184</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>277</v>
+        <v>240</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="5" t="s">
-        <v>222</v>
+        <v>185</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>278</v>
+        <v>241</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="5" t="s">
-        <v>223</v>
+        <v>186</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>279</v>
+        <v>242</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="5" t="s">
-        <v>224</v>
+        <v>187</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>280</v>
+        <v>243</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="5" t="s">
-        <v>225</v>
+        <v>188</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>281</v>
+        <v>244</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="5" t="s">
-        <v>226</v>
+        <v>189</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>282</v>
+        <v>245</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="5" t="s">
-        <v>227</v>
+        <v>190</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>283</v>
+        <v>246</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="5" t="s">
-        <v>228</v>
+        <v>191</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>284</v>
+        <v>247</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="5" t="s">
-        <v>229</v>
+        <v>192</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>285</v>
+        <v>248</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
win11_en.xlsx: update YouTube link for part9 (ch8) video, because previous video has broken frame.
</commit_message>
<xml_diff>
--- a/win11_en.xlsx
+++ b/win11_en.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta2025\fresta-github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1AA1390-E481-4E0C-B151-E96DA3F23549}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{716A07C8-E4B8-41EF-8AEF-426F1616DE03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="15576" windowHeight="11784" tabRatio="729" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -96,10 +96,6 @@
   </si>
   <si>
     <t>raw:&lt;iframe width="100%" height="315" src="https://www.youtube.com/embed/pIJzS-l5ELM?list=PLjGYIiYIuSrByd_Llk0LaHf1-ZJzhU4fQ" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen=""&gt;&lt;/iframe&gt;</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>raw:&lt;iframe width="100%" height="315" src="https://www.youtube.com/embed/SjSaCahtcbA?list=PLjGYIiYIuSrByd_Llk0LaHf1-ZJzhU4fQ" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen=""&gt;&lt;/iframe&gt;</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -1937,6 +1933,10 @@
 &lt;/ul&gt;
 If you have configured your PC with your home network, and this is the first time to connect the campus network (HU-CUP), please refer &lt;a href="ch8.html"&gt;the chapter 8&lt;/a&gt; how to connect to HU-CUP.
 </t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>raw:&lt;iframe width="100%" height="315" src="https://www.youtube.com/embed/usNVgdA1BEA?list=PLjGYIiYIuSrByd_Llk0LaHf1-ZJzhU4fQ" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen=""&gt;&lt;/iframe&gt;</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -2348,7 +2348,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="66" x14ac:dyDescent="0.2">
@@ -2408,7 +2408,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -2418,7 +2418,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -2438,7 +2438,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -2458,7 +2458,7 @@
     <row r="7" spans="1:4" ht="118.8" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="5" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -2466,11 +2466,11 @@
     <row r="8" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4" t="s" ph="1">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -2482,7 +2482,7 @@
     <row r="10" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4" ph="1"/>
@@ -2490,85 +2490,85 @@
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="5" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="5" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="5" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="5" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="5" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="5" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
@@ -2580,87 +2580,87 @@
     <row r="19" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="5" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="C19" s="4"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="5" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="5" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
       <c r="B22" s="5" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
       <c r="B23" s="5" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="C23" s="4"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
       <c r="B24" s="3" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
       <c r="B25" s="5" t="s">
-        <v>502</v>
+        <v>501</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>504</v>
+        <v>503</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
       <c r="B26" s="5" t="s">
+        <v>502</v>
+      </c>
+      <c r="C26" s="4" t="s">
         <v>503</v>
       </c>
-      <c r="C26" s="4" t="s">
-        <v>504</v>
-      </c>
       <c r="D26" s="3" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -2670,18 +2670,18 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="30" spans="1:4" s="3" customFormat="1" ht="12.9" customHeight="1" ph="1" x14ac:dyDescent="0.2">
@@ -2689,18 +2689,18 @@
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B31" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B32" s="2" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>9</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -3044,7 +3044,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3052,7 +3052,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3068,7 +3068,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -3081,13 +3081,13 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="D7" s="3" ph="1"/>
     </row>
     <row r="8" spans="1:4" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D8" s="4" t="s" ph="1">
         <v>14</v>
@@ -3098,332 +3098,332 @@
         <v>4</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="3" t="s" ph="1">
-        <v>430</v>
+        <v>429</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B10" s="2" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B11" s="2" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
     </row>
     <row r="23" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B23" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B25" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
     </row>
     <row r="29" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B29" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="30" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
     </row>
     <row r="31" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B31" s="2" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="32" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B32" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B34" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" s="2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B37" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
   </sheetData>
@@ -3454,7 +3454,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3462,7 +3462,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3478,12 +3478,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="184.8" x14ac:dyDescent="0.2">
       <c r="B6" s="1" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -3491,7 +3491,7 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7" s="4" t="s" ph="1">
         <v>15</v>
@@ -3503,24 +3503,24 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="16.8" x14ac:dyDescent="0.4">
       <c r="B10" s="1" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -3528,30 +3528,30 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C12" s="4"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -3559,30 +3559,30 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C16" s="4"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -3590,13 +3590,13 @@
         <v>4</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -3604,7 +3604,7 @@
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C21" s="4"/>
     </row>
@@ -3613,13 +3613,13 @@
         <v>4</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -3627,24 +3627,24 @@
         <v>4</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -3652,13 +3652,13 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -3666,13 +3666,13 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -3680,13 +3680,13 @@
         <v>4</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -3694,13 +3694,13 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -3708,13 +3708,13 @@
         <v>4</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -3722,46 +3722,46 @@
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
     </row>
     <row r="33" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.2">
@@ -3769,96 +3769,96 @@
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C35" s="4"/>
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="38" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
     </row>
     <row r="41" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
   </sheetData>
@@ -3889,7 +3889,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D1"/>
     </row>
@@ -3898,7 +3898,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D2"/>
     </row>
@@ -3916,7 +3916,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D4"/>
     </row>
@@ -3929,13 +3929,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D6"/>
     </row>
     <row r="7" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="B7" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7" s="4" t="s" ph="1">
         <v>16</v>
@@ -3946,13 +3946,13 @@
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -3962,20 +3962,20 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -3983,24 +3983,24 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -4010,31 +4010,31 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -4042,13 +4042,13 @@
         <v>4</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4058,75 +4058,75 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="92.4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -4136,114 +4136,114 @@
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C28" s="4"/>
       <c r="D28"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B30" s="1" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B32" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
     </row>
     <row r="33" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="34" spans="2:4" ht="66" x14ac:dyDescent="0.2">
       <c r="B34" s="1" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="C34" s="4"/>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B35" s="1" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="36" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B36" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="37" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="38" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B38" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.2">
@@ -4252,52 +4252,52 @@
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C40" s="4"/>
     </row>
     <row r="41" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B41" s="1" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
     </row>
     <row r="42" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B42" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
     </row>
     <row r="43" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
     </row>
     <row r="44" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B44" s="1" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
     </row>
     <row r="45" spans="2:4" x14ac:dyDescent="0.2">
@@ -4306,74 +4306,74 @@
     </row>
     <row r="46" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C46" s="4"/>
     </row>
     <row r="47" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B47" s="1" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="48" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B48" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="49" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B49" s="1" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="50" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B50" s="1" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="51" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B51" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="52" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B52" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D52" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="53" spans="2:4" x14ac:dyDescent="0.2">
@@ -4382,135 +4382,135 @@
     </row>
     <row r="54" spans="2:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B54" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C54" s="4"/>
     </row>
     <row r="55" spans="2:4" ht="16.8" x14ac:dyDescent="0.4">
       <c r="B55" s="1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C55" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="56" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B56" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C56" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="57" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B57" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C57" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D57" s="3" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="58" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B58" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C58" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D58" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="59" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B59" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C59" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="60" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B60" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C60" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D60" s="3" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="61" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B61" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C61" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="62" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B62" s="1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C62" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D62" s="3" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
     </row>
     <row r="64" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B64" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C64" s="4"/>
     </row>
     <row r="65" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B65" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C65" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
     </row>
     <row r="66" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B66" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
     </row>
     <row r="67" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B67" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D67" s="3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
   </sheetData>
@@ -4524,8 +4524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:D77"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -4541,7 +4541,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -4565,7 +4565,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -4579,26 +4579,26 @@
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="B8" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D8" s="4" t="s" ph="1">
-        <v>17</v>
+        <v>505</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -4606,19 +4606,19 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -4626,13 +4626,13 @@
         <v>4</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -4640,13 +4640,13 @@
         <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -4654,24 +4654,24 @@
         <v>4</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -4679,18 +4679,18 @@
         <v>4</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C18" s="4"/>
     </row>
@@ -4699,30 +4699,30 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C20" s="4"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="52.8" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -4730,7 +4730,7 @@
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C24" s="4"/>
     </row>
@@ -4739,13 +4739,13 @@
         <v>4</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -4753,24 +4753,24 @@
         <v>4</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D26" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D27" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -4778,24 +4778,24 @@
         <v>4</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D28" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D29" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -4803,24 +4803,24 @@
         <v>4</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D30" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D31" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -4828,24 +4828,24 @@
         <v>4</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D32" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B33" s="1" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -4853,13 +4853,13 @@
         <v>4</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D34" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -4867,13 +4867,13 @@
         <v>4</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D35" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -4881,7 +4881,7 @@
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C37" s="4"/>
     </row>
@@ -4890,13 +4890,13 @@
         <v>4</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D38" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -4904,24 +4904,24 @@
         <v>4</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D39" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B40" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D40" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -4929,13 +4929,13 @@
         <v>4</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D41" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -4943,24 +4943,24 @@
         <v>4</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D42" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B43" s="1" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D43" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -4968,24 +4968,24 @@
         <v>4</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D44" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B45" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D45" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -4993,35 +4993,35 @@
         <v>4</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D46" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B47" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C47" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D47" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B48" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C48" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D48" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -5029,24 +5029,24 @@
         <v>4</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C49" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D49" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B50" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D50" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -5054,35 +5054,35 @@
         <v>4</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D51" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B52" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C52" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D52" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B53" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D53" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
     </row>
     <row r="65" spans="4:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -5122,7 +5122,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5130,7 +5130,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -5146,7 +5146,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -5157,7 +5157,7 @@
     </row>
     <row r="7" spans="1:4" ht="79.2" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -5165,21 +5165,21 @@
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D8" s="4" t="s" ph="1">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -5187,13 +5187,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -5201,106 +5201,106 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="20" spans="2:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
   </sheetData>
@@ -5330,7 +5330,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5338,7 +5338,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -5354,12 +5354,12 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -5367,10 +5367,10 @@
         <v>4</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D8" s="4" t="s" ph="1">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -5378,13 +5378,13 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -5392,13 +5392,13 @@
         <v>4</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -5406,13 +5406,13 @@
         <v>4</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -5420,134 +5420,134 @@
         <v>4</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
   </sheetData>
@@ -5575,10 +5575,10 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -5586,7 +5586,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -5602,7 +5602,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -5610,21 +5610,21 @@
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D7" s="4" t="s" ph="1">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="26.4" x14ac:dyDescent="0.2">
@@ -5632,222 +5632,222 @@
         <v>4</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D14" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D15" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D17" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D18" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D19" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D20" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D21" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="22" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B22" s="1" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D22" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D23" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D24" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D25" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B26" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D26" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B27" s="1" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D27" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="28" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D28" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>
@@ -5879,7 +5879,7 @@
         <v>5</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -5889,7 +5889,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -5909,7 +5909,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
@@ -5929,7 +5929,7 @@
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
@@ -5937,215 +5937,215 @@
     <row r="8" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4" t="s" ph="1">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="5" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="5" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="5" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="5" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="5" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="5" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="5" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="5" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="5" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="5" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="5" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="5" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
       <c r="B22" s="5" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
       <c r="B23" s="5" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
       <c r="B24" s="5" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
       <c r="B25" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>9</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
bugfix for previous commit
</commit_message>
<xml_diff>
--- a/win11_en.xlsx
+++ b/win11_en.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\fresta2025\fresta-github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{716A07C8-E4B8-41EF-8AEF-426F1616DE03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B8054B4-ACEE-4626-A9EB-379AA37A49E6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="15576" windowHeight="11784" tabRatio="729" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -99,6 +99,10 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
+    <t>raw:&lt;iframe width="100%" height="315" src="https://www.youtube.com/embed/SjSaCahtcbA?list=PLjGYIiYIuSrByd_Llk0LaHf1-ZJzhU4fQ" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen=""&gt;&lt;/iframe&gt;</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
     <t>raw:&lt;iframe width="100%" height="315" src="https://www.youtube.com/embed/_nezh3_BDSA?list=PLjGYIiYIuSrByd_Llk0LaHf1-ZJzhU4fQ" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen=""&gt;&lt;/iframe&gt;</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -112,10 +116,6 @@
   </si>
   <si>
     <t>raw:&lt;iframe width="100%" height="315" src="https://www.youtube.com/embed/fyQYFEl3wKU?list=PLjGYIiYIuSrByd_Llk0LaHf1-ZJzhU4fQ" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen=""&gt;&lt;/iframe&gt;</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>raw:&lt;iframe width="100%" height="315" src="https://www.youtube.com/embed/PhOuXSnlPyA?list=PLjGYIiYIuSrByd_Llk0LaHf1-ZJzhU4fQ" title="YouTube video player" frameborder="0" allow="accelerometer; autoplay; clipboard-write; encrypted-media; gyroscope; picture-in-picture; web-share" referrerpolicy="strict-origin-when-cross-origin" allowfullscreen=""&gt;&lt;/iframe&gt;</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -2390,8 +2390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EFCA2B8-55C7-4AC3-9E13-35156DBD8BC5}">
   <dimension ref="A1:D84"/>
   <sheetViews>
-    <sheetView topLeftCell="C18" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="C4" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -2470,7 +2470,7 @@
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4" t="s" ph="1">
-        <v>21</v>
+        <v>505</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="20.399999999999999" x14ac:dyDescent="0.2">
@@ -4525,7 +4525,7 @@
   <dimension ref="A1:D77"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="13.2" x14ac:dyDescent="0.2"/>
@@ -4587,7 +4587,7 @@
         <v>44</v>
       </c>
       <c r="D8" s="4" t="s" ph="1">
-        <v>505</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -5168,7 +5168,7 @@
         <v>44</v>
       </c>
       <c r="D8" s="4" t="s" ph="1">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="39.6" x14ac:dyDescent="0.2">
@@ -5370,7 +5370,7 @@
         <v>44</v>
       </c>
       <c r="D8" s="4" t="s" ph="1">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -5613,7 +5613,7 @@
         <v>44</v>
       </c>
       <c r="D7" s="4" t="s" ph="1">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -5941,7 +5941,7 @@
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4" t="s" ph="1">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>